<commit_message>
ignoring decommissioned power plants
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1103,7 +1103,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="5" t="n">
-        <v>2024</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="2">
@@ -1189,7 +1189,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1234,24 +1234,24 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>19871400086</v>
+        <v>20132800145</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.33</v>
+        <v>0.44</v>
       </c>
       <c r="F2" t="n">
-        <v>1795</v>
+        <v>4734</v>
       </c>
       <c r="G2" t="n">
-        <v>1795</v>
+        <v>4734</v>
       </c>
     </row>
     <row r="3">
@@ -1259,24 +1259,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>19861400087</v>
+        <v>20122800156</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.33</v>
+        <v>0.44</v>
       </c>
       <c r="F3" t="n">
-        <v>2746</v>
+        <v>1597.7</v>
       </c>
       <c r="G3" t="n">
-        <v>2746</v>
+        <v>1597.7</v>
       </c>
     </row>
     <row r="4">
@@ -1284,24 +1284,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20132800145</v>
+        <v>20102900161</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F4" t="n">
-        <v>4734</v>
+        <v>2780.3</v>
       </c>
       <c r="G4" t="n">
-        <v>4734</v>
+        <v>2780.3</v>
       </c>
     </row>
     <row r="5">
@@ -1309,24 +1309,24 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20122800156</v>
+        <v>20082900162</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F5" t="n">
-        <v>1597.7</v>
+        <v>94.8</v>
       </c>
       <c r="G5" t="n">
-        <v>1597.7</v>
+        <v>94.8</v>
       </c>
     </row>
     <row r="6">
@@ -1334,7 +1334,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20102900161</v>
+        <v>20072900163</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1348,10 +1348,10 @@
         <v>0.45</v>
       </c>
       <c r="F6" t="n">
-        <v>2780.3</v>
+        <v>648</v>
       </c>
       <c r="G6" t="n">
-        <v>2780.3</v>
+        <v>648</v>
       </c>
     </row>
     <row r="7">
@@ -1359,7 +1359,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20082900162</v>
+        <v>20062900164</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1373,10 +1373,10 @@
         <v>0.45</v>
       </c>
       <c r="F7" t="n">
-        <v>94.8</v>
+        <v>628</v>
       </c>
       <c r="G7" t="n">
-        <v>94.8</v>
+        <v>628</v>
       </c>
     </row>
     <row r="8">
@@ -1384,7 +1384,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20072900163</v>
+        <v>20002900165</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>0.45</v>
       </c>
       <c r="F8" t="n">
-        <v>648</v>
+        <v>967.22</v>
       </c>
       <c r="G8" t="n">
-        <v>648</v>
+        <v>967.22</v>
       </c>
     </row>
     <row r="9">
@@ -1409,7 +1409,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20062900164</v>
+        <v>19982900166</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1423,10 +1423,10 @@
         <v>0.45</v>
       </c>
       <c r="F9" t="n">
-        <v>628</v>
+        <v>1732</v>
       </c>
       <c r="G9" t="n">
-        <v>628</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="10">
@@ -1434,24 +1434,24 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20002900165</v>
+        <v>20112800167</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="F10" t="n">
-        <v>967.22</v>
+        <v>1909</v>
       </c>
       <c r="G10" t="n">
-        <v>967.22</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="11">
@@ -1459,7 +1459,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>19982900166</v>
+        <v>19972900168</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1473,10 +1473,10 @@
         <v>0.45</v>
       </c>
       <c r="F11" t="n">
-        <v>1732</v>
+        <v>949</v>
       </c>
       <c r="G11" t="n">
-        <v>1732</v>
+        <v>949</v>
       </c>
     </row>
     <row r="12">
@@ -1484,24 +1484,24 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20112800167</v>
+        <v>19962900169</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F12" t="n">
-        <v>1909</v>
+        <v>750</v>
       </c>
       <c r="G12" t="n">
-        <v>1909</v>
+        <v>750</v>
       </c>
     </row>
     <row r="13">
@@ -1509,7 +1509,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19972900168</v>
+        <v>19952900170</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1523,10 +1523,10 @@
         <v>0.45</v>
       </c>
       <c r="F13" t="n">
-        <v>949</v>
+        <v>750</v>
       </c>
       <c r="G13" t="n">
-        <v>949</v>
+        <v>750</v>
       </c>
     </row>
     <row r="14">
@@ -1534,7 +1534,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19962900169</v>
+        <v>19942900171</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1548,10 +1548,10 @@
         <v>0.45</v>
       </c>
       <c r="F14" t="n">
-        <v>750</v>
+        <v>2780</v>
       </c>
       <c r="G14" t="n">
-        <v>750</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="15">
@@ -1559,7 +1559,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>19952900170</v>
+        <v>19922900172</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1573,10 +1573,10 @@
         <v>0.45</v>
       </c>
       <c r="F15" t="n">
-        <v>750</v>
+        <v>496</v>
       </c>
       <c r="G15" t="n">
-        <v>750</v>
+        <v>496</v>
       </c>
     </row>
     <row r="16">
@@ -1584,7 +1584,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>19942900171</v>
+        <v>19912900173</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         <v>0.45</v>
       </c>
       <c r="F16" t="n">
-        <v>2780</v>
+        <v>488.3</v>
       </c>
       <c r="G16" t="n">
-        <v>2780</v>
+        <v>488.3</v>
       </c>
     </row>
     <row r="17">
@@ -1609,7 +1609,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>19922900172</v>
+        <v>19882900174</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1623,10 +1623,10 @@
         <v>0.45</v>
       </c>
       <c r="F17" t="n">
-        <v>496</v>
+        <v>652.8</v>
       </c>
       <c r="G17" t="n">
-        <v>496</v>
+        <v>652.8</v>
       </c>
     </row>
     <row r="18">
@@ -1634,24 +1634,24 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>19912900173</v>
+        <v>20102800178</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="F18" t="n">
-        <v>488.3</v>
+        <v>433</v>
       </c>
       <c r="G18" t="n">
-        <v>488.3</v>
+        <v>433</v>
       </c>
     </row>
     <row r="19">
@@ -1659,24 +1659,24 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>19882900174</v>
+        <v>20092800189</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="F19" t="n">
-        <v>652.8</v>
+        <v>716</v>
       </c>
       <c r="G19" t="n">
-        <v>652.8</v>
+        <v>716</v>
       </c>
     </row>
     <row r="20">
@@ -1684,24 +1684,24 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>19872900175</v>
+        <v>20093000194</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="F20" t="n">
-        <v>498.5</v>
+        <v>83.8</v>
       </c>
       <c r="G20" t="n">
-        <v>498.5</v>
+        <v>83.8</v>
       </c>
     </row>
     <row r="21">
@@ -1709,24 +1709,24 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>19862900176</v>
+        <v>20063000195</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="F21" t="n">
-        <v>232.8</v>
+        <v>60</v>
       </c>
       <c r="G21" t="n">
-        <v>232.8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22">
@@ -1734,24 +1734,24 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>19852900177</v>
+        <v>20023000196</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="F22" t="n">
-        <v>465</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="G22" t="n">
-        <v>465</v>
+        <v>97.09999999999999</v>
       </c>
     </row>
     <row r="23">
@@ -1759,7 +1759,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20102800178</v>
+        <v>20082800200</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1773,10 +1773,10 @@
         <v>0.44</v>
       </c>
       <c r="F23" t="n">
-        <v>433</v>
+        <v>250</v>
       </c>
       <c r="G23" t="n">
-        <v>433</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24">
@@ -1784,7 +1784,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20092800189</v>
+        <v>20072800211</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1798,10 +1798,10 @@
         <v>0.44</v>
       </c>
       <c r="F24" t="n">
-        <v>716</v>
+        <v>1572</v>
       </c>
       <c r="G24" t="n">
-        <v>716</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="25">
@@ -1809,24 +1809,24 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20093000194</v>
+        <v>20052800213</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="F25" t="n">
-        <v>83.8</v>
+        <v>350</v>
       </c>
       <c r="G25" t="n">
-        <v>83.8</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26">
@@ -1834,24 +1834,24 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20063000195</v>
+        <v>20042800214</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="F26" t="n">
-        <v>60</v>
+        <v>336</v>
       </c>
       <c r="G26" t="n">
-        <v>60</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27">
@@ -1859,24 +1859,24 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20023000196</v>
+        <v>20032800216</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="F27" t="n">
-        <v>97.09999999999999</v>
+        <v>822</v>
       </c>
       <c r="G27" t="n">
-        <v>97.09999999999999</v>
+        <v>822</v>
       </c>
     </row>
     <row r="28">
@@ -1884,24 +1884,24 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>19963000197</v>
+        <v>20012800217</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D28" t="n">
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="F28" t="n">
-        <v>212</v>
+        <v>690</v>
       </c>
       <c r="G28" t="n">
-        <v>212</v>
+        <v>690</v>
       </c>
     </row>
     <row r="29">
@@ -1909,24 +1909,24 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>19953000198</v>
+        <v>19982800218</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="F29" t="n">
-        <v>97.3</v>
+        <v>123</v>
       </c>
       <c r="G29" t="n">
-        <v>97.3</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30">
@@ -1934,7 +1934,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>20082800200</v>
+        <v>19922800219</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1948,10 +1948,10 @@
         <v>0.44</v>
       </c>
       <c r="F30" t="n">
-        <v>250</v>
+        <v>1127.4</v>
       </c>
       <c r="G30" t="n">
-        <v>250</v>
+        <v>1127.4</v>
       </c>
     </row>
     <row r="31">
@@ -1959,7 +1959,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>20072800211</v>
+        <v>19912800220</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1973,10 +1973,10 @@
         <v>0.44</v>
       </c>
       <c r="F31" t="n">
-        <v>1572</v>
+        <v>889</v>
       </c>
       <c r="G31" t="n">
-        <v>1572</v>
+        <v>889</v>
       </c>
     </row>
     <row r="32">
@@ -1984,7 +1984,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>20052800213</v>
+        <v>19902800221</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1998,10 +1998,10 @@
         <v>0.44</v>
       </c>
       <c r="F32" t="n">
-        <v>350</v>
+        <v>561.7</v>
       </c>
       <c r="G32" t="n">
-        <v>350</v>
+        <v>561.7</v>
       </c>
     </row>
     <row r="33">
@@ -2009,7 +2009,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>20042800214</v>
+        <v>19892800222</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -2023,10 +2023,10 @@
         <v>0.44</v>
       </c>
       <c r="F33" t="n">
-        <v>336</v>
+        <v>332.7</v>
       </c>
       <c r="G33" t="n">
-        <v>336</v>
+        <v>332.7</v>
       </c>
     </row>
     <row r="34">
@@ -2034,7 +2034,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>20032800216</v>
+        <v>19882800223</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -2048,10 +2048,10 @@
         <v>0.44</v>
       </c>
       <c r="F34" t="n">
-        <v>822</v>
+        <v>169.9</v>
       </c>
       <c r="G34" t="n">
-        <v>822</v>
+        <v>169.9</v>
       </c>
     </row>
     <row r="35">
@@ -2059,24 +2059,24 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>20012800217</v>
+        <v>20180300241</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E35" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F35" t="n">
-        <v>690</v>
+        <v>140.5</v>
       </c>
       <c r="G35" t="n">
-        <v>690</v>
+        <v>140.5</v>
       </c>
     </row>
     <row r="36">
@@ -2084,24 +2084,24 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>19982800218</v>
+        <v>20140300242</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E36" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F36" t="n">
-        <v>123</v>
+        <v>1117.5</v>
       </c>
       <c r="G36" t="n">
-        <v>123</v>
+        <v>1117.5</v>
       </c>
     </row>
     <row r="37">
@@ -2109,24 +2109,24 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>19922800219</v>
+        <v>20130300243</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E37" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F37" t="n">
-        <v>1127.4</v>
+        <v>296.3</v>
       </c>
       <c r="G37" t="n">
-        <v>1127.4</v>
+        <v>296.3</v>
       </c>
     </row>
     <row r="38">
@@ -2134,24 +2134,24 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>19912800220</v>
+        <v>20110300244</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E38" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F38" t="n">
-        <v>889</v>
+        <v>2110.5</v>
       </c>
       <c r="G38" t="n">
-        <v>889</v>
+        <v>2110.5</v>
       </c>
     </row>
     <row r="39">
@@ -2159,24 +2159,24 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>19902800221</v>
+        <v>20100300245</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E39" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F39" t="n">
-        <v>561.7</v>
+        <v>3470</v>
       </c>
       <c r="G39" t="n">
-        <v>561.7</v>
+        <v>3470</v>
       </c>
     </row>
     <row r="40">
@@ -2184,24 +2184,24 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>19892800222</v>
+        <v>20090300246</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E40" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F40" t="n">
-        <v>332.7</v>
+        <v>639</v>
       </c>
       <c r="G40" t="n">
-        <v>332.7</v>
+        <v>639</v>
       </c>
     </row>
     <row r="41">
@@ -2209,24 +2209,24 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>19882800223</v>
+        <v>20080300247</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E41" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F41" t="n">
-        <v>169.9</v>
+        <v>4269.5</v>
       </c>
       <c r="G41" t="n">
-        <v>169.9</v>
+        <v>4269.5</v>
       </c>
     </row>
     <row r="42">
@@ -2234,24 +2234,24 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>19872800224</v>
+        <v>20070300249</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E42" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F42" t="n">
-        <v>762.5</v>
+        <v>196</v>
       </c>
       <c r="G42" t="n">
-        <v>762.5</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43">
@@ -2259,24 +2259,24 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>19862800225</v>
+        <v>20060300250</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E43" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F43" t="n">
-        <v>713.5</v>
+        <v>1569</v>
       </c>
       <c r="G43" t="n">
-        <v>713.5</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="44">
@@ -2284,24 +2284,24 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>19852800227</v>
+        <v>20050300251</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E44" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F44" t="n">
-        <v>1157</v>
+        <v>1517</v>
       </c>
       <c r="G44" t="n">
-        <v>1157</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="45">
@@ -2309,7 +2309,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20180300241</v>
+        <v>20030300252</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -2323,10 +2323,10 @@
         <v>0.61</v>
       </c>
       <c r="F45" t="n">
-        <v>140.5</v>
+        <v>1207.759</v>
       </c>
       <c r="G45" t="n">
-        <v>140.5</v>
+        <v>1207.759</v>
       </c>
     </row>
     <row r="46">
@@ -2334,7 +2334,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20140300242</v>
+        <v>20171700278</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2342,16 +2342,16 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E46" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F46" t="n">
-        <v>1117.5</v>
+        <v>535.2</v>
       </c>
       <c r="G46" t="n">
-        <v>1117.5</v>
+        <v>535.2</v>
       </c>
     </row>
     <row r="47">
@@ -2359,7 +2359,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20130300243</v>
+        <v>20161700279</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2367,16 +2367,16 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E47" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F47" t="n">
-        <v>296.3</v>
+        <v>167.451</v>
       </c>
       <c r="G47" t="n">
-        <v>296.3</v>
+        <v>167.451</v>
       </c>
     </row>
     <row r="48">
@@ -2384,7 +2384,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>20110300244</v>
+        <v>20151700280</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -2392,16 +2392,16 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E48" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F48" t="n">
-        <v>2110.5</v>
+        <v>220.2</v>
       </c>
       <c r="G48" t="n">
-        <v>2110.5</v>
+        <v>220.2</v>
       </c>
     </row>
     <row r="49">
@@ -2409,7 +2409,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>20100300245</v>
+        <v>20141700282</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2417,16 +2417,16 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E49" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F49" t="n">
-        <v>3470</v>
+        <v>574.3099999999999</v>
       </c>
       <c r="G49" t="n">
-        <v>3470</v>
+        <v>574.3099999999999</v>
       </c>
     </row>
     <row r="50">
@@ -2434,7 +2434,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20090300246</v>
+        <v>20121700283</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2442,16 +2442,16 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E50" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F50" t="n">
-        <v>639</v>
+        <v>141.6</v>
       </c>
       <c r="G50" t="n">
-        <v>639</v>
+        <v>141.6</v>
       </c>
     </row>
     <row r="51">
@@ -2459,7 +2459,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>20080300247</v>
+        <v>20111700284</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -2467,16 +2467,16 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E51" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F51" t="n">
-        <v>4269.5</v>
+        <v>454.24</v>
       </c>
       <c r="G51" t="n">
-        <v>4269.5</v>
+        <v>454.24</v>
       </c>
     </row>
     <row r="52">
@@ -2484,7 +2484,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>20070300249</v>
+        <v>20101700285</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -2492,16 +2492,16 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E52" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F52" t="n">
-        <v>196</v>
+        <v>275.78</v>
       </c>
       <c r="G52" t="n">
-        <v>196</v>
+        <v>275.78</v>
       </c>
     </row>
     <row r="53">
@@ -2509,7 +2509,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>20060300250</v>
+        <v>20051700286</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -2517,16 +2517,16 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E53" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F53" t="n">
-        <v>1569</v>
+        <v>158</v>
       </c>
       <c r="G53" t="n">
-        <v>1569</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54">
@@ -2534,7 +2534,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>20050300251</v>
+        <v>20041700287</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -2542,16 +2542,16 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E54" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F54" t="n">
-        <v>1517</v>
+        <v>746.015</v>
       </c>
       <c r="G54" t="n">
-        <v>1517</v>
+        <v>746.015</v>
       </c>
     </row>
     <row r="55">
@@ -2559,7 +2559,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>20030300252</v>
+        <v>20031700288</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -2567,391 +2567,16 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E55" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F55" t="n">
-        <v>1207.759</v>
+        <v>163.9</v>
       </c>
       <c r="G55" t="n">
-        <v>1207.759</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="5" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="n">
-        <v>20020300253</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D56" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E56" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="F56" t="n">
-        <v>1375.4</v>
-      </c>
-      <c r="G56" t="n">
-        <v>1375.4</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="n">
-        <v>20010300254</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D57" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E57" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="F57" t="n">
-        <v>245.46</v>
-      </c>
-      <c r="G57" t="n">
-        <v>245.46</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="5" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="n">
-        <v>20171700278</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D58" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F58" t="n">
-        <v>535.2</v>
-      </c>
-      <c r="G58" t="n">
-        <v>535.2</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="5" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="n">
-        <v>20161700279</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D59" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F59" t="n">
-        <v>167.451</v>
-      </c>
-      <c r="G59" t="n">
-        <v>167.451</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="5" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="n">
-        <v>20151700280</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D60" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E60" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F60" t="n">
-        <v>220.2</v>
-      </c>
-      <c r="G60" t="n">
-        <v>220.2</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="5" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="n">
-        <v>20141700282</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D61" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E61" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F61" t="n">
-        <v>574.3099999999999</v>
-      </c>
-      <c r="G61" t="n">
-        <v>574.3099999999999</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="5" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="n">
-        <v>20121700283</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D62" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E62" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F62" t="n">
-        <v>141.6</v>
-      </c>
-      <c r="G62" t="n">
-        <v>141.6</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="5" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="n">
-        <v>20111700284</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D63" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E63" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F63" t="n">
-        <v>454.24</v>
-      </c>
-      <c r="G63" t="n">
-        <v>454.24</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="5" t="n">
-        <v>62</v>
-      </c>
-      <c r="B64" t="n">
-        <v>20101700285</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D64" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E64" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F64" t="n">
-        <v>275.78</v>
-      </c>
-      <c r="G64" t="n">
-        <v>275.78</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="5" t="n">
-        <v>63</v>
-      </c>
-      <c r="B65" t="n">
-        <v>20051700286</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D65" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E65" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F65" t="n">
-        <v>158</v>
-      </c>
-      <c r="G65" t="n">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="5" t="n">
-        <v>64</v>
-      </c>
-      <c r="B66" t="n">
-        <v>20041700287</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D66" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E66" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F66" t="n">
-        <v>746.015</v>
-      </c>
-      <c r="G66" t="n">
-        <v>746.015</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="5" t="n">
-        <v>65</v>
-      </c>
-      <c r="B67" t="n">
-        <v>20031700288</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D67" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E67" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F67" t="n">
         <v>163.9</v>
-      </c>
-      <c r="G67" t="n">
-        <v>163.9</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="5" t="n">
-        <v>66</v>
-      </c>
-      <c r="B68" t="n">
-        <v>20021700289</v>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D68" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E68" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F68" t="n">
-        <v>126.7</v>
-      </c>
-      <c r="G68" t="n">
-        <v>126.7</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="5" t="n">
-        <v>67</v>
-      </c>
-      <c r="B69" t="n">
-        <v>20011700290</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D69" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E69" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F69" t="n">
-        <v>110.55</v>
-      </c>
-      <c r="G69" t="n">
-        <v>110.55</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="5" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="n">
-        <v>20001700291</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D70" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E70" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F70" t="n">
-        <v>124.5</v>
-      </c>
-      <c r="G70" t="n">
-        <v>124.5</v>
       </c>
     </row>
   </sheetData>
@@ -2965,7 +2590,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3449,17 +3074,17 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19771200058</v>
+        <v>20202400092</v>
       </c>
       <c r="C13" t="n">
-        <v>1057.4</v>
+        <v>400</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Undefined</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -3488,17 +3113,17 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19761200059</v>
+        <v>20192400093</v>
       </c>
       <c r="C14" t="n">
-        <v>179.4</v>
+        <v>554.6</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Undefined</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -3527,10 +3152,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20202400092</v>
+        <v>20182400094</v>
       </c>
       <c r="C15" t="n">
-        <v>400</v>
+        <v>577</v>
       </c>
       <c r="D15" t="n">
         <v>1.35</v>
@@ -3566,10 +3191,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20192400093</v>
+        <v>20172400095</v>
       </c>
       <c r="C16" t="n">
-        <v>554.6</v>
+        <v>888.5916000000008</v>
       </c>
       <c r="D16" t="n">
         <v>1.35</v>
@@ -3605,10 +3230,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20182400094</v>
+        <v>20162400096</v>
       </c>
       <c r="C17" t="n">
-        <v>577</v>
+        <v>4593.90489999998</v>
       </c>
       <c r="D17" t="n">
         <v>1.35</v>
@@ -3644,10 +3269,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20172400095</v>
+        <v>20152400097</v>
       </c>
       <c r="C18" t="n">
-        <v>888.5916000000008</v>
+        <v>5251.351200000026</v>
       </c>
       <c r="D18" t="n">
         <v>1.35</v>
@@ -3683,10 +3308,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20162400096</v>
+        <v>20142400098</v>
       </c>
       <c r="C19" t="n">
-        <v>4593.90489999998</v>
+        <v>3907.871117000042</v>
       </c>
       <c r="D19" t="n">
         <v>1.35</v>
@@ -3722,10 +3347,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20152400097</v>
+        <v>20132400099</v>
       </c>
       <c r="C20" t="n">
-        <v>5251.351200000026</v>
+        <v>3468.728360000041</v>
       </c>
       <c r="D20" t="n">
         <v>1.35</v>
@@ -3761,10 +3386,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20142400098</v>
+        <v>20122400101</v>
       </c>
       <c r="C21" t="n">
-        <v>3907.871117000042</v>
+        <v>3969.104243000032</v>
       </c>
       <c r="D21" t="n">
         <v>1.35</v>
@@ -3800,10 +3425,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20132400099</v>
+        <v>20112400102</v>
       </c>
       <c r="C22" t="n">
-        <v>3468.728360000041</v>
+        <v>2785.43162000001</v>
       </c>
       <c r="D22" t="n">
         <v>1.35</v>
@@ -3839,10 +3464,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20122400101</v>
+        <v>20102400103</v>
       </c>
       <c r="C23" t="n">
-        <v>3969.104243000032</v>
+        <v>2104.219086999985</v>
       </c>
       <c r="D23" t="n">
         <v>1.35</v>
@@ -3878,10 +3503,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20112400102</v>
+        <v>20092400104</v>
       </c>
       <c r="C24" t="n">
-        <v>2785.43162000001</v>
+        <v>1734.347213999992</v>
       </c>
       <c r="D24" t="n">
         <v>1.35</v>
@@ -3917,10 +3542,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20102400103</v>
+        <v>20082400105</v>
       </c>
       <c r="C25" t="n">
-        <v>2104.219086999985</v>
+        <v>1087.143895999995</v>
       </c>
       <c r="D25" t="n">
         <v>1.35</v>
@@ -3956,10 +3581,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20092400104</v>
+        <v>20072400106</v>
       </c>
       <c r="C26" t="n">
-        <v>1734.347213999992</v>
+        <v>2049.836699999993</v>
       </c>
       <c r="D26" t="n">
         <v>1.35</v>
@@ -3995,10 +3620,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20082400105</v>
+        <v>20062400107</v>
       </c>
       <c r="C27" t="n">
-        <v>1087.143895999995</v>
+        <v>751.4120000000005</v>
       </c>
       <c r="D27" t="n">
         <v>1.35</v>
@@ -4034,10 +3659,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20072400106</v>
+        <v>20052400108</v>
       </c>
       <c r="C28" t="n">
-        <v>2049.836699999993</v>
+        <v>1340.202199999995</v>
       </c>
       <c r="D28" t="n">
         <v>1.35</v>
@@ -4073,10 +3698,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>20062400107</v>
+        <v>20042400109</v>
       </c>
       <c r="C29" t="n">
-        <v>751.4120000000005</v>
+        <v>1659.914999999992</v>
       </c>
       <c r="D29" t="n">
         <v>1.35</v>
@@ -4112,10 +3737,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>20052400108</v>
+        <v>20032400110</v>
       </c>
       <c r="C30" t="n">
-        <v>1340.202199999995</v>
+        <v>1287.459599999997</v>
       </c>
       <c r="D30" t="n">
         <v>1.35</v>
@@ -4151,10 +3776,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>20042400109</v>
+        <v>20022400112</v>
       </c>
       <c r="C31" t="n">
-        <v>1659.914999999992</v>
+        <v>1434.670999999991</v>
       </c>
       <c r="D31" t="n">
         <v>1.35</v>
@@ -4190,10 +3815,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>20032400110</v>
+        <v>20012400113</v>
       </c>
       <c r="C32" t="n">
-        <v>1287.459599999997</v>
+        <v>1773.431999999988</v>
       </c>
       <c r="D32" t="n">
         <v>1.35</v>
@@ -4229,10 +3854,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>20022400112</v>
+        <v>20002400114</v>
       </c>
       <c r="C33" t="n">
-        <v>1434.670999999991</v>
+        <v>1975.231089999979</v>
       </c>
       <c r="D33" t="n">
         <v>1.35</v>
@@ -4268,10 +3893,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>20012400113</v>
+        <v>19992400115</v>
       </c>
       <c r="C34" t="n">
-        <v>1773.431999999988</v>
+        <v>1648.599299999983</v>
       </c>
       <c r="D34" t="n">
         <v>1.35</v>
@@ -4307,10 +3932,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>20002400114</v>
+        <v>19982400116</v>
       </c>
       <c r="C35" t="n">
-        <v>1975.231089999979</v>
+        <v>853.3870000000011</v>
       </c>
       <c r="D35" t="n">
         <v>1.35</v>
@@ -4346,17 +3971,17 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>19992400115</v>
+        <v>20192300124</v>
       </c>
       <c r="C36" t="n">
-        <v>1648.599299999983</v>
+        <v>1130.5</v>
       </c>
       <c r="D36" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -4385,17 +4010,17 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>19982400116</v>
+        <v>20182300125</v>
       </c>
       <c r="C37" t="n">
-        <v>853.3870000000011</v>
+        <v>952</v>
       </c>
       <c r="D37" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4424,17 +4049,17 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>19972400117</v>
+        <v>20172300126</v>
       </c>
       <c r="C38" t="n">
-        <v>564.2280000000012</v>
+        <v>1455</v>
       </c>
       <c r="D38" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4463,17 +4088,17 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>19962400118</v>
+        <v>20162300127</v>
       </c>
       <c r="C39" t="n">
-        <v>251.9353999999998</v>
+        <v>735</v>
       </c>
       <c r="D39" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4502,17 +4127,17 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>19952400119</v>
+        <v>20152300128</v>
       </c>
       <c r="C40" t="n">
-        <v>170.8699999999997</v>
+        <v>1622</v>
       </c>
       <c r="D40" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4541,10 +4166,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>20192300124</v>
+        <v>20142300129</v>
       </c>
       <c r="C41" t="n">
-        <v>1130.5</v>
+        <v>726</v>
       </c>
       <c r="D41" t="n">
         <v>2.7</v>
@@ -4580,10 +4205,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20182300125</v>
+        <v>20132300130</v>
       </c>
       <c r="C42" t="n">
-        <v>952</v>
+        <v>2502</v>
       </c>
       <c r="D42" t="n">
         <v>2.7</v>
@@ -4619,10 +4244,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20172300126</v>
+        <v>20122300131</v>
       </c>
       <c r="C43" t="n">
-        <v>1455</v>
+        <v>401</v>
       </c>
       <c r="D43" t="n">
         <v>2.7</v>
@@ -4658,10 +4283,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>20162300127</v>
+        <v>20112300132</v>
       </c>
       <c r="C44" t="n">
-        <v>735</v>
+        <v>400</v>
       </c>
       <c r="D44" t="n">
         <v>2.7</v>
@@ -4697,10 +4322,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20152300128</v>
+        <v>20082300135</v>
       </c>
       <c r="C45" t="n">
-        <v>1622</v>
+        <v>108.3</v>
       </c>
       <c r="D45" t="n">
         <v>2.7</v>
@@ -4736,10 +4361,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20142300129</v>
+        <v>20062300136</v>
       </c>
       <c r="C46" t="n">
-        <v>726</v>
+        <v>240</v>
       </c>
       <c r="D46" t="n">
         <v>2.7</v>
@@ -4775,17 +4400,15 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20132300130</v>
+        <v>20202100137</v>
       </c>
       <c r="C47" t="n">
-        <v>2502</v>
-      </c>
-      <c r="D47" t="n">
-        <v>2.7</v>
-      </c>
+        <v>251.8</v>
+      </c>
+      <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -4814,17 +4437,17 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>20122300131</v>
+        <v>20271200291</v>
       </c>
       <c r="C48" t="n">
-        <v>401</v>
+        <v>100</v>
       </c>
       <c r="D48" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>Undefined</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4853,17 +4476,15 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>20112300132</v>
+        <v>20192100138</v>
       </c>
       <c r="C49" t="n">
-        <v>400</v>
-      </c>
-      <c r="D49" t="n">
-        <v>2.7</v>
-      </c>
+        <v>195.4</v>
+      </c>
+      <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4892,17 +4513,15 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20082300135</v>
+        <v>20182100139</v>
       </c>
       <c r="C50" t="n">
-        <v>108.3</v>
-      </c>
-      <c r="D50" t="n">
-        <v>2.7</v>
-      </c>
+        <v>414.723</v>
+      </c>
+      <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4931,17 +4550,15 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>20062300136</v>
+        <v>20172100140</v>
       </c>
       <c r="C51" t="n">
-        <v>240</v>
-      </c>
-      <c r="D51" t="n">
-        <v>2.7</v>
-      </c>
+        <v>3311.82512350009</v>
+      </c>
+      <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4970,10 +4587,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>20202100137</v>
+        <v>20162100141</v>
       </c>
       <c r="C52" t="n">
-        <v>251.8</v>
+        <v>6222.270852000401</v>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
@@ -5007,10 +4624,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>20192100138</v>
+        <v>20152100142</v>
       </c>
       <c r="C53" t="n">
-        <v>195.4</v>
+        <v>1688.32281700176</v>
       </c>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
@@ -5044,10 +4661,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>20182100139</v>
+        <v>20142100143</v>
       </c>
       <c r="C54" t="n">
-        <v>414.723</v>
+        <v>1467.604103002783</v>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
@@ -5081,10 +4698,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>20172100140</v>
+        <v>20132100144</v>
       </c>
       <c r="C55" t="n">
-        <v>3311.82512350009</v>
+        <v>1387.194197003628</v>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
@@ -5118,10 +4735,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>20162100141</v>
+        <v>20122100146</v>
       </c>
       <c r="C56" t="n">
-        <v>6222.270852000401</v>
+        <v>1732.597611001665</v>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
@@ -5155,10 +4772,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>20152100142</v>
+        <v>20112100147</v>
       </c>
       <c r="C57" t="n">
-        <v>1688.32281700176</v>
+        <v>3084.73933250188</v>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
@@ -5192,10 +4809,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>20142100143</v>
+        <v>20102100148</v>
       </c>
       <c r="C58" t="n">
-        <v>1467.604103002783</v>
+        <v>6784.098386973769</v>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
@@ -5229,10 +4846,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>20132100144</v>
+        <v>20092100149</v>
       </c>
       <c r="C59" t="n">
-        <v>1387.194197003628</v>
+        <v>9295.344562513454</v>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
@@ -5266,10 +4883,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>20122100146</v>
+        <v>20082100150</v>
       </c>
       <c r="C60" t="n">
-        <v>1732.597611001665</v>
+        <v>7475.485288501332</v>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
@@ -5303,10 +4920,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>20112100147</v>
+        <v>20072100151</v>
       </c>
       <c r="C61" t="n">
-        <v>3084.73933250188</v>
+        <v>4341.280789791133</v>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
@@ -5340,10 +4957,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>20102100148</v>
+        <v>20062100152</v>
       </c>
       <c r="C62" t="n">
-        <v>6784.098386973769</v>
+        <v>1924.091949500588</v>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
@@ -5377,10 +4994,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>20092100149</v>
+        <v>20052100153</v>
       </c>
       <c r="C63" t="n">
-        <v>9295.344562513454</v>
+        <v>1221.046400499492</v>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
@@ -5414,10 +5031,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>20082100150</v>
+        <v>20042100154</v>
       </c>
       <c r="C64" t="n">
-        <v>7475.485288501332</v>
+        <v>829.7290730002117</v>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
@@ -5451,10 +5068,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>20072100151</v>
+        <v>20032100155</v>
       </c>
       <c r="C65" t="n">
-        <v>4341.280789791133</v>
+        <v>907.4490049999474</v>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
@@ -5488,10 +5105,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>20062100152</v>
+        <v>20022100157</v>
       </c>
       <c r="C66" t="n">
-        <v>1924.091949500588</v>
+        <v>633.0435090000258</v>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
@@ -5525,10 +5142,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>20052100153</v>
+        <v>20012100158</v>
       </c>
       <c r="C67" t="n">
-        <v>1221.046400499492</v>
+        <v>122.1209029997136</v>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
@@ -5562,10 +5179,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>20042100154</v>
+        <v>20002100159</v>
       </c>
       <c r="C68" t="n">
-        <v>829.7290730002117</v>
+        <v>93.42517899995289</v>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
@@ -5599,10 +5216,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>20032100155</v>
+        <v>19992100160</v>
       </c>
       <c r="C69" t="n">
-        <v>907.4490049999474</v>
+        <v>171.9239930052555</v>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr">
@@ -5626,154 +5243,6 @@
         </is>
       </c>
       <c r="I69" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="5" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="n">
-        <v>20022100157</v>
-      </c>
-      <c r="C70" t="n">
-        <v>633.0435090000258</v>
-      </c>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="5" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" t="n">
-        <v>20012100158</v>
-      </c>
-      <c r="C71" t="n">
-        <v>122.1209029997136</v>
-      </c>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="5" t="n">
-        <v>70</v>
-      </c>
-      <c r="B72" t="n">
-        <v>20002100159</v>
-      </c>
-      <c r="C72" t="n">
-        <v>93.42517899995289</v>
-      </c>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="5" t="n">
-        <v>71</v>
-      </c>
-      <c r="B73" t="n">
-        <v>19992100160</v>
-      </c>
-      <c r="C73" t="n">
-        <v>171.9239930052555</v>
-      </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I73" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -5864,7 +5333,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6036,10 +5505,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20020100023</v>
+        <v>20120100133</v>
       </c>
       <c r="C5" t="n">
-        <v>256</v>
+        <v>89.8</v>
       </c>
       <c r="D5" t="n">
         <v>1.9</v>
@@ -6075,10 +5544,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20010100034</v>
+        <v>20100100215</v>
       </c>
       <c r="C6" t="n">
-        <v>169.3934</v>
+        <v>89.05</v>
       </c>
       <c r="D6" t="n">
         <v>1.9</v>
@@ -6114,10 +5583,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20000100045</v>
+        <v>20080100226</v>
       </c>
       <c r="C7" t="n">
-        <v>81.2</v>
+        <v>127.8</v>
       </c>
       <c r="D7" t="n">
         <v>1.9</v>
@@ -6153,10 +5622,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20120100133</v>
+        <v>20070100237</v>
       </c>
       <c r="C8" t="n">
-        <v>89.8</v>
+        <v>217.8</v>
       </c>
       <c r="D8" t="n">
         <v>1.9</v>
@@ -6192,10 +5661,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20100100215</v>
+        <v>20060100248</v>
       </c>
       <c r="C9" t="n">
-        <v>89.05</v>
+        <v>91.5</v>
       </c>
       <c r="D9" t="n">
         <v>1.9</v>
@@ -6231,10 +5700,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20080100226</v>
+        <v>20050100259</v>
       </c>
       <c r="C10" t="n">
-        <v>127.8</v>
+        <v>66.78</v>
       </c>
       <c r="D10" t="n">
         <v>1.9</v>
@@ -6270,10 +5739,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20070100237</v>
+        <v>20040100270</v>
       </c>
       <c r="C11" t="n">
-        <v>217.8</v>
+        <v>166.92</v>
       </c>
       <c r="D11" t="n">
         <v>1.9</v>
@@ -6309,10 +5778,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20060100248</v>
+        <v>20030100281</v>
       </c>
       <c r="C12" t="n">
-        <v>91.5</v>
+        <v>206.65</v>
       </c>
       <c r="D12" t="n">
         <v>1.9</v>
@@ -6338,123 +5807,6 @@
         </is>
       </c>
       <c r="I12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>20050100259</v>
-      </c>
-      <c r="C13" t="n">
-        <v>66.78</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>20040100270</v>
-      </c>
-      <c r="C14" t="n">
-        <v>166.92</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>20030100281</v>
-      </c>
-      <c r="C15" t="n">
-        <v>206.65</v>
-      </c>
-      <c r="D15" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -6491,7 +5843,7 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>45291.99861111111</v>
+        <v>46387.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -6501,7 +5853,7 @@
         </is>
       </c>
       <c r="B3" s="7" t="n">
-        <v>45656.99861111111</v>
+        <v>46751.99861111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
git commit -m "Untrack files in .gitignore"
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -5255,7 +5255,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I178"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8001,10 +8001,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>20240102436</v>
+        <v>100215</v>
       </c>
       <c r="C71" t="n">
-        <v>50</v>
+        <v>89.05</v>
       </c>
       <c r="D71" t="n">
         <v>1.9</v>
@@ -8040,10 +8040,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>20240102502</v>
+        <v>100226</v>
       </c>
       <c r="C72" t="n">
-        <v>50</v>
+        <v>127.8</v>
       </c>
       <c r="D72" t="n">
         <v>1.9</v>
@@ -8079,10 +8079,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>20240102569</v>
+        <v>100237</v>
       </c>
       <c r="C73" t="n">
-        <v>50</v>
+        <v>217.8</v>
       </c>
       <c r="D73" t="n">
         <v>1.9</v>
@@ -8118,10 +8118,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>20240102637</v>
+        <v>100248</v>
       </c>
       <c r="C74" t="n">
-        <v>50</v>
+        <v>91.5</v>
       </c>
       <c r="D74" t="n">
         <v>1.9</v>
@@ -8157,10 +8157,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>20240102706</v>
+        <v>100259</v>
       </c>
       <c r="C75" t="n">
-        <v>50</v>
+        <v>66.78</v>
       </c>
       <c r="D75" t="n">
         <v>1.9</v>
@@ -8196,10 +8196,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>20240102776</v>
+        <v>100270</v>
       </c>
       <c r="C76" t="n">
-        <v>50</v>
+        <v>166.92</v>
       </c>
       <c r="D76" t="n">
         <v>1.9</v>
@@ -8235,10 +8235,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>20240102847</v>
+        <v>100281</v>
       </c>
       <c r="C77" t="n">
-        <v>50</v>
+        <v>206.65</v>
       </c>
       <c r="D77" t="n">
         <v>1.9</v>
@@ -8264,3945 +8264,6 @@
         </is>
       </c>
       <c r="I77" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="5" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" t="n">
-        <v>20240102919</v>
-      </c>
-      <c r="C78" t="n">
-        <v>50</v>
-      </c>
-      <c r="D78" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="5" t="n">
-        <v>77</v>
-      </c>
-      <c r="B79" t="n">
-        <v>20240102992</v>
-      </c>
-      <c r="C79" t="n">
-        <v>50</v>
-      </c>
-      <c r="D79" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="5" t="n">
-        <v>78</v>
-      </c>
-      <c r="B80" t="n">
-        <v>20240103066</v>
-      </c>
-      <c r="C80" t="n">
-        <v>50</v>
-      </c>
-      <c r="D80" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="5" t="n">
-        <v>79</v>
-      </c>
-      <c r="B81" t="n">
-        <v>20240103141</v>
-      </c>
-      <c r="C81" t="n">
-        <v>50</v>
-      </c>
-      <c r="D81" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="B82" t="n">
-        <v>20240103217</v>
-      </c>
-      <c r="C82" t="n">
-        <v>50</v>
-      </c>
-      <c r="D82" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" s="5" t="n">
-        <v>81</v>
-      </c>
-      <c r="B83" t="n">
-        <v>20240103294</v>
-      </c>
-      <c r="C83" t="n">
-        <v>50</v>
-      </c>
-      <c r="D83" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="5" t="n">
-        <v>82</v>
-      </c>
-      <c r="B84" t="n">
-        <v>20240103372</v>
-      </c>
-      <c r="C84" t="n">
-        <v>50</v>
-      </c>
-      <c r="D84" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="5" t="n">
-        <v>83</v>
-      </c>
-      <c r="B85" t="n">
-        <v>20240103451</v>
-      </c>
-      <c r="C85" t="n">
-        <v>50</v>
-      </c>
-      <c r="D85" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="5" t="n">
-        <v>84</v>
-      </c>
-      <c r="B86" t="n">
-        <v>20240103531</v>
-      </c>
-      <c r="C86" t="n">
-        <v>50</v>
-      </c>
-      <c r="D86" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="5" t="n">
-        <v>85</v>
-      </c>
-      <c r="B87" t="n">
-        <v>20240103612</v>
-      </c>
-      <c r="C87" t="n">
-        <v>50</v>
-      </c>
-      <c r="D87" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G87" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="5" t="n">
-        <v>86</v>
-      </c>
-      <c r="B88" t="n">
-        <v>20240103694</v>
-      </c>
-      <c r="C88" t="n">
-        <v>50</v>
-      </c>
-      <c r="D88" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="5" t="n">
-        <v>87</v>
-      </c>
-      <c r="B89" t="n">
-        <v>20240103777</v>
-      </c>
-      <c r="C89" t="n">
-        <v>50</v>
-      </c>
-      <c r="D89" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I89" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="5" t="n">
-        <v>88</v>
-      </c>
-      <c r="B90" t="n">
-        <v>20240103861</v>
-      </c>
-      <c r="C90" t="n">
-        <v>50</v>
-      </c>
-      <c r="D90" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="5" t="n">
-        <v>89</v>
-      </c>
-      <c r="B91" t="n">
-        <v>20240103946</v>
-      </c>
-      <c r="C91" t="n">
-        <v>50</v>
-      </c>
-      <c r="D91" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="5" t="n">
-        <v>90</v>
-      </c>
-      <c r="B92" t="n">
-        <v>20240104032</v>
-      </c>
-      <c r="C92" t="n">
-        <v>50</v>
-      </c>
-      <c r="D92" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="5" t="n">
-        <v>91</v>
-      </c>
-      <c r="B93" t="n">
-        <v>20240104119</v>
-      </c>
-      <c r="C93" t="n">
-        <v>50</v>
-      </c>
-      <c r="D93" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="5" t="n">
-        <v>92</v>
-      </c>
-      <c r="B94" t="n">
-        <v>20240104207</v>
-      </c>
-      <c r="C94" t="n">
-        <v>50</v>
-      </c>
-      <c r="D94" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="5" t="n">
-        <v>93</v>
-      </c>
-      <c r="B95" t="n">
-        <v>20240104296</v>
-      </c>
-      <c r="C95" t="n">
-        <v>50</v>
-      </c>
-      <c r="D95" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" s="5" t="n">
-        <v>94</v>
-      </c>
-      <c r="B96" t="n">
-        <v>20240104386</v>
-      </c>
-      <c r="C96" t="n">
-        <v>50</v>
-      </c>
-      <c r="D96" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" s="5" t="n">
-        <v>95</v>
-      </c>
-      <c r="B97" t="n">
-        <v>20240104477</v>
-      </c>
-      <c r="C97" t="n">
-        <v>50</v>
-      </c>
-      <c r="D97" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" s="5" t="n">
-        <v>96</v>
-      </c>
-      <c r="B98" t="n">
-        <v>20240104569</v>
-      </c>
-      <c r="C98" t="n">
-        <v>50</v>
-      </c>
-      <c r="D98" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I98" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" s="5" t="n">
-        <v>97</v>
-      </c>
-      <c r="B99" t="n">
-        <v>20240104662</v>
-      </c>
-      <c r="C99" t="n">
-        <v>50</v>
-      </c>
-      <c r="D99" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="5" t="n">
-        <v>98</v>
-      </c>
-      <c r="B100" t="n">
-        <v>20240104756</v>
-      </c>
-      <c r="C100" t="n">
-        <v>50</v>
-      </c>
-      <c r="D100" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="5" t="n">
-        <v>99</v>
-      </c>
-      <c r="B101" t="n">
-        <v>20240104851</v>
-      </c>
-      <c r="C101" t="n">
-        <v>50</v>
-      </c>
-      <c r="D101" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" s="5" t="n">
-        <v>100</v>
-      </c>
-      <c r="B102" t="n">
-        <v>20240104947</v>
-      </c>
-      <c r="C102" t="n">
-        <v>50</v>
-      </c>
-      <c r="D102" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="5" t="n">
-        <v>101</v>
-      </c>
-      <c r="B103" t="n">
-        <v>20240105044</v>
-      </c>
-      <c r="C103" t="n">
-        <v>50</v>
-      </c>
-      <c r="D103" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="5" t="n">
-        <v>102</v>
-      </c>
-      <c r="B104" t="n">
-        <v>20240105142</v>
-      </c>
-      <c r="C104" t="n">
-        <v>50</v>
-      </c>
-      <c r="D104" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="5" t="n">
-        <v>103</v>
-      </c>
-      <c r="B105" t="n">
-        <v>20240105241</v>
-      </c>
-      <c r="C105" t="n">
-        <v>50</v>
-      </c>
-      <c r="D105" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="5" t="n">
-        <v>104</v>
-      </c>
-      <c r="B106" t="n">
-        <v>20240105341</v>
-      </c>
-      <c r="C106" t="n">
-        <v>50</v>
-      </c>
-      <c r="D106" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="5" t="n">
-        <v>105</v>
-      </c>
-      <c r="B107" t="n">
-        <v>20240105442</v>
-      </c>
-      <c r="C107" t="n">
-        <v>50</v>
-      </c>
-      <c r="D107" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="5" t="n">
-        <v>106</v>
-      </c>
-      <c r="B108" t="n">
-        <v>20240105544</v>
-      </c>
-      <c r="C108" t="n">
-        <v>50</v>
-      </c>
-      <c r="D108" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I108" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="5" t="n">
-        <v>107</v>
-      </c>
-      <c r="B109" t="n">
-        <v>20240105647</v>
-      </c>
-      <c r="C109" t="n">
-        <v>50</v>
-      </c>
-      <c r="D109" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="5" t="n">
-        <v>108</v>
-      </c>
-      <c r="B110" t="n">
-        <v>20240105751</v>
-      </c>
-      <c r="C110" t="n">
-        <v>50</v>
-      </c>
-      <c r="D110" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H110" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="5" t="n">
-        <v>109</v>
-      </c>
-      <c r="B111" t="n">
-        <v>20240105856</v>
-      </c>
-      <c r="C111" t="n">
-        <v>50</v>
-      </c>
-      <c r="D111" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E111" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G111" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="5" t="n">
-        <v>110</v>
-      </c>
-      <c r="B112" t="n">
-        <v>20240105962</v>
-      </c>
-      <c r="C112" t="n">
-        <v>50</v>
-      </c>
-      <c r="D112" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="5" t="n">
-        <v>111</v>
-      </c>
-      <c r="B113" t="n">
-        <v>20240106069</v>
-      </c>
-      <c r="C113" t="n">
-        <v>50</v>
-      </c>
-      <c r="D113" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H113" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="5" t="n">
-        <v>112</v>
-      </c>
-      <c r="B114" t="n">
-        <v>20240106177</v>
-      </c>
-      <c r="C114" t="n">
-        <v>50</v>
-      </c>
-      <c r="D114" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H114" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="5" t="n">
-        <v>113</v>
-      </c>
-      <c r="B115" t="n">
-        <v>20240106286</v>
-      </c>
-      <c r="C115" t="n">
-        <v>50</v>
-      </c>
-      <c r="D115" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E115" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H115" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="5" t="n">
-        <v>114</v>
-      </c>
-      <c r="B116" t="n">
-        <v>20240106396</v>
-      </c>
-      <c r="C116" t="n">
-        <v>50</v>
-      </c>
-      <c r="D116" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E116" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H116" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="5" t="n">
-        <v>115</v>
-      </c>
-      <c r="B117" t="n">
-        <v>20240106507</v>
-      </c>
-      <c r="C117" t="n">
-        <v>50</v>
-      </c>
-      <c r="D117" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H117" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="5" t="n">
-        <v>116</v>
-      </c>
-      <c r="B118" t="n">
-        <v>20240106619</v>
-      </c>
-      <c r="C118" t="n">
-        <v>50</v>
-      </c>
-      <c r="D118" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H118" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" s="5" t="n">
-        <v>117</v>
-      </c>
-      <c r="B119" t="n">
-        <v>20240106732</v>
-      </c>
-      <c r="C119" t="n">
-        <v>50</v>
-      </c>
-      <c r="D119" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E119" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H119" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="5" t="n">
-        <v>118</v>
-      </c>
-      <c r="B120" t="n">
-        <v>20240106846</v>
-      </c>
-      <c r="C120" t="n">
-        <v>50</v>
-      </c>
-      <c r="D120" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E120" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H120" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" s="5" t="n">
-        <v>119</v>
-      </c>
-      <c r="B121" t="n">
-        <v>20240106961</v>
-      </c>
-      <c r="C121" t="n">
-        <v>50</v>
-      </c>
-      <c r="D121" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E121" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H121" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" s="5" t="n">
-        <v>120</v>
-      </c>
-      <c r="B122" t="n">
-        <v>20240107077</v>
-      </c>
-      <c r="C122" t="n">
-        <v>50</v>
-      </c>
-      <c r="D122" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E122" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H122" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="5" t="n">
-        <v>121</v>
-      </c>
-      <c r="B123" t="n">
-        <v>20240107194</v>
-      </c>
-      <c r="C123" t="n">
-        <v>50</v>
-      </c>
-      <c r="D123" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E123" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G123" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H123" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" s="5" t="n">
-        <v>122</v>
-      </c>
-      <c r="B124" t="n">
-        <v>20240107312</v>
-      </c>
-      <c r="C124" t="n">
-        <v>50</v>
-      </c>
-      <c r="D124" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E124" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F124" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H124" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" s="5" t="n">
-        <v>123</v>
-      </c>
-      <c r="B125" t="n">
-        <v>20240107431</v>
-      </c>
-      <c r="C125" t="n">
-        <v>50</v>
-      </c>
-      <c r="D125" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H125" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="5" t="n">
-        <v>124</v>
-      </c>
-      <c r="B126" t="n">
-        <v>20240107551</v>
-      </c>
-      <c r="C126" t="n">
-        <v>50</v>
-      </c>
-      <c r="D126" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E126" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H126" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" s="5" t="n">
-        <v>125</v>
-      </c>
-      <c r="B127" t="n">
-        <v>20240107672</v>
-      </c>
-      <c r="C127" t="n">
-        <v>50</v>
-      </c>
-      <c r="D127" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F127" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H127" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="5" t="n">
-        <v>126</v>
-      </c>
-      <c r="B128" t="n">
-        <v>20240107794</v>
-      </c>
-      <c r="C128" t="n">
-        <v>50</v>
-      </c>
-      <c r="D128" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E128" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F128" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H128" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I128" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="5" t="n">
-        <v>127</v>
-      </c>
-      <c r="B129" t="n">
-        <v>20240107917</v>
-      </c>
-      <c r="C129" t="n">
-        <v>50</v>
-      </c>
-      <c r="D129" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E129" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F129" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G129" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H129" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I129" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" s="5" t="n">
-        <v>128</v>
-      </c>
-      <c r="B130" t="n">
-        <v>20240108041</v>
-      </c>
-      <c r="C130" t="n">
-        <v>50</v>
-      </c>
-      <c r="D130" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F130" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G130" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H130" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I130" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" s="5" t="n">
-        <v>129</v>
-      </c>
-      <c r="B131" t="n">
-        <v>20240108166</v>
-      </c>
-      <c r="C131" t="n">
-        <v>50</v>
-      </c>
-      <c r="D131" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E131" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F131" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G131" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H131" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I131" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="5" t="n">
-        <v>130</v>
-      </c>
-      <c r="B132" t="n">
-        <v>20240108292</v>
-      </c>
-      <c r="C132" t="n">
-        <v>50</v>
-      </c>
-      <c r="D132" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E132" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F132" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G132" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H132" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I132" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" s="5" t="n">
-        <v>131</v>
-      </c>
-      <c r="B133" t="n">
-        <v>20240108419</v>
-      </c>
-      <c r="C133" t="n">
-        <v>50</v>
-      </c>
-      <c r="D133" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E133" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F133" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G133" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H133" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I133" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" s="5" t="n">
-        <v>132</v>
-      </c>
-      <c r="B134" t="n">
-        <v>20240108547</v>
-      </c>
-      <c r="C134" t="n">
-        <v>50</v>
-      </c>
-      <c r="D134" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E134" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F134" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G134" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H134" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="5" t="n">
-        <v>133</v>
-      </c>
-      <c r="B135" t="n">
-        <v>20240108676</v>
-      </c>
-      <c r="C135" t="n">
-        <v>50</v>
-      </c>
-      <c r="D135" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E135" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F135" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G135" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H135" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" s="5" t="n">
-        <v>134</v>
-      </c>
-      <c r="B136" t="n">
-        <v>20240108806</v>
-      </c>
-      <c r="C136" t="n">
-        <v>50</v>
-      </c>
-      <c r="D136" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F136" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G136" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H136" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I136" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" s="5" t="n">
-        <v>135</v>
-      </c>
-      <c r="B137" t="n">
-        <v>20240108937</v>
-      </c>
-      <c r="C137" t="n">
-        <v>50</v>
-      </c>
-      <c r="D137" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E137" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F137" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G137" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H137" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I137" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="5" t="n">
-        <v>136</v>
-      </c>
-      <c r="B138" t="n">
-        <v>20240109069</v>
-      </c>
-      <c r="C138" t="n">
-        <v>50</v>
-      </c>
-      <c r="D138" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E138" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F138" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G138" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H138" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" s="5" t="n">
-        <v>137</v>
-      </c>
-      <c r="B139" t="n">
-        <v>20240109202</v>
-      </c>
-      <c r="C139" t="n">
-        <v>50</v>
-      </c>
-      <c r="D139" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E139" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F139" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G139" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H139" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I139" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" s="5" t="n">
-        <v>138</v>
-      </c>
-      <c r="B140" t="n">
-        <v>20240109336</v>
-      </c>
-      <c r="C140" t="n">
-        <v>50</v>
-      </c>
-      <c r="D140" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E140" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F140" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G140" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H140" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I140" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="5" t="n">
-        <v>139</v>
-      </c>
-      <c r="B141" t="n">
-        <v>20240109471</v>
-      </c>
-      <c r="C141" t="n">
-        <v>50</v>
-      </c>
-      <c r="D141" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E141" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F141" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G141" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H141" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I141" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" s="5" t="n">
-        <v>140</v>
-      </c>
-      <c r="B142" t="n">
-        <v>20240109607</v>
-      </c>
-      <c r="C142" t="n">
-        <v>50</v>
-      </c>
-      <c r="D142" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E142" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F142" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H142" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I142" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" s="5" t="n">
-        <v>141</v>
-      </c>
-      <c r="B143" t="n">
-        <v>20240109744</v>
-      </c>
-      <c r="C143" t="n">
-        <v>50</v>
-      </c>
-      <c r="D143" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E143" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F143" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G143" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H143" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I143" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="5" t="n">
-        <v>142</v>
-      </c>
-      <c r="B144" t="n">
-        <v>20240109882</v>
-      </c>
-      <c r="C144" t="n">
-        <v>50</v>
-      </c>
-      <c r="D144" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E144" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F144" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G144" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H144" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I144" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" s="5" t="n">
-        <v>143</v>
-      </c>
-      <c r="B145" t="n">
-        <v>20240110021</v>
-      </c>
-      <c r="C145" t="n">
-        <v>50</v>
-      </c>
-      <c r="D145" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E145" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F145" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G145" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H145" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I145" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" s="5" t="n">
-        <v>144</v>
-      </c>
-      <c r="B146" t="n">
-        <v>20240110022</v>
-      </c>
-      <c r="C146" t="n">
-        <v>50</v>
-      </c>
-      <c r="D146" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E146" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F146" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G146" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H146" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I146" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="5" t="n">
-        <v>145</v>
-      </c>
-      <c r="B147" t="n">
-        <v>20240110023</v>
-      </c>
-      <c r="C147" t="n">
-        <v>50</v>
-      </c>
-      <c r="D147" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E147" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F147" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G147" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H147" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I147" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" s="5" t="n">
-        <v>146</v>
-      </c>
-      <c r="B148" t="n">
-        <v>20240110024</v>
-      </c>
-      <c r="C148" t="n">
-        <v>50</v>
-      </c>
-      <c r="D148" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E148" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F148" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G148" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H148" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I148" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" s="5" t="n">
-        <v>147</v>
-      </c>
-      <c r="B149" t="n">
-        <v>20240110025</v>
-      </c>
-      <c r="C149" t="n">
-        <v>50</v>
-      </c>
-      <c r="D149" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E149" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F149" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G149" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H149" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I149" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" s="5" t="n">
-        <v>148</v>
-      </c>
-      <c r="B150" t="n">
-        <v>20240110026</v>
-      </c>
-      <c r="C150" t="n">
-        <v>50</v>
-      </c>
-      <c r="D150" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E150" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F150" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G150" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H150" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I150" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" s="5" t="n">
-        <v>149</v>
-      </c>
-      <c r="B151" t="n">
-        <v>20240110027</v>
-      </c>
-      <c r="C151" t="n">
-        <v>50</v>
-      </c>
-      <c r="D151" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E151" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F151" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G151" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H151" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I151" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" s="5" t="n">
-        <v>150</v>
-      </c>
-      <c r="B152" t="n">
-        <v>20240110028</v>
-      </c>
-      <c r="C152" t="n">
-        <v>50</v>
-      </c>
-      <c r="D152" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E152" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F152" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G152" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H152" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I152" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" s="5" t="n">
-        <v>151</v>
-      </c>
-      <c r="B153" t="n">
-        <v>20240110029</v>
-      </c>
-      <c r="C153" t="n">
-        <v>50</v>
-      </c>
-      <c r="D153" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E153" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F153" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G153" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H153" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I153" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" s="5" t="n">
-        <v>152</v>
-      </c>
-      <c r="B154" t="n">
-        <v>20240110030</v>
-      </c>
-      <c r="C154" t="n">
-        <v>50</v>
-      </c>
-      <c r="D154" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E154" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F154" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G154" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H154" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I154" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" s="5" t="n">
-        <v>153</v>
-      </c>
-      <c r="B155" t="n">
-        <v>20240110031</v>
-      </c>
-      <c r="C155" t="n">
-        <v>50</v>
-      </c>
-      <c r="D155" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E155" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F155" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G155" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H155" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I155" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="5" t="n">
-        <v>154</v>
-      </c>
-      <c r="B156" t="n">
-        <v>20240110032</v>
-      </c>
-      <c r="C156" t="n">
-        <v>50</v>
-      </c>
-      <c r="D156" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E156" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F156" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G156" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H156" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I156" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" s="5" t="n">
-        <v>155</v>
-      </c>
-      <c r="B157" t="n">
-        <v>20240110033</v>
-      </c>
-      <c r="C157" t="n">
-        <v>50</v>
-      </c>
-      <c r="D157" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E157" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F157" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G157" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H157" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I157" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" s="5" t="n">
-        <v>156</v>
-      </c>
-      <c r="B158" t="n">
-        <v>20240110034</v>
-      </c>
-      <c r="C158" t="n">
-        <v>50</v>
-      </c>
-      <c r="D158" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E158" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F158" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G158" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H158" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I158" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" s="5" t="n">
-        <v>157</v>
-      </c>
-      <c r="B159" t="n">
-        <v>20240110035</v>
-      </c>
-      <c r="C159" t="n">
-        <v>50</v>
-      </c>
-      <c r="D159" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E159" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F159" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G159" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H159" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" s="5" t="n">
-        <v>158</v>
-      </c>
-      <c r="B160" t="n">
-        <v>20240110036</v>
-      </c>
-      <c r="C160" t="n">
-        <v>50</v>
-      </c>
-      <c r="D160" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E160" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F160" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G160" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H160" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I160" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" s="5" t="n">
-        <v>159</v>
-      </c>
-      <c r="B161" t="n">
-        <v>20240110037</v>
-      </c>
-      <c r="C161" t="n">
-        <v>50</v>
-      </c>
-      <c r="D161" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E161" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F161" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G161" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H161" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I161" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" s="5" t="n">
-        <v>160</v>
-      </c>
-      <c r="B162" t="n">
-        <v>20240110038</v>
-      </c>
-      <c r="C162" t="n">
-        <v>50</v>
-      </c>
-      <c r="D162" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E162" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F162" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G162" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H162" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I162" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" s="5" t="n">
-        <v>161</v>
-      </c>
-      <c r="B163" t="n">
-        <v>20240110039</v>
-      </c>
-      <c r="C163" t="n">
-        <v>50</v>
-      </c>
-      <c r="D163" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E163" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F163" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G163" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H163" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I163" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" s="5" t="n">
-        <v>162</v>
-      </c>
-      <c r="B164" t="n">
-        <v>20240110040</v>
-      </c>
-      <c r="C164" t="n">
-        <v>50</v>
-      </c>
-      <c r="D164" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E164" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F164" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G164" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H164" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I164" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" s="5" t="n">
-        <v>163</v>
-      </c>
-      <c r="B165" t="n">
-        <v>20240110041</v>
-      </c>
-      <c r="C165" t="n">
-        <v>50</v>
-      </c>
-      <c r="D165" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E165" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F165" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G165" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H165" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I165" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" s="5" t="n">
-        <v>164</v>
-      </c>
-      <c r="B166" t="n">
-        <v>20240110042</v>
-      </c>
-      <c r="C166" t="n">
-        <v>50</v>
-      </c>
-      <c r="D166" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E166" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F166" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G166" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H166" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I166" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" s="5" t="n">
-        <v>165</v>
-      </c>
-      <c r="B167" t="n">
-        <v>20240110043</v>
-      </c>
-      <c r="C167" t="n">
-        <v>50</v>
-      </c>
-      <c r="D167" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E167" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F167" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G167" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H167" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I167" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" s="5" t="n">
-        <v>166</v>
-      </c>
-      <c r="B168" t="n">
-        <v>20240110044</v>
-      </c>
-      <c r="C168" t="n">
-        <v>50</v>
-      </c>
-      <c r="D168" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E168" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F168" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G168" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H168" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I168" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" s="5" t="n">
-        <v>167</v>
-      </c>
-      <c r="B169" t="n">
-        <v>20240110045</v>
-      </c>
-      <c r="C169" t="n">
-        <v>50</v>
-      </c>
-      <c r="D169" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E169" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F169" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G169" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H169" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I169" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" s="5" t="n">
-        <v>168</v>
-      </c>
-      <c r="B170" t="n">
-        <v>20240110046</v>
-      </c>
-      <c r="C170" t="n">
-        <v>50</v>
-      </c>
-      <c r="D170" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E170" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F170" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G170" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H170" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I170" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" s="5" t="n">
-        <v>169</v>
-      </c>
-      <c r="B171" t="n">
-        <v>20240110047</v>
-      </c>
-      <c r="C171" t="n">
-        <v>50</v>
-      </c>
-      <c r="D171" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E171" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F171" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G171" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H171" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I171" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" s="5" t="n">
-        <v>170</v>
-      </c>
-      <c r="B172" t="n">
-        <v>100215</v>
-      </c>
-      <c r="C172" t="n">
-        <v>89.05</v>
-      </c>
-      <c r="D172" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E172" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F172" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G172" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H172" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I172" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" s="5" t="n">
-        <v>171</v>
-      </c>
-      <c r="B173" t="n">
-        <v>100226</v>
-      </c>
-      <c r="C173" t="n">
-        <v>127.8</v>
-      </c>
-      <c r="D173" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E173" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F173" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G173" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H173" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I173" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" s="5" t="n">
-        <v>172</v>
-      </c>
-      <c r="B174" t="n">
-        <v>100237</v>
-      </c>
-      <c r="C174" t="n">
-        <v>217.8</v>
-      </c>
-      <c r="D174" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E174" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F174" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G174" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H174" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I174" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" s="5" t="n">
-        <v>173</v>
-      </c>
-      <c r="B175" t="n">
-        <v>100248</v>
-      </c>
-      <c r="C175" t="n">
-        <v>91.5</v>
-      </c>
-      <c r="D175" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E175" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F175" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G175" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H175" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I175" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" s="5" t="n">
-        <v>174</v>
-      </c>
-      <c r="B176" t="n">
-        <v>100259</v>
-      </c>
-      <c r="C176" t="n">
-        <v>66.78</v>
-      </c>
-      <c r="D176" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E176" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F176" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G176" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H176" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I176" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" s="5" t="n">
-        <v>175</v>
-      </c>
-      <c r="B177" t="n">
-        <v>100270</v>
-      </c>
-      <c r="C177" t="n">
-        <v>166.92</v>
-      </c>
-      <c r="D177" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E177" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F177" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G177" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H177" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I177" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" s="5" t="n">
-        <v>176</v>
-      </c>
-      <c r="B178" t="n">
-        <v>100281</v>
-      </c>
-      <c r="C178" t="n">
-        <v>206.65</v>
-      </c>
-      <c r="D178" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E178" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F178" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G178" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H178" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I178" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
set invest to false after check failed
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1245,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1665,24 +1665,24 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>19882900174</v>
+        <v>20102800178</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="F17" t="n">
-        <v>652.8</v>
+        <v>433</v>
       </c>
       <c r="G17" t="n">
-        <v>652.8</v>
+        <v>433</v>
       </c>
     </row>
     <row r="18">
@@ -1690,7 +1690,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20102800178</v>
+        <v>20092800189</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1704,10 +1704,10 @@
         <v>0.44</v>
       </c>
       <c r="F18" t="n">
-        <v>433</v>
+        <v>716</v>
       </c>
       <c r="G18" t="n">
-        <v>433</v>
+        <v>716</v>
       </c>
     </row>
     <row r="19">
@@ -1715,24 +1715,24 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20092800189</v>
+        <v>20093000194</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.44</v>
+        <v>0.35</v>
       </c>
       <c r="F19" t="n">
-        <v>716</v>
+        <v>83.8</v>
       </c>
       <c r="G19" t="n">
-        <v>716</v>
+        <v>83.8</v>
       </c>
     </row>
     <row r="20">
@@ -1740,7 +1740,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20093000194</v>
+        <v>20063000195</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1754,10 +1754,10 @@
         <v>0.35</v>
       </c>
       <c r="F20" t="n">
-        <v>83.8</v>
+        <v>60</v>
       </c>
       <c r="G20" t="n">
-        <v>83.8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21">
@@ -1765,7 +1765,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20063000195</v>
+        <v>20023000196</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1779,10 +1779,10 @@
         <v>0.35</v>
       </c>
       <c r="F21" t="n">
-        <v>60</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="G21" t="n">
-        <v>60</v>
+        <v>97.09999999999999</v>
       </c>
     </row>
     <row r="22">
@@ -1790,24 +1790,24 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20023000196</v>
+        <v>20082800200</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="F22" t="n">
-        <v>97.09999999999999</v>
+        <v>250</v>
       </c>
       <c r="G22" t="n">
-        <v>97.09999999999999</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23">
@@ -1815,7 +1815,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20082800200</v>
+        <v>20072800211</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1829,10 +1829,10 @@
         <v>0.44</v>
       </c>
       <c r="F23" t="n">
-        <v>250</v>
+        <v>1572</v>
       </c>
       <c r="G23" t="n">
-        <v>250</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="24">
@@ -1840,7 +1840,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20072800211</v>
+        <v>20052800213</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1854,10 +1854,10 @@
         <v>0.44</v>
       </c>
       <c r="F24" t="n">
-        <v>1572</v>
+        <v>350</v>
       </c>
       <c r="G24" t="n">
-        <v>1572</v>
+        <v>350</v>
       </c>
     </row>
     <row r="25">
@@ -1865,7 +1865,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20052800213</v>
+        <v>20042800214</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1879,10 +1879,10 @@
         <v>0.44</v>
       </c>
       <c r="F25" t="n">
-        <v>350</v>
+        <v>336</v>
       </c>
       <c r="G25" t="n">
-        <v>350</v>
+        <v>336</v>
       </c>
     </row>
     <row r="26">
@@ -1890,7 +1890,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20042800214</v>
+        <v>20032800216</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1904,10 +1904,10 @@
         <v>0.44</v>
       </c>
       <c r="F26" t="n">
-        <v>336</v>
+        <v>822</v>
       </c>
       <c r="G26" t="n">
-        <v>336</v>
+        <v>822</v>
       </c>
     </row>
     <row r="27">
@@ -1915,7 +1915,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20032800216</v>
+        <v>20012800217</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1929,10 +1929,10 @@
         <v>0.44</v>
       </c>
       <c r="F27" t="n">
-        <v>822</v>
+        <v>690</v>
       </c>
       <c r="G27" t="n">
-        <v>822</v>
+        <v>690</v>
       </c>
     </row>
     <row r="28">
@@ -1940,7 +1940,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20012800217</v>
+        <v>19982800218</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1954,10 +1954,10 @@
         <v>0.44</v>
       </c>
       <c r="F28" t="n">
-        <v>690</v>
+        <v>123</v>
       </c>
       <c r="G28" t="n">
-        <v>690</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29">
@@ -1965,7 +1965,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>19982800218</v>
+        <v>19922800219</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1979,10 +1979,10 @@
         <v>0.44</v>
       </c>
       <c r="F29" t="n">
-        <v>123</v>
+        <v>1127.4</v>
       </c>
       <c r="G29" t="n">
-        <v>123</v>
+        <v>1127.4</v>
       </c>
     </row>
     <row r="30">
@@ -1990,7 +1990,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>19922800219</v>
+        <v>19912800220</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -2004,10 +2004,10 @@
         <v>0.44</v>
       </c>
       <c r="F30" t="n">
-        <v>1127.4</v>
+        <v>889</v>
       </c>
       <c r="G30" t="n">
-        <v>1127.4</v>
+        <v>889</v>
       </c>
     </row>
     <row r="31">
@@ -2015,7 +2015,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>19912800220</v>
+        <v>19902800221</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -2029,10 +2029,10 @@
         <v>0.44</v>
       </c>
       <c r="F31" t="n">
-        <v>889</v>
+        <v>561.7</v>
       </c>
       <c r="G31" t="n">
-        <v>889</v>
+        <v>561.7</v>
       </c>
     </row>
     <row r="32">
@@ -2040,7 +2040,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>19902800221</v>
+        <v>19892800222</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -2054,10 +2054,10 @@
         <v>0.44</v>
       </c>
       <c r="F32" t="n">
-        <v>561.7</v>
+        <v>332.7</v>
       </c>
       <c r="G32" t="n">
-        <v>561.7</v>
+        <v>332.7</v>
       </c>
     </row>
     <row r="33">
@@ -2065,24 +2065,24 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>19892800222</v>
+        <v>20180300241</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E33" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F33" t="n">
-        <v>332.7</v>
+        <v>140.5</v>
       </c>
       <c r="G33" t="n">
-        <v>332.7</v>
+        <v>140.5</v>
       </c>
     </row>
     <row r="34">
@@ -2090,24 +2090,24 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>19882800223</v>
+        <v>20140300242</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="E34" t="n">
-        <v>0.44</v>
+        <v>0.61</v>
       </c>
       <c r="F34" t="n">
-        <v>169.9</v>
+        <v>1117.5</v>
       </c>
       <c r="G34" t="n">
-        <v>169.9</v>
+        <v>1117.5</v>
       </c>
     </row>
     <row r="35">
@@ -2115,7 +2115,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>20180300241</v>
+        <v>20130300243</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -2129,10 +2129,10 @@
         <v>0.61</v>
       </c>
       <c r="F35" t="n">
-        <v>140.5</v>
+        <v>296.3</v>
       </c>
       <c r="G35" t="n">
-        <v>140.5</v>
+        <v>296.3</v>
       </c>
     </row>
     <row r="36">
@@ -2140,7 +2140,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>20140300242</v>
+        <v>20110300244</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         <v>0.61</v>
       </c>
       <c r="F36" t="n">
-        <v>1117.5</v>
+        <v>2110.5</v>
       </c>
       <c r="G36" t="n">
-        <v>1117.5</v>
+        <v>2110.5</v>
       </c>
     </row>
     <row r="37">
@@ -2165,7 +2165,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>20130300243</v>
+        <v>20100300245</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -2179,10 +2179,10 @@
         <v>0.61</v>
       </c>
       <c r="F37" t="n">
-        <v>296.3</v>
+        <v>3470</v>
       </c>
       <c r="G37" t="n">
-        <v>296.3</v>
+        <v>3470</v>
       </c>
     </row>
     <row r="38">
@@ -2190,7 +2190,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>20110300244</v>
+        <v>20090300246</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -2204,10 +2204,10 @@
         <v>0.61</v>
       </c>
       <c r="F38" t="n">
-        <v>2110.5</v>
+        <v>639</v>
       </c>
       <c r="G38" t="n">
-        <v>2110.5</v>
+        <v>639</v>
       </c>
     </row>
     <row r="39">
@@ -2215,7 +2215,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>20100300245</v>
+        <v>20080300247</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -2229,10 +2229,10 @@
         <v>0.61</v>
       </c>
       <c r="F39" t="n">
-        <v>3470</v>
+        <v>4269.5</v>
       </c>
       <c r="G39" t="n">
-        <v>3470</v>
+        <v>4269.5</v>
       </c>
     </row>
     <row r="40">
@@ -2240,7 +2240,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>20090300246</v>
+        <v>20070300249</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -2254,10 +2254,10 @@
         <v>0.61</v>
       </c>
       <c r="F40" t="n">
-        <v>639</v>
+        <v>196</v>
       </c>
       <c r="G40" t="n">
-        <v>639</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41">
@@ -2265,7 +2265,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>20080300247</v>
+        <v>20060300250</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -2279,10 +2279,10 @@
         <v>0.61</v>
       </c>
       <c r="F41" t="n">
-        <v>4269.5</v>
+        <v>1569</v>
       </c>
       <c r="G41" t="n">
-        <v>4269.5</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="42">
@@ -2290,7 +2290,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20070300249</v>
+        <v>20050300251</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -2304,10 +2304,10 @@
         <v>0.61</v>
       </c>
       <c r="F42" t="n">
-        <v>196</v>
+        <v>1517</v>
       </c>
       <c r="G42" t="n">
-        <v>196</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="43">
@@ -2315,7 +2315,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20060300250</v>
+        <v>20171700278</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -2323,16 +2323,16 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E43" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F43" t="n">
-        <v>1569</v>
+        <v>535.2</v>
       </c>
       <c r="G43" t="n">
-        <v>1569</v>
+        <v>535.2</v>
       </c>
     </row>
     <row r="44">
@@ -2340,7 +2340,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>20050300251</v>
+        <v>20161700279</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -2348,16 +2348,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E44" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F44" t="n">
-        <v>1517</v>
+        <v>167.451</v>
       </c>
       <c r="G44" t="n">
-        <v>1517</v>
+        <v>167.451</v>
       </c>
     </row>
     <row r="45">
@@ -2365,7 +2365,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20030300252</v>
+        <v>20151700280</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -2373,16 +2373,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E45" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F45" t="n">
-        <v>1207.759</v>
+        <v>220.2</v>
       </c>
       <c r="G45" t="n">
-        <v>1207.759</v>
+        <v>220.2</v>
       </c>
     </row>
     <row r="46">
@@ -2390,7 +2390,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20171700278</v>
+        <v>20141700282</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2404,10 +2404,10 @@
         <v>0.43</v>
       </c>
       <c r="F46" t="n">
-        <v>535.2</v>
+        <v>574.3099999999999</v>
       </c>
       <c r="G46" t="n">
-        <v>535.2</v>
+        <v>574.3099999999999</v>
       </c>
     </row>
     <row r="47">
@@ -2415,7 +2415,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20161700279</v>
+        <v>20121700283</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2429,10 +2429,10 @@
         <v>0.43</v>
       </c>
       <c r="F47" t="n">
-        <v>167.451</v>
+        <v>141.6</v>
       </c>
       <c r="G47" t="n">
-        <v>167.451</v>
+        <v>141.6</v>
       </c>
     </row>
     <row r="48">
@@ -2440,7 +2440,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>20151700280</v>
+        <v>20111700284</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -2454,10 +2454,10 @@
         <v>0.43</v>
       </c>
       <c r="F48" t="n">
-        <v>220.2</v>
+        <v>454.24</v>
       </c>
       <c r="G48" t="n">
-        <v>220.2</v>
+        <v>454.24</v>
       </c>
     </row>
     <row r="49">
@@ -2465,7 +2465,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>20141700282</v>
+        <v>20101700285</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2479,10 +2479,10 @@
         <v>0.43</v>
       </c>
       <c r="F49" t="n">
-        <v>574.3099999999999</v>
+        <v>275.78</v>
       </c>
       <c r="G49" t="n">
-        <v>574.3099999999999</v>
+        <v>275.78</v>
       </c>
     </row>
     <row r="50">
@@ -2490,7 +2490,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20121700283</v>
+        <v>20051700286</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2504,10 +2504,10 @@
         <v>0.43</v>
       </c>
       <c r="F50" t="n">
-        <v>141.6</v>
+        <v>158</v>
       </c>
       <c r="G50" t="n">
-        <v>141.6</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51">
@@ -2515,7 +2515,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>20111700284</v>
+        <v>20041700287</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -2529,110 +2529,10 @@
         <v>0.43</v>
       </c>
       <c r="F51" t="n">
-        <v>454.24</v>
+        <v>746.015</v>
       </c>
       <c r="G51" t="n">
-        <v>454.24</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="n">
-        <v>20101700285</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F52" t="n">
-        <v>275.78</v>
-      </c>
-      <c r="G52" t="n">
-        <v>275.78</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="6" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="n">
-        <v>20051700286</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D53" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F53" t="n">
-        <v>158</v>
-      </c>
-      <c r="G53" t="n">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="6" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="n">
-        <v>20041700287</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D54" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F54" t="n">
         <v>746.015</v>
-      </c>
-      <c r="G54" t="n">
-        <v>746.015</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="6" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="n">
-        <v>20031700288</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D55" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F55" t="n">
-        <v>163.9</v>
-      </c>
-      <c r="G55" t="n">
-        <v>163.9</v>
       </c>
     </row>
   </sheetData>
@@ -2683,7 +2583,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I247"/>
+  <dimension ref="A1:I262"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4025,17 +3925,17 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>19982400116</v>
+        <v>20192300124</v>
       </c>
       <c r="C35" t="n">
-        <v>853.3870000000011</v>
+        <v>1130.5</v>
       </c>
       <c r="D35" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -4064,10 +3964,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>20192300124</v>
+        <v>20182300125</v>
       </c>
       <c r="C36" t="n">
-        <v>1130.5</v>
+        <v>952</v>
       </c>
       <c r="D36" t="n">
         <v>2.7</v>
@@ -4103,10 +4003,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>20182300125</v>
+        <v>20172300126</v>
       </c>
       <c r="C37" t="n">
-        <v>952</v>
+        <v>1455</v>
       </c>
       <c r="D37" t="n">
         <v>2.7</v>
@@ -4142,10 +4042,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>20172300126</v>
+        <v>20162300127</v>
       </c>
       <c r="C38" t="n">
-        <v>1455</v>
+        <v>735</v>
       </c>
       <c r="D38" t="n">
         <v>2.7</v>
@@ -4181,10 +4081,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>20162300127</v>
+        <v>20152300128</v>
       </c>
       <c r="C39" t="n">
-        <v>735</v>
+        <v>1622</v>
       </c>
       <c r="D39" t="n">
         <v>2.7</v>
@@ -4220,10 +4120,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>20152300128</v>
+        <v>20142300129</v>
       </c>
       <c r="C40" t="n">
-        <v>1622</v>
+        <v>726</v>
       </c>
       <c r="D40" t="n">
         <v>2.7</v>
@@ -4259,10 +4159,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>20142300129</v>
+        <v>20132300130</v>
       </c>
       <c r="C41" t="n">
-        <v>726</v>
+        <v>2502</v>
       </c>
       <c r="D41" t="n">
         <v>2.7</v>
@@ -4298,10 +4198,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20132300130</v>
+        <v>20122300131</v>
       </c>
       <c r="C42" t="n">
-        <v>2502</v>
+        <v>401</v>
       </c>
       <c r="D42" t="n">
         <v>2.7</v>
@@ -4337,10 +4237,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20122300131</v>
+        <v>20112300132</v>
       </c>
       <c r="C43" t="n">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D43" t="n">
         <v>2.7</v>
@@ -4376,10 +4276,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>20112300132</v>
+        <v>20082300135</v>
       </c>
       <c r="C44" t="n">
-        <v>400</v>
+        <v>108.3</v>
       </c>
       <c r="D44" t="n">
         <v>2.7</v>
@@ -4415,10 +4315,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20082300135</v>
+        <v>20062300136</v>
       </c>
       <c r="C45" t="n">
-        <v>108.3</v>
+        <v>240</v>
       </c>
       <c r="D45" t="n">
         <v>2.7</v>
@@ -4454,17 +4354,15 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20062300136</v>
+        <v>20202100137</v>
       </c>
       <c r="C46" t="n">
-        <v>240</v>
-      </c>
-      <c r="D46" t="n">
-        <v>2.7</v>
-      </c>
+        <v>251.8</v>
+      </c>
+      <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -4493,15 +4391,17 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20202100137</v>
+        <v>20222410061</v>
       </c>
       <c r="C47" t="n">
-        <v>251.8</v>
-      </c>
-      <c r="D47" t="inlineStr"/>
+        <v>300</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1.35</v>
+      </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -4530,17 +4430,17 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>20232300291</v>
+        <v>20222410062</v>
       </c>
       <c r="C48" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D48" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4569,17 +4469,17 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>20232300292</v>
+        <v>20222410063</v>
       </c>
       <c r="C49" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D49" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4608,17 +4508,17 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20232300294</v>
+        <v>20222410064</v>
       </c>
       <c r="C50" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D50" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4647,17 +4547,17 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>20232300297</v>
+        <v>20222410065</v>
       </c>
       <c r="C51" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D51" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4686,17 +4586,17 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>20232300301</v>
+        <v>20222410066</v>
       </c>
       <c r="C52" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D52" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4725,17 +4625,17 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>20232300306</v>
+        <v>20222410067</v>
       </c>
       <c r="C53" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D53" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4764,17 +4664,17 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>20232300312</v>
+        <v>20222410068</v>
       </c>
       <c r="C54" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D54" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4803,17 +4703,17 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>20232300319</v>
+        <v>20222410069</v>
       </c>
       <c r="C55" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D55" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4842,17 +4742,17 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>20232300327</v>
+        <v>20222410070</v>
       </c>
       <c r="C56" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D56" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4881,17 +4781,17 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>20232300336</v>
+        <v>20222410071</v>
       </c>
       <c r="C57" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D57" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4920,17 +4820,17 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>20232300346</v>
+        <v>20222410072</v>
       </c>
       <c r="C58" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D58" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4959,17 +4859,17 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>20232300357</v>
+        <v>20222410073</v>
       </c>
       <c r="C59" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D59" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4998,17 +4898,17 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>20232300369</v>
+        <v>20222410074</v>
       </c>
       <c r="C60" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D60" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -5037,17 +4937,17 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>20232300382</v>
+        <v>20222410075</v>
       </c>
       <c r="C61" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D61" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5076,17 +4976,17 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>20232300396</v>
+        <v>20222410076</v>
       </c>
       <c r="C62" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D62" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5115,7 +5015,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>20232300411</v>
+        <v>20232300291</v>
       </c>
       <c r="C63" t="n">
         <v>200</v>
@@ -5154,7 +5054,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>20232300427</v>
+        <v>20232300292</v>
       </c>
       <c r="C64" t="n">
         <v>200</v>
@@ -5193,7 +5093,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>20232300444</v>
+        <v>20232300294</v>
       </c>
       <c r="C65" t="n">
         <v>200</v>
@@ -5232,7 +5132,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>20232300462</v>
+        <v>20232300297</v>
       </c>
       <c r="C66" t="n">
         <v>200</v>
@@ -5271,7 +5171,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>20232300481</v>
+        <v>20232300301</v>
       </c>
       <c r="C67" t="n">
         <v>200</v>
@@ -5310,7 +5210,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>20232300501</v>
+        <v>20232300306</v>
       </c>
       <c r="C68" t="n">
         <v>200</v>
@@ -5349,7 +5249,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>20232300522</v>
+        <v>20232300312</v>
       </c>
       <c r="C69" t="n">
         <v>200</v>
@@ -5388,7 +5288,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>20232300544</v>
+        <v>20232300319</v>
       </c>
       <c r="C70" t="n">
         <v>200</v>
@@ -5427,7 +5327,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>20232300567</v>
+        <v>20232300327</v>
       </c>
       <c r="C71" t="n">
         <v>200</v>
@@ -5466,7 +5366,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>20232300591</v>
+        <v>20232300336</v>
       </c>
       <c r="C72" t="n">
         <v>200</v>
@@ -5505,7 +5405,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>20232300616</v>
+        <v>20232300346</v>
       </c>
       <c r="C73" t="n">
         <v>200</v>
@@ -5544,7 +5444,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>20232300642</v>
+        <v>20232300357</v>
       </c>
       <c r="C74" t="n">
         <v>200</v>
@@ -5583,7 +5483,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>20232300669</v>
+        <v>20232300369</v>
       </c>
       <c r="C75" t="n">
         <v>200</v>
@@ -5622,7 +5522,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>20232300697</v>
+        <v>20232300382</v>
       </c>
       <c r="C76" t="n">
         <v>200</v>
@@ -5661,7 +5561,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>20232300726</v>
+        <v>20232300396</v>
       </c>
       <c r="C77" t="n">
         <v>200</v>
@@ -5700,7 +5600,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>20232300756</v>
+        <v>20232300411</v>
       </c>
       <c r="C78" t="n">
         <v>200</v>
@@ -5739,7 +5639,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>20232300787</v>
+        <v>20232300427</v>
       </c>
       <c r="C79" t="n">
         <v>200</v>
@@ -5778,7 +5678,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>20232300819</v>
+        <v>20232300444</v>
       </c>
       <c r="C80" t="n">
         <v>200</v>
@@ -5817,7 +5717,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>20232300852</v>
+        <v>20232300462</v>
       </c>
       <c r="C81" t="n">
         <v>200</v>
@@ -5856,7 +5756,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>20232300886</v>
+        <v>20232300481</v>
       </c>
       <c r="C82" t="n">
         <v>200</v>
@@ -5895,7 +5795,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>20232300921</v>
+        <v>20232300501</v>
       </c>
       <c r="C83" t="n">
         <v>200</v>
@@ -5934,7 +5834,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>20232300957</v>
+        <v>20232300522</v>
       </c>
       <c r="C84" t="n">
         <v>200</v>
@@ -5973,7 +5873,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>20232300994</v>
+        <v>20232300544</v>
       </c>
       <c r="C85" t="n">
         <v>200</v>
@@ -6012,7 +5912,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>20232301032</v>
+        <v>20232300567</v>
       </c>
       <c r="C86" t="n">
         <v>200</v>
@@ -6051,7 +5951,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>20232301071</v>
+        <v>20232300591</v>
       </c>
       <c r="C87" t="n">
         <v>200</v>
@@ -6090,7 +5990,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>20232301111</v>
+        <v>20232300616</v>
       </c>
       <c r="C88" t="n">
         <v>200</v>
@@ -6129,7 +6029,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>20232301152</v>
+        <v>20232300642</v>
       </c>
       <c r="C89" t="n">
         <v>200</v>
@@ -6168,7 +6068,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>20232301194</v>
+        <v>20232300669</v>
       </c>
       <c r="C90" t="n">
         <v>200</v>
@@ -6207,7 +6107,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>20232301237</v>
+        <v>20232300697</v>
       </c>
       <c r="C91" t="n">
         <v>200</v>
@@ -6246,7 +6146,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>20232301281</v>
+        <v>20232300726</v>
       </c>
       <c r="C92" t="n">
         <v>200</v>
@@ -6285,7 +6185,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>20232301326</v>
+        <v>20232300756</v>
       </c>
       <c r="C93" t="n">
         <v>200</v>
@@ -6324,7 +6224,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>20232301372</v>
+        <v>20232300787</v>
       </c>
       <c r="C94" t="n">
         <v>200</v>
@@ -6363,7 +6263,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>20232301419</v>
+        <v>20232300819</v>
       </c>
       <c r="C95" t="n">
         <v>200</v>
@@ -6402,7 +6302,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>20232301467</v>
+        <v>20232300852</v>
       </c>
       <c r="C96" t="n">
         <v>200</v>
@@ -6441,7 +6341,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>20232301516</v>
+        <v>20232300886</v>
       </c>
       <c r="C97" t="n">
         <v>200</v>
@@ -6480,7 +6380,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>20232301566</v>
+        <v>20232300921</v>
       </c>
       <c r="C98" t="n">
         <v>200</v>
@@ -6519,7 +6419,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>20232301617</v>
+        <v>20232300957</v>
       </c>
       <c r="C99" t="n">
         <v>200</v>
@@ -6558,7 +6458,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>20232301669</v>
+        <v>20232300994</v>
       </c>
       <c r="C100" t="n">
         <v>200</v>
@@ -6597,7 +6497,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>20232301722</v>
+        <v>20232301032</v>
       </c>
       <c r="C101" t="n">
         <v>200</v>
@@ -6636,7 +6536,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>20232301776</v>
+        <v>20232301071</v>
       </c>
       <c r="C102" t="n">
         <v>200</v>
@@ -6675,7 +6575,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>20232301831</v>
+        <v>20232301111</v>
       </c>
       <c r="C103" t="n">
         <v>200</v>
@@ -6714,7 +6614,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>20232301887</v>
+        <v>20232301152</v>
       </c>
       <c r="C104" t="n">
         <v>200</v>
@@ -6753,7 +6653,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>20232301944</v>
+        <v>20232301194</v>
       </c>
       <c r="C105" t="n">
         <v>200</v>
@@ -6792,7 +6692,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>20232302002</v>
+        <v>20232301237</v>
       </c>
       <c r="C106" t="n">
         <v>200</v>
@@ -6831,7 +6731,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>20232302061</v>
+        <v>20232301281</v>
       </c>
       <c r="C107" t="n">
         <v>200</v>
@@ -6870,7 +6770,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>20232302121</v>
+        <v>20232301326</v>
       </c>
       <c r="C108" t="n">
         <v>200</v>
@@ -6909,7 +6809,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>20232302182</v>
+        <v>20232301372</v>
       </c>
       <c r="C109" t="n">
         <v>200</v>
@@ -6948,7 +6848,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>20232302244</v>
+        <v>20232301419</v>
       </c>
       <c r="C110" t="n">
         <v>200</v>
@@ -6987,7 +6887,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>20232302307</v>
+        <v>20232301467</v>
       </c>
       <c r="C111" t="n">
         <v>200</v>
@@ -7026,7 +6926,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>20232302371</v>
+        <v>20232301516</v>
       </c>
       <c r="C112" t="n">
         <v>200</v>
@@ -7065,7 +6965,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>20232302436</v>
+        <v>20232301566</v>
       </c>
       <c r="C113" t="n">
         <v>200</v>
@@ -7104,7 +7004,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>20232302502</v>
+        <v>20232301617</v>
       </c>
       <c r="C114" t="n">
         <v>200</v>
@@ -7143,7 +7043,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>20232302569</v>
+        <v>20232301669</v>
       </c>
       <c r="C115" t="n">
         <v>200</v>
@@ -7182,7 +7082,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>20232302637</v>
+        <v>20232301722</v>
       </c>
       <c r="C116" t="n">
         <v>200</v>
@@ -7221,7 +7121,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>20232302706</v>
+        <v>20232301776</v>
       </c>
       <c r="C117" t="n">
         <v>200</v>
@@ -7260,7 +7160,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>20232302776</v>
+        <v>20232301831</v>
       </c>
       <c r="C118" t="n">
         <v>200</v>
@@ -7299,7 +7199,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>20232302847</v>
+        <v>20232301887</v>
       </c>
       <c r="C119" t="n">
         <v>200</v>
@@ -7338,7 +7238,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>20232302919</v>
+        <v>20232301944</v>
       </c>
       <c r="C120" t="n">
         <v>200</v>
@@ -7377,7 +7277,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>20232302992</v>
+        <v>20232302002</v>
       </c>
       <c r="C121" t="n">
         <v>200</v>
@@ -7416,7 +7316,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>20232303066</v>
+        <v>20232302061</v>
       </c>
       <c r="C122" t="n">
         <v>200</v>
@@ -7455,7 +7355,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>20232303141</v>
+        <v>20232302121</v>
       </c>
       <c r="C123" t="n">
         <v>200</v>
@@ -7494,7 +7394,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>20232303217</v>
+        <v>20232302182</v>
       </c>
       <c r="C124" t="n">
         <v>200</v>
@@ -7533,7 +7433,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>20232303294</v>
+        <v>20232302244</v>
       </c>
       <c r="C125" t="n">
         <v>200</v>
@@ -7572,7 +7472,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>20232303372</v>
+        <v>20232302307</v>
       </c>
       <c r="C126" t="n">
         <v>200</v>
@@ -7611,7 +7511,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>20232303451</v>
+        <v>20232302371</v>
       </c>
       <c r="C127" t="n">
         <v>200</v>
@@ -7650,7 +7550,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>20232303531</v>
+        <v>20232302436</v>
       </c>
       <c r="C128" t="n">
         <v>200</v>
@@ -7689,7 +7589,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>20232303612</v>
+        <v>20232302502</v>
       </c>
       <c r="C129" t="n">
         <v>200</v>
@@ -7728,7 +7628,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>20232303694</v>
+        <v>20232302569</v>
       </c>
       <c r="C130" t="n">
         <v>200</v>
@@ -7767,7 +7667,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>20232303777</v>
+        <v>20232302637</v>
       </c>
       <c r="C131" t="n">
         <v>200</v>
@@ -7806,7 +7706,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>20232303861</v>
+        <v>20232302706</v>
       </c>
       <c r="C132" t="n">
         <v>200</v>
@@ -7845,7 +7745,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>20232303946</v>
+        <v>20232302776</v>
       </c>
       <c r="C133" t="n">
         <v>200</v>
@@ -7884,7 +7784,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>20232304032</v>
+        <v>20232302847</v>
       </c>
       <c r="C134" t="n">
         <v>200</v>
@@ -7923,7 +7823,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>20232304119</v>
+        <v>20232302919</v>
       </c>
       <c r="C135" t="n">
         <v>200</v>
@@ -7962,7 +7862,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>20232304207</v>
+        <v>20232302992</v>
       </c>
       <c r="C136" t="n">
         <v>200</v>
@@ -8001,7 +7901,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>20232304296</v>
+        <v>20232303066</v>
       </c>
       <c r="C137" t="n">
         <v>200</v>
@@ -8040,7 +7940,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>20232304386</v>
+        <v>20232303141</v>
       </c>
       <c r="C138" t="n">
         <v>200</v>
@@ -8079,7 +7979,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>20232304477</v>
+        <v>20232303217</v>
       </c>
       <c r="C139" t="n">
         <v>200</v>
@@ -8118,7 +8018,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>20232304569</v>
+        <v>20232303294</v>
       </c>
       <c r="C140" t="n">
         <v>200</v>
@@ -8157,7 +8057,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>20232304662</v>
+        <v>20232303372</v>
       </c>
       <c r="C141" t="n">
         <v>200</v>
@@ -8196,7 +8096,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>20232304756</v>
+        <v>20232303451</v>
       </c>
       <c r="C142" t="n">
         <v>200</v>
@@ -8235,7 +8135,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>20232304851</v>
+        <v>20232303531</v>
       </c>
       <c r="C143" t="n">
         <v>200</v>
@@ -8274,7 +8174,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>20232304947</v>
+        <v>20232303612</v>
       </c>
       <c r="C144" t="n">
         <v>200</v>
@@ -8313,7 +8213,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>20232305044</v>
+        <v>20232303694</v>
       </c>
       <c r="C145" t="n">
         <v>200</v>
@@ -8352,7 +8252,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>20232305142</v>
+        <v>20232303777</v>
       </c>
       <c r="C146" t="n">
         <v>200</v>
@@ -8391,7 +8291,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>20232305241</v>
+        <v>20232303861</v>
       </c>
       <c r="C147" t="n">
         <v>200</v>
@@ -8430,7 +8330,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>20232305341</v>
+        <v>20232303946</v>
       </c>
       <c r="C148" t="n">
         <v>200</v>
@@ -8469,7 +8369,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>20232305442</v>
+        <v>20232304032</v>
       </c>
       <c r="C149" t="n">
         <v>200</v>
@@ -8508,7 +8408,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>20232305544</v>
+        <v>20232304119</v>
       </c>
       <c r="C150" t="n">
         <v>200</v>
@@ -8547,7 +8447,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>20232305647</v>
+        <v>20232304207</v>
       </c>
       <c r="C151" t="n">
         <v>200</v>
@@ -8586,7 +8486,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>20232305751</v>
+        <v>20232304296</v>
       </c>
       <c r="C152" t="n">
         <v>200</v>
@@ -8625,7 +8525,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>20232305856</v>
+        <v>20232304386</v>
       </c>
       <c r="C153" t="n">
         <v>200</v>
@@ -8664,7 +8564,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>20232305962</v>
+        <v>20232304477</v>
       </c>
       <c r="C154" t="n">
         <v>200</v>
@@ -8703,7 +8603,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>20232306069</v>
+        <v>20232304569</v>
       </c>
       <c r="C155" t="n">
         <v>200</v>
@@ -8742,7 +8642,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>20232306177</v>
+        <v>20232304662</v>
       </c>
       <c r="C156" t="n">
         <v>200</v>
@@ -8781,7 +8681,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>20232306286</v>
+        <v>20232304756</v>
       </c>
       <c r="C157" t="n">
         <v>200</v>
@@ -8820,7 +8720,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>20232306396</v>
+        <v>20232304851</v>
       </c>
       <c r="C158" t="n">
         <v>200</v>
@@ -8859,7 +8759,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>20232306507</v>
+        <v>20232304947</v>
       </c>
       <c r="C159" t="n">
         <v>200</v>
@@ -8898,7 +8798,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>20232306619</v>
+        <v>20232305044</v>
       </c>
       <c r="C160" t="n">
         <v>200</v>
@@ -8937,7 +8837,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>20232306732</v>
+        <v>20232305142</v>
       </c>
       <c r="C161" t="n">
         <v>200</v>
@@ -8976,7 +8876,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>20232306846</v>
+        <v>20232305241</v>
       </c>
       <c r="C162" t="n">
         <v>200</v>
@@ -9015,7 +8915,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>20232306961</v>
+        <v>20232305341</v>
       </c>
       <c r="C163" t="n">
         <v>200</v>
@@ -9054,7 +8954,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>20232307077</v>
+        <v>20232305442</v>
       </c>
       <c r="C164" t="n">
         <v>200</v>
@@ -9093,7 +8993,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>20232307194</v>
+        <v>20232305544</v>
       </c>
       <c r="C165" t="n">
         <v>200</v>
@@ -9132,7 +9032,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>20232307312</v>
+        <v>20232305647</v>
       </c>
       <c r="C166" t="n">
         <v>200</v>
@@ -9171,7 +9071,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>20232307431</v>
+        <v>20232305751</v>
       </c>
       <c r="C167" t="n">
         <v>200</v>
@@ -9210,7 +9110,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>20232307551</v>
+        <v>20232305856</v>
       </c>
       <c r="C168" t="n">
         <v>200</v>
@@ -9249,7 +9149,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>20232307672</v>
+        <v>20232305962</v>
       </c>
       <c r="C169" t="n">
         <v>200</v>
@@ -9288,7 +9188,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>20232307794</v>
+        <v>20232306069</v>
       </c>
       <c r="C170" t="n">
         <v>200</v>
@@ -9327,7 +9227,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>20232307917</v>
+        <v>20232306177</v>
       </c>
       <c r="C171" t="n">
         <v>200</v>
@@ -9366,7 +9266,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>20232308041</v>
+        <v>20232306286</v>
       </c>
       <c r="C172" t="n">
         <v>200</v>
@@ -9405,7 +9305,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>20232308166</v>
+        <v>20232306396</v>
       </c>
       <c r="C173" t="n">
         <v>200</v>
@@ -9444,7 +9344,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>20232308292</v>
+        <v>20232306507</v>
       </c>
       <c r="C174" t="n">
         <v>200</v>
@@ -9483,7 +9383,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>20232308419</v>
+        <v>20232306619</v>
       </c>
       <c r="C175" t="n">
         <v>200</v>
@@ -9522,7 +9422,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>20232308547</v>
+        <v>20232306732</v>
       </c>
       <c r="C176" t="n">
         <v>200</v>
@@ -9561,7 +9461,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>20232308676</v>
+        <v>20232306846</v>
       </c>
       <c r="C177" t="n">
         <v>200</v>
@@ -9600,7 +9500,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>20232308806</v>
+        <v>20232306961</v>
       </c>
       <c r="C178" t="n">
         <v>200</v>
@@ -9639,7 +9539,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>20232308937</v>
+        <v>20232307077</v>
       </c>
       <c r="C179" t="n">
         <v>200</v>
@@ -9678,7 +9578,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>20232309069</v>
+        <v>20232307194</v>
       </c>
       <c r="C180" t="n">
         <v>200</v>
@@ -9717,7 +9617,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>20232309202</v>
+        <v>20232307312</v>
       </c>
       <c r="C181" t="n">
         <v>200</v>
@@ -9756,7 +9656,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>20232309336</v>
+        <v>20232307431</v>
       </c>
       <c r="C182" t="n">
         <v>200</v>
@@ -9795,7 +9695,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>20232309471</v>
+        <v>20232307551</v>
       </c>
       <c r="C183" t="n">
         <v>200</v>
@@ -9834,7 +9734,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>20232309607</v>
+        <v>20232307672</v>
       </c>
       <c r="C184" t="n">
         <v>200</v>
@@ -9873,7 +9773,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>20232309744</v>
+        <v>20232307794</v>
       </c>
       <c r="C185" t="n">
         <v>200</v>
@@ -9912,7 +9812,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>20232309882</v>
+        <v>20232307917</v>
       </c>
       <c r="C186" t="n">
         <v>200</v>
@@ -9951,7 +9851,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>20232310021</v>
+        <v>20232308041</v>
       </c>
       <c r="C187" t="n">
         <v>200</v>
@@ -9990,7 +9890,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>20232310022</v>
+        <v>20232308166</v>
       </c>
       <c r="C188" t="n">
         <v>200</v>
@@ -10029,7 +9929,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>20232310023</v>
+        <v>20232308292</v>
       </c>
       <c r="C189" t="n">
         <v>200</v>
@@ -10068,7 +9968,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>20232310024</v>
+        <v>20232308419</v>
       </c>
       <c r="C190" t="n">
         <v>200</v>
@@ -10107,7 +10007,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>20232310025</v>
+        <v>20232308547</v>
       </c>
       <c r="C191" t="n">
         <v>200</v>
@@ -10146,7 +10046,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>20232310026</v>
+        <v>20232308676</v>
       </c>
       <c r="C192" t="n">
         <v>200</v>
@@ -10185,7 +10085,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>20232310027</v>
+        <v>20232308806</v>
       </c>
       <c r="C193" t="n">
         <v>200</v>
@@ -10224,7 +10124,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>20232310028</v>
+        <v>20232308937</v>
       </c>
       <c r="C194" t="n">
         <v>200</v>
@@ -10263,7 +10163,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>20232310029</v>
+        <v>20232309069</v>
       </c>
       <c r="C195" t="n">
         <v>200</v>
@@ -10302,7 +10202,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>20232310030</v>
+        <v>20232309202</v>
       </c>
       <c r="C196" t="n">
         <v>200</v>
@@ -10341,7 +10241,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>20232310031</v>
+        <v>20232309336</v>
       </c>
       <c r="C197" t="n">
         <v>200</v>
@@ -10380,7 +10280,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>20232310032</v>
+        <v>20232309471</v>
       </c>
       <c r="C198" t="n">
         <v>200</v>
@@ -10419,7 +10319,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>20232310033</v>
+        <v>20232309607</v>
       </c>
       <c r="C199" t="n">
         <v>200</v>
@@ -10458,7 +10358,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>20232310034</v>
+        <v>20232309744</v>
       </c>
       <c r="C200" t="n">
         <v>200</v>
@@ -10497,7 +10397,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>20232310035</v>
+        <v>20232309882</v>
       </c>
       <c r="C201" t="n">
         <v>200</v>
@@ -10536,7 +10436,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>20232310036</v>
+        <v>20232310021</v>
       </c>
       <c r="C202" t="n">
         <v>200</v>
@@ -10575,7 +10475,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
-        <v>20232310037</v>
+        <v>20232310022</v>
       </c>
       <c r="C203" t="n">
         <v>200</v>
@@ -10614,7 +10514,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
-        <v>20232310038</v>
+        <v>20232310023</v>
       </c>
       <c r="C204" t="n">
         <v>200</v>
@@ -10653,7 +10553,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="n">
-        <v>20232310039</v>
+        <v>20232310024</v>
       </c>
       <c r="C205" t="n">
         <v>200</v>
@@ -10692,7 +10592,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>20232310040</v>
+        <v>20232310025</v>
       </c>
       <c r="C206" t="n">
         <v>200</v>
@@ -10731,7 +10631,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>20232310041</v>
+        <v>20232310026</v>
       </c>
       <c r="C207" t="n">
         <v>200</v>
@@ -10770,7 +10670,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>20232310042</v>
+        <v>20232310027</v>
       </c>
       <c r="C208" t="n">
         <v>200</v>
@@ -10809,7 +10709,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>20232310043</v>
+        <v>20232310028</v>
       </c>
       <c r="C209" t="n">
         <v>200</v>
@@ -10848,7 +10748,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>20232310044</v>
+        <v>20232310029</v>
       </c>
       <c r="C210" t="n">
         <v>200</v>
@@ -10887,7 +10787,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>20232310045</v>
+        <v>20232310030</v>
       </c>
       <c r="C211" t="n">
         <v>200</v>
@@ -10926,7 +10826,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>20232310046</v>
+        <v>20232310031</v>
       </c>
       <c r="C212" t="n">
         <v>200</v>
@@ -10965,7 +10865,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="n">
-        <v>20232310047</v>
+        <v>20232310032</v>
       </c>
       <c r="C213" t="n">
         <v>200</v>
@@ -11004,7 +10904,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="n">
-        <v>20232310048</v>
+        <v>20232310033</v>
       </c>
       <c r="C214" t="n">
         <v>200</v>
@@ -11043,7 +10943,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="n">
-        <v>20232310049</v>
+        <v>20232310034</v>
       </c>
       <c r="C215" t="n">
         <v>200</v>
@@ -11082,7 +10982,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="n">
-        <v>20232310050</v>
+        <v>20232310035</v>
       </c>
       <c r="C216" t="n">
         <v>200</v>
@@ -11121,7 +11021,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="n">
-        <v>20232310051</v>
+        <v>20232310036</v>
       </c>
       <c r="C217" t="n">
         <v>200</v>
@@ -11160,7 +11060,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="n">
-        <v>20232310052</v>
+        <v>20232310037</v>
       </c>
       <c r="C218" t="n">
         <v>200</v>
@@ -11199,7 +11099,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="n">
-        <v>20232310053</v>
+        <v>20232310038</v>
       </c>
       <c r="C219" t="n">
         <v>200</v>
@@ -11238,7 +11138,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="n">
-        <v>20232310054</v>
+        <v>20232310039</v>
       </c>
       <c r="C220" t="n">
         <v>200</v>
@@ -11277,7 +11177,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="n">
-        <v>20232310055</v>
+        <v>20232310040</v>
       </c>
       <c r="C221" t="n">
         <v>200</v>
@@ -11316,7 +11216,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="n">
-        <v>20232310056</v>
+        <v>20232310041</v>
       </c>
       <c r="C222" t="n">
         <v>200</v>
@@ -11355,7 +11255,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="n">
-        <v>20232310057</v>
+        <v>20232310042</v>
       </c>
       <c r="C223" t="n">
         <v>200</v>
@@ -11394,7 +11294,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="n">
-        <v>20232310058</v>
+        <v>20232310043</v>
       </c>
       <c r="C224" t="n">
         <v>200</v>
@@ -11433,7 +11333,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="n">
-        <v>20232310059</v>
+        <v>20232310044</v>
       </c>
       <c r="C225" t="n">
         <v>200</v>
@@ -11472,7 +11372,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="n">
-        <v>20232310060</v>
+        <v>20232310045</v>
       </c>
       <c r="C226" t="n">
         <v>200</v>
@@ -11511,15 +11411,17 @@
         <v>225</v>
       </c>
       <c r="B227" t="n">
-        <v>20192100138</v>
+        <v>20232310046</v>
       </c>
       <c r="C227" t="n">
-        <v>195.4</v>
-      </c>
-      <c r="D227" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D227" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -11548,15 +11450,17 @@
         <v>226</v>
       </c>
       <c r="B228" t="n">
-        <v>20182100139</v>
+        <v>20232310047</v>
       </c>
       <c r="C228" t="n">
-        <v>414.723</v>
-      </c>
-      <c r="D228" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D228" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -11585,15 +11489,17 @@
         <v>227</v>
       </c>
       <c r="B229" t="n">
-        <v>20172100140</v>
+        <v>20232310048</v>
       </c>
       <c r="C229" t="n">
-        <v>3311.82512350009</v>
-      </c>
-      <c r="D229" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D229" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -11622,15 +11528,17 @@
         <v>228</v>
       </c>
       <c r="B230" t="n">
-        <v>20162100141</v>
+        <v>20232310049</v>
       </c>
       <c r="C230" t="n">
-        <v>6222.270852000401</v>
-      </c>
-      <c r="D230" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D230" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -11659,15 +11567,17 @@
         <v>229</v>
       </c>
       <c r="B231" t="n">
-        <v>20152100142</v>
+        <v>20232310050</v>
       </c>
       <c r="C231" t="n">
-        <v>1688.32281700176</v>
-      </c>
-      <c r="D231" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D231" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -11696,15 +11606,17 @@
         <v>230</v>
       </c>
       <c r="B232" t="n">
-        <v>20142100143</v>
+        <v>20232310051</v>
       </c>
       <c r="C232" t="n">
-        <v>1467.604103002783</v>
-      </c>
-      <c r="D232" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D232" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -11733,15 +11645,17 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>20132100144</v>
+        <v>20232310052</v>
       </c>
       <c r="C233" t="n">
-        <v>1387.194197003628</v>
-      </c>
-      <c r="D233" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D233" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -11770,15 +11684,17 @@
         <v>232</v>
       </c>
       <c r="B234" t="n">
-        <v>20122100146</v>
+        <v>20232310053</v>
       </c>
       <c r="C234" t="n">
-        <v>1732.597611001665</v>
-      </c>
-      <c r="D234" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D234" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -11807,15 +11723,17 @@
         <v>233</v>
       </c>
       <c r="B235" t="n">
-        <v>20112100147</v>
+        <v>20232310054</v>
       </c>
       <c r="C235" t="n">
-        <v>3084.73933250188</v>
-      </c>
-      <c r="D235" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D235" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -11844,15 +11762,17 @@
         <v>234</v>
       </c>
       <c r="B236" t="n">
-        <v>20102100148</v>
+        <v>20232310055</v>
       </c>
       <c r="C236" t="n">
-        <v>6784.098386973769</v>
-      </c>
-      <c r="D236" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D236" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -11881,15 +11801,17 @@
         <v>235</v>
       </c>
       <c r="B237" t="n">
-        <v>20092100149</v>
+        <v>20232310056</v>
       </c>
       <c r="C237" t="n">
-        <v>9295.344562513454</v>
-      </c>
-      <c r="D237" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D237" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -11918,15 +11840,17 @@
         <v>236</v>
       </c>
       <c r="B238" t="n">
-        <v>20082100150</v>
+        <v>20232310057</v>
       </c>
       <c r="C238" t="n">
-        <v>7475.485288501332</v>
-      </c>
-      <c r="D238" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D238" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -11955,15 +11879,17 @@
         <v>237</v>
       </c>
       <c r="B239" t="n">
-        <v>20072100151</v>
+        <v>20232310058</v>
       </c>
       <c r="C239" t="n">
-        <v>4341.280789791133</v>
-      </c>
-      <c r="D239" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D239" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -11992,15 +11918,17 @@
         <v>238</v>
       </c>
       <c r="B240" t="n">
-        <v>20062100152</v>
+        <v>20232310059</v>
       </c>
       <c r="C240" t="n">
-        <v>1924.091949500588</v>
-      </c>
-      <c r="D240" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D240" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -12029,15 +11957,17 @@
         <v>239</v>
       </c>
       <c r="B241" t="n">
-        <v>20052100153</v>
+        <v>20232310060</v>
       </c>
       <c r="C241" t="n">
-        <v>1221.046400499492</v>
-      </c>
-      <c r="D241" t="inlineStr"/>
+        <v>200</v>
+      </c>
+      <c r="D241" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -12066,10 +11996,10 @@
         <v>240</v>
       </c>
       <c r="B242" t="n">
-        <v>20042100154</v>
+        <v>20192100138</v>
       </c>
       <c r="C242" t="n">
-        <v>829.7290730002117</v>
+        <v>195.4</v>
       </c>
       <c r="D242" t="inlineStr"/>
       <c r="E242" t="inlineStr">
@@ -12103,10 +12033,10 @@
         <v>241</v>
       </c>
       <c r="B243" t="n">
-        <v>20032100155</v>
+        <v>20182100139</v>
       </c>
       <c r="C243" t="n">
-        <v>907.4490049999474</v>
+        <v>414.723</v>
       </c>
       <c r="D243" t="inlineStr"/>
       <c r="E243" t="inlineStr">
@@ -12140,10 +12070,10 @@
         <v>242</v>
       </c>
       <c r="B244" t="n">
-        <v>20022100157</v>
+        <v>20172100140</v>
       </c>
       <c r="C244" t="n">
-        <v>633.0435090000258</v>
+        <v>3311.82512350009</v>
       </c>
       <c r="D244" t="inlineStr"/>
       <c r="E244" t="inlineStr">
@@ -12177,10 +12107,10 @@
         <v>243</v>
       </c>
       <c r="B245" t="n">
-        <v>20012100158</v>
+        <v>20162100141</v>
       </c>
       <c r="C245" t="n">
-        <v>122.1209029997136</v>
+        <v>6222.270852000401</v>
       </c>
       <c r="D245" t="inlineStr"/>
       <c r="E245" t="inlineStr">
@@ -12214,10 +12144,10 @@
         <v>244</v>
       </c>
       <c r="B246" t="n">
-        <v>20002100159</v>
+        <v>20152100142</v>
       </c>
       <c r="C246" t="n">
-        <v>93.42517899995289</v>
+        <v>1688.32281700176</v>
       </c>
       <c r="D246" t="inlineStr"/>
       <c r="E246" t="inlineStr">
@@ -12251,10 +12181,10 @@
         <v>245</v>
       </c>
       <c r="B247" t="n">
-        <v>19992100160</v>
+        <v>20142100143</v>
       </c>
       <c r="C247" t="n">
-        <v>171.9239930052555</v>
+        <v>1467.604103002783</v>
       </c>
       <c r="D247" t="inlineStr"/>
       <c r="E247" t="inlineStr">
@@ -12278,6 +12208,561 @@
         </is>
       </c>
       <c r="I247" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="6" t="n">
+        <v>246</v>
+      </c>
+      <c r="B248" t="n">
+        <v>20132100144</v>
+      </c>
+      <c r="C248" t="n">
+        <v>1387.194197003628</v>
+      </c>
+      <c r="D248" t="inlineStr"/>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G248" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I248" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="6" t="n">
+        <v>247</v>
+      </c>
+      <c r="B249" t="n">
+        <v>20122100146</v>
+      </c>
+      <c r="C249" t="n">
+        <v>1732.597611001665</v>
+      </c>
+      <c r="D249" t="inlineStr"/>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I249" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="6" t="n">
+        <v>248</v>
+      </c>
+      <c r="B250" t="n">
+        <v>20112100147</v>
+      </c>
+      <c r="C250" t="n">
+        <v>3084.73933250188</v>
+      </c>
+      <c r="D250" t="inlineStr"/>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I250" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="6" t="n">
+        <v>249</v>
+      </c>
+      <c r="B251" t="n">
+        <v>20102100148</v>
+      </c>
+      <c r="C251" t="n">
+        <v>6784.098386973769</v>
+      </c>
+      <c r="D251" t="inlineStr"/>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="6" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="n">
+        <v>20092100149</v>
+      </c>
+      <c r="C252" t="n">
+        <v>9295.344562513454</v>
+      </c>
+      <c r="D252" t="inlineStr"/>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="6" t="n">
+        <v>251</v>
+      </c>
+      <c r="B253" t="n">
+        <v>20082100150</v>
+      </c>
+      <c r="C253" t="n">
+        <v>7475.485288501332</v>
+      </c>
+      <c r="D253" t="inlineStr"/>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I253" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="6" t="n">
+        <v>252</v>
+      </c>
+      <c r="B254" t="n">
+        <v>20072100151</v>
+      </c>
+      <c r="C254" t="n">
+        <v>4341.280789791133</v>
+      </c>
+      <c r="D254" t="inlineStr"/>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G254" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H254" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I254" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="6" t="n">
+        <v>253</v>
+      </c>
+      <c r="B255" t="n">
+        <v>20062100152</v>
+      </c>
+      <c r="C255" t="n">
+        <v>1924.091949500588</v>
+      </c>
+      <c r="D255" t="inlineStr"/>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H255" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I255" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="6" t="n">
+        <v>254</v>
+      </c>
+      <c r="B256" t="n">
+        <v>20052100153</v>
+      </c>
+      <c r="C256" t="n">
+        <v>1221.046400499492</v>
+      </c>
+      <c r="D256" t="inlineStr"/>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H256" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I256" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="6" t="n">
+        <v>255</v>
+      </c>
+      <c r="B257" t="n">
+        <v>20042100154</v>
+      </c>
+      <c r="C257" t="n">
+        <v>829.7290730002117</v>
+      </c>
+      <c r="D257" t="inlineStr"/>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I257" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="6" t="n">
+        <v>256</v>
+      </c>
+      <c r="B258" t="n">
+        <v>20032100155</v>
+      </c>
+      <c r="C258" t="n">
+        <v>907.4490049999474</v>
+      </c>
+      <c r="D258" t="inlineStr"/>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I258" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="6" t="n">
+        <v>257</v>
+      </c>
+      <c r="B259" t="n">
+        <v>20022100157</v>
+      </c>
+      <c r="C259" t="n">
+        <v>633.0435090000258</v>
+      </c>
+      <c r="D259" t="inlineStr"/>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="6" t="n">
+        <v>258</v>
+      </c>
+      <c r="B260" t="n">
+        <v>20012100158</v>
+      </c>
+      <c r="C260" t="n">
+        <v>122.1209029997136</v>
+      </c>
+      <c r="D260" t="inlineStr"/>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H260" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I260" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="6" t="n">
+        <v>259</v>
+      </c>
+      <c r="B261" t="n">
+        <v>20002100159</v>
+      </c>
+      <c r="C261" t="n">
+        <v>93.42517899995289</v>
+      </c>
+      <c r="D261" t="inlineStr"/>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G261" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I261" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="6" t="n">
+        <v>260</v>
+      </c>
+      <c r="B262" t="n">
+        <v>19992100160</v>
+      </c>
+      <c r="C262" t="n">
+        <v>171.9239930052555</v>
+      </c>
+      <c r="D262" t="inlineStr"/>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I262" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -12368,7 +12853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12769,45 +13254,6 @@
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>20030100281</v>
-      </c>
-      <c r="C11" t="n">
-        <v>206.65</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
interpolate for first 5 years
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>46752.99861111111</v>
+        <v>44196.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>47117.99861111111</v>
+        <v>44560.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1159,10 +1159,10 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2027</v>
+        <v>2020</v>
       </c>
       <c r="C1" s="6" t="n">
-        <v>2028</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="2">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>52.23999999999999</v>
+        <v>24.38</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -1205,7 +1205,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>16.432</v>
+        <v>11.504</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -1216,7 +1216,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>22.624</v>
+        <v>20.468</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -1227,7 +1227,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>59.832</v>
+        <v>48.114</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -1259,7 +1259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1304,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99991700006</v>
+        <v>19991700024</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1315,13 +1315,13 @@
         <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>115.8</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>115.8</v>
       </c>
     </row>
     <row r="3">
@@ -1329,7 +1329,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99990300008</v>
+        <v>19971700025</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1337,16 +1337,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.43</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>72.59999999999999</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>72.59999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -1354,24 +1354,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20132800145</v>
+        <v>19871400086</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.44</v>
+        <v>0.33</v>
       </c>
       <c r="F4" t="n">
-        <v>4734</v>
+        <v>1795</v>
       </c>
       <c r="G4" t="n">
-        <v>4734</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="5">
@@ -1379,24 +1379,24 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20122800156</v>
+        <v>19861400087</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0.44</v>
+        <v>0.33</v>
       </c>
       <c r="F5" t="n">
-        <v>1597.7</v>
+        <v>2746</v>
       </c>
       <c r="G5" t="n">
-        <v>1597.7</v>
+        <v>2746</v>
       </c>
     </row>
     <row r="6">
@@ -1404,24 +1404,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20102900161</v>
+        <v>19841400088</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.45</v>
+        <v>0.33</v>
       </c>
       <c r="F6" t="n">
-        <v>2780.3</v>
+        <v>1410</v>
       </c>
       <c r="G6" t="n">
-        <v>2780.3</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="7">
@@ -1429,24 +1429,24 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20082900162</v>
+        <v>19831400090</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.45</v>
+        <v>0.33</v>
       </c>
       <c r="F7" t="n">
-        <v>94.8</v>
+        <v>1360</v>
       </c>
       <c r="G7" t="n">
-        <v>94.8</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="8">
@@ -1454,24 +1454,24 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20072900163</v>
+        <v>19821400091</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0.45</v>
+        <v>0.33</v>
       </c>
       <c r="F8" t="n">
-        <v>648</v>
+        <v>1288</v>
       </c>
       <c r="G8" t="n">
-        <v>648</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="9">
@@ -1479,24 +1479,24 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20062900164</v>
+        <v>20132800145</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="F9" t="n">
-        <v>628</v>
+        <v>4734</v>
       </c>
       <c r="G9" t="n">
-        <v>628</v>
+        <v>4734</v>
       </c>
     </row>
     <row r="10">
@@ -1504,24 +1504,24 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20002900165</v>
+        <v>20122800156</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="F10" t="n">
-        <v>967.22</v>
+        <v>1597.7</v>
       </c>
       <c r="G10" t="n">
-        <v>967.22</v>
+        <v>1597.7</v>
       </c>
     </row>
     <row r="11">
@@ -1529,7 +1529,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>19982900166</v>
+        <v>20102900161</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1543,10 +1543,10 @@
         <v>0.45</v>
       </c>
       <c r="F11" t="n">
-        <v>1732</v>
+        <v>2780.3</v>
       </c>
       <c r="G11" t="n">
-        <v>1732</v>
+        <v>2780.3</v>
       </c>
     </row>
     <row r="12">
@@ -1554,24 +1554,24 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20112800167</v>
+        <v>20082900162</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F12" t="n">
-        <v>1909</v>
+        <v>94.8</v>
       </c>
       <c r="G12" t="n">
-        <v>1909</v>
+        <v>94.8</v>
       </c>
     </row>
     <row r="13">
@@ -1579,7 +1579,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19972900168</v>
+        <v>20072900163</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1593,10 +1593,10 @@
         <v>0.45</v>
       </c>
       <c r="F13" t="n">
-        <v>949</v>
+        <v>648</v>
       </c>
       <c r="G13" t="n">
-        <v>949</v>
+        <v>648</v>
       </c>
     </row>
     <row r="14">
@@ -1604,7 +1604,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19962900169</v>
+        <v>20062900164</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1618,10 +1618,10 @@
         <v>0.45</v>
       </c>
       <c r="F14" t="n">
-        <v>750</v>
+        <v>628</v>
       </c>
       <c r="G14" t="n">
-        <v>750</v>
+        <v>628</v>
       </c>
     </row>
     <row r="15">
@@ -1629,7 +1629,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>19952900170</v>
+        <v>20002900165</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1643,10 +1643,10 @@
         <v>0.45</v>
       </c>
       <c r="F15" t="n">
-        <v>750</v>
+        <v>967.22</v>
       </c>
       <c r="G15" t="n">
-        <v>750</v>
+        <v>967.22</v>
       </c>
     </row>
     <row r="16">
@@ -1654,7 +1654,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>19942900171</v>
+        <v>19982900166</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1668,10 +1668,10 @@
         <v>0.45</v>
       </c>
       <c r="F16" t="n">
-        <v>2780</v>
+        <v>1732</v>
       </c>
       <c r="G16" t="n">
-        <v>2780</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="17">
@@ -1679,24 +1679,24 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>19922900172</v>
+        <v>20112800167</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="F17" t="n">
-        <v>496</v>
+        <v>1909</v>
       </c>
       <c r="G17" t="n">
-        <v>496</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="18">
@@ -1704,7 +1704,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>19912900173</v>
+        <v>19972900168</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1718,10 +1718,10 @@
         <v>0.45</v>
       </c>
       <c r="F18" t="n">
-        <v>488.3</v>
+        <v>949</v>
       </c>
       <c r="G18" t="n">
-        <v>488.3</v>
+        <v>949</v>
       </c>
     </row>
     <row r="19">
@@ -1729,24 +1729,24 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20102800178</v>
+        <v>19962900169</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F19" t="n">
-        <v>433</v>
+        <v>750</v>
       </c>
       <c r="G19" t="n">
-        <v>433</v>
+        <v>750</v>
       </c>
     </row>
     <row r="20">
@@ -1754,24 +1754,24 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20092800189</v>
+        <v>19952900170</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F20" t="n">
-        <v>716</v>
+        <v>750</v>
       </c>
       <c r="G20" t="n">
-        <v>716</v>
+        <v>750</v>
       </c>
     </row>
     <row r="21">
@@ -1779,24 +1779,24 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20093000194</v>
+        <v>19942900171</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="F21" t="n">
-        <v>83.8</v>
+        <v>2780</v>
       </c>
       <c r="G21" t="n">
-        <v>83.8</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="22">
@@ -1804,24 +1804,24 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20063000195</v>
+        <v>19922900172</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="F22" t="n">
-        <v>60</v>
+        <v>496</v>
       </c>
       <c r="G22" t="n">
-        <v>60</v>
+        <v>496</v>
       </c>
     </row>
     <row r="23">
@@ -1829,24 +1829,24 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20023000196</v>
+        <v>19912900173</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0.35</v>
+        <v>0.45</v>
       </c>
       <c r="F23" t="n">
-        <v>97.09999999999999</v>
+        <v>488.3</v>
       </c>
       <c r="G23" t="n">
-        <v>97.09999999999999</v>
+        <v>488.3</v>
       </c>
     </row>
     <row r="24">
@@ -1854,24 +1854,24 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20082800200</v>
+        <v>19882900174</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F24" t="n">
-        <v>250</v>
+        <v>652.8</v>
       </c>
       <c r="G24" t="n">
-        <v>250</v>
+        <v>652.8</v>
       </c>
     </row>
     <row r="25">
@@ -1879,24 +1879,24 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20072800211</v>
+        <v>19872900175</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F25" t="n">
-        <v>1572</v>
+        <v>498.5</v>
       </c>
       <c r="G25" t="n">
-        <v>1572</v>
+        <v>498.5</v>
       </c>
     </row>
     <row r="26">
@@ -1904,24 +1904,24 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20052800213</v>
+        <v>19862900176</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F26" t="n">
-        <v>350</v>
+        <v>232.8</v>
       </c>
       <c r="G26" t="n">
-        <v>350</v>
+        <v>232.8</v>
       </c>
     </row>
     <row r="27">
@@ -1929,24 +1929,24 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20042800214</v>
+        <v>19852900177</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F27" t="n">
-        <v>336</v>
+        <v>465</v>
       </c>
       <c r="G27" t="n">
-        <v>336</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28">
@@ -1954,7 +1954,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20032800216</v>
+        <v>20102800178</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1968,10 +1968,10 @@
         <v>0.44</v>
       </c>
       <c r="F28" t="n">
-        <v>822</v>
+        <v>433</v>
       </c>
       <c r="G28" t="n">
-        <v>822</v>
+        <v>433</v>
       </c>
     </row>
     <row r="29">
@@ -1979,24 +1979,24 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>20012800217</v>
+        <v>19832900179</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0.44</v>
+        <v>0.45</v>
       </c>
       <c r="F29" t="n">
-        <v>690</v>
+        <v>361.3</v>
       </c>
       <c r="G29" t="n">
-        <v>690</v>
+        <v>361.3</v>
       </c>
     </row>
     <row r="30">
@@ -2004,7 +2004,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>19982800218</v>
+        <v>20092800189</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -2018,10 +2018,10 @@
         <v>0.44</v>
       </c>
       <c r="F30" t="n">
-        <v>123</v>
+        <v>716</v>
       </c>
       <c r="G30" t="n">
-        <v>123</v>
+        <v>716</v>
       </c>
     </row>
     <row r="31">
@@ -2029,24 +2029,24 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>19922800219</v>
+        <v>20093000194</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>0.44</v>
+        <v>0.35</v>
       </c>
       <c r="F31" t="n">
-        <v>1127.4</v>
+        <v>83.8</v>
       </c>
       <c r="G31" t="n">
-        <v>1127.4</v>
+        <v>83.8</v>
       </c>
     </row>
     <row r="32">
@@ -2054,24 +2054,24 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>19912800220</v>
+        <v>20063000195</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0.44</v>
+        <v>0.35</v>
       </c>
       <c r="F32" t="n">
-        <v>889</v>
+        <v>60</v>
       </c>
       <c r="G32" t="n">
-        <v>889</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33">
@@ -2079,24 +2079,24 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>19902800221</v>
+        <v>20023000196</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>0.44</v>
+        <v>0.35</v>
       </c>
       <c r="F33" t="n">
-        <v>561.7</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="G33" t="n">
-        <v>561.7</v>
+        <v>97.09999999999999</v>
       </c>
     </row>
     <row r="34">
@@ -2104,24 +2104,24 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>19892800222</v>
+        <v>19963000197</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>0.44</v>
+        <v>0.35</v>
       </c>
       <c r="F34" t="n">
-        <v>332.7</v>
+        <v>212</v>
       </c>
       <c r="G34" t="n">
-        <v>332.7</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35">
@@ -2129,24 +2129,24 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>20180300241</v>
+        <v>19953000198</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>0.61</v>
+        <v>0.35</v>
       </c>
       <c r="F35" t="n">
-        <v>140.5</v>
+        <v>97.3</v>
       </c>
       <c r="G35" t="n">
-        <v>140.5</v>
+        <v>97.3</v>
       </c>
     </row>
     <row r="36">
@@ -2154,24 +2154,24 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>20140300242</v>
+        <v>19933000199</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>0.61</v>
+        <v>0.35</v>
       </c>
       <c r="F36" t="n">
-        <v>1117.5</v>
+        <v>87.8</v>
       </c>
       <c r="G36" t="n">
-        <v>1117.5</v>
+        <v>87.8</v>
       </c>
     </row>
     <row r="37">
@@ -2179,24 +2179,24 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>20130300243</v>
+        <v>20082800200</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0.61</v>
+        <v>0.44</v>
       </c>
       <c r="F37" t="n">
-        <v>296.3</v>
+        <v>250</v>
       </c>
       <c r="G37" t="n">
-        <v>296.3</v>
+        <v>250</v>
       </c>
     </row>
     <row r="38">
@@ -2204,24 +2204,24 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>20110300244</v>
+        <v>19923000201</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>0.61</v>
+        <v>0.35</v>
       </c>
       <c r="F38" t="n">
-        <v>2110.5</v>
+        <v>190.4</v>
       </c>
       <c r="G38" t="n">
-        <v>2110.5</v>
+        <v>190.4</v>
       </c>
     </row>
     <row r="39">
@@ -2229,24 +2229,24 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>20100300245</v>
+        <v>20072800211</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>0.61</v>
+        <v>0.44</v>
       </c>
       <c r="F39" t="n">
-        <v>3470</v>
+        <v>1572</v>
       </c>
       <c r="G39" t="n">
-        <v>3470</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="40">
@@ -2254,24 +2254,24 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>20090300246</v>
+        <v>20052800213</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>0.61</v>
+        <v>0.44</v>
       </c>
       <c r="F40" t="n">
-        <v>639</v>
+        <v>350</v>
       </c>
       <c r="G40" t="n">
-        <v>639</v>
+        <v>350</v>
       </c>
     </row>
     <row r="41">
@@ -2279,24 +2279,24 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>20080300247</v>
+        <v>20042800214</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>0.61</v>
+        <v>0.44</v>
       </c>
       <c r="F41" t="n">
-        <v>4269.5</v>
+        <v>336</v>
       </c>
       <c r="G41" t="n">
-        <v>4269.5</v>
+        <v>336</v>
       </c>
     </row>
     <row r="42">
@@ -2304,24 +2304,24 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20070300249</v>
+        <v>20032800216</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>0.61</v>
+        <v>0.44</v>
       </c>
       <c r="F42" t="n">
-        <v>196</v>
+        <v>822</v>
       </c>
       <c r="G42" t="n">
-        <v>196</v>
+        <v>822</v>
       </c>
     </row>
     <row r="43">
@@ -2329,24 +2329,24 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20060300250</v>
+        <v>20012800217</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>0.61</v>
+        <v>0.44</v>
       </c>
       <c r="F43" t="n">
-        <v>1569</v>
+        <v>690</v>
       </c>
       <c r="G43" t="n">
-        <v>1569</v>
+        <v>690</v>
       </c>
     </row>
     <row r="44">
@@ -2354,24 +2354,24 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>20050300251</v>
+        <v>19982800218</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>0.61</v>
+        <v>0.44</v>
       </c>
       <c r="F44" t="n">
-        <v>1517</v>
+        <v>123</v>
       </c>
       <c r="G44" t="n">
-        <v>1517</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45">
@@ -2379,24 +2379,24 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20171700278</v>
+        <v>19922800219</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="F45" t="n">
-        <v>535.2</v>
+        <v>1127.4</v>
       </c>
       <c r="G45" t="n">
-        <v>535.2</v>
+        <v>1127.4</v>
       </c>
     </row>
     <row r="46">
@@ -2404,24 +2404,24 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20161700279</v>
+        <v>19912800220</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="F46" t="n">
-        <v>167.451</v>
+        <v>889</v>
       </c>
       <c r="G46" t="n">
-        <v>167.451</v>
+        <v>889</v>
       </c>
     </row>
     <row r="47">
@@ -2429,24 +2429,24 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20151700280</v>
+        <v>19902800221</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="F47" t="n">
-        <v>220.2</v>
+        <v>561.7</v>
       </c>
       <c r="G47" t="n">
-        <v>220.2</v>
+        <v>561.7</v>
       </c>
     </row>
     <row r="48">
@@ -2454,24 +2454,24 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>20141700282</v>
+        <v>19892800222</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="F48" t="n">
-        <v>574.3099999999999</v>
+        <v>332.7</v>
       </c>
       <c r="G48" t="n">
-        <v>574.3099999999999</v>
+        <v>332.7</v>
       </c>
     </row>
     <row r="49">
@@ -2479,24 +2479,24 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>20121700283</v>
+        <v>19882800223</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="F49" t="n">
-        <v>141.6</v>
+        <v>169.9</v>
       </c>
       <c r="G49" t="n">
-        <v>141.6</v>
+        <v>169.9</v>
       </c>
     </row>
     <row r="50">
@@ -2504,24 +2504,24 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20111700284</v>
+        <v>19872800224</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="F50" t="n">
-        <v>454.24</v>
+        <v>762.5</v>
       </c>
       <c r="G50" t="n">
-        <v>454.24</v>
+        <v>762.5</v>
       </c>
     </row>
     <row r="51">
@@ -2529,24 +2529,24 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>20101700285</v>
+        <v>19862800225</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="F51" t="n">
-        <v>275.78</v>
+        <v>713.5</v>
       </c>
       <c r="G51" t="n">
-        <v>275.78</v>
+        <v>713.5</v>
       </c>
     </row>
     <row r="52">
@@ -2554,24 +2554,24 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>20051700286</v>
+        <v>19852800227</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="F52" t="n">
-        <v>158</v>
+        <v>1157</v>
       </c>
       <c r="G52" t="n">
-        <v>158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="53">
@@ -2579,24 +2579,774 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
+        <v>19832800228</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>HARD_COAL</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="F53" t="n">
+        <v>380</v>
+      </c>
+      <c r="G53" t="n">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="6" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>19822800229</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>HARD_COAL</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="F54" t="n">
+        <v>88.3</v>
+      </c>
+      <c r="G54" t="n">
+        <v>88.3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>20180300241</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F55" t="n">
+        <v>140.5</v>
+      </c>
+      <c r="G55" t="n">
+        <v>140.5</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>20140300242</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1117.5</v>
+      </c>
+      <c r="G56" t="n">
+        <v>1117.5</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>20130300243</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F57" t="n">
+        <v>296.3</v>
+      </c>
+      <c r="G57" t="n">
+        <v>296.3</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="6" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>20110300244</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F58" t="n">
+        <v>2110.5</v>
+      </c>
+      <c r="G58" t="n">
+        <v>2110.5</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>20100300245</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F59" t="n">
+        <v>3470</v>
+      </c>
+      <c r="G59" t="n">
+        <v>3470</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="6" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>20090300246</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F60" t="n">
+        <v>639</v>
+      </c>
+      <c r="G60" t="n">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>20080300247</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F61" t="n">
+        <v>4269.5</v>
+      </c>
+      <c r="G61" t="n">
+        <v>4269.5</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>20070300249</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F62" t="n">
+        <v>196</v>
+      </c>
+      <c r="G62" t="n">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>20060300250</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1569</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="6" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>20050300251</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1517</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>20030300252</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F65" t="n">
+        <v>1207.759</v>
+      </c>
+      <c r="G65" t="n">
+        <v>1207.759</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="6" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>20020300253</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F66" t="n">
+        <v>1375.4</v>
+      </c>
+      <c r="G66" t="n">
+        <v>1375.4</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="6" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>20010300254</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F67" t="n">
+        <v>245.46</v>
+      </c>
+      <c r="G67" t="n">
+        <v>245.46</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="6" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>19990300255</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F68" t="n">
+        <v>135.8</v>
+      </c>
+      <c r="G68" t="n">
+        <v>135.8</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>19980300256</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F69" t="n">
+        <v>1239.2</v>
+      </c>
+      <c r="G69" t="n">
+        <v>1239.2</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="6" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>19970300257</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F70" t="n">
+        <v>778.6</v>
+      </c>
+      <c r="G70" t="n">
+        <v>778.6</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>20171700278</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F71" t="n">
+        <v>535.2</v>
+      </c>
+      <c r="G71" t="n">
+        <v>535.2</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="6" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>20161700279</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F72" t="n">
+        <v>167.451</v>
+      </c>
+      <c r="G72" t="n">
+        <v>167.451</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="6" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>20151700280</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F73" t="n">
+        <v>220.2</v>
+      </c>
+      <c r="G73" t="n">
+        <v>220.2</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="6" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>20141700282</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F74" t="n">
+        <v>574.3099999999999</v>
+      </c>
+      <c r="G74" t="n">
+        <v>574.3099999999999</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>20121700283</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F75" t="n">
+        <v>141.6</v>
+      </c>
+      <c r="G75" t="n">
+        <v>141.6</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="6" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>20111700284</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F76" t="n">
+        <v>454.24</v>
+      </c>
+      <c r="G76" t="n">
+        <v>454.24</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="6" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>20101700285</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F77" t="n">
+        <v>275.78</v>
+      </c>
+      <c r="G77" t="n">
+        <v>275.78</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="6" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>20051700286</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F78" t="n">
+        <v>158</v>
+      </c>
+      <c r="G78" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="6" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
         <v>20041700287</v>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="C79" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D53" t="n">
+      <c r="D79" t="n">
         <v>4.5</v>
       </c>
-      <c r="E53" t="n">
+      <c r="E79" t="n">
         <v>0.43</v>
       </c>
-      <c r="F53" t="n">
+      <c r="F79" t="n">
         <v>746.015</v>
       </c>
-      <c r="G53" t="n">
+      <c r="G79" t="n">
         <v>746.015</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="6" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>20031700288</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F80" t="n">
+        <v>163.9</v>
+      </c>
+      <c r="G80" t="n">
+        <v>163.9</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="6" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>20021700289</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F81" t="n">
+        <v>126.7</v>
+      </c>
+      <c r="G81" t="n">
+        <v>126.7</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="6" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>20011700290</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F82" t="n">
+        <v>110.55</v>
+      </c>
+      <c r="G82" t="n">
+        <v>110.55</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="6" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>20001700291</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F83" t="n">
+        <v>124.5</v>
+      </c>
+      <c r="G83" t="n">
+        <v>124.5</v>
       </c>
     </row>
   </sheetData>
@@ -2647,7 +3397,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2702,12 +3452,14 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99991000001</v>
+        <v>20181200048</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
+        <v>105.3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>RunOfRiver</t>
@@ -2739,15 +3491,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99992100002</v>
+        <v>20071200049</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
+        <v>691.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>RunOfRiver</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2776,17 +3530,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>99992400003</v>
+        <v>20021200050</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>1052</v>
       </c>
       <c r="D4" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>RunOfRiver</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -2815,17 +3569,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>99992300007</v>
+        <v>20011200051</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>138</v>
       </c>
       <c r="D5" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>RunOfRiver</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2854,10 +3608,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20181200048</v>
+        <v>19901200052</v>
       </c>
       <c r="C6" t="n">
-        <v>105.3</v>
+        <v>117.4</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -2893,10 +3647,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20071200049</v>
+        <v>19871200053</v>
       </c>
       <c r="C7" t="n">
-        <v>691.6</v>
+        <v>189.8</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -2932,10 +3686,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20021200050</v>
+        <v>19821200054</v>
       </c>
       <c r="C8" t="n">
-        <v>1052</v>
+        <v>91.80000000000001</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -2971,10 +3725,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20011200051</v>
+        <v>19811200055</v>
       </c>
       <c r="C9" t="n">
-        <v>138</v>
+        <v>60.3</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -3010,10 +3764,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>19901200052</v>
+        <v>19801200057</v>
       </c>
       <c r="C10" t="n">
-        <v>117.4</v>
+        <v>70</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -3049,10 +3803,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>19871200053</v>
+        <v>19771200058</v>
       </c>
       <c r="C11" t="n">
-        <v>189.8</v>
+        <v>1057.4</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -3088,10 +3842,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>19821200054</v>
+        <v>19761200059</v>
       </c>
       <c r="C12" t="n">
-        <v>91.80000000000001</v>
+        <v>179.4</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -3127,10 +3881,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19811200055</v>
+        <v>19731200060</v>
       </c>
       <c r="C13" t="n">
-        <v>60.3</v>
+        <v>926.7</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -3166,10 +3920,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19801200057</v>
+        <v>19721200061</v>
       </c>
       <c r="C14" t="n">
-        <v>70</v>
+        <v>164</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -4063,17 +4817,17 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>20192300124</v>
+        <v>19982400116</v>
       </c>
       <c r="C37" t="n">
-        <v>1130.5</v>
+        <v>853.3870000000011</v>
       </c>
       <c r="D37" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4102,17 +4856,17 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>20182300125</v>
+        <v>19972400117</v>
       </c>
       <c r="C38" t="n">
-        <v>952</v>
+        <v>564.2280000000012</v>
       </c>
       <c r="D38" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4141,17 +4895,17 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>20172300126</v>
+        <v>19962400118</v>
       </c>
       <c r="C39" t="n">
-        <v>1455</v>
+        <v>251.9353999999998</v>
       </c>
       <c r="D39" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4180,17 +4934,17 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>20162300127</v>
+        <v>19952400119</v>
       </c>
       <c r="C40" t="n">
-        <v>735</v>
+        <v>170.8699999999997</v>
       </c>
       <c r="D40" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -4219,17 +4973,17 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>20152300128</v>
+        <v>19942400120</v>
       </c>
       <c r="C41" t="n">
-        <v>1622</v>
+        <v>157.8950399999997</v>
       </c>
       <c r="D41" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4258,17 +5012,17 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20142300129</v>
+        <v>19932400121</v>
       </c>
       <c r="C42" t="n">
-        <v>726</v>
+        <v>172.6729999999995</v>
       </c>
       <c r="D42" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4297,17 +5051,17 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20132300130</v>
+        <v>19922400123</v>
       </c>
       <c r="C43" t="n">
-        <v>2502</v>
+        <v>133.46792</v>
       </c>
       <c r="D43" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -4336,10 +5090,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>20122300131</v>
+        <v>20192300124</v>
       </c>
       <c r="C44" t="n">
-        <v>401</v>
+        <v>1130.5</v>
       </c>
       <c r="D44" t="n">
         <v>2.7</v>
@@ -4375,10 +5129,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20112300132</v>
+        <v>20182300125</v>
       </c>
       <c r="C45" t="n">
-        <v>400</v>
+        <v>952</v>
       </c>
       <c r="D45" t="n">
         <v>2.7</v>
@@ -4414,10 +5168,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20082300135</v>
+        <v>20172300126</v>
       </c>
       <c r="C46" t="n">
-        <v>108.3</v>
+        <v>1455</v>
       </c>
       <c r="D46" t="n">
         <v>2.7</v>
@@ -4453,10 +5207,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20062300136</v>
+        <v>20162300127</v>
       </c>
       <c r="C47" t="n">
-        <v>240</v>
+        <v>735</v>
       </c>
       <c r="D47" t="n">
         <v>2.7</v>
@@ -4492,15 +5246,17 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>20202100137</v>
+        <v>20152300128</v>
       </c>
       <c r="C48" t="n">
-        <v>251.8</v>
-      </c>
-      <c r="D48" t="inlineStr"/>
+        <v>1622</v>
+      </c>
+      <c r="D48" t="n">
+        <v>2.7</v>
+      </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4529,17 +5285,17 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>20222400346</v>
+        <v>20142300129</v>
       </c>
       <c r="C49" t="n">
-        <v>1000</v>
+        <v>726</v>
       </c>
       <c r="D49" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4568,17 +5324,17 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20222400357</v>
+        <v>20132300130</v>
       </c>
       <c r="C50" t="n">
-        <v>1000</v>
+        <v>2502</v>
       </c>
       <c r="D50" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4607,17 +5363,17 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>20222400369</v>
+        <v>20122300131</v>
       </c>
       <c r="C51" t="n">
-        <v>1000</v>
+        <v>401</v>
       </c>
       <c r="D51" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4646,17 +5402,17 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>20222400382</v>
+        <v>20112300132</v>
       </c>
       <c r="C52" t="n">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="D52" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4685,17 +5441,17 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>20222400396</v>
+        <v>20082300135</v>
       </c>
       <c r="C53" t="n">
-        <v>1000</v>
+        <v>108.3</v>
       </c>
       <c r="D53" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4724,17 +5480,17 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>20222400411</v>
+        <v>20062300136</v>
       </c>
       <c r="C54" t="n">
-        <v>1000</v>
+        <v>240</v>
       </c>
       <c r="D54" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4763,17 +5519,15 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>20222400427</v>
+        <v>20202100137</v>
       </c>
       <c r="C55" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D55" t="n">
-        <v>1.35</v>
-      </c>
+        <v>251.8</v>
+      </c>
+      <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4802,17 +5556,15 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>20222400444</v>
+        <v>20192100138</v>
       </c>
       <c r="C56" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D56" t="n">
-        <v>1.35</v>
-      </c>
+        <v>195.4</v>
+      </c>
+      <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4841,17 +5593,15 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>20222400462</v>
+        <v>20182100139</v>
       </c>
       <c r="C57" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D57" t="n">
-        <v>1.35</v>
-      </c>
+        <v>414.723</v>
+      </c>
+      <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4880,17 +5630,15 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>20222400481</v>
+        <v>20172100140</v>
       </c>
       <c r="C58" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D58" t="n">
-        <v>1.35</v>
-      </c>
+        <v>3311.82512350009</v>
+      </c>
+      <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4919,10 +5667,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>20192100138</v>
+        <v>20162100141</v>
       </c>
       <c r="C59" t="n">
-        <v>195.4</v>
+        <v>6222.270852000401</v>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
@@ -4956,10 +5704,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>20182100139</v>
+        <v>20152100142</v>
       </c>
       <c r="C60" t="n">
-        <v>414.723</v>
+        <v>1688.32281700176</v>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
@@ -4993,10 +5741,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>20172100140</v>
+        <v>20142100143</v>
       </c>
       <c r="C61" t="n">
-        <v>3311.82512350009</v>
+        <v>1467.604103002783</v>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="inlineStr">
@@ -5030,10 +5778,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>20162100141</v>
+        <v>20132100144</v>
       </c>
       <c r="C62" t="n">
-        <v>6222.270852000401</v>
+        <v>1387.194197003628</v>
       </c>
       <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr">
@@ -5067,10 +5815,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>20152100142</v>
+        <v>20122100146</v>
       </c>
       <c r="C63" t="n">
-        <v>1688.32281700176</v>
+        <v>1732.597611001665</v>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
@@ -5104,10 +5852,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>20142100143</v>
+        <v>20112100147</v>
       </c>
       <c r="C64" t="n">
-        <v>1467.604103002783</v>
+        <v>3084.73933250188</v>
       </c>
       <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
@@ -5141,10 +5889,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>20132100144</v>
+        <v>20102100148</v>
       </c>
       <c r="C65" t="n">
-        <v>1387.194197003628</v>
+        <v>6784.098386973769</v>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
@@ -5178,10 +5926,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>20122100146</v>
+        <v>20092100149</v>
       </c>
       <c r="C66" t="n">
-        <v>1732.597611001665</v>
+        <v>9295.344562513454</v>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
@@ -5215,10 +5963,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>20112100147</v>
+        <v>20082100150</v>
       </c>
       <c r="C67" t="n">
-        <v>3084.73933250188</v>
+        <v>7475.485288501332</v>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
@@ -5252,10 +6000,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>20102100148</v>
+        <v>20072100151</v>
       </c>
       <c r="C68" t="n">
-        <v>6784.098386973769</v>
+        <v>4341.280789791133</v>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
@@ -5289,10 +6037,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>20092100149</v>
+        <v>20062100152</v>
       </c>
       <c r="C69" t="n">
-        <v>9295.344562513454</v>
+        <v>1924.091949500588</v>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr">
@@ -5326,10 +6074,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>20082100150</v>
+        <v>20052100153</v>
       </c>
       <c r="C70" t="n">
-        <v>7475.485288501332</v>
+        <v>1221.046400499492</v>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr">
@@ -5363,10 +6111,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>20072100151</v>
+        <v>20042100154</v>
       </c>
       <c r="C71" t="n">
-        <v>4341.280789791133</v>
+        <v>829.7290730002117</v>
       </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr">
@@ -5400,10 +6148,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>20062100152</v>
+        <v>20032100155</v>
       </c>
       <c r="C72" t="n">
-        <v>1924.091949500588</v>
+        <v>907.4490049999474</v>
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr">
@@ -5437,10 +6185,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>20052100153</v>
+        <v>20022100157</v>
       </c>
       <c r="C73" t="n">
-        <v>1221.046400499492</v>
+        <v>633.0435090000258</v>
       </c>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr">
@@ -5474,10 +6222,10 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>20042100154</v>
+        <v>20012100158</v>
       </c>
       <c r="C74" t="n">
-        <v>829.7290730002117</v>
+        <v>122.1209029997136</v>
       </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr">
@@ -5511,10 +6259,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>20032100155</v>
+        <v>20002100159</v>
       </c>
       <c r="C75" t="n">
-        <v>907.4490049999474</v>
+        <v>93.42517899995289</v>
       </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr">
@@ -5548,10 +6296,10 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>20022100157</v>
+        <v>19992100160</v>
       </c>
       <c r="C76" t="n">
-        <v>633.0435090000258</v>
+        <v>171.9239930052555</v>
       </c>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr">
@@ -5575,117 +6323,6 @@
         </is>
       </c>
       <c r="I76" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="6" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="n">
-        <v>20012100158</v>
-      </c>
-      <c r="C77" t="n">
-        <v>122.1209029997136</v>
-      </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="6" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" t="n">
-        <v>20002100159</v>
-      </c>
-      <c r="C78" t="n">
-        <v>93.42517899995289</v>
-      </c>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="6" t="n">
-        <v>77</v>
-      </c>
-      <c r="B79" t="n">
-        <v>19992100160</v>
-      </c>
-      <c r="C79" t="n">
-        <v>171.9239930052555</v>
-      </c>
-      <c r="D79" t="inlineStr"/>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I79" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -5702,7 +6339,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5745,34 +6382,6 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>99992600009</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5804,7 +6413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5859,10 +6468,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99990100004</v>
+        <v>20140100021</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>1125.6</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -5898,10 +6507,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20140100021</v>
+        <v>20130100022</v>
       </c>
       <c r="C3" t="n">
-        <v>1125.6</v>
+        <v>731</v>
       </c>
       <c r="D3" t="n">
         <v>1.9</v>
@@ -5937,10 +6546,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20130100022</v>
+        <v>20020100023</v>
       </c>
       <c r="C4" t="n">
-        <v>731</v>
+        <v>256</v>
       </c>
       <c r="D4" t="n">
         <v>1.9</v>
@@ -5976,10 +6585,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20120100133</v>
+        <v>20010100034</v>
       </c>
       <c r="C5" t="n">
-        <v>89.8</v>
+        <v>169.3934</v>
       </c>
       <c r="D5" t="n">
         <v>1.9</v>
@@ -6015,10 +6624,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20240100291</v>
+        <v>20000100045</v>
       </c>
       <c r="C6" t="n">
-        <v>1000</v>
+        <v>81.2</v>
       </c>
       <c r="D6" t="n">
         <v>1.9</v>
@@ -6054,10 +6663,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20240100292</v>
+        <v>19980100056</v>
       </c>
       <c r="C7" t="n">
-        <v>1000</v>
+        <v>90.80000000000001</v>
       </c>
       <c r="D7" t="n">
         <v>1.9</v>
@@ -6093,10 +6702,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20240100294</v>
+        <v>19970100067</v>
       </c>
       <c r="C8" t="n">
-        <v>1000</v>
+        <v>95.8</v>
       </c>
       <c r="D8" t="n">
         <v>1.9</v>
@@ -6132,10 +6741,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20240100297</v>
+        <v>20120100133</v>
       </c>
       <c r="C9" t="n">
-        <v>1000</v>
+        <v>89.8</v>
       </c>
       <c r="D9" t="n">
         <v>1.9</v>
@@ -6171,10 +6780,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20240100301</v>
+        <v>20100100215</v>
       </c>
       <c r="C10" t="n">
-        <v>1000</v>
+        <v>89.05</v>
       </c>
       <c r="D10" t="n">
         <v>1.9</v>
@@ -6210,10 +6819,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20240100306</v>
+        <v>20080100226</v>
       </c>
       <c r="C11" t="n">
-        <v>1000</v>
+        <v>127.8</v>
       </c>
       <c r="D11" t="n">
         <v>1.9</v>
@@ -6249,10 +6858,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20240100312</v>
+        <v>20070100237</v>
       </c>
       <c r="C12" t="n">
-        <v>1000</v>
+        <v>217.8</v>
       </c>
       <c r="D12" t="n">
         <v>1.9</v>
@@ -6288,10 +6897,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20240100319</v>
+        <v>20060100248</v>
       </c>
       <c r="C13" t="n">
-        <v>1000</v>
+        <v>91.5</v>
       </c>
       <c r="D13" t="n">
         <v>1.9</v>
@@ -6327,10 +6936,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20240100327</v>
+        <v>20050100259</v>
       </c>
       <c r="C14" t="n">
-        <v>1000</v>
+        <v>66.78</v>
       </c>
       <c r="D14" t="n">
         <v>1.9</v>
@@ -6366,10 +6975,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20240100336</v>
+        <v>20040100270</v>
       </c>
       <c r="C15" t="n">
-        <v>1000</v>
+        <v>166.92</v>
       </c>
       <c r="D15" t="n">
         <v>1.9</v>
@@ -6405,10 +7014,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20100100215</v>
+        <v>20030100281</v>
       </c>
       <c r="C16" t="n">
-        <v>89.05</v>
+        <v>206.65</v>
       </c>
       <c r="D16" t="n">
         <v>1.9</v>
@@ -6434,201 +7043,6 @@
         </is>
       </c>
       <c r="I16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>20080100226</v>
-      </c>
-      <c r="C17" t="n">
-        <v>127.8</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>20070100237</v>
-      </c>
-      <c r="C18" t="n">
-        <v>217.8</v>
-      </c>
-      <c r="D18" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>20060100248</v>
-      </c>
-      <c r="C19" t="n">
-        <v>91.5</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>20050100259</v>
-      </c>
-      <c r="C20" t="n">
-        <v>66.78</v>
-      </c>
-      <c r="D20" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>20040100270</v>
-      </c>
-      <c r="C21" t="n">
-        <v>166.92</v>
-      </c>
-      <c r="D21" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
fixed wrong setting of age in dismantling module
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>50040.99861111111</v>
+        <v>45657.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>50404.99861111111</v>
+        <v>46021.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1149,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1159,37 +1159,10 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2027</v>
+        <v>2024</v>
       </c>
       <c r="C1" s="6" t="n">
-        <v>2028</v>
-      </c>
-      <c r="D1" s="6" t="n">
-        <v>2029</v>
-      </c>
-      <c r="E1" s="6" t="n">
-        <v>2030</v>
-      </c>
-      <c r="F1" s="6" t="n">
-        <v>2031</v>
-      </c>
-      <c r="G1" s="6" t="n">
-        <v>2032</v>
-      </c>
-      <c r="H1" s="6" t="n">
-        <v>2033</v>
-      </c>
-      <c r="I1" s="6" t="n">
-        <v>2034</v>
-      </c>
-      <c r="J1" s="6" t="n">
-        <v>2035</v>
-      </c>
-      <c r="K1" s="6" t="n">
-        <v>2036</v>
-      </c>
-      <c r="L1" s="6" t="n">
-        <v>2037</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="2">
@@ -1199,18 +1172,9 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>88.06</v>
+        <v>40.3</v>
       </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -1222,15 +1186,6 @@
         <v>1.69</v>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -1242,15 +1197,6 @@
         <v>3.96</v>
       </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -1259,18 +1205,9 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>22.76800000000003</v>
+        <v>14.32</v>
       </c>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -1279,18 +1216,9 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25.39599999999996</v>
+        <v>21.7</v>
       </c>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -1299,18 +1227,9 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>74.89799999999923</v>
+        <v>54.81</v>
       </c>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -1324,51 +1243,6 @@
         </is>
       </c>
       <c r="C8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
         <is>
           <t>./timeseries/demand/load.csv</t>
         </is>
@@ -1673,7 +1547,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2313,17 +2187,17 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20222100086</v>
+        <v>20151200026</v>
       </c>
       <c r="C17" t="n">
-        <v>1000</v>
+        <v>8858.749999999998</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>RunOfRiver</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2352,10 +2226,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20222100087</v>
+        <v>20152100030</v>
       </c>
       <c r="C18" t="n">
-        <v>1000</v>
+        <v>53555.51607579708</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -2391,17 +2265,17 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20222100089</v>
+        <v>20152300031</v>
       </c>
       <c r="C19" t="n">
-        <v>1000</v>
+        <v>10271.8</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -2420,786 +2294,6 @@
         </is>
       </c>
       <c r="I19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>20222100092</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>20222100096</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>20222100101</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="6" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>20222100107</v>
-      </c>
-      <c r="C23" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>20222100114</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>20222100122</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>20222100131</v>
-      </c>
-      <c r="C26" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>20222100141</v>
-      </c>
-      <c r="C27" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="n">
-        <v>20232100141</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="n">
-        <v>20232100142</v>
-      </c>
-      <c r="C29" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="6" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="n">
-        <v>20232100144</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="n">
-        <v>20232100147</v>
-      </c>
-      <c r="C31" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="n">
-        <v>20232100151</v>
-      </c>
-      <c r="C32" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="6" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="n">
-        <v>20232100156</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="6" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="n">
-        <v>20232100162</v>
-      </c>
-      <c r="C34" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="6" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="n">
-        <v>20232100169</v>
-      </c>
-      <c r="C35" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="6" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="n">
-        <v>20232100177</v>
-      </c>
-      <c r="C36" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="6" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="n">
-        <v>20151200026</v>
-      </c>
-      <c r="C37" t="n">
-        <v>8858.749999999998</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>RunOfRiver</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="6" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="n">
-        <v>20152100030</v>
-      </c>
-      <c r="C38" t="n">
-        <v>53555.51607579708</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="6" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="n">
-        <v>20152300031</v>
-      </c>
-      <c r="C39" t="n">
-        <v>10271.8</v>
-      </c>
-      <c r="D39" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>WindOff</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
WIP plot yearly dispatch
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>44196.99861111111</v>
+        <v>45291.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>44560.99861111111</v>
+        <v>45656.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1149,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1159,10 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2020</v>
-      </c>
-      <c r="C1" s="6" t="n">
-        <v>2021</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="2">
@@ -1172,9 +1169,8 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24.38</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
+        <v>36.31999999999999</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -1185,7 +1181,6 @@
       <c r="B3" t="n">
         <v>1.69</v>
       </c>
-      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -1196,7 +1191,6 @@
       <c r="B4" t="n">
         <v>3.96</v>
       </c>
-      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -1205,9 +1199,8 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.504</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
+        <v>13.616</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -1216,9 +1209,8 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>20.468</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
+        <v>21.392</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -1227,9 +1219,8 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>48.114</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
+        <v>53.136</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -1238,11 +1229,6 @@
         </is>
       </c>
       <c r="B8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
         <is>
           <t>./timeseries/demand/load.csv</t>
         </is>
@@ -1259,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1304,24 +1290,24 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20122800022</v>
+        <v>99991700006</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>22051</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>22051</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1329,24 +1315,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20123000028</v>
+        <v>99990300008</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
+        <v>4.2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>3747</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>3747</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1354,24 +1340,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20122900030</v>
+        <v>20122800022</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D4" t="n">
         <v>3.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="F4" t="n">
-        <v>18049</v>
+        <v>22051</v>
       </c>
       <c r="G4" t="n">
-        <v>18049</v>
+        <v>22051</v>
       </c>
     </row>
     <row r="5">
@@ -1379,24 +1365,24 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20121400031</v>
+        <v>20123000028</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="E5" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="F5" t="n">
-        <v>9516</v>
+        <v>3747</v>
       </c>
       <c r="G5" t="n">
-        <v>9516</v>
+        <v>3747</v>
       </c>
     </row>
     <row r="6">
@@ -1404,24 +1390,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20120300032</v>
+        <v>20122900030</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="F6" t="n">
-        <v>7820.6</v>
+        <v>18049</v>
       </c>
       <c r="G6" t="n">
-        <v>7820.6</v>
+        <v>18049</v>
       </c>
     </row>
     <row r="7">
@@ -1429,23 +1415,73 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
+        <v>20121400031</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NUCLEAR</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F7" t="n">
+        <v>9516</v>
+      </c>
+      <c r="G7" t="n">
+        <v>9516</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20120300032</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F8" t="n">
+        <v>7820.6</v>
+      </c>
+      <c r="G8" t="n">
+        <v>7820.6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
         <v>20121700033</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D9" t="n">
         <v>4.5</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E9" t="n">
         <v>0.5</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F9" t="n">
         <v>16062.2</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G9" t="n">
         <v>16062.2</v>
       </c>
     </row>
@@ -1497,7 +1533,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1552,17 +1588,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20122400023</v>
+        <v>99992100002</v>
       </c>
       <c r="C2" t="n">
-        <v>2328</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1591,10 +1627,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20122400024</v>
+        <v>99992400003</v>
       </c>
       <c r="C3" t="n">
-        <v>50617</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>1.35</v>
@@ -1630,10 +1666,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20122300025</v>
+        <v>99992300007</v>
       </c>
       <c r="C4" t="n">
-        <v>2859</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>2.7</v>
@@ -1669,17 +1705,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20122300026</v>
+        <v>20122400023</v>
       </c>
       <c r="C5" t="n">
-        <v>4644</v>
+        <v>2328</v>
       </c>
       <c r="D5" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1708,17 +1744,17 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20121000027</v>
+        <v>20122400024</v>
       </c>
       <c r="C6" t="n">
-        <v>5317</v>
+        <v>50617</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1747,17 +1783,17 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20122100034</v>
+        <v>20122300025</v>
       </c>
       <c r="C7" t="n">
-        <v>14504</v>
+        <v>2859</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1786,35 +1822,152 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
+        <v>20122300026</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4644</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20121000027</v>
+      </c>
+      <c r="C9" t="n">
+        <v>5317</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>RunOfRiver</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20122100034</v>
+      </c>
+      <c r="C10" t="n">
+        <v>14504</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
         <v>20122100035</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C11" t="n">
         <v>30932</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D11" t="n">
         <v>0</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>OtherPV</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1831,7 +1984,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1881,26 +2034,54 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>99992600009</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>20122700029</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>STORAGE</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="D3" t="n">
         <v>5</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E3" t="n">
         <v>0.89</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F3" t="n">
         <v>0.89</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G3" t="n">
         <v>30000</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H3" t="n">
         <v>8000</v>
       </c>
     </row>
@@ -1933,7 +2114,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1988,10 +2169,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20120100021</v>
+        <v>99990100004</v>
       </c>
       <c r="C2" t="n">
-        <v>7908</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -2017,6 +2198,45 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20120100021</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7908</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
candidate power plants assigned to wrong producer
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>43830.99861111111</v>
+        <v>45291.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>44195.99861111111</v>
+        <v>45656.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2020</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="2">
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20.4</v>
+        <v>36.31999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -1199,7 +1199,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.8</v>
+        <v>13.616</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>20.16</v>
+        <v>21.392</v>
       </c>
     </row>
     <row r="7">
@@ -1219,7 +1219,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46.44</v>
+        <v>53.136</v>
       </c>
     </row>
     <row r="8">
@@ -1245,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20150300022</v>
+        <v>99991700006</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1298,16 +1298,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5382609560151593</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1315,24 +1315,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20152800024</v>
+        <v>99990300008</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.40383904661803</v>
+        <v>0.61</v>
       </c>
       <c r="F3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1340,24 +1340,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20153000025</v>
+        <v>20150300022</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>4.2</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3539907794712127</v>
+        <v>0.61</v>
       </c>
       <c r="F4" t="n">
-        <v>3652.9</v>
+        <v>31358.329</v>
       </c>
       <c r="G4" t="n">
-        <v>3652.9</v>
+        <v>31358.329</v>
       </c>
     </row>
     <row r="5">
@@ -1365,24 +1365,24 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20152900027</v>
+        <v>20152800024</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>3.5</v>
       </c>
       <c r="E5" t="n">
-        <v>0.360040798965821</v>
+        <v>0.33</v>
       </c>
       <c r="F5" t="n">
-        <v>20779.02</v>
+        <v>24845.77</v>
       </c>
       <c r="G5" t="n">
-        <v>20779.02</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="6">
@@ -1390,24 +1390,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20151400028</v>
+        <v>20153000025</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="E6" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="F6" t="n">
-        <v>8599</v>
+        <v>3652.9</v>
       </c>
       <c r="G6" t="n">
-        <v>8599</v>
+        <v>3652.9</v>
       </c>
     </row>
     <row r="7">
@@ -1415,23 +1415,73 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
+        <v>20152900027</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>LIGNITE</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F7" t="n">
+        <v>20779.02</v>
+      </c>
+      <c r="G7" t="n">
+        <v>20779.02</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20151400028</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NUCLEAR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8599</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8599</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
         <v>20151700029</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D9" t="n">
         <v>4.5</v>
       </c>
-      <c r="E7" t="n">
-        <v>0.3741421697393409</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="E9" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F9" t="n">
         <v>8194.3025</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G9" t="n">
         <v>8194.3025</v>
       </c>
     </row>
@@ -1483,7 +1533,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1538,17 +1588,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20152400023</v>
+        <v>99992100002</v>
       </c>
       <c r="C2" t="n">
-        <v>47547.50848700004</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1577,17 +1627,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20151200026</v>
+        <v>99992400003</v>
       </c>
       <c r="C3" t="n">
-        <v>8858.749999999998</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1616,17 +1666,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20152100030</v>
+        <v>99992300007</v>
       </c>
       <c r="C4" t="n">
-        <v>53555.51607579708</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1655,35 +1705,152 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>20152400023</v>
+      </c>
+      <c r="C5" t="n">
+        <v>47547.50848700004</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20151200026</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8858.749999999998</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>RunOfRiver</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20152100030</v>
+      </c>
+      <c r="C7" t="n">
+        <v>53555.51607579708</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
         <v>20152300031</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C8" t="n">
         <v>10271.8</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D8" t="n">
         <v>2.7</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1700,7 +1867,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1743,6 +1910,34 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99992600009</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1774,7 +1969,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1829,10 +2024,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20150100021</v>
+        <v>99990100004</v>
       </c>
       <c r="C2" t="n">
-        <v>4644.4034</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -1858,6 +2053,45 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20150100021</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4644.4034</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
corrected again capacity market
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45291.99861111111</v>
+        <v>44196.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>45656.99861111111</v>
+        <v>44560.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1149,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1159,7 +1159,10 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2024</v>
+        <v>2020</v>
+      </c>
+      <c r="C1" s="6" t="n">
+        <v>2021</v>
       </c>
     </row>
     <row r="2">
@@ -1169,8 +1172,9 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>36.31999999999999</v>
-      </c>
+        <v>24.38</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -1181,6 +1185,7 @@
       <c r="B3" t="n">
         <v>1.69</v>
       </c>
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -1191,6 +1196,7 @@
       <c r="B4" t="n">
         <v>3.96</v>
       </c>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -1199,8 +1205,9 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13.616</v>
-      </c>
+        <v>11.504</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -1209,8 +1216,9 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.392</v>
-      </c>
+        <v>20.468</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -1219,8 +1227,9 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>53.136</v>
-      </c>
+        <v>48.114</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -1229,6 +1238,11 @@
         </is>
       </c>
       <c r="B8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>./timeseries/demand/load.csv</t>
         </is>
@@ -1245,7 +1259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99991700006</v>
+        <v>20150300022</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1298,16 +1312,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E2" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>31358.329</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>31358.329</v>
       </c>
     </row>
     <row r="3">
@@ -1315,24 +1329,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99990300008</v>
+        <v>20152800024</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="E3" t="n">
-        <v>0.61</v>
+        <v>0.33</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>24845.77</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="4">
@@ -1340,24 +1354,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20150300022</v>
+        <v>20153000025</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4.2</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>0.61</v>
+        <v>0.35</v>
       </c>
       <c r="F4" t="n">
-        <v>31358.329</v>
+        <v>3652.9</v>
       </c>
       <c r="G4" t="n">
-        <v>31358.329</v>
+        <v>3652.9</v>
       </c>
     </row>
     <row r="5">
@@ -1365,11 +1379,11 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20152800024</v>
+        <v>20152900027</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1379,10 +1393,10 @@
         <v>0.33</v>
       </c>
       <c r="F5" t="n">
-        <v>24845.77</v>
+        <v>20779.02</v>
       </c>
       <c r="G5" t="n">
-        <v>24845.77</v>
+        <v>20779.02</v>
       </c>
     </row>
     <row r="6">
@@ -1390,24 +1404,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20153000025</v>
+        <v>20151400028</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="F6" t="n">
-        <v>3652.9</v>
+        <v>8599</v>
       </c>
       <c r="G6" t="n">
-        <v>3652.9</v>
+        <v>8599</v>
       </c>
     </row>
     <row r="7">
@@ -1415,73 +1429,23 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20152900027</v>
+        <v>20151700029</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="E7" t="n">
-        <v>0.33</v>
+        <v>0.43</v>
       </c>
       <c r="F7" t="n">
-        <v>20779.02</v>
+        <v>8194.3025</v>
       </c>
       <c r="G7" t="n">
-        <v>20779.02</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>20151400028</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NUCLEAR</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F8" t="n">
-        <v>8599</v>
-      </c>
-      <c r="G8" t="n">
-        <v>8599</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>20151700029</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F9" t="n">
-        <v>8194.3025</v>
-      </c>
-      <c r="G9" t="n">
         <v>8194.3025</v>
       </c>
     </row>
@@ -1533,7 +1497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1588,17 +1552,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99992100002</v>
+        <v>20152400023</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>47547.50848700004</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1627,17 +1591,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99992400003</v>
+        <v>20212100031</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D3" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1666,17 +1630,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>99992300007</v>
+        <v>20212100032</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D4" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1705,17 +1669,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20152400023</v>
+        <v>20212100034</v>
       </c>
       <c r="C5" t="n">
-        <v>47547.50848700004</v>
+        <v>1000</v>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1744,17 +1708,17 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20151200026</v>
+        <v>20212100037</v>
       </c>
       <c r="C6" t="n">
-        <v>8858.749999999998</v>
+        <v>1000</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1783,10 +1747,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20152100030</v>
+        <v>20212100041</v>
       </c>
       <c r="C7" t="n">
-        <v>53555.51607579708</v>
+        <v>1000</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -1822,35 +1786,308 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
+        <v>20212100046</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20212100052</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20212100059</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20212100067</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20212100076</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20151200026</v>
+      </c>
+      <c r="C13" t="n">
+        <v>8858.749999999998</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>RunOfRiver</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20152100030</v>
+      </c>
+      <c r="C14" t="n">
+        <v>53555.51607579708</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
         <v>20152300031</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C15" t="n">
         <v>10271.8</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D15" t="n">
         <v>2.7</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1867,7 +2104,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1910,34 +2147,6 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>99992600009</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1969,7 +2178,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2024,10 +2233,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99990100004</v>
+        <v>20150100021</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>4644.4034</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -2053,45 +2262,6 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>20150100021</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4644.4034</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
saving capacity market revenues
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45657.99861111111</v>
+        <v>43830.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>46021.99861111111</v>
+        <v>44195.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1149,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1159,10 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2024</v>
-      </c>
-      <c r="C1" s="6" t="n">
-        <v>2025</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="2">
@@ -1172,9 +1169,8 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40.3</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
+        <v>20.4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -1185,7 +1181,6 @@
       <c r="B3" t="n">
         <v>1.69</v>
       </c>
-      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -1196,7 +1191,6 @@
       <c r="B4" t="n">
         <v>3.96</v>
       </c>
-      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -1205,9 +1199,8 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14.32</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
+        <v>10.8</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -1216,9 +1209,8 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.7</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
+        <v>20.16</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -1227,9 +1219,8 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>54.81</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
+        <v>46.44</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -1238,11 +1229,6 @@
         </is>
       </c>
       <c r="B8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
         <is>
           <t>./timeseries/demand/load.csv</t>
         </is>
@@ -1497,7 +1483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1552,17 +1538,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99992100002</v>
+        <v>20152400023</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>47547.50848700004</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1591,17 +1577,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20152400023</v>
+        <v>20151200026</v>
       </c>
       <c r="C3" t="n">
-        <v>47547.50848700004</v>
+        <v>8858.749999999998</v>
       </c>
       <c r="D3" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>RunOfRiver</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1630,10 +1616,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20212100031</v>
+        <v>20152100030</v>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>53555.51607579708</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -1669,17 +1655,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20212100032</v>
+        <v>20152300031</v>
       </c>
       <c r="C5" t="n">
-        <v>1000</v>
+        <v>10271.8</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1698,864 +1684,6 @@
         </is>
       </c>
       <c r="I5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>20212100034</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>20212100037</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>20212100041</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>20212100046</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>20212100052</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>20212100059</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>20212100067</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>20212100076</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>20212100086</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>20222100086</v>
-      </c>
-      <c r="C15" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>20222100087</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>20222100089</v>
-      </c>
-      <c r="C17" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>20222100092</v>
-      </c>
-      <c r="C18" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>20222100096</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>20222100101</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>20222100107</v>
-      </c>
-      <c r="C21" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>20222100114</v>
-      </c>
-      <c r="C22" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="6" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>20222100122</v>
-      </c>
-      <c r="C23" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>20222100131</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>20151200026</v>
-      </c>
-      <c r="C25" t="n">
-        <v>8858.749999999998</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>RunOfRiver</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>20152100030</v>
-      </c>
-      <c r="C26" t="n">
-        <v>53555.51607579708</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>20152300031</v>
-      </c>
-      <c r="C27" t="n">
-        <v>10271.8</v>
-      </c>
-      <c r="D27" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>WindOff</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
correcting FR module json
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>43830.99861111111</v>
+        <v>45291.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>44195.99861111111</v>
+        <v>45656.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2020</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="2">
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20.4</v>
+        <v>36.31999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -1199,7 +1199,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.8</v>
+        <v>13.616</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>20.16</v>
+        <v>21.392</v>
       </c>
     </row>
     <row r="7">
@@ -1219,7 +1219,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46.44</v>
+        <v>53.136</v>
       </c>
     </row>
     <row r="8">
@@ -1245,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20150300022</v>
+        <v>99991700006</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1298,16 +1298,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1315,24 +1315,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20152800024</v>
+        <v>99990300008</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1340,24 +1340,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20153000025</v>
+        <v>20150300022</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>4.2</v>
       </c>
       <c r="E4" t="n">
-        <v>0.35</v>
+        <v>0.61</v>
       </c>
       <c r="F4" t="n">
-        <v>3652.9</v>
+        <v>31358.329</v>
       </c>
       <c r="G4" t="n">
-        <v>3652.9</v>
+        <v>31358.329</v>
       </c>
     </row>
     <row r="5">
@@ -1365,11 +1365,11 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20152900027</v>
+        <v>20152800024</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1379,10 +1379,10 @@
         <v>0.33</v>
       </c>
       <c r="F5" t="n">
-        <v>20779.02</v>
+        <v>24845.77</v>
       </c>
       <c r="G5" t="n">
-        <v>20779.02</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="6">
@@ -1390,24 +1390,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20151400028</v>
+        <v>20153000025</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="E6" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="F6" t="n">
-        <v>8599</v>
+        <v>3652.9</v>
       </c>
       <c r="G6" t="n">
-        <v>8599</v>
+        <v>3652.9</v>
       </c>
     </row>
     <row r="7">
@@ -1415,23 +1415,73 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
+        <v>20152900027</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>LIGNITE</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F7" t="n">
+        <v>20779.02</v>
+      </c>
+      <c r="G7" t="n">
+        <v>20779.02</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20151400028</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NUCLEAR</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8599</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8599</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
         <v>20151700029</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D9" t="n">
         <v>4.5</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E9" t="n">
         <v>0.43</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F9" t="n">
         <v>8194.3025</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G9" t="n">
         <v>8194.3025</v>
       </c>
     </row>
@@ -1483,7 +1533,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1538,17 +1588,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20152400023</v>
+        <v>99992100002</v>
       </c>
       <c r="C2" t="n">
-        <v>47547.50848700004</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1577,17 +1627,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20151200026</v>
+        <v>99992400003</v>
       </c>
       <c r="C3" t="n">
-        <v>8858.749999999998</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1616,17 +1666,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20152100030</v>
+        <v>99992300007</v>
       </c>
       <c r="C4" t="n">
-        <v>53555.51607579708</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1655,35 +1705,152 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>20152400023</v>
+      </c>
+      <c r="C5" t="n">
+        <v>47547.50848700004</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20151200026</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8858.749999999998</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>RunOfRiver</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20152100030</v>
+      </c>
+      <c r="C7" t="n">
+        <v>53555.51607579708</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
         <v>20152300031</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C8" t="n">
         <v>10271.8</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D8" t="n">
         <v>2.7</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1700,7 +1867,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1743,6 +1910,34 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99992600009</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1774,7 +1969,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1829,10 +2024,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20150100021</v>
+        <v>99990100004</v>
       </c>
       <c r="C2" t="n">
-        <v>4644.4034</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -1858,6 +2053,45 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20150100021</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4644.4034</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
corrected reading Cap mechanism revenues
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45291.99861111111</v>
+        <v>45657.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>45656.99861111111</v>
+        <v>46021.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1149,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1161,6 +1161,9 @@
       <c r="B1" s="6" t="n">
         <v>2024</v>
       </c>
+      <c r="C1" s="6" t="n">
+        <v>2025</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -1169,8 +1172,9 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>36.31999999999999</v>
-      </c>
+        <v>40.3</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -1181,6 +1185,7 @@
       <c r="B3" t="n">
         <v>1.69</v>
       </c>
+      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -1191,6 +1196,7 @@
       <c r="B4" t="n">
         <v>3.96</v>
       </c>
+      <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -1199,8 +1205,9 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13.616</v>
-      </c>
+        <v>14.32</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -1209,8 +1216,9 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.392</v>
-      </c>
+        <v>21.7</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -1219,8 +1227,9 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>53.136</v>
-      </c>
+        <v>54.81</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -1229,6 +1238,11 @@
         </is>
       </c>
       <c r="B8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>./timeseries/demand/load.csv</t>
         </is>
@@ -1245,7 +1259,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99991700006</v>
+        <v>20150300022</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1298,16 +1312,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E2" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>31358.329</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>31358.329</v>
       </c>
     </row>
     <row r="3">
@@ -1315,24 +1329,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99990300008</v>
+        <v>20152800024</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="E3" t="n">
-        <v>0.61</v>
+        <v>0.33</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>24845.77</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="4">
@@ -1340,24 +1354,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20150300022</v>
+        <v>20153000025</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4.2</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>0.61</v>
+        <v>0.35</v>
       </c>
       <c r="F4" t="n">
-        <v>31358.329</v>
+        <v>3652.9</v>
       </c>
       <c r="G4" t="n">
-        <v>31358.329</v>
+        <v>3652.9</v>
       </c>
     </row>
     <row r="5">
@@ -1365,11 +1379,11 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20152800024</v>
+        <v>20152900027</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1379,10 +1393,10 @@
         <v>0.33</v>
       </c>
       <c r="F5" t="n">
-        <v>24845.77</v>
+        <v>20779.02</v>
       </c>
       <c r="G5" t="n">
-        <v>24845.77</v>
+        <v>20779.02</v>
       </c>
     </row>
     <row r="6">
@@ -1390,24 +1404,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20153000025</v>
+        <v>20151400028</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="F6" t="n">
-        <v>3652.9</v>
+        <v>8599</v>
       </c>
       <c r="G6" t="n">
-        <v>3652.9</v>
+        <v>8599</v>
       </c>
     </row>
     <row r="7">
@@ -1415,73 +1429,23 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20152900027</v>
+        <v>20151700029</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="E7" t="n">
-        <v>0.33</v>
+        <v>0.43</v>
       </c>
       <c r="F7" t="n">
-        <v>20779.02</v>
+        <v>8194.3025</v>
       </c>
       <c r="G7" t="n">
-        <v>20779.02</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>20151400028</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NUCLEAR</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F8" t="n">
-        <v>8599</v>
-      </c>
-      <c r="G8" t="n">
-        <v>8599</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>20151700029</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F9" t="n">
-        <v>8194.3025</v>
-      </c>
-      <c r="G9" t="n">
         <v>8194.3025</v>
       </c>
     </row>
@@ -1533,7 +1497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1627,10 +1591,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99992400003</v>
+        <v>20152400023</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>47547.50848700004</v>
       </c>
       <c r="D3" t="n">
         <v>1.35</v>
@@ -1666,17 +1630,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>99992300007</v>
+        <v>20212100031</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D4" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1705,17 +1669,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20152400023</v>
+        <v>20212100032</v>
       </c>
       <c r="C5" t="n">
-        <v>47547.50848700004</v>
+        <v>1000</v>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1744,17 +1708,17 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20151200026</v>
+        <v>20212100034</v>
       </c>
       <c r="C6" t="n">
-        <v>8858.749999999998</v>
+        <v>1000</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1783,10 +1747,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20152100030</v>
+        <v>20212100037</v>
       </c>
       <c r="C7" t="n">
-        <v>53555.51607579708</v>
+        <v>1000</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -1822,35 +1786,815 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
+        <v>20212100041</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20212100046</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20212100052</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20212100059</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20212100067</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20212100076</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20212100086</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>20222100086</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20222100087</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20222100089</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20222100092</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20222100096</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20222100101</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20222100107</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20222100114</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>20222100122</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>20222100131</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>20222100141</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>20151200026</v>
+      </c>
+      <c r="C26" t="n">
+        <v>8858.749999999998</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>RunOfRiver</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>20152100030</v>
+      </c>
+      <c r="C27" t="n">
+        <v>53555.51607579708</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
         <v>20152300031</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C28" t="n">
         <v>10271.8</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D28" t="n">
         <v>2.7</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1867,7 +2611,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1910,34 +2654,6 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>99992600009</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1969,7 +2685,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2024,10 +2740,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99990100004</v>
+        <v>20150100021</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>4644.4034</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -2053,45 +2769,6 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>20150100021</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4644.4034</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
corrected missing cm revenues in financial reports
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45657.99861111111</v>
+        <v>46752.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>46021.99861111111</v>
+        <v>47117.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1149,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1164,6 +1164,15 @@
       <c r="C1" s="6" t="n">
         <v>2025</v>
       </c>
+      <c r="D1" s="6" t="n">
+        <v>2026</v>
+      </c>
+      <c r="E1" s="6" t="n">
+        <v>2027</v>
+      </c>
+      <c r="F1" s="6" t="n">
+        <v>2028</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -1172,9 +1181,12 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40.3</v>
+        <v>52.23999999999999</v>
       </c>
       <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -1186,6 +1198,9 @@
         <v>1.69</v>
       </c>
       <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -1197,6 +1212,9 @@
         <v>3.96</v>
       </c>
       <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -1205,9 +1223,12 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14.32</v>
+        <v>16.432</v>
       </c>
       <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -1216,9 +1237,12 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.7</v>
+        <v>22.624</v>
       </c>
       <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -1227,9 +1251,12 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>54.81</v>
+        <v>59.832</v>
       </c>
       <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -1243,6 +1270,21 @@
         </is>
       </c>
       <c r="C8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>./timeseries/demand/load.csv</t>
         </is>
@@ -1259,7 +1301,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1304,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20150300022</v>
+        <v>99991700006</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1312,16 +1354,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1329,24 +1371,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20152800024</v>
+        <v>99990300008</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1354,24 +1396,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20153000025</v>
+        <v>19892800024</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="F4" t="n">
-        <v>3652.9</v>
+        <v>24845.77</v>
       </c>
       <c r="G4" t="n">
-        <v>3652.9</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="5">
@@ -1379,24 +1421,24 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20152900027</v>
+        <v>20230300031</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E5" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F5" t="n">
-        <v>20779.02</v>
+        <v>1000</v>
       </c>
       <c r="G5" t="n">
-        <v>20779.02</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6">
@@ -1404,24 +1446,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20151400028</v>
+        <v>20230300032</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E6" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F6" t="n">
-        <v>8599</v>
+        <v>1000</v>
       </c>
       <c r="G6" t="n">
-        <v>8599</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7">
@@ -1429,7 +1471,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20151700029</v>
+        <v>20230300034</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1437,16 +1479,1016 @@
         </is>
       </c>
       <c r="D7" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20230300037</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20230300041</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20230300046</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20230300052</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20230300059</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20230300067</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20230300076</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>20230300086</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20231700097</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
         <v>4.5</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E16" t="n">
         <v>0.43</v>
       </c>
-      <c r="F7" t="n">
-        <v>8194.3025</v>
-      </c>
-      <c r="G7" t="n">
-        <v>8194.3025</v>
+      <c r="F16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20231700109</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20231700122</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20231700136</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20231700151</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20231700167</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20231700184</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>20231700202</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>20231700221</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>20231700241</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>20231700262</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>20260301984</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>20260301988</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>20260301993</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>20260301999</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>20260302006</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>20260302014</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>20260302023</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>20260302033</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>20260302044</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>20260302056</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>20260302069</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>20261701981</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>20261702083</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>20261702098</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>20261702114</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>20261702131</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>20261702149</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>20261702168</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>20261702188</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>20261702209</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>20261702231</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1497,7 +2539,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1591,10 +2633,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20152400023</v>
+        <v>99992400003</v>
       </c>
       <c r="C3" t="n">
-        <v>47547.50848700004</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>1.35</v>
@@ -1630,17 +2672,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20212100031</v>
+        <v>99992300007</v>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1669,17 +2711,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20212100032</v>
+        <v>20062400023</v>
       </c>
       <c r="C5" t="n">
-        <v>1000</v>
+        <v>47547.50848700004</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1708,7 +2750,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20212100034</v>
+        <v>20212101021</v>
       </c>
       <c r="C6" t="n">
         <v>1000</v>
@@ -1747,7 +2789,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20212100037</v>
+        <v>20212101066</v>
       </c>
       <c r="C7" t="n">
         <v>1000</v>
@@ -1786,7 +2828,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20212100041</v>
+        <v>20212101112</v>
       </c>
       <c r="C8" t="n">
         <v>1000</v>
@@ -1825,7 +2867,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20212100046</v>
+        <v>20212101159</v>
       </c>
       <c r="C9" t="n">
         <v>1000</v>
@@ -1864,7 +2906,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20212100052</v>
+        <v>20212101207</v>
       </c>
       <c r="C10" t="n">
         <v>1000</v>
@@ -1903,7 +2945,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20212100059</v>
+        <v>20212101256</v>
       </c>
       <c r="C11" t="n">
         <v>1000</v>
@@ -1942,7 +2984,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20212100067</v>
+        <v>20212101306</v>
       </c>
       <c r="C12" t="n">
         <v>1000</v>
@@ -1981,7 +3023,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20212100076</v>
+        <v>20212101357</v>
       </c>
       <c r="C13" t="n">
         <v>1000</v>
@@ -2020,7 +3062,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20212100086</v>
+        <v>20212101409</v>
       </c>
       <c r="C14" t="n">
         <v>1000</v>
@@ -2059,7 +3101,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20222100086</v>
+        <v>20212101462</v>
       </c>
       <c r="C15" t="n">
         <v>1000</v>
@@ -2098,7 +3140,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20222100087</v>
+        <v>20212101516</v>
       </c>
       <c r="C16" t="n">
         <v>1000</v>
@@ -2137,7 +3179,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20222100089</v>
+        <v>20222101516</v>
       </c>
       <c r="C17" t="n">
         <v>1000</v>
@@ -2176,7 +3218,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20222100092</v>
+        <v>20222101517</v>
       </c>
       <c r="C18" t="n">
         <v>1000</v>
@@ -2215,7 +3257,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20222100096</v>
+        <v>20222101519</v>
       </c>
       <c r="C19" t="n">
         <v>1000</v>
@@ -2254,7 +3296,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20222100101</v>
+        <v>20222101621</v>
       </c>
       <c r="C20" t="n">
         <v>1000</v>
@@ -2293,7 +3335,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20222100107</v>
+        <v>20222101636</v>
       </c>
       <c r="C21" t="n">
         <v>1000</v>
@@ -2332,7 +3374,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20222100114</v>
+        <v>20222101652</v>
       </c>
       <c r="C22" t="n">
         <v>1000</v>
@@ -2371,7 +3413,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20222100122</v>
+        <v>20222101669</v>
       </c>
       <c r="C23" t="n">
         <v>1000</v>
@@ -2410,7 +3452,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20222100131</v>
+        <v>20222101687</v>
       </c>
       <c r="C24" t="n">
         <v>1000</v>
@@ -2449,7 +3491,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20222100141</v>
+        <v>20222101706</v>
       </c>
       <c r="C25" t="n">
         <v>1000</v>
@@ -2488,17 +3530,17 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20151200026</v>
+        <v>20222101726</v>
       </c>
       <c r="C26" t="n">
-        <v>8858.749999999998</v>
+        <v>1000</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2527,10 +3569,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20152100030</v>
+        <v>20222101747</v>
       </c>
       <c r="C27" t="n">
-        <v>53555.51607579708</v>
+        <v>1000</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -2566,35 +3608,1985 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20152300031</v>
+        <v>20222400592</v>
       </c>
       <c r="C28" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>20222400626</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>20222400661</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>20222400697</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>20222400734</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>20222400772</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>20222400811</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>20222400851</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>20222400892</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>20222400934</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>20222400977</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>20232101813</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>20232101825</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>20232101838</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>20232101852</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>20232101867</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>20232101883</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>20232101900</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>20232101918</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>20232101937</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="6" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>20232101957</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>20232101978</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="6" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>20242101978</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>20242101979</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>20242102254</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>20242102278</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="6" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>20242102303</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>20242301522</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D55" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>20242301526</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D56" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>20242301531</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D57" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="6" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>20242301537</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D58" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>20242301544</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D59" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="6" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>20242301552</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D60" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>20242301561</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D61" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>20242301571</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D62" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>20242301582</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D63" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="6" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>20242301594</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D64" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>20242301607</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D65" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="6" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>20242401747</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="6" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>20242401748</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="6" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>20242401750</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>20242401753</v>
+      </c>
+      <c r="C69" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="6" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>20242401757</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>20242401762</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="6" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>20242401768</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D72" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="6" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>20242401775</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="6" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>20242401783</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>20242401792</v>
+      </c>
+      <c r="C75" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D75" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="6" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>20242401802</v>
+      </c>
+      <c r="C76" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="6" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>20102100030</v>
+      </c>
+      <c r="C77" t="n">
+        <v>53555.51607579708</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="6" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>20142300031</v>
+      </c>
+      <c r="C78" t="n">
         <v>10271.8</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D78" t="n">
         <v>2.7</v>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E78" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2611,7 +5603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2654,6 +5646,34 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99992600009</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2685,7 +5705,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2740,10 +5760,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20150100021</v>
+        <v>99990100004</v>
       </c>
       <c r="C2" t="n">
-        <v>4644.4034</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -2769,6 +5789,435 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20240100284</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>20240100307</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>20240100331</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20240100356</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20240100382</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20240100409</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20240100437</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20240100466</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20240100496</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20240100527</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20240100559</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
Integrated new cap mechs
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45657.99861111111</v>
+        <v>46752.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>46021.99861111111</v>
+        <v>47117.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1149,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1164,6 +1164,15 @@
       <c r="C1" s="6" t="n">
         <v>2025</v>
       </c>
+      <c r="D1" s="6" t="n">
+        <v>2026</v>
+      </c>
+      <c r="E1" s="6" t="n">
+        <v>2027</v>
+      </c>
+      <c r="F1" s="6" t="n">
+        <v>2028</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -1172,9 +1181,12 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40.3</v>
+        <v>52.23999999999999</v>
       </c>
       <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -1186,6 +1198,9 @@
         <v>1.69</v>
       </c>
       <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -1197,6 +1212,9 @@
         <v>3.96</v>
       </c>
       <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -1205,9 +1223,12 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>14.32</v>
+        <v>16.432</v>
       </c>
       <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -1216,9 +1237,12 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.7</v>
+        <v>22.624</v>
       </c>
       <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -1227,9 +1251,12 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>54.81</v>
+        <v>59.832</v>
       </c>
       <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -1243,6 +1270,21 @@
         </is>
       </c>
       <c r="C8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>./timeseries/demand/load.csv</t>
         </is>
@@ -1259,7 +1301,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1304,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20150300022</v>
+        <v>99991700006</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1312,16 +1354,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1329,24 +1371,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20152800024</v>
+        <v>99990300008</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1354,24 +1396,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20153000025</v>
+        <v>19892800024</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="F4" t="n">
-        <v>3652.9</v>
+        <v>24845.77</v>
       </c>
       <c r="G4" t="n">
-        <v>3652.9</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="5">
@@ -1379,24 +1421,24 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20152900027</v>
+        <v>20230300031</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E5" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F5" t="n">
-        <v>20779.02</v>
+        <v>1000</v>
       </c>
       <c r="G5" t="n">
-        <v>20779.02</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6">
@@ -1404,24 +1446,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20151400028</v>
+        <v>20230300032</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E6" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F6" t="n">
-        <v>8599</v>
+        <v>1000</v>
       </c>
       <c r="G6" t="n">
-        <v>8599</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7">
@@ -1429,7 +1471,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20151700029</v>
+        <v>20230300034</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1437,16 +1479,1016 @@
         </is>
       </c>
       <c r="D7" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20230300037</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20230300041</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20230300046</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20230300052</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20230300059</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20230300067</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20230300076</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>20230300086</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20231700097</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
         <v>4.5</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E16" t="n">
         <v>0.43</v>
       </c>
-      <c r="F7" t="n">
-        <v>8194.3025</v>
-      </c>
-      <c r="G7" t="n">
-        <v>8194.3025</v>
+      <c r="F16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20231700109</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20231700122</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20231700136</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20231700151</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20231700167</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20231700184</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>20231700202</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>20231700221</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>20231700241</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>20231700262</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>20260301984</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>20260301988</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>20260301993</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>20260301999</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>20260302006</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F31" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>20260302014</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>20260302023</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F33" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>20260302033</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>20260302044</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F35" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>20260302056</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>20260302069</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>20261701981</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>20261702083</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>20261702098</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>20261702114</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>20261702131</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>20261702149</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>20261702168</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>20261702188</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F45" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>20261702209</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G46" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>20261702231</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F47" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1497,7 +2539,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1591,10 +2633,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20152400023</v>
+        <v>99992400003</v>
       </c>
       <c r="C3" t="n">
-        <v>47547.50848700004</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>1.35</v>
@@ -1630,17 +2672,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20212100031</v>
+        <v>99992300007</v>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1669,17 +2711,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20212100032</v>
+        <v>20062400023</v>
       </c>
       <c r="C5" t="n">
-        <v>1000</v>
+        <v>47547.50848700004</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1708,7 +2750,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20212100034</v>
+        <v>20212101021</v>
       </c>
       <c r="C6" t="n">
         <v>1000</v>
@@ -1747,7 +2789,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20212100037</v>
+        <v>20212101066</v>
       </c>
       <c r="C7" t="n">
         <v>1000</v>
@@ -1786,7 +2828,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20212100041</v>
+        <v>20212101112</v>
       </c>
       <c r="C8" t="n">
         <v>1000</v>
@@ -1825,7 +2867,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20212100046</v>
+        <v>20212101159</v>
       </c>
       <c r="C9" t="n">
         <v>1000</v>
@@ -1864,7 +2906,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20212100052</v>
+        <v>20212101207</v>
       </c>
       <c r="C10" t="n">
         <v>1000</v>
@@ -1903,7 +2945,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20212100059</v>
+        <v>20212101256</v>
       </c>
       <c r="C11" t="n">
         <v>1000</v>
@@ -1942,7 +2984,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20212100067</v>
+        <v>20212101306</v>
       </c>
       <c r="C12" t="n">
         <v>1000</v>
@@ -1981,7 +3023,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20212100076</v>
+        <v>20212101357</v>
       </c>
       <c r="C13" t="n">
         <v>1000</v>
@@ -2020,7 +3062,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20212100086</v>
+        <v>20212101409</v>
       </c>
       <c r="C14" t="n">
         <v>1000</v>
@@ -2059,7 +3101,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20222100086</v>
+        <v>20212101462</v>
       </c>
       <c r="C15" t="n">
         <v>1000</v>
@@ -2098,7 +3140,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20222100087</v>
+        <v>20212101516</v>
       </c>
       <c r="C16" t="n">
         <v>1000</v>
@@ -2137,7 +3179,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20222100089</v>
+        <v>20222101516</v>
       </c>
       <c r="C17" t="n">
         <v>1000</v>
@@ -2176,7 +3218,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20222100092</v>
+        <v>20222101517</v>
       </c>
       <c r="C18" t="n">
         <v>1000</v>
@@ -2215,7 +3257,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20222100096</v>
+        <v>20222101519</v>
       </c>
       <c r="C19" t="n">
         <v>1000</v>
@@ -2254,7 +3296,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20222100101</v>
+        <v>20222101621</v>
       </c>
       <c r="C20" t="n">
         <v>1000</v>
@@ -2293,7 +3335,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20222100107</v>
+        <v>20222101636</v>
       </c>
       <c r="C21" t="n">
         <v>1000</v>
@@ -2332,7 +3374,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20222100114</v>
+        <v>20222101652</v>
       </c>
       <c r="C22" t="n">
         <v>1000</v>
@@ -2371,7 +3413,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20222100122</v>
+        <v>20222101669</v>
       </c>
       <c r="C23" t="n">
         <v>1000</v>
@@ -2410,7 +3452,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20222100131</v>
+        <v>20222101687</v>
       </c>
       <c r="C24" t="n">
         <v>1000</v>
@@ -2449,17 +3491,17 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20151200026</v>
+        <v>20222101706</v>
       </c>
       <c r="C25" t="n">
-        <v>8858.749999999998</v>
+        <v>1000</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2488,10 +3530,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20152100030</v>
+        <v>20222101726</v>
       </c>
       <c r="C26" t="n">
-        <v>53555.51607579708</v>
+        <v>1000</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -2527,35 +3569,2024 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20152300031</v>
+        <v>20222101747</v>
       </c>
       <c r="C27" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>20222400592</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>20222400626</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>20222400661</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>20222400697</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>20222400734</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>20222400772</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>20222400811</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>20222400851</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>20222400892</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>20222400934</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>20222400977</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>20232101813</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>20232101825</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>20232101838</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>20232101852</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>20232101867</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>20232101883</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>20232101900</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>20232101918</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>20232101937</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="6" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>20232101957</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>20232101978</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="6" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>20242101978</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>20242101979</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>20242102254</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>20242102278</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="6" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>20242102303</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>20242301522</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D55" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>20242301526</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D56" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>20242301531</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D57" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="6" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>20242301537</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D58" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>20242301544</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D59" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="6" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>20242301552</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D60" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>20242301561</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D61" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>20242301571</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D62" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>20242301582</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D63" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="6" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>20242301594</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D64" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>20242301607</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D65" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="6" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>20242401747</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="6" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>20242401748</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="6" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>20242401750</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>20242401753</v>
+      </c>
+      <c r="C69" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="6" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>20242401757</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>20242401762</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="6" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>20242401768</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D72" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="6" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>20242401775</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="6" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>20242401783</v>
+      </c>
+      <c r="C74" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>20242401792</v>
+      </c>
+      <c r="C75" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D75" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="6" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>20242401802</v>
+      </c>
+      <c r="C76" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="6" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>20102100030</v>
+      </c>
+      <c r="C77" t="n">
+        <v>53555.51607579708</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="6" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>20142300031</v>
+      </c>
+      <c r="C78" t="n">
         <v>10271.8</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D78" t="n">
         <v>2.7</v>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="E78" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2572,7 +5603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2615,6 +5646,34 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99992600009</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2646,7 +5705,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2701,10 +5760,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20150100021</v>
+        <v>99990100004</v>
       </c>
       <c r="C2" t="n">
-        <v>4644.4034</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -2730,6 +5789,435 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20240100284</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>20240100307</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>20240100331</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20240100356</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20240100382</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20240100409</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20240100437</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20240100466</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20240100496</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20240100527</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20240100559</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
testing slow dismantling expectations
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45291.99861111111</v>
+        <v>43830.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>45656.99861111111</v>
+        <v>44195.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2024</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="2">
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>36.31999999999999</v>
+        <v>20.4</v>
       </c>
     </row>
     <row r="3">
@@ -1199,7 +1199,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13.616</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.392</v>
+        <v>20.16</v>
       </c>
     </row>
     <row r="7">
@@ -1219,7 +1219,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>53.136</v>
+        <v>46.44</v>
       </c>
     </row>
     <row r="8">
@@ -1245,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99991700006</v>
+        <v>19920300022</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1298,16 +1298,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E2" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>31358.329</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>31358.329</v>
       </c>
     </row>
     <row r="3">
@@ -1315,24 +1315,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99990300008</v>
+        <v>19892800024</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="E3" t="n">
-        <v>0.61</v>
+        <v>0.33</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>24845.77</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="4">
@@ -1340,24 +1340,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>19892800024</v>
+        <v>19843000025</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="F4" t="n">
-        <v>24845.77</v>
+        <v>3652.9</v>
       </c>
       <c r="G4" t="n">
-        <v>24845.77</v>
+        <v>3652.9</v>
       </c>
     </row>
     <row r="5">
@@ -1365,24 +1365,24 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20230300031</v>
+        <v>19822900027</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="E5" t="n">
-        <v>0.61</v>
+        <v>0.33</v>
       </c>
       <c r="F5" t="n">
-        <v>1000</v>
+        <v>20779.02</v>
       </c>
       <c r="G5" t="n">
-        <v>1000</v>
+        <v>20779.02</v>
       </c>
     </row>
     <row r="6">
@@ -1390,24 +1390,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20230300032</v>
+        <v>19851400028</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.61</v>
+        <v>0.33</v>
       </c>
       <c r="F6" t="n">
-        <v>1000</v>
+        <v>8599</v>
       </c>
       <c r="G6" t="n">
-        <v>1000</v>
+        <v>8599</v>
       </c>
     </row>
     <row r="7">
@@ -1415,7 +1415,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20230300034</v>
+        <v>19921700029</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1423,141 +1423,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E7" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F7" t="n">
-        <v>1000</v>
+        <v>8194.3025</v>
       </c>
       <c r="G7" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>20230300037</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>20230300041</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>20230300046</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>20230300052</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G11" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>19851400028</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>NUCLEAR</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F12" t="n">
-        <v>8599</v>
-      </c>
-      <c r="G12" t="n">
-        <v>8599</v>
+        <v>8194.3025</v>
       </c>
     </row>
   </sheetData>
@@ -1608,7 +1483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1663,17 +1538,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99992100002</v>
+        <v>20062400023</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>47547.50848700004</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1702,17 +1577,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99992400003</v>
+        <v>19641200026</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>8858.749999999998</v>
       </c>
       <c r="D3" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>RunOfRiver</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1741,17 +1616,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20062400023</v>
+        <v>20102100030</v>
       </c>
       <c r="C4" t="n">
-        <v>47547.50848700004</v>
+        <v>53555.51607579708</v>
       </c>
       <c r="D4" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1780,17 +1655,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20102100030</v>
+        <v>20142300031</v>
       </c>
       <c r="C5" t="n">
-        <v>53555.51607579708</v>
+        <v>10271.8</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1809,45 +1684,6 @@
         </is>
       </c>
       <c r="I5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>20142300031</v>
-      </c>
-      <c r="C6" t="n">
-        <v>10271.8</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>WindOff</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1938,7 +1774,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1993,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99990100004</v>
+        <v>20000100021</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>4644.4034</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -2022,45 +1858,6 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>20000100021</v>
-      </c>
-      <c r="C3" t="n">
-        <v>4644.4034</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
revising future market clearing
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>44926.99861111111</v>
+        <v>46752.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>45290.99861111111</v>
+        <v>47117.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1149,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1159,16 +1159,19 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2020</v>
+        <v>2024</v>
       </c>
       <c r="C1" s="6" t="n">
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="D1" s="6" t="n">
-        <v>2022</v>
+        <v>2026</v>
       </c>
       <c r="E1" s="6" t="n">
-        <v>2023</v>
+        <v>2027</v>
+      </c>
+      <c r="F1" s="6" t="n">
+        <v>2028</v>
       </c>
     </row>
     <row r="2">
@@ -1178,11 +1181,12 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>32.34</v>
+        <v>52.23999999999999</v>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -1196,6 +1200,7 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -1209,6 +1214,7 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -1217,11 +1223,12 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.912</v>
+        <v>16.432</v>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -1230,11 +1237,12 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.084</v>
+        <v>22.624</v>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -1243,11 +1251,12 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>51.462</v>
+        <v>59.832</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -1271,6 +1280,11 @@
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>./timeseries/demand/load.csv</t>
         </is>
@@ -1287,7 +1301,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1332,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>19920300022</v>
+        <v>99991700006</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1340,16 +1354,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1357,24 +1371,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>19892800024</v>
+        <v>99990300008</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1382,7 +1396,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20230300031</v>
+        <v>19920300022</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1396,10 +1410,10 @@
         <v>0.61</v>
       </c>
       <c r="F4" t="n">
-        <v>1000</v>
+        <v>31358.329</v>
       </c>
       <c r="G4" t="n">
-        <v>1000</v>
+        <v>31358.329</v>
       </c>
     </row>
     <row r="5">
@@ -1407,7 +1421,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20230300032</v>
+        <v>20230300031</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1432,7 +1446,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20230300034</v>
+        <v>20230300032</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1457,7 +1471,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20230300037</v>
+        <v>20230300034</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1482,7 +1496,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20230300041</v>
+        <v>20230300037</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1507,7 +1521,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20230300046</v>
+        <v>20230300041</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1532,7 +1546,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20230300052</v>
+        <v>20230300046</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1557,7 +1571,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20230300059</v>
+        <v>20230300052</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1582,7 +1596,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20230300067</v>
+        <v>20230300059</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1607,7 +1621,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20230300076</v>
+        <v>20230300067</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1632,7 +1646,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20230300086</v>
+        <v>20230300076</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1657,7 +1671,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20231700097</v>
+        <v>20230300086</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1665,10 +1679,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E15" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F15" t="n">
         <v>1000</v>
@@ -1682,7 +1696,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20231700109</v>
+        <v>20231700097</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1707,7 +1721,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20231700122</v>
+        <v>20231700109</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1732,7 +1746,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20231700136</v>
+        <v>20231700122</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1757,7 +1771,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20231700151</v>
+        <v>20231700136</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1782,7 +1796,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20231700167</v>
+        <v>20231700151</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1807,7 +1821,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20231700184</v>
+        <v>20231700167</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1832,7 +1846,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20231700202</v>
+        <v>20231700184</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1857,7 +1871,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20231700221</v>
+        <v>20231700202</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1882,7 +1896,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20231700241</v>
+        <v>20231700221</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1907,7 +1921,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20231700262</v>
+        <v>20231700241</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1932,24 +1946,24 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>19843000025</v>
+        <v>20231700262</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="E26" t="n">
-        <v>0.35</v>
+        <v>0.43</v>
       </c>
       <c r="F26" t="n">
-        <v>3652.9</v>
+        <v>1000</v>
       </c>
       <c r="G26" t="n">
-        <v>3652.9</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="27">
@@ -1957,24 +1971,24 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>19822900027</v>
+        <v>19843000025</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="E27" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="F27" t="n">
-        <v>20779.02</v>
+        <v>3652.9</v>
       </c>
       <c r="G27" t="n">
-        <v>20779.02</v>
+        <v>3652.9</v>
       </c>
     </row>
     <row r="28">
@@ -1982,11 +1996,11 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>19851400028</v>
+        <v>19822900027</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1996,10 +2010,10 @@
         <v>0.33</v>
       </c>
       <c r="F28" t="n">
-        <v>8599</v>
+        <v>20779.02</v>
       </c>
       <c r="G28" t="n">
-        <v>8599</v>
+        <v>20779.02</v>
       </c>
     </row>
     <row r="29">
@@ -2007,23 +2021,48 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
+        <v>19851400028</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>NUCLEAR</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F29" t="n">
+        <v>8599</v>
+      </c>
+      <c r="G29" t="n">
+        <v>8599</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
         <v>19921700029</v>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="D30" t="n">
         <v>4.5</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E30" t="n">
         <v>0.43</v>
       </c>
-      <c r="F29" t="n">
+      <c r="F30" t="n">
         <v>8194.3025</v>
       </c>
-      <c r="G29" t="n">
+      <c r="G30" t="n">
         <v>8194.3025</v>
       </c>
     </row>
@@ -2075,7 +2114,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2130,17 +2169,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20062400023</v>
+        <v>99992100002</v>
       </c>
       <c r="C2" t="n">
-        <v>47547.50848700004</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2169,17 +2208,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20212100811</v>
+        <v>99992400003</v>
       </c>
       <c r="C3" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2208,17 +2247,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20212100851</v>
+        <v>99992300007</v>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -2247,17 +2286,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20212100892</v>
+        <v>20062400023</v>
       </c>
       <c r="C5" t="n">
-        <v>1000</v>
+        <v>47547.50848700004</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2286,7 +2325,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20212100934</v>
+        <v>20212100811</v>
       </c>
       <c r="C6" t="n">
         <v>1000</v>
@@ -2325,7 +2364,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20212100977</v>
+        <v>20212100851</v>
       </c>
       <c r="C7" t="n">
         <v>1000</v>
@@ -2364,7 +2403,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20212101021</v>
+        <v>20212100892</v>
       </c>
       <c r="C8" t="n">
         <v>1000</v>
@@ -2403,7 +2442,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20212101066</v>
+        <v>20212100934</v>
       </c>
       <c r="C9" t="n">
         <v>1000</v>
@@ -2442,7 +2481,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20212101112</v>
+        <v>20212100977</v>
       </c>
       <c r="C10" t="n">
         <v>1000</v>
@@ -2481,7 +2520,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20212101159</v>
+        <v>20212101021</v>
       </c>
       <c r="C11" t="n">
         <v>1000</v>
@@ -2520,7 +2559,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20212101207</v>
+        <v>20212101066</v>
       </c>
       <c r="C12" t="n">
         <v>1000</v>
@@ -2559,7 +2598,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20212101256</v>
+        <v>20212101112</v>
       </c>
       <c r="C13" t="n">
         <v>1000</v>
@@ -2598,7 +2637,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20222101392</v>
+        <v>20212101159</v>
       </c>
       <c r="C14" t="n">
         <v>1000</v>
@@ -2637,7 +2676,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20222101409</v>
+        <v>20212101207</v>
       </c>
       <c r="C15" t="n">
         <v>1000</v>
@@ -2676,7 +2715,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20222101427</v>
+        <v>20212101256</v>
       </c>
       <c r="C16" t="n">
         <v>1000</v>
@@ -2715,7 +2754,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20222101446</v>
+        <v>20222101392</v>
       </c>
       <c r="C17" t="n">
         <v>1000</v>
@@ -2754,7 +2793,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20222101466</v>
+        <v>20222101409</v>
       </c>
       <c r="C18" t="n">
         <v>1000</v>
@@ -2793,7 +2832,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20222101487</v>
+        <v>20222101427</v>
       </c>
       <c r="C19" t="n">
         <v>1000</v>
@@ -2832,7 +2871,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20222101509</v>
+        <v>20222101446</v>
       </c>
       <c r="C20" t="n">
         <v>1000</v>
@@ -2871,7 +2910,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20222101532</v>
+        <v>20222101466</v>
       </c>
       <c r="C21" t="n">
         <v>1000</v>
@@ -2910,7 +2949,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20222101556</v>
+        <v>20222101487</v>
       </c>
       <c r="C22" t="n">
         <v>1000</v>
@@ -2949,7 +2988,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20222101581</v>
+        <v>20222101509</v>
       </c>
       <c r="C23" t="n">
         <v>1000</v>
@@ -2988,7 +3027,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20222101607</v>
+        <v>20222101532</v>
       </c>
       <c r="C24" t="n">
         <v>1000</v>
@@ -3027,17 +3066,17 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20222400592</v>
+        <v>20222101556</v>
       </c>
       <c r="C25" t="n">
         <v>1000</v>
       </c>
       <c r="D25" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3066,17 +3105,17 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20222400626</v>
+        <v>20222101581</v>
       </c>
       <c r="C26" t="n">
         <v>1000</v>
       </c>
       <c r="D26" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3105,17 +3144,17 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20222400661</v>
+        <v>20222101607</v>
       </c>
       <c r="C27" t="n">
         <v>1000</v>
       </c>
       <c r="D27" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3144,7 +3183,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20222400697</v>
+        <v>20222400592</v>
       </c>
       <c r="C28" t="n">
         <v>1000</v>
@@ -3183,7 +3222,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>20222400734</v>
+        <v>20222400626</v>
       </c>
       <c r="C29" t="n">
         <v>1000</v>
@@ -3222,7 +3261,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>20222400772</v>
+        <v>20222400661</v>
       </c>
       <c r="C30" t="n">
         <v>1000</v>
@@ -3261,17 +3300,17 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>20232101628</v>
+        <v>20222400697</v>
       </c>
       <c r="C31" t="n">
         <v>1000</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3300,17 +3339,17 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>20232101635</v>
+        <v>20222400734</v>
       </c>
       <c r="C32" t="n">
         <v>1000</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3339,17 +3378,17 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>20232101643</v>
+        <v>20222400772</v>
       </c>
       <c r="C33" t="n">
         <v>1000</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3378,7 +3417,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>20232101652</v>
+        <v>20232101628</v>
       </c>
       <c r="C34" t="n">
         <v>1000</v>
@@ -3417,7 +3456,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>20232101662</v>
+        <v>20232101635</v>
       </c>
       <c r="C35" t="n">
         <v>1000</v>
@@ -3456,7 +3495,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>20232101673</v>
+        <v>20232101643</v>
       </c>
       <c r="C36" t="n">
         <v>1000</v>
@@ -3495,7 +3534,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>20232101685</v>
+        <v>20232101652</v>
       </c>
       <c r="C37" t="n">
         <v>1000</v>
@@ -3534,7 +3573,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>20232101698</v>
+        <v>20232101662</v>
       </c>
       <c r="C38" t="n">
         <v>1000</v>
@@ -3573,7 +3612,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>20232101712</v>
+        <v>20232101673</v>
       </c>
       <c r="C39" t="n">
         <v>1000</v>
@@ -3612,7 +3651,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>20232101727</v>
+        <v>20232101685</v>
       </c>
       <c r="C40" t="n">
         <v>1000</v>
@@ -3651,7 +3690,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>20232101743</v>
+        <v>20232101698</v>
       </c>
       <c r="C41" t="n">
         <v>1000</v>
@@ -3690,17 +3729,17 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20232401256</v>
+        <v>20232101712</v>
       </c>
       <c r="C42" t="n">
         <v>1000</v>
       </c>
       <c r="D42" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3729,17 +3768,17 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20232401257</v>
+        <v>20232101727</v>
       </c>
       <c r="C43" t="n">
         <v>1000</v>
       </c>
       <c r="D43" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3768,17 +3807,17 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>20232401347</v>
+        <v>20232101743</v>
       </c>
       <c r="C44" t="n">
         <v>1000</v>
       </c>
       <c r="D44" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3807,7 +3846,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20232401361</v>
+        <v>20232401256</v>
       </c>
       <c r="C45" t="n">
         <v>1000</v>
@@ -3846,7 +3885,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20232401376</v>
+        <v>20232401257</v>
       </c>
       <c r="C46" t="n">
         <v>1000</v>
@@ -3885,17 +3924,17 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>19641200026</v>
+        <v>20232401347</v>
       </c>
       <c r="C47" t="n">
-        <v>8858.749999999998</v>
+        <v>1000</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3924,17 +3963,17 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>20102100030</v>
+        <v>20232401361</v>
       </c>
       <c r="C48" t="n">
-        <v>53555.51607579708</v>
+        <v>1000</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -3963,35 +4002,815 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
+        <v>20232401376</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="6" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>20242301259</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D50" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>20242301262</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D51" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>20242301266</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D52" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>20242301271</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D53" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="6" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>20242301277</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D54" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>20242301284</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D55" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>20242301292</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D56" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>20242301301</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D57" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="6" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>20242301311</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D58" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>20242301322</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D59" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="6" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>20242301334</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D60" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>20242401607</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>20242401608</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>20242401610</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="6" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>20242401613</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>20242401617</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="6" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>20242401622</v>
+      </c>
+      <c r="C66" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="6" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>19641200026</v>
+      </c>
+      <c r="C67" t="n">
+        <v>8858.749999999998</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>RunOfRiver</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="6" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>20102100030</v>
+      </c>
+      <c r="C68" t="n">
+        <v>53555.51607579708</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
         <v>20142300031</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C69" t="n">
         <v>10271.8</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D69" t="n">
         <v>2.7</v>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="E69" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -4008,7 +4827,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4051,6 +4870,34 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99992600009</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4082,7 +4929,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4137,10 +4984,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20000100021</v>
+        <v>99990100004</v>
       </c>
       <c r="C2" t="n">
-        <v>4644.4034</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -4166,6 +5013,474 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20000100021</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4644.4034</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>20240100284</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>20240100307</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20240100331</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20240100356</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20240100382</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20240100409</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20240100437</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20240100466</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20240100496</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20240100527</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20240100559</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
changing paths of new module
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45291.99861111111</v>
+        <v>47118.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>45656.99861111111</v>
+        <v>47482.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1149,7 +1149,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1159,7 +1159,34 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C1" s="6" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="6" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E1" s="6" t="n">
+        <v>2023</v>
+      </c>
+      <c r="F1" s="6" t="n">
         <v>2024</v>
+      </c>
+      <c r="G1" s="6" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H1" s="6" t="n">
+        <v>2026</v>
+      </c>
+      <c r="I1" s="6" t="n">
+        <v>2027</v>
+      </c>
+      <c r="J1" s="6" t="n">
+        <v>2028</v>
+      </c>
+      <c r="K1" s="6" t="n">
+        <v>2029</v>
       </c>
     </row>
     <row r="2">
@@ -1169,8 +1196,17 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>36.31999999999999</v>
-      </c>
+        <v>56.21999999999999</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -1181,6 +1217,15 @@
       <c r="B3" t="n">
         <v>1.69</v>
       </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -1191,6 +1236,15 @@
       <c r="B4" t="n">
         <v>3.96</v>
       </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -1199,8 +1253,17 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13.616</v>
-      </c>
+        <v>17.136</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -1209,8 +1272,17 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.392</v>
-      </c>
+        <v>22.932</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -1219,8 +1291,17 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>53.136</v>
-      </c>
+        <v>61.506</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -1229,6 +1310,51 @@
         </is>
       </c>
       <c r="B8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>./timeseries/demand/load.csv</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>./timeseries/demand/load.csv</t>
         </is>
@@ -1245,7 +1371,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99991700006</v>
+        <v>19920300022</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1298,16 +1424,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E2" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>31358.329</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>31358.329</v>
       </c>
     </row>
     <row r="3">
@@ -1315,24 +1441,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99990300008</v>
+        <v>19892800024</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="E3" t="n">
-        <v>0.61</v>
+        <v>0.33</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>24845.77</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="4">
@@ -1340,24 +1466,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>19892800024</v>
+        <v>20230300031</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E4" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F4" t="n">
-        <v>24845.77</v>
+        <v>1000</v>
       </c>
       <c r="G4" t="n">
-        <v>24845.77</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5">
@@ -1365,24 +1491,624 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>20230300032</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20230300034</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20230300037</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20230300041</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20230300046</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20230300052</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20230300059</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20230300067</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20230300076</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20230300086</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>20231700097</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20231700109</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20231700122</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20231700136</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20231700151</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20231700167</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20231700184</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20231700202</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>20231700221</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>20231700241</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>20231700262</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>19843000025</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>OIL</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>6</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F26" t="n">
+        <v>3652.9</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3652.9</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>19822900027</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>LIGNITE</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F27" t="n">
+        <v>20779.02</v>
+      </c>
+      <c r="G27" t="n">
+        <v>20779.02</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
         <v>19851400028</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>NUCLEAR</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D28" t="n">
         <v>3.5</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E28" t="n">
         <v>0.33</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F28" t="n">
         <v>8599</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G28" t="n">
         <v>8599</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>19921700029</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F29" t="n">
+        <v>8194.3025</v>
+      </c>
+      <c r="G29" t="n">
+        <v>8194.3025</v>
       </c>
     </row>
   </sheetData>
@@ -1433,7 +2159,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1488,17 +2214,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99992100002</v>
+        <v>20062400023</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>47547.50848700004</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1527,17 +2253,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99992400003</v>
+        <v>20212100811</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D3" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1566,17 +2292,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>99992300007</v>
+        <v>20212100851</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D4" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1605,17 +2331,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20062400023</v>
+        <v>20212100892</v>
       </c>
       <c r="C5" t="n">
-        <v>47547.50848700004</v>
+        <v>1000</v>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1644,10 +2370,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20102100030</v>
+        <v>20212100934</v>
       </c>
       <c r="C6" t="n">
-        <v>53555.51607579708</v>
+        <v>1000</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -1683,35 +2409,2336 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
+        <v>20212100977</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20212101021</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20212101066</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20212101112</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20212101159</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20212101207</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20212101256</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20222101392</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>20222101409</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20222101427</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20222101446</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20222101466</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20222101487</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20222101509</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20222101532</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20222101556</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>20222101581</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>20222101607</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>20222400592</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>20222400626</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>20222400661</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>20222400697</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>20222400734</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>20222400772</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>20232101628</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>20232101635</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>20232101643</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>20232101652</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>20232101662</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>20232101673</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>20232101685</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>20232101698</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>20232101712</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>20232101727</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>20232101743</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>20232401256</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>20232401257</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>20232401347</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>20232401361</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>20232401376</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>20242301259</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D47" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="6" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>20242301262</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D48" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>20242301266</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D49" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="6" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>20242301271</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D50" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>20242301277</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D51" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>20242301284</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D52" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>20242301292</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D53" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="6" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>20242301301</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D54" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>20242301311</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D55" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>20242301322</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D56" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>20242301334</v>
+      </c>
+      <c r="C57" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D57" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="6" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>20242401607</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>20242401608</v>
+      </c>
+      <c r="C59" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="6" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>20242401610</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>20242401613</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="6" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>20242401617</v>
+      </c>
+      <c r="C62" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>20242401622</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="6" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>19641200026</v>
+      </c>
+      <c r="C64" t="n">
+        <v>8858.749999999998</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>RunOfRiver</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>20102100030</v>
+      </c>
+      <c r="C65" t="n">
+        <v>53555.51607579708</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="6" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
         <v>20142300031</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C66" t="n">
         <v>10271.8</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D66" t="n">
         <v>2.7</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E66" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1728,7 +4755,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1771,34 +4798,6 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>99992600009</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1830,7 +4829,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1885,10 +4884,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99990100004</v>
+        <v>20000100021</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>4644.4034</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -1924,10 +4923,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20000100021</v>
+        <v>20240100284</v>
       </c>
       <c r="C3" t="n">
-        <v>4644.4034</v>
+        <v>1000</v>
       </c>
       <c r="D3" t="n">
         <v>1.9</v>
@@ -1953,6 +4952,396 @@
         </is>
       </c>
       <c r="I3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>20240100307</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>20240100331</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20240100356</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20240100382</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20240100409</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20240100437</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20240100466</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20240100496</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20240100527</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20240100559</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
WIP saving loans , downpayments and cash flows
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>43830.99861111111</v>
+        <v>45291.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>44195.99861111111</v>
+        <v>45656.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2020</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="2">
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20.4</v>
+        <v>36.31999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -1199,7 +1199,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.8</v>
+        <v>13.616</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>20.16</v>
+        <v>21.392</v>
       </c>
     </row>
     <row r="7">
@@ -1219,7 +1219,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46.44</v>
+        <v>53.136</v>
       </c>
     </row>
     <row r="8">
@@ -1245,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>19920300022</v>
+        <v>99991700006</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1298,16 +1298,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1315,24 +1315,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>19892800024</v>
+        <v>99990300008</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1340,24 +1340,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>19843000025</v>
+        <v>19892800024</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="F4" t="n">
-        <v>3652.9</v>
+        <v>24845.77</v>
       </c>
       <c r="G4" t="n">
-        <v>3652.9</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="5">
@@ -1365,11 +1365,11 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>19822900027</v>
+        <v>19851400028</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1379,60 +1379,10 @@
         <v>0.33</v>
       </c>
       <c r="F5" t="n">
-        <v>20779.02</v>
+        <v>8599</v>
       </c>
       <c r="G5" t="n">
-        <v>20779.02</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>19851400028</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NUCLEAR</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F6" t="n">
         <v>8599</v>
-      </c>
-      <c r="G6" t="n">
-        <v>8599</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>19921700029</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F7" t="n">
-        <v>8194.3025</v>
-      </c>
-      <c r="G7" t="n">
-        <v>8194.3025</v>
       </c>
     </row>
   </sheetData>
@@ -1483,7 +1433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1538,17 +1488,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20062400023</v>
+        <v>99992100002</v>
       </c>
       <c r="C2" t="n">
-        <v>47547.50848700004</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1577,17 +1527,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>19641200026</v>
+        <v>99992400003</v>
       </c>
       <c r="C3" t="n">
-        <v>8858.749999999998</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1616,17 +1566,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20102100030</v>
+        <v>99992300007</v>
       </c>
       <c r="C4" t="n">
-        <v>53555.51607579708</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1655,35 +1605,113 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>20062400023</v>
+      </c>
+      <c r="C5" t="n">
+        <v>47547.50848700004</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20102100030</v>
+      </c>
+      <c r="C6" t="n">
+        <v>53555.51607579708</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
         <v>20142300031</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C7" t="n">
         <v>10271.8</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D7" t="n">
         <v>2.7</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1700,7 +1728,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1743,6 +1771,34 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99992600009</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1774,7 +1830,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1829,10 +1885,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20000100021</v>
+        <v>99990100004</v>
       </c>
       <c r="C2" t="n">
-        <v>4644.4034</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -1858,6 +1914,45 @@
         </is>
       </c>
       <c r="I2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20000100021</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4644.4034</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
adding electricity market revenues to financial results . Channging SR parameters in excel
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>36.31999999999999</v>
+        <v>17.68</v>
       </c>
     </row>
     <row r="3">
@@ -1199,7 +1199,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13.616</v>
+        <v>10.876</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.392</v>
+        <v>23.17066666666667</v>
       </c>
     </row>
     <row r="7">
@@ -1219,7 +1219,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>53.136</v>
+        <v>54.24266666666666</v>
       </c>
     </row>
     <row r="8">
@@ -1245,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1365,23 +1365,73 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>19851400028</v>
+        <v>20230300025</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20230300032</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>19851400029</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>NUCLEAR</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D7" t="n">
         <v>3.5</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E7" t="n">
         <v>0.33</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F7" t="n">
         <v>8599</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G7" t="n">
         <v>8599</v>
       </c>
     </row>
@@ -1433,7 +1483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1566,17 +1616,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>99992300007</v>
+        <v>20062400023</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>47547.50848700004</v>
       </c>
       <c r="D4" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1605,17 +1655,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20062400023</v>
+        <v>20102100031</v>
       </c>
       <c r="C5" t="n">
-        <v>47547.50848700004</v>
+        <v>53555.51607579708</v>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1644,17 +1694,17 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20102100030</v>
+        <v>20142300032</v>
       </c>
       <c r="C6" t="n">
-        <v>53555.51607579708</v>
+        <v>10271.8</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1673,45 +1723,6 @@
         </is>
       </c>
       <c r="I6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>20142300031</v>
-      </c>
-      <c r="C7" t="n">
-        <v>10271.8</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>WindOff</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1728,7 +1739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1771,34 +1782,6 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>99992600009</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing demand for amiris
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -26,8 +26,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -109,7 +109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -121,7 +121,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,8 +1015,8 @@
           <t>StartTime</t>
         </is>
       </c>
-      <c r="B2" s="7" t="n">
-        <v>47118.99861111111</v>
+      <c r="B2" s="8" t="n">
+        <v>43830.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1024,8 +1025,8 @@
           <t>StopTime</t>
         </is>
       </c>
-      <c r="B3" s="7" t="n">
-        <v>47482.99861111111</v>
+      <c r="B3" s="8" t="n">
+        <v>44195.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1148,7 +1149,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1160,33 +1161,6 @@
       <c r="B1" s="6" t="n">
         <v>2020</v>
       </c>
-      <c r="C1" s="6" t="n">
-        <v>2021</v>
-      </c>
-      <c r="D1" s="6" t="n">
-        <v>2022</v>
-      </c>
-      <c r="E1" s="6" t="n">
-        <v>2023</v>
-      </c>
-      <c r="F1" s="6" t="n">
-        <v>2024</v>
-      </c>
-      <c r="G1" s="6" t="n">
-        <v>2025</v>
-      </c>
-      <c r="H1" s="6" t="n">
-        <v>2026</v>
-      </c>
-      <c r="I1" s="6" t="n">
-        <v>2027</v>
-      </c>
-      <c r="J1" s="6" t="n">
-        <v>2028</v>
-      </c>
-      <c r="K1" s="6" t="n">
-        <v>2029</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -1195,17 +1169,8 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14.28</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+        <v>20.4</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
@@ -1216,15 +1181,6 @@
       <c r="B3" t="n">
         <v>1.69</v>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="inlineStr">
@@ -1235,15 +1191,6 @@
       <c r="B4" t="n">
         <v>3.96</v>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="inlineStr">
@@ -1252,17 +1199,8 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.971</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+        <v>10.8</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
@@ -1271,17 +1209,8 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>26.934</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+        <v>20.16</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
@@ -1290,17 +1219,8 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>63.996</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+        <v>46.44</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -1310,52 +1230,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>./timeseries/demand/load.csv</t>
+          <t>./amiris_workflow/amiris-config/data/load.csv</t>
         </is>
       </c>
     </row>
@@ -1370,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1440,24 +1315,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20230300031</v>
+        <v>19892800024</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="E3" t="n">
-        <v>0.61</v>
+        <v>0.33</v>
       </c>
       <c r="F3" t="n">
-        <v>1000</v>
+        <v>24845.77</v>
       </c>
       <c r="G3" t="n">
-        <v>1000</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="4">
@@ -1465,7 +1340,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20230300032</v>
+        <v>20140300058</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1490,7 +1365,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20230300034</v>
+        <v>20140300059</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1515,7 +1390,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20230300037</v>
+        <v>20140300060</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1540,7 +1415,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20230300041</v>
+        <v>20140300061</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1565,7 +1440,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20230300046</v>
+        <v>20140300062</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1590,7 +1465,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20230300052</v>
+        <v>20140300063</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1615,7 +1490,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20230300059</v>
+        <v>20140300064</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1640,7 +1515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20230300067</v>
+        <v>20140300065</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1665,7 +1540,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20230300076</v>
+        <v>20140300066</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1690,7 +1565,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20230300086</v>
+        <v>20140300067</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1715,7 +1590,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20231700097</v>
+        <v>20140300068</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1723,10 +1598,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E14" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F14" t="n">
         <v>1000</v>
@@ -1740,7 +1615,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20231700109</v>
+        <v>20141700069</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1765,7 +1640,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20231700122</v>
+        <v>20141700070</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1790,7 +1665,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20231700136</v>
+        <v>20141700071</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1815,7 +1690,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20231700151</v>
+        <v>20141700072</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1840,7 +1715,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20231700167</v>
+        <v>20141700073</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1865,7 +1740,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20231700184</v>
+        <v>20141700074</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1890,7 +1765,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20231700202</v>
+        <v>20141700075</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1915,7 +1790,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20231700221</v>
+        <v>20141700076</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1940,7 +1815,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20231700241</v>
+        <v>20141700077</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1965,7 +1840,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20231700262</v>
+        <v>20141700078</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1990,7 +1865,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20281702015</v>
+        <v>20141700079</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -2015,7 +1890,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20281702016</v>
+        <v>20191700124</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -2040,7 +1915,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20281702018</v>
+        <v>20191700125</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -2065,7 +1940,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20281702021</v>
+        <v>20191700126</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -2090,7 +1965,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>20281702025</v>
+        <v>20191700127</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -2115,24 +1990,124 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>19851400028</v>
+        <v>20191700128</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>19843000129</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>OIL</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>6</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F31" t="n">
+        <v>3652.9</v>
+      </c>
+      <c r="G31" t="n">
+        <v>3652.9</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>19822900131</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>LIGNITE</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F32" t="n">
+        <v>20779.02</v>
+      </c>
+      <c r="G32" t="n">
+        <v>20779.02</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>19851400132</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t>NUCLEAR</t>
         </is>
       </c>
-      <c r="D30" t="n">
+      <c r="D33" t="n">
         <v>3.5</v>
       </c>
-      <c r="E30" t="n">
+      <c r="E33" t="n">
         <v>0.33</v>
       </c>
-      <c r="F30" t="n">
+      <c r="F33" t="n">
         <v>8599</v>
       </c>
-      <c r="G30" t="n">
+      <c r="G33" t="n">
         <v>8599</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>19921700133</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F34" t="n">
+        <v>8194.3025</v>
+      </c>
+      <c r="G34" t="n">
+        <v>8194.3025</v>
       </c>
     </row>
   </sheetData>
@@ -2277,7 +2252,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20212100934</v>
+        <v>20122100025</v>
       </c>
       <c r="C3" t="n">
         <v>1000</v>
@@ -2316,7 +2291,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20212100977</v>
+        <v>20122100026</v>
       </c>
       <c r="C4" t="n">
         <v>1000</v>
@@ -2355,7 +2330,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20212101021</v>
+        <v>20122100027</v>
       </c>
       <c r="C5" t="n">
         <v>1000</v>
@@ -2394,7 +2369,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20212101066</v>
+        <v>20122100028</v>
       </c>
       <c r="C6" t="n">
         <v>1000</v>
@@ -2433,7 +2408,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20212101112</v>
+        <v>20122100029</v>
       </c>
       <c r="C7" t="n">
         <v>1000</v>
@@ -2472,7 +2447,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20212101159</v>
+        <v>20122100030</v>
       </c>
       <c r="C8" t="n">
         <v>1000</v>
@@ -2511,7 +2486,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20212101207</v>
+        <v>20122100031</v>
       </c>
       <c r="C9" t="n">
         <v>1000</v>
@@ -2550,7 +2525,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20212101256</v>
+        <v>20122100032</v>
       </c>
       <c r="C10" t="n">
         <v>1000</v>
@@ -2589,7 +2564,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20212101306</v>
+        <v>20122100033</v>
       </c>
       <c r="C11" t="n">
         <v>1000</v>
@@ -2628,7 +2603,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20212101357</v>
+        <v>20122100034</v>
       </c>
       <c r="C12" t="n">
         <v>1000</v>
@@ -2667,7 +2642,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20212101409</v>
+        <v>20122100035</v>
       </c>
       <c r="C13" t="n">
         <v>1000</v>
@@ -2706,7 +2681,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20222101409</v>
+        <v>20132100036</v>
       </c>
       <c r="C14" t="n">
         <v>1000</v>
@@ -2745,7 +2720,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20222101415</v>
+        <v>20132100037</v>
       </c>
       <c r="C15" t="n">
         <v>1000</v>
@@ -2784,7 +2759,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20222101419</v>
+        <v>20132100038</v>
       </c>
       <c r="C16" t="n">
         <v>1000</v>
@@ -2823,7 +2798,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20222101424</v>
+        <v>20132100039</v>
       </c>
       <c r="C17" t="n">
         <v>1000</v>
@@ -2862,7 +2837,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20222101430</v>
+        <v>20132100040</v>
       </c>
       <c r="C18" t="n">
         <v>1000</v>
@@ -2901,7 +2876,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20222101437</v>
+        <v>20132100041</v>
       </c>
       <c r="C19" t="n">
         <v>1000</v>
@@ -2940,7 +2915,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20222101445</v>
+        <v>20132100042</v>
       </c>
       <c r="C20" t="n">
         <v>1000</v>
@@ -2979,7 +2954,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20222101454</v>
+        <v>20132100043</v>
       </c>
       <c r="C21" t="n">
         <v>1000</v>
@@ -3018,7 +2993,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20222101464</v>
+        <v>20132100044</v>
       </c>
       <c r="C22" t="n">
         <v>1000</v>
@@ -3057,7 +3032,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20222101475</v>
+        <v>20132100045</v>
       </c>
       <c r="C23" t="n">
         <v>1000</v>
@@ -3096,7 +3071,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20222101487</v>
+        <v>20132100046</v>
       </c>
       <c r="C24" t="n">
         <v>1000</v>
@@ -3135,7 +3110,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20222400527</v>
+        <v>20132400047</v>
       </c>
       <c r="C25" t="n">
         <v>1000</v>
@@ -3174,7 +3149,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20222400559</v>
+        <v>20132400048</v>
       </c>
       <c r="C26" t="n">
         <v>1000</v>
@@ -3213,7 +3188,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20222400592</v>
+        <v>20132400049</v>
       </c>
       <c r="C27" t="n">
         <v>1000</v>
@@ -3252,7 +3227,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20222400626</v>
+        <v>20132400050</v>
       </c>
       <c r="C28" t="n">
         <v>1000</v>
@@ -3291,7 +3266,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>20222400661</v>
+        <v>20132400051</v>
       </c>
       <c r="C29" t="n">
         <v>1000</v>
@@ -3330,7 +3305,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>20222400697</v>
+        <v>20132400052</v>
       </c>
       <c r="C30" t="n">
         <v>1000</v>
@@ -3369,7 +3344,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>20222400734</v>
+        <v>20132400053</v>
       </c>
       <c r="C31" t="n">
         <v>1000</v>
@@ -3408,7 +3383,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>20222400772</v>
+        <v>20132400054</v>
       </c>
       <c r="C32" t="n">
         <v>1000</v>
@@ -3447,7 +3422,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>20222400811</v>
+        <v>20132400055</v>
       </c>
       <c r="C33" t="n">
         <v>1000</v>
@@ -3486,7 +3461,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>20222400851</v>
+        <v>20132400056</v>
       </c>
       <c r="C34" t="n">
         <v>1000</v>
@@ -3525,7 +3500,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>20222400892</v>
+        <v>20132400057</v>
       </c>
       <c r="C35" t="n">
         <v>1000</v>
@@ -3564,7 +3539,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>20232101740</v>
+        <v>20142100080</v>
       </c>
       <c r="C36" t="n">
         <v>1000</v>
@@ -3603,7 +3578,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>20232101763</v>
+        <v>20142100081</v>
       </c>
       <c r="C37" t="n">
         <v>1000</v>
@@ -3642,7 +3617,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>20232101787</v>
+        <v>20142100082</v>
       </c>
       <c r="C38" t="n">
         <v>1000</v>
@@ -3681,7 +3656,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>20232101812</v>
+        <v>20142100083</v>
       </c>
       <c r="C39" t="n">
         <v>1000</v>
@@ -3720,7 +3695,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>20232101838</v>
+        <v>20142100084</v>
       </c>
       <c r="C40" t="n">
         <v>1000</v>
@@ -3759,7 +3734,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>20232101865</v>
+        <v>20142100085</v>
       </c>
       <c r="C41" t="n">
         <v>1000</v>
@@ -3798,7 +3773,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20232101893</v>
+        <v>20142100086</v>
       </c>
       <c r="C42" t="n">
         <v>1000</v>
@@ -3837,7 +3812,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20232101922</v>
+        <v>20142100087</v>
       </c>
       <c r="C43" t="n">
         <v>1000</v>
@@ -3876,7 +3851,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>20232101952</v>
+        <v>20142100088</v>
       </c>
       <c r="C44" t="n">
         <v>1000</v>
@@ -3915,7 +3890,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20232101983</v>
+        <v>20142100089</v>
       </c>
       <c r="C45" t="n">
         <v>1000</v>
@@ -3954,7 +3929,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20232102015</v>
+        <v>20142100090</v>
       </c>
       <c r="C46" t="n">
         <v>1000</v>
@@ -3993,7 +3968,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20242401487</v>
+        <v>20152400100</v>
       </c>
       <c r="C47" t="n">
         <v>1000</v>
@@ -4032,7 +4007,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>20242401488</v>
+        <v>20152400101</v>
       </c>
       <c r="C48" t="n">
         <v>1000</v>
@@ -4071,7 +4046,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>20242401578</v>
+        <v>20152400102</v>
       </c>
       <c r="C49" t="n">
         <v>1000</v>
@@ -4110,7 +4085,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20242401592</v>
+        <v>20152400103</v>
       </c>
       <c r="C50" t="n">
         <v>1000</v>
@@ -4149,7 +4124,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>20242401607</v>
+        <v>20152400104</v>
       </c>
       <c r="C51" t="n">
         <v>1000</v>
@@ -4188,7 +4163,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>20242401623</v>
+        <v>20152400105</v>
       </c>
       <c r="C52" t="n">
         <v>1000</v>
@@ -4227,7 +4202,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>20242401640</v>
+        <v>20152400106</v>
       </c>
       <c r="C53" t="n">
         <v>1000</v>
@@ -4266,7 +4241,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>20242401658</v>
+        <v>20152400107</v>
       </c>
       <c r="C54" t="n">
         <v>1000</v>
@@ -4305,7 +4280,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>20242401677</v>
+        <v>20152400108</v>
       </c>
       <c r="C55" t="n">
         <v>1000</v>
@@ -4344,7 +4319,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>20242401697</v>
+        <v>20152400109</v>
       </c>
       <c r="C56" t="n">
         <v>1000</v>
@@ -4383,7 +4358,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>20242401718</v>
+        <v>20152400110</v>
       </c>
       <c r="C57" t="n">
         <v>1000</v>
@@ -4422,7 +4397,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>20252301490</v>
+        <v>20162300113</v>
       </c>
       <c r="C58" t="n">
         <v>1000</v>
@@ -4461,7 +4436,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>20252301493</v>
+        <v>20162300114</v>
       </c>
       <c r="C59" t="n">
         <v>1000</v>
@@ -4500,7 +4475,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>20252301497</v>
+        <v>20162300115</v>
       </c>
       <c r="C60" t="n">
         <v>1000</v>
@@ -4539,7 +4514,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>20252301502</v>
+        <v>20162300116</v>
       </c>
       <c r="C61" t="n">
         <v>1000</v>
@@ -4578,7 +4553,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>20252301508</v>
+        <v>20162300117</v>
       </c>
       <c r="C62" t="n">
         <v>1000</v>
@@ -4617,7 +4592,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>20252301515</v>
+        <v>20162300118</v>
       </c>
       <c r="C63" t="n">
         <v>1000</v>
@@ -4656,7 +4631,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>20252301523</v>
+        <v>20162300119</v>
       </c>
       <c r="C64" t="n">
         <v>1000</v>
@@ -4695,7 +4670,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>20252301532</v>
+        <v>20162300120</v>
       </c>
       <c r="C65" t="n">
         <v>1000</v>
@@ -4734,7 +4709,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>20252301542</v>
+        <v>20162300121</v>
       </c>
       <c r="C66" t="n">
         <v>1000</v>
@@ -4773,7 +4748,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>20252301553</v>
+        <v>20162300122</v>
       </c>
       <c r="C67" t="n">
         <v>1000</v>
@@ -4812,7 +4787,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>20252301565</v>
+        <v>20162300123</v>
       </c>
       <c r="C68" t="n">
         <v>1000</v>
@@ -4851,7 +4826,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>19641200026</v>
+        <v>19641200130</v>
       </c>
       <c r="C69" t="n">
         <v>8858.749999999998</v>
@@ -4890,7 +4865,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>20102100030</v>
+        <v>20102100134</v>
       </c>
       <c r="C70" t="n">
         <v>53555.51607579708</v>
@@ -4929,7 +4904,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>20142300031</v>
+        <v>20142300135</v>
       </c>
       <c r="C71" t="n">
         <v>10271.8</v>
@@ -5142,7 +5117,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20240100284</v>
+        <v>20150100091</v>
       </c>
       <c r="C3" t="n">
         <v>1000</v>
@@ -5181,7 +5156,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20240100307</v>
+        <v>20150100092</v>
       </c>
       <c r="C4" t="n">
         <v>1000</v>
@@ -5220,7 +5195,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20240100331</v>
+        <v>20150100093</v>
       </c>
       <c r="C5" t="n">
         <v>1000</v>
@@ -5259,7 +5234,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20240100356</v>
+        <v>20150100094</v>
       </c>
       <c r="C6" t="n">
         <v>1000</v>
@@ -5298,7 +5273,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20240100382</v>
+        <v>20150100095</v>
       </c>
       <c r="C7" t="n">
         <v>1000</v>
@@ -5337,7 +5312,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20240100409</v>
+        <v>20150100096</v>
       </c>
       <c r="C8" t="n">
         <v>1000</v>
@@ -5376,7 +5351,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20240100437</v>
+        <v>20150100097</v>
       </c>
       <c r="C9" t="n">
         <v>1000</v>
@@ -5415,7 +5390,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20240100466</v>
+        <v>20150100098</v>
       </c>
       <c r="C10" t="n">
         <v>1000</v>
@@ -5454,7 +5429,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20240100496</v>
+        <v>20150100099</v>
       </c>
       <c r="C11" t="n">
         <v>1000</v>
@@ -5493,7 +5468,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20250101410</v>
+        <v>20160100111</v>
       </c>
       <c r="C12" t="n">
         <v>1000</v>
@@ -5532,7 +5507,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20250101412</v>
+        <v>20160100112</v>
       </c>
       <c r="C13" t="n">
         <v>1000</v>

</xml_diff>

<commit_message>
testing demand increase through excel input
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45657.99861111111</v>
+        <v>47118.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>46021.99861111111</v>
+        <v>47482.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2025</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="2">
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>37</v>
+        <v>50.28</v>
       </c>
     </row>
     <row r="3">
@@ -1199,7 +1199,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.876</v>
+        <v>10.971</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23.17066666666667</v>
+        <v>26.934</v>
       </c>
     </row>
     <row r="7">
@@ -1219,7 +1219,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>54.24266666666666</v>
+        <v>63.996</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
improving graphs and retesting CM save
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>46022.99861111111</v>
+        <v>44196.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>46386.99861111111</v>
+        <v>44560.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2026</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="2">
@@ -1169,7 +1169,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40.31999999999999</v>
+        <v>23.72</v>
       </c>
     </row>
     <row r="3">
@@ -1199,7 +1199,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.914</v>
+        <v>10.819</v>
       </c>
     </row>
     <row r="6">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>24.676</v>
+        <v>20.91266666666667</v>
       </c>
     </row>
     <row r="7">
@@ -1219,7 +1219,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>58.144</v>
+        <v>48.39066666666666</v>
       </c>
     </row>
     <row r="8">
@@ -1245,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99991700006</v>
+        <v>19920300022</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1298,16 +1298,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E2" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>31358.329</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>31358.329</v>
       </c>
     </row>
     <row r="3">
@@ -1315,24 +1315,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99990300008</v>
+        <v>19892800024</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="E3" t="n">
-        <v>0.61</v>
+        <v>0.33</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>24845.77</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="4">
@@ -1340,24 +1340,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>19892800024</v>
+        <v>19843000025</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="F4" t="n">
-        <v>24845.77</v>
+        <v>3652.9</v>
       </c>
       <c r="G4" t="n">
-        <v>24845.77</v>
+        <v>3652.9</v>
       </c>
     </row>
     <row r="5">
@@ -1365,24 +1365,74 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20230300031</v>
+        <v>19822900027</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>LIGNITE</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F5" t="n">
+        <v>20779.02</v>
+      </c>
+      <c r="G5" t="n">
+        <v>20779.02</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>19851400028</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NUCLEAR</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F6" t="n">
+        <v>8599</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8599</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>19921700029</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1000</v>
+      <c r="D7" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F7" t="n">
+        <v>8194.3025</v>
+      </c>
+      <c r="G7" t="n">
+        <v>8194.3025</v>
       </c>
     </row>
   </sheetData>
@@ -1433,7 +1483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1488,17 +1538,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99992100002</v>
+        <v>20062400023</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>47547.50848700004</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1527,17 +1577,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99992400003</v>
+        <v>19641200026</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>8858.749999999998</v>
       </c>
       <c r="D3" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>RunOfRiver</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1566,17 +1616,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>99992300007</v>
+        <v>20102100030</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>53555.51607579708</v>
       </c>
       <c r="D4" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1605,17 +1655,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20062400023</v>
+        <v>20142300031</v>
       </c>
       <c r="C5" t="n">
-        <v>47547.50848700004</v>
+        <v>10271.8</v>
       </c>
       <c r="D5" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1634,84 +1684,6 @@
         </is>
       </c>
       <c r="I5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>20102100030</v>
-      </c>
-      <c r="C6" t="n">
-        <v>53555.51607579708</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>20142300031</v>
-      </c>
-      <c r="C7" t="n">
-        <v>10271.8</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>WindOff</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1728,7 +1700,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1771,34 +1743,6 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>99992600009</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1885,10 +1829,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99990100004</v>
+        <v>20000100021</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>4644.4034</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>

</xml_diff>

<commit_message>
minor fixed to strategic reserves
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schi_co\Arbeitsbereich\Git\traderes\toolbox-amiris-emlab\amiris_workflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Documents\TraderesCode\toolbox-amiris-emlab\amiris_workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC1D690E-7E91-411A-99EB-8F7F394B4F6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{027AB769-D8D6-4671-9393-3997938AE643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28815" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-15720" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_skeleton" sheetId="1" r:id="rId1"/>
@@ -26,11 +26,23 @@
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="86">
   <si>
     <t>group</t>
   </si>
@@ -210,6 +222,9 @@
   </si>
   <si>
     <t>Efficiency</t>
+  </si>
+  <si>
+    <t>BlockSizeInMW</t>
   </si>
   <si>
     <t>InstalledPowerInMW</t>
@@ -294,7 +309,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,12 +331,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -371,22 +380,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -704,13 +710,13 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,7 +727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -732,7 +738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -743,7 +749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -754,7 +760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -765,7 +771,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -773,7 +779,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -784,7 +790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -795,7 +801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -806,7 +812,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -817,7 +823,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -828,7 +834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -839,7 +845,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -850,7 +856,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -861,7 +867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -872,7 +878,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -883,7 +889,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -894,7 +900,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -905,7 +911,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -916,7 +922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -927,7 +933,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -938,7 +944,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -949,7 +955,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -960,7 +966,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -971,7 +977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -982,7 +988,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -993,7 +999,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -1027,24 +1033,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B2" s="5">
         <v>43830.998611111107</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B3" s="5">
         <v>44195.998611111107</v>
@@ -1063,14 +1069,14 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1092,7 +1098,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1103,7 +1109,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1114,7 +1120,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1134,22 +1140,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="4">
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>48</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>49</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>51</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>52</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>20.16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>53</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>46.44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>54</v>
       </c>
@@ -1212,41 +1212,40 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.6328125" customWidth="1"/>
+    <col min="4" max="7" width="19.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1254,7 +1253,7 @@
         <v>19920300022</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D2">
         <v>4.2</v>
@@ -1265,8 +1264,11 @@
       <c r="F2">
         <v>31358.329000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>31358.329000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1274,7 +1276,7 @@
         <v>19892800024</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>3.5</v>
@@ -1285,8 +1287,11 @@
       <c r="F3">
         <v>24845.77</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>24845.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1294,7 +1299,7 @@
         <v>19843000025</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -1305,8 +1310,11 @@
       <c r="F4">
         <v>3652.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>3652.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1314,7 +1322,7 @@
         <v>19822900027</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D5">
         <v>3.5</v>
@@ -1325,8 +1333,11 @@
       <c r="F5">
         <v>20779.02</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>20779.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1334,7 +1345,7 @@
         <v>19851400028</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D6">
         <v>3.5</v>
@@ -1345,8 +1356,11 @@
       <c r="F6">
         <v>8599</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>8599</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1354,15 +1368,18 @@
         <v>19921700029</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D7">
-        <v>4.5</v>
+        <v>800</v>
       </c>
       <c r="E7">
         <v>0.43</v>
       </c>
       <c r="F7">
+        <v>8194.3024999999998</v>
+      </c>
+      <c r="G7">
         <v>8194.3024999999998</v>
       </c>
     </row>
@@ -1379,22 +1396,22 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1">
         <f>SUM(conventionals!G:G,renewables!C:C,biogas!C:C)</f>
-        <v>124877.97796279713</v>
+        <v>222307.29946279712</v>
       </c>
       <c r="B1">
         <f>A1/1000</f>
-        <v>124.87797796279713</v>
+        <v>222.30729946279712</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1406,49 +1423,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1462,22 +1467,22 @@
         <v>1.35</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1491,22 +1496,22 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1520,22 +1525,22 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1549,19 +1554,19 @@
         <v>2.7</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1575,29 +1580,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1611,7 +1616,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1623,35 +1628,35 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -1665,19 +1670,19 @@
         <v>1.9</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected reading of make financial results
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -26,8 +26,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -109,7 +109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -121,7 +121,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,8 +1015,8 @@
           <t>StartTime</t>
         </is>
       </c>
-      <c r="B2" s="7" t="n">
-        <v>43830.99861111111</v>
+      <c r="B2" s="8" t="n">
+        <v>45657.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1024,8 +1025,8 @@
           <t>StopTime</t>
         </is>
       </c>
-      <c r="B3" s="7" t="n">
-        <v>44195.99861111111</v>
+      <c r="B3" s="8" t="n">
+        <v>46021.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2020</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="2">
@@ -1168,7 +1169,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20.4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
@@ -1198,7 +1199,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.8</v>
+        <v>10.895</v>
       </c>
     </row>
     <row r="6">
@@ -1208,7 +1209,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>20.16</v>
+        <v>23.92333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -1218,7 +1219,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46.44</v>
+        <v>56.19333333333333</v>
       </c>
     </row>
     <row r="8">
@@ -1244,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1289,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>19920300022</v>
+        <v>99991700006</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1297,16 +1298,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>31358.329</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1314,124 +1315,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>19892800024</v>
+        <v>99990300008</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E3" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F3" t="n">
-        <v>24845.77</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>24845.77</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>19843000025</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>OIL</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="F4" t="n">
-        <v>3652.9</v>
-      </c>
-      <c r="G4" t="n">
-        <v>3652.9</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>19822900027</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>LIGNITE</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F5" t="n">
-        <v>20779.02</v>
-      </c>
-      <c r="G5" t="n">
-        <v>20779.02</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>19851400028</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>NUCLEAR</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F6" t="n">
-        <v>8599</v>
-      </c>
-      <c r="G6" t="n">
-        <v>8599</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>19921700029</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="F7" t="n">
-        <v>8194.3025</v>
-      </c>
-      <c r="G7" t="n">
-        <v>8194.3025</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1482,7 +1383,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1537,17 +1438,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20062400023</v>
+        <v>99992100002</v>
       </c>
       <c r="C2" t="n">
-        <v>47547.50848700004</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1576,17 +1477,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>19641200026</v>
+        <v>99992400003</v>
       </c>
       <c r="C3" t="n">
-        <v>8858.749999999998</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1615,17 +1516,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20102100030</v>
+        <v>99992300007</v>
       </c>
       <c r="C4" t="n">
-        <v>53555.51607579708</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1644,45 +1545,6 @@
         </is>
       </c>
       <c r="I4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>20142300031</v>
-      </c>
-      <c r="C5" t="n">
-        <v>10271.8</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>WindOff</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1699,7 +1561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1742,6 +1604,34 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99992600009</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1828,10 +1718,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20000100021</v>
+        <v>99990100004</v>
       </c>
       <c r="C2" t="n">
-        <v>4644.4034</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>

</xml_diff>

<commit_message>
making test to invest in smaller volumes
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45657.99861111111</v>
+        <v>43830.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>46021.99861111111</v>
+        <v>44195.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2025</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
adding fixed operating cost GEOMETRIC trend
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>48579.99861111111</v>
+        <v>47118.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>48943.99861111111</v>
+        <v>47482.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2033</v>
+        <v>2029</v>
       </c>
     </row>
     <row r="2">
@@ -1245,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1315,24 +1315,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20230300031</v>
+        <v>19892800024</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.2</v>
+        <v>3.5</v>
       </c>
       <c r="E3" t="n">
-        <v>0.61</v>
+        <v>0.33</v>
       </c>
       <c r="F3" t="n">
-        <v>300</v>
+        <v>24845.77</v>
       </c>
       <c r="G3" t="n">
-        <v>300</v>
+        <v>24845.77</v>
       </c>
     </row>
     <row r="4">
@@ -1340,7 +1340,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20230300032</v>
+        <v>20230300031</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1365,7 +1365,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20230300034</v>
+        <v>20230300032</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1390,7 +1390,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20231700037</v>
+        <v>20230300034</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1398,16 +1398,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E6" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F6" t="n">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="G6" t="n">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7">
@@ -1415,7 +1415,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20231700041</v>
+        <v>20231700037</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1440,7 +1440,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20231700046</v>
+        <v>20231700041</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1465,7 +1465,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20231700052</v>
+        <v>20231700046</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1490,7 +1490,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20231700059</v>
+        <v>20231700052</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1515,7 +1515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20231700067</v>
+        <v>20231700059</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1540,7 +1540,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20231700076</v>
+        <v>20231700067</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1565,24 +1565,24 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19843000025</v>
+        <v>20231700076</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="E13" t="n">
-        <v>0.35</v>
+        <v>0.43</v>
       </c>
       <c r="F13" t="n">
-        <v>3652.9</v>
+        <v>100</v>
       </c>
       <c r="G13" t="n">
-        <v>3652.9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14">
@@ -1590,24 +1590,24 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19822900027</v>
+        <v>20260300401</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E14" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F14" t="n">
-        <v>20779.02</v>
+        <v>300</v>
       </c>
       <c r="G14" t="n">
-        <v>20779.02</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15">
@@ -1615,24 +1615,24 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>19851400028</v>
+        <v>20261700398</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="E15" t="n">
-        <v>0.33</v>
+        <v>0.43</v>
       </c>
       <c r="F15" t="n">
-        <v>8599</v>
+        <v>100</v>
       </c>
       <c r="G15" t="n">
-        <v>8599</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16">
@@ -1640,7 +1640,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>19921700029</v>
+        <v>20261700405</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1654,10 +1654,385 @@
         <v>0.43</v>
       </c>
       <c r="F16" t="n">
-        <v>8194.3025</v>
+        <v>100</v>
       </c>
       <c r="G16" t="n">
-        <v>8194.3025</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20261700410</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F17" t="n">
+        <v>100</v>
+      </c>
+      <c r="G17" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20261700416</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F18" t="n">
+        <v>100</v>
+      </c>
+      <c r="G18" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20261700423</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F19" t="n">
+        <v>100</v>
+      </c>
+      <c r="G19" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20261700431</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F20" t="n">
+        <v>100</v>
+      </c>
+      <c r="G20" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20261700440</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F21" t="n">
+        <v>100</v>
+      </c>
+      <c r="G21" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20270300474</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F22" t="n">
+        <v>300</v>
+      </c>
+      <c r="G22" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>20270300476</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F23" t="n">
+        <v>300</v>
+      </c>
+      <c r="G23" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>20291700504</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F24" t="n">
+        <v>100</v>
+      </c>
+      <c r="G24" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>20291700505</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F25" t="n">
+        <v>100</v>
+      </c>
+      <c r="G25" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>20291700507</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F26" t="n">
+        <v>100</v>
+      </c>
+      <c r="G26" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>20291700510</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F27" t="n">
+        <v>100</v>
+      </c>
+      <c r="G27" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>20291700514</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F28" t="n">
+        <v>100</v>
+      </c>
+      <c r="G28" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>20291700519</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F29" t="n">
+        <v>100</v>
+      </c>
+      <c r="G29" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>20291700525</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F30" t="n">
+        <v>100</v>
+      </c>
+      <c r="G30" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>19851400028</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>NUCLEAR</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F31" t="n">
+        <v>8599</v>
+      </c>
+      <c r="G31" t="n">
+        <v>8599</v>
       </c>
     </row>
   </sheetData>
@@ -1708,7 +2083,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1763,17 +2138,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99992100002</v>
+        <v>20062400023</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>47547.50848700004</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1802,17 +2177,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20062400023</v>
+        <v>20212100241</v>
       </c>
       <c r="C3" t="n">
-        <v>47547.50848700004</v>
+        <v>150</v>
       </c>
       <c r="D3" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1841,7 +2216,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20212100241</v>
+        <v>20212100262</v>
       </c>
       <c r="C4" t="n">
         <v>150</v>
@@ -1880,7 +2255,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20212100262</v>
+        <v>20212100284</v>
       </c>
       <c r="C5" t="n">
         <v>150</v>
@@ -1919,7 +2294,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20212100284</v>
+        <v>20212100307</v>
       </c>
       <c r="C6" t="n">
         <v>150</v>
@@ -1958,7 +2333,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20212100307</v>
+        <v>20212100331</v>
       </c>
       <c r="C7" t="n">
         <v>150</v>
@@ -1997,7 +2372,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20212100331</v>
+        <v>20222100331</v>
       </c>
       <c r="C8" t="n">
         <v>150</v>
@@ -2036,7 +2411,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20222100331</v>
+        <v>20222100332</v>
       </c>
       <c r="C9" t="n">
         <v>150</v>
@@ -2075,7 +2450,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20222100332</v>
+        <v>20222100334</v>
       </c>
       <c r="C10" t="n">
         <v>150</v>
@@ -2114,7 +2489,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20222100334</v>
+        <v>20222100359</v>
       </c>
       <c r="C11" t="n">
         <v>150</v>
@@ -2153,7 +2528,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20222100359</v>
+        <v>20222100367</v>
       </c>
       <c r="C12" t="n">
         <v>150</v>
@@ -2192,17 +2567,17 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20222100367</v>
+        <v>20222400184</v>
       </c>
       <c r="C13" t="n">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -2231,7 +2606,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20222400184</v>
+        <v>20222400202</v>
       </c>
       <c r="C14" t="n">
         <v>300</v>
@@ -2270,7 +2645,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20222400202</v>
+        <v>20222400221</v>
       </c>
       <c r="C15" t="n">
         <v>300</v>
@@ -2309,17 +2684,17 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20222400221</v>
+        <v>20232100373</v>
       </c>
       <c r="C16" t="n">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D16" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2348,7 +2723,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20232100373</v>
+        <v>20232100377</v>
       </c>
       <c r="C17" t="n">
         <v>150</v>
@@ -2387,7 +2762,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20232100377</v>
+        <v>20232100382</v>
       </c>
       <c r="C18" t="n">
         <v>150</v>
@@ -2426,7 +2801,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20232100382</v>
+        <v>20232100388</v>
       </c>
       <c r="C19" t="n">
         <v>150</v>
@@ -2465,7 +2840,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20232100388</v>
+        <v>20232100395</v>
       </c>
       <c r="C20" t="n">
         <v>150</v>
@@ -2504,7 +2879,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20232100395</v>
+        <v>20242100395</v>
       </c>
       <c r="C21" t="n">
         <v>150</v>
@@ -2543,7 +2918,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20242100395</v>
+        <v>20242100396</v>
       </c>
       <c r="C22" t="n">
         <v>150</v>
@@ -2582,7 +2957,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20242100396</v>
+        <v>20242100450</v>
       </c>
       <c r="C23" t="n">
         <v>150</v>
@@ -2621,7 +2996,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20242100398</v>
+        <v>20242100461</v>
       </c>
       <c r="C24" t="n">
         <v>150</v>
@@ -2660,7 +3035,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20242100401</v>
+        <v>20242100473</v>
       </c>
       <c r="C25" t="n">
         <v>150</v>
@@ -2699,17 +3074,17 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20242100405</v>
+        <v>20242300337</v>
       </c>
       <c r="C26" t="n">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2738,7 +3113,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20242300337</v>
+        <v>20242300341</v>
       </c>
       <c r="C27" t="n">
         <v>200</v>
@@ -2777,7 +3152,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20242300341</v>
+        <v>20242300346</v>
       </c>
       <c r="C28" t="n">
         <v>200</v>
@@ -2816,7 +3191,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>20242300346</v>
+        <v>20242300352</v>
       </c>
       <c r="C29" t="n">
         <v>200</v>
@@ -2855,17 +3230,17 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>20242300352</v>
+        <v>20242400367</v>
       </c>
       <c r="C30" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D30" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2894,7 +3269,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>20242400367</v>
+        <v>20242400368</v>
       </c>
       <c r="C31" t="n">
         <v>300</v>
@@ -2933,7 +3308,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>20242400368</v>
+        <v>20242400370</v>
       </c>
       <c r="C32" t="n">
         <v>300</v>
@@ -2972,17 +3347,17 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>20242400370</v>
+        <v>20252100473</v>
       </c>
       <c r="C33" t="n">
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="D33" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3011,7 +3386,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>20252100405</v>
+        <v>20252100479</v>
       </c>
       <c r="C34" t="n">
         <v>150</v>
@@ -3050,7 +3425,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>20252100406</v>
+        <v>20252100483</v>
       </c>
       <c r="C35" t="n">
         <v>150</v>
@@ -3089,7 +3464,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>20252100408</v>
+        <v>20252100488</v>
       </c>
       <c r="C36" t="n">
         <v>150</v>
@@ -3128,7 +3503,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>20252100411</v>
+        <v>20252100494</v>
       </c>
       <c r="C37" t="n">
         <v>150</v>
@@ -3167,7 +3542,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>20252100415</v>
+        <v>20262100494</v>
       </c>
       <c r="C38" t="n">
         <v>150</v>
@@ -3206,7 +3581,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>20262100415</v>
+        <v>20262100495</v>
       </c>
       <c r="C39" t="n">
         <v>150</v>
@@ -3245,7 +3620,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>20262100416</v>
+        <v>20262100497</v>
       </c>
       <c r="C40" t="n">
         <v>150</v>
@@ -3284,7 +3659,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>20262100418</v>
+        <v>20262100500</v>
       </c>
       <c r="C41" t="n">
         <v>150</v>
@@ -3323,7 +3698,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20262100421</v>
+        <v>20262100504</v>
       </c>
       <c r="C42" t="n">
         <v>150</v>
@@ -3362,7 +3737,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20262100425</v>
+        <v>20272100532</v>
       </c>
       <c r="C43" t="n">
         <v>150</v>
@@ -3401,7 +3776,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>20272100425</v>
+        <v>20272100540</v>
       </c>
       <c r="C44" t="n">
         <v>150</v>
@@ -3440,7 +3815,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20272100426</v>
+        <v>20272100549</v>
       </c>
       <c r="C45" t="n">
         <v>150</v>
@@ -3479,7 +3854,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20272100428</v>
+        <v>20272100559</v>
       </c>
       <c r="C46" t="n">
         <v>150</v>
@@ -3518,7 +3893,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20272100431</v>
+        <v>20272100570</v>
       </c>
       <c r="C47" t="n">
         <v>150</v>
@@ -3557,7 +3932,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>20272100435</v>
+        <v>20282100570</v>
       </c>
       <c r="C48" t="n">
         <v>150</v>
@@ -3596,7 +3971,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>20282100435</v>
+        <v>20282100580</v>
       </c>
       <c r="C49" t="n">
         <v>150</v>
@@ -3635,7 +4010,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20282100436</v>
+        <v>20282100585</v>
       </c>
       <c r="C50" t="n">
         <v>150</v>
@@ -3674,7 +4049,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>20282100438</v>
+        <v>20282100591</v>
       </c>
       <c r="C51" t="n">
         <v>150</v>
@@ -3713,7 +4088,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>20282100441</v>
+        <v>20282100598</v>
       </c>
       <c r="C52" t="n">
         <v>150</v>
@@ -3752,7 +4127,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>20282100445</v>
+        <v>20292100598</v>
       </c>
       <c r="C53" t="n">
         <v>150</v>
@@ -3791,7 +4166,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>20292100445</v>
+        <v>20292100599</v>
       </c>
       <c r="C54" t="n">
         <v>150</v>
@@ -3830,7 +4205,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>20292100446</v>
+        <v>20292100601</v>
       </c>
       <c r="C55" t="n">
         <v>150</v>
@@ -3869,7 +4244,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>20292100448</v>
+        <v>20292100604</v>
       </c>
       <c r="C56" t="n">
         <v>150</v>
@@ -3908,7 +4283,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>20292100451</v>
+        <v>20292100608</v>
       </c>
       <c r="C57" t="n">
         <v>150</v>
@@ -3947,17 +4322,17 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>20292100455</v>
+        <v>19641200026</v>
       </c>
       <c r="C58" t="n">
-        <v>150</v>
+        <v>8858.749999999998</v>
       </c>
       <c r="D58" t="n">
         <v>0</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>RunOfRiver</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -3986,10 +4361,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>20302100455</v>
+        <v>20102100030</v>
       </c>
       <c r="C59" t="n">
-        <v>150</v>
+        <v>53555.51607579708</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
@@ -4025,17 +4400,17 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>20302100456</v>
+        <v>20142300031</v>
       </c>
       <c r="C60" t="n">
-        <v>150</v>
+        <v>10271.8</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4054,240 +4429,6 @@
         </is>
       </c>
       <c r="I60" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="6" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="n">
-        <v>20302100458</v>
-      </c>
-      <c r="C61" t="n">
-        <v>150</v>
-      </c>
-      <c r="D61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="6" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="n">
-        <v>20302100461</v>
-      </c>
-      <c r="C62" t="n">
-        <v>150</v>
-      </c>
-      <c r="D62" t="n">
-        <v>0</v>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="6" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="n">
-        <v>20302100465</v>
-      </c>
-      <c r="C63" t="n">
-        <v>150</v>
-      </c>
-      <c r="D63" t="n">
-        <v>0</v>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="6" t="n">
-        <v>62</v>
-      </c>
-      <c r="B64" t="n">
-        <v>19641200026</v>
-      </c>
-      <c r="C64" t="n">
-        <v>8858.749999999998</v>
-      </c>
-      <c r="D64" t="n">
-        <v>0</v>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>RunOfRiver</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="6" t="n">
-        <v>63</v>
-      </c>
-      <c r="B65" t="n">
-        <v>20102100030</v>
-      </c>
-      <c r="C65" t="n">
-        <v>53555.51607579708</v>
-      </c>
-      <c r="D65" t="n">
-        <v>0</v>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="6" t="n">
-        <v>64</v>
-      </c>
-      <c r="B66" t="n">
-        <v>20142300031</v>
-      </c>
-      <c r="C66" t="n">
-        <v>10271.8</v>
-      </c>
-      <c r="D66" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>WindOff</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I66" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
saving fixed costs of old power plants
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45291.99861111111</v>
+        <v>46387.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1026,7 +1026,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>45656.99861111111</v>
+        <v>46751.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1159,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2024</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="2">
@@ -1245,7 +1245,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20230300031</v>
+        <v>99990300008</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1304,10 +1304,10 @@
         <v>0.61</v>
       </c>
       <c r="F2" t="n">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>300</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1315,7 +1315,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20230300032</v>
+        <v>20230300031</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20231700034</v>
+        <v>20230300032</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1348,16 +1348,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E4" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F4" t="n">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="G4" t="n">
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5">
@@ -1365,7 +1365,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20231700037</v>
+        <v>20231700034</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1390,7 +1390,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20231700041</v>
+        <v>20231700037</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1415,7 +1415,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20231700046</v>
+        <v>20231700041</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1440,24 +1440,24 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>19892800024</v>
+        <v>20231700046</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="E8" t="n">
-        <v>0.33</v>
+        <v>0.43</v>
       </c>
       <c r="F8" t="n">
-        <v>24845.77</v>
+        <v>100</v>
       </c>
       <c r="G8" t="n">
-        <v>24845.77</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9">
@@ -1465,24 +1465,124 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
+        <v>19920300022</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F9" t="n">
+        <v>31358.329</v>
+      </c>
+      <c r="G9" t="n">
+        <v>31358.329</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>19921700029</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F10" t="n">
+        <v>8194.3025</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8194.3025</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>19892800024</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>HARD_COAL</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F11" t="n">
+        <v>24845.77</v>
+      </c>
+      <c r="G11" t="n">
+        <v>24845.77</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
         <v>19851400028</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>NUCLEAR</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D12" t="n">
         <v>3.5</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E12" t="n">
         <v>0.33</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F12" t="n">
         <v>8599</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G12" t="n">
         <v>8599</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>19843000025</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>OIL</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>6</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3652.9</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3652.9</v>
       </c>
     </row>
   </sheetData>
@@ -1533,7 +1633,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1588,17 +1688,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20222400086</v>
+        <v>20252300173</v>
       </c>
       <c r="C2" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D2" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1627,17 +1727,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20222400097</v>
+        <v>20252300177</v>
       </c>
       <c r="C3" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D3" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1666,7 +1766,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20212100109</v>
+        <v>20242100195</v>
       </c>
       <c r="C4" t="n">
         <v>150</v>
@@ -1705,7 +1805,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20212100122</v>
+        <v>20242100203</v>
       </c>
       <c r="C5" t="n">
         <v>150</v>
@@ -1744,10 +1844,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>99992100002</v>
+        <v>20242100212</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -1783,17 +1883,17 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20142300031</v>
+        <v>20242400167</v>
       </c>
       <c r="C7" t="n">
-        <v>10271.8</v>
+        <v>300</v>
       </c>
       <c r="D7" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -1822,17 +1922,17 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20102100030</v>
+        <v>20242400168</v>
       </c>
       <c r="C8" t="n">
-        <v>53555.51607579708</v>
+        <v>300</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -1861,35 +1961,581 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
+        <v>99992100002</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20232100170</v>
+      </c>
+      <c r="C10" t="n">
+        <v>150</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20232100182</v>
+      </c>
+      <c r="C11" t="n">
+        <v>150</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20232100188</v>
+      </c>
+      <c r="C12" t="n">
+        <v>150</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20222100136</v>
+      </c>
+      <c r="C13" t="n">
+        <v>150</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20222100151</v>
+      </c>
+      <c r="C14" t="n">
+        <v>150</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>20222100167</v>
+      </c>
+      <c r="C15" t="n">
+        <v>150</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20222400086</v>
+      </c>
+      <c r="C16" t="n">
+        <v>300</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20222400097</v>
+      </c>
+      <c r="C17" t="n">
+        <v>300</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20212100109</v>
+      </c>
+      <c r="C18" t="n">
+        <v>150</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20212100122</v>
+      </c>
+      <c r="C19" t="n">
+        <v>150</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20142300031</v>
+      </c>
+      <c r="C20" t="n">
+        <v>10271.8</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20102100030</v>
+      </c>
+      <c r="C21" t="n">
+        <v>53555.51607579708</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
         <v>20062400023</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C22" t="n">
         <v>47547.50848700004</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D22" t="n">
         <v>1.35</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>WindOn</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>19641200026</v>
+      </c>
+      <c r="C23" t="n">
+        <v>8858.749999999998</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>RunOfRiver</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -1906,7 +2552,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1949,6 +2595,34 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99992600009</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing npv with annuity
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>44196.99861111111</v>
+        <v>55884.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>44560.99861111111</v>
+        <v>56248.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1158,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2021</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="2">
@@ -1244,7 +1244,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1289,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20030300025</v>
+        <v>99991700006</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1297,16 +1297,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>5667.109666666667</v>
+        <v>100</v>
       </c>
       <c r="G2" t="n">
-        <v>5667.109666666667</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -1314,7 +1314,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>19980300022</v>
+        <v>99990300008</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1328,10 +1328,10 @@
         <v>0.61</v>
       </c>
       <c r="F3" t="n">
-        <v>5667.109666666667</v>
+        <v>300</v>
       </c>
       <c r="G3" t="n">
-        <v>5667.109666666667</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4">
@@ -1339,7 +1339,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>19971700031</v>
+        <v>20030300025</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1347,16 +1347,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E4" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F4" t="n">
-        <v>2481.7675</v>
+        <v>5667.109666666667</v>
       </c>
       <c r="G4" t="n">
-        <v>2481.7675</v>
+        <v>5667.109666666667</v>
       </c>
     </row>
     <row r="5">
@@ -1364,24 +1364,24 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>19942800026</v>
+        <v>19980300022</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E5" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F5" t="n">
-        <v>7561.923333333333</v>
+        <v>5667.109666666667</v>
       </c>
       <c r="G5" t="n">
-        <v>7561.923333333333</v>
+        <v>5667.109666666667</v>
       </c>
     </row>
     <row r="6">
@@ -1389,7 +1389,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>19930300037</v>
+        <v>19971700031</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1397,16 +1397,16 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
       <c r="E6" t="n">
-        <v>0.61</v>
+        <v>0.43</v>
       </c>
       <c r="F6" t="n">
-        <v>5667.109666666667</v>
+        <v>2481.7675</v>
       </c>
       <c r="G6" t="n">
-        <v>5667.109666666667</v>
+        <v>2481.7675</v>
       </c>
     </row>
     <row r="7">
@@ -1414,24 +1414,24 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>19921700051</v>
+        <v>19942800026</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="E7" t="n">
-        <v>0.43</v>
+        <v>0.33</v>
       </c>
       <c r="F7" t="n">
-        <v>2481.7675</v>
+        <v>7561.923333333333</v>
       </c>
       <c r="G7" t="n">
-        <v>2481.7675</v>
+        <v>7561.923333333333</v>
       </c>
     </row>
     <row r="8">
@@ -1439,24 +1439,24 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>19901400030</v>
+        <v>19930300037</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E8" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F8" t="n">
-        <v>2704.666666666667</v>
+        <v>5667.109666666667</v>
       </c>
       <c r="G8" t="n">
-        <v>2704.666666666667</v>
+        <v>5667.109666666667</v>
       </c>
     </row>
     <row r="9">
@@ -1464,24 +1464,24 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>19893000027</v>
+        <v>19921700051</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="E9" t="n">
-        <v>0.35</v>
+        <v>0.43</v>
       </c>
       <c r="F9" t="n">
-        <v>1217.633333333333</v>
+        <v>2481.7675</v>
       </c>
       <c r="G9" t="n">
-        <v>1217.633333333333</v>
+        <v>2481.7675</v>
       </c>
     </row>
     <row r="10">
@@ -1489,11 +1489,11 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>19892800033</v>
+        <v>19901400030</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -1503,10 +1503,10 @@
         <v>0.33</v>
       </c>
       <c r="F10" t="n">
-        <v>7561.923333333333</v>
+        <v>2704.666666666667</v>
       </c>
       <c r="G10" t="n">
-        <v>7561.923333333333</v>
+        <v>2704.666666666667</v>
       </c>
     </row>
     <row r="11">
@@ -1514,24 +1514,24 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>19872900029</v>
+        <v>19893000027</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="E11" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="F11" t="n">
-        <v>6926.339999999999</v>
+        <v>1217.633333333333</v>
       </c>
       <c r="G11" t="n">
-        <v>6926.339999999999</v>
+        <v>1217.633333333333</v>
       </c>
     </row>
     <row r="12">
@@ -1539,24 +1539,24 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>19871700043</v>
+        <v>19892800033</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>NATURAL_GAS</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="E12" t="n">
-        <v>0.43</v>
+        <v>0.33</v>
       </c>
       <c r="F12" t="n">
-        <v>2481.7675</v>
+        <v>7561.923333333333</v>
       </c>
       <c r="G12" t="n">
-        <v>2481.7675</v>
+        <v>7561.923333333333</v>
       </c>
     </row>
     <row r="13">
@@ -1564,11 +1564,11 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19851400050</v>
+        <v>19872900029</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1578,10 +1578,10 @@
         <v>0.33</v>
       </c>
       <c r="F13" t="n">
-        <v>2704.666666666667</v>
+        <v>6926.339999999999</v>
       </c>
       <c r="G13" t="n">
-        <v>2704.666666666667</v>
+        <v>6926.339999999999</v>
       </c>
     </row>
     <row r="14">
@@ -1589,24 +1589,24 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19842800038</v>
+        <v>19871700043</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="E14" t="n">
-        <v>0.33</v>
+        <v>0.43</v>
       </c>
       <c r="F14" t="n">
-        <v>7561.923333333333</v>
+        <v>2481.7675</v>
       </c>
       <c r="G14" t="n">
-        <v>7561.923333333333</v>
+        <v>2481.7675</v>
       </c>
     </row>
     <row r="15">
@@ -1614,24 +1614,24 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>19843000044</v>
+        <v>19851400050</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="E15" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="F15" t="n">
-        <v>1217.633333333333</v>
+        <v>2704.666666666667</v>
       </c>
       <c r="G15" t="n">
-        <v>1217.633333333333</v>
+        <v>2704.666666666667</v>
       </c>
     </row>
     <row r="16">
@@ -1639,11 +1639,11 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>19822900049</v>
+        <v>19842800038</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>HARD_COAL</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1653,10 +1653,10 @@
         <v>0.33</v>
       </c>
       <c r="F16" t="n">
-        <v>6926.339999999999</v>
+        <v>7561.923333333333</v>
       </c>
       <c r="G16" t="n">
-        <v>6926.339999999999</v>
+        <v>7561.923333333333</v>
       </c>
     </row>
     <row r="17">
@@ -1664,24 +1664,24 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>19801400042</v>
+        <v>19843000044</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>OIL</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="E17" t="n">
-        <v>0.33</v>
+        <v>0.35</v>
       </c>
       <c r="F17" t="n">
-        <v>2704.666666666667</v>
+        <v>1217.633333333333</v>
       </c>
       <c r="G17" t="n">
-        <v>2704.666666666667</v>
+        <v>1217.633333333333</v>
       </c>
     </row>
     <row r="18">
@@ -1689,24 +1689,24 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>19793000039</v>
+        <v>19822900049</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>LIGNITE</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="E18" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
       <c r="F18" t="n">
-        <v>1217.633333333333</v>
+        <v>6926.339999999999</v>
       </c>
       <c r="G18" t="n">
-        <v>1217.633333333333</v>
+        <v>6926.339999999999</v>
       </c>
     </row>
     <row r="19">
@@ -1714,11 +1714,11 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>19772900041</v>
+        <v>19801400042</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1728,9 +1728,59 @@
         <v>0.33</v>
       </c>
       <c r="F19" t="n">
+        <v>2704.666666666667</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2704.666666666667</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>19793000039</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>OIL</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>6</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1217.633333333333</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1217.633333333333</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>19772900041</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>LIGNITE</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F21" t="n">
         <v>6926.339999999999</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G21" t="n">
         <v>6926.339999999999</v>
       </c>
     </row>
@@ -1782,7 +1832,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1837,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20212100053</v>
+        <v>20502100067</v>
       </c>
       <c r="C2" t="n">
         <v>150</v>
@@ -1876,7 +1926,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20212100054</v>
+        <v>20502100068</v>
       </c>
       <c r="C3" t="n">
         <v>150</v>
@@ -1915,17 +1965,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20202300034</v>
+        <v>99992400003</v>
       </c>
       <c r="C4" t="n">
-        <v>2591.333333333333</v>
+        <v>300</v>
       </c>
       <c r="D4" t="n">
-        <v>2.7</v>
+        <v>1.35</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -1954,17 +2004,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20152100032</v>
+        <v>99992300007</v>
       </c>
       <c r="C5" t="n">
-        <v>18148.27119466832</v>
+        <v>200</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -1993,17 +2043,17 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20152300053</v>
+        <v>20482100066</v>
       </c>
       <c r="C6" t="n">
-        <v>2591.333333333333</v>
+        <v>150</v>
       </c>
       <c r="D6" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -2032,17 +2082,17 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20112400035</v>
+        <v>20482100067</v>
       </c>
       <c r="C7" t="n">
-        <v>17185.46324999998</v>
+        <v>150</v>
       </c>
       <c r="D7" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -2071,17 +2121,17 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20102300046</v>
+        <v>20462100065</v>
       </c>
       <c r="C8" t="n">
-        <v>2591.333333333333</v>
+        <v>150</v>
       </c>
       <c r="D8" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2110,10 +2160,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20102100052</v>
+        <v>20462100066</v>
       </c>
       <c r="C9" t="n">
-        <v>18148.27119466832</v>
+        <v>150</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -2149,17 +2199,17 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20062400023</v>
+        <v>20442100064</v>
       </c>
       <c r="C10" t="n">
-        <v>17185.46324999998</v>
+        <v>150</v>
       </c>
       <c r="D10" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -2188,10 +2238,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20052100045</v>
+        <v>20442100065</v>
       </c>
       <c r="C11" t="n">
-        <v>18148.27119466832</v>
+        <v>150</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -2227,17 +2277,17 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20012400047</v>
+        <v>20422100063</v>
       </c>
       <c r="C12" t="n">
-        <v>17185.46324999998</v>
+        <v>150</v>
       </c>
       <c r="D12" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -2266,17 +2316,17 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19691200028</v>
+        <v>20422100064</v>
       </c>
       <c r="C13" t="n">
-        <v>2940.25</v>
+        <v>150</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -2305,17 +2355,17 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19641200048</v>
+        <v>20402100062</v>
       </c>
       <c r="C14" t="n">
-        <v>2940.25</v>
+        <v>150</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2344,35 +2394,1205 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
+        <v>20402100063</v>
+      </c>
+      <c r="C15" t="n">
+        <v>150</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20382100061</v>
+      </c>
+      <c r="C16" t="n">
+        <v>150</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20382100062</v>
+      </c>
+      <c r="C17" t="n">
+        <v>150</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20362100060</v>
+      </c>
+      <c r="C18" t="n">
+        <v>150</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20362100061</v>
+      </c>
+      <c r="C19" t="n">
+        <v>150</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20342100059</v>
+      </c>
+      <c r="C20" t="n">
+        <v>150</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20342100060</v>
+      </c>
+      <c r="C21" t="n">
+        <v>150</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20322100058</v>
+      </c>
+      <c r="C22" t="n">
+        <v>150</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>20322100059</v>
+      </c>
+      <c r="C23" t="n">
+        <v>150</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>20302100057</v>
+      </c>
+      <c r="C24" t="n">
+        <v>150</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>20302100058</v>
+      </c>
+      <c r="C25" t="n">
+        <v>150</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>20282100056</v>
+      </c>
+      <c r="C26" t="n">
+        <v>150</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>20282100057</v>
+      </c>
+      <c r="C27" t="n">
+        <v>150</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>20262100055</v>
+      </c>
+      <c r="C28" t="n">
+        <v>150</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>20262100056</v>
+      </c>
+      <c r="C29" t="n">
+        <v>150</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>20242100054</v>
+      </c>
+      <c r="C30" t="n">
+        <v>150</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>20242100055</v>
+      </c>
+      <c r="C31" t="n">
+        <v>150</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>20222100053</v>
+      </c>
+      <c r="C32" t="n">
+        <v>150</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>20222100054</v>
+      </c>
+      <c r="C33" t="n">
+        <v>150</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>20202300034</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2591.333333333333</v>
+      </c>
+      <c r="D34" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>20152100032</v>
+      </c>
+      <c r="C35" t="n">
+        <v>18148.27119466832</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>20152300053</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2591.333333333333</v>
+      </c>
+      <c r="D36" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>20112400035</v>
+      </c>
+      <c r="C37" t="n">
+        <v>17185.46324999998</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>20102300046</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2591.333333333333</v>
+      </c>
+      <c r="D38" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>20102100052</v>
+      </c>
+      <c r="C39" t="n">
+        <v>18148.27119466832</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>20062400023</v>
+      </c>
+      <c r="C40" t="n">
+        <v>17185.46324999998</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>20052100045</v>
+      </c>
+      <c r="C41" t="n">
+        <v>18148.27119466832</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>20012400047</v>
+      </c>
+      <c r="C42" t="n">
+        <v>17185.46324999998</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>19691200028</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2940.25</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>RunOfRiver</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>19641200048</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2940.25</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>RunOfRiver</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
         <v>19591200040</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C45" t="n">
         <v>2940.25</v>
       </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="inlineStr">
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="inlineStr">
         <is>
           <t>RunOfRiver</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2389,7 +3609,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2432,6 +3652,34 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>99992600009</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>STORAGE</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2463,7 +3711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2518,10 +3766,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20100100024</v>
+        <v>99990100004</v>
       </c>
       <c r="C2" t="n">
-        <v>3232.501133333333</v>
+        <v>100</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -2557,7 +3805,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20050100021</v>
+        <v>20100100024</v>
       </c>
       <c r="C3" t="n">
         <v>3232.501133333333</v>
@@ -2596,7 +3844,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20000100036</v>
+        <v>20050100021</v>
       </c>
       <c r="C4" t="n">
         <v>3232.501133333333</v>
@@ -2625,6 +3873,45 @@
         </is>
       </c>
       <c r="I4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>20000100036</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3232.501133333333</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Biogas</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
saving residual load in excel
preparing scenario to run unlimited investment
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>55884.99861111111</v>
+        <v>45657.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>56248.99861111111</v>
+        <v>46021.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1158,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2053</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="2">
@@ -1303,10 +1303,10 @@
         <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="G2" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3">
@@ -1328,10 +1328,10 @@
         <v>0.61</v>
       </c>
       <c r="F3" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="G3" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4">
@@ -1832,7 +1832,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1887,10 +1887,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20502100067</v>
+        <v>99992100002</v>
       </c>
       <c r="C2" t="n">
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1926,17 +1926,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20502100068</v>
+        <v>99992400003</v>
       </c>
       <c r="C3" t="n">
-        <v>150</v>
+        <v>500</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1965,17 +1965,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>99992400003</v>
+        <v>99992300007</v>
       </c>
       <c r="C4" t="n">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="D4" t="n">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -2004,10 +2004,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>99992300007</v>
+        <v>20202300034</v>
       </c>
       <c r="C5" t="n">
-        <v>200</v>
+        <v>2591.333333333333</v>
       </c>
       <c r="D5" t="n">
         <v>2.7</v>
@@ -2043,10 +2043,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20482100066</v>
+        <v>20152100032</v>
       </c>
       <c r="C6" t="n">
-        <v>150</v>
+        <v>18148.27119466832</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -2082,17 +2082,17 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20482100067</v>
+        <v>20152300053</v>
       </c>
       <c r="C7" t="n">
-        <v>150</v>
+        <v>2591.333333333333</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -2121,17 +2121,17 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20462100065</v>
+        <v>20112400035</v>
       </c>
       <c r="C8" t="n">
-        <v>150</v>
+        <v>17185.46324999998</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2160,17 +2160,17 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20462100066</v>
+        <v>20102300046</v>
       </c>
       <c r="C9" t="n">
-        <v>150</v>
+        <v>2591.333333333333</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2199,10 +2199,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20442100064</v>
+        <v>20102100052</v>
       </c>
       <c r="C10" t="n">
-        <v>150</v>
+        <v>18148.27119466832</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -2238,17 +2238,17 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20442100065</v>
+        <v>20062400023</v>
       </c>
       <c r="C11" t="n">
-        <v>150</v>
+        <v>17185.46324999998</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -2277,10 +2277,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20422100063</v>
+        <v>20052100045</v>
       </c>
       <c r="C12" t="n">
-        <v>150</v>
+        <v>18148.27119466832</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -2316,17 +2316,17 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20422100064</v>
+        <v>20012400047</v>
       </c>
       <c r="C13" t="n">
-        <v>150</v>
+        <v>17185.46324999998</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -2355,17 +2355,17 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20402100062</v>
+        <v>19691200028</v>
       </c>
       <c r="C14" t="n">
-        <v>150</v>
+        <v>2940.25</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>RunOfRiver</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2394,17 +2394,17 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20402100063</v>
+        <v>19641200048</v>
       </c>
       <c r="C15" t="n">
-        <v>150</v>
+        <v>2940.25</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>RunOfRiver</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2433,17 +2433,17 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20382100061</v>
+        <v>19591200040</v>
       </c>
       <c r="C16" t="n">
-        <v>150</v>
+        <v>2940.25</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>RunOfRiver</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2462,1137 +2462,6 @@
         </is>
       </c>
       <c r="I16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>20382100062</v>
-      </c>
-      <c r="C17" t="n">
-        <v>150</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>20362100060</v>
-      </c>
-      <c r="C18" t="n">
-        <v>150</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>20362100061</v>
-      </c>
-      <c r="C19" t="n">
-        <v>150</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>20342100059</v>
-      </c>
-      <c r="C20" t="n">
-        <v>150</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>20342100060</v>
-      </c>
-      <c r="C21" t="n">
-        <v>150</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>20322100058</v>
-      </c>
-      <c r="C22" t="n">
-        <v>150</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="6" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>20322100059</v>
-      </c>
-      <c r="C23" t="n">
-        <v>150</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>20302100057</v>
-      </c>
-      <c r="C24" t="n">
-        <v>150</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>20302100058</v>
-      </c>
-      <c r="C25" t="n">
-        <v>150</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="6" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>20282100056</v>
-      </c>
-      <c r="C26" t="n">
-        <v>150</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="6" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>20282100057</v>
-      </c>
-      <c r="C27" t="n">
-        <v>150</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="6" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="n">
-        <v>20262100055</v>
-      </c>
-      <c r="C28" t="n">
-        <v>150</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="6" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="n">
-        <v>20262100056</v>
-      </c>
-      <c r="C29" t="n">
-        <v>150</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="6" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="n">
-        <v>20242100054</v>
-      </c>
-      <c r="C30" t="n">
-        <v>150</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="6" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="n">
-        <v>20242100055</v>
-      </c>
-      <c r="C31" t="n">
-        <v>150</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="6" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="n">
-        <v>20222100053</v>
-      </c>
-      <c r="C32" t="n">
-        <v>150</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="6" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="n">
-        <v>20222100054</v>
-      </c>
-      <c r="C33" t="n">
-        <v>150</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="6" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="n">
-        <v>20202300034</v>
-      </c>
-      <c r="C34" t="n">
-        <v>2591.333333333333</v>
-      </c>
-      <c r="D34" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>WindOff</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="6" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="n">
-        <v>20152100032</v>
-      </c>
-      <c r="C35" t="n">
-        <v>18148.27119466832</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="6" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="n">
-        <v>20152300053</v>
-      </c>
-      <c r="C36" t="n">
-        <v>2591.333333333333</v>
-      </c>
-      <c r="D36" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>WindOff</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="6" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="n">
-        <v>20112400035</v>
-      </c>
-      <c r="C37" t="n">
-        <v>17185.46324999998</v>
-      </c>
-      <c r="D37" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>WindOn</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="6" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="n">
-        <v>20102300046</v>
-      </c>
-      <c r="C38" t="n">
-        <v>2591.333333333333</v>
-      </c>
-      <c r="D38" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>WindOff</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="6" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="n">
-        <v>20102100052</v>
-      </c>
-      <c r="C39" t="n">
-        <v>18148.27119466832</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="6" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="n">
-        <v>20062400023</v>
-      </c>
-      <c r="C40" t="n">
-        <v>17185.46324999998</v>
-      </c>
-      <c r="D40" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>WindOn</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="6" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="n">
-        <v>20052100045</v>
-      </c>
-      <c r="C41" t="n">
-        <v>18148.27119466832</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="6" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="n">
-        <v>20012400047</v>
-      </c>
-      <c r="C42" t="n">
-        <v>17185.46324999998</v>
-      </c>
-      <c r="D42" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>WindOn</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="6" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="n">
-        <v>19691200028</v>
-      </c>
-      <c r="C43" t="n">
-        <v>2940.25</v>
-      </c>
-      <c r="D43" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>RunOfRiver</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="6" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="n">
-        <v>19641200048</v>
-      </c>
-      <c r="C44" t="n">
-        <v>2940.25</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>RunOfRiver</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="6" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="n">
-        <v>19591200040</v>
-      </c>
-      <c r="C45" t="n">
-        <v>2940.25</v>
-      </c>
-      <c r="D45" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>RunOfRiver</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -3679,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -3769,7 +2638,7 @@
         <v>99990100004</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>

</xml_diff>

<commit_message>
preparing dynamic data for NL case
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
-        <v>45657.99861111111</v>
+        <v>46752.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
-        <v>46021.99861111111</v>
+        <v>47117.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1158,7 +1158,7 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="6" t="n">
-        <v>2025</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="2">
@@ -1244,7 +1244,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1289,7 +1289,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99991700006</v>
+        <v>20030300025</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1297,16 +1297,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E2" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F2" t="n">
-        <v>500</v>
+        <v>5667.109666666667</v>
       </c>
       <c r="G2" t="n">
-        <v>500</v>
+        <v>5667.109666666667</v>
       </c>
     </row>
     <row r="3">
@@ -1314,7 +1314,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99990300008</v>
+        <v>19980300022</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1328,10 +1328,10 @@
         <v>0.61</v>
       </c>
       <c r="F3" t="n">
-        <v>500</v>
+        <v>5667.109666666667</v>
       </c>
       <c r="G3" t="n">
-        <v>500</v>
+        <v>5667.109666666667</v>
       </c>
     </row>
     <row r="4">
@@ -1339,7 +1339,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20030300025</v>
+        <v>19970300031</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1353,10 +1353,10 @@
         <v>0.61</v>
       </c>
       <c r="F4" t="n">
-        <v>5667.109666666667</v>
+        <v>2481.7675</v>
       </c>
       <c r="G4" t="n">
-        <v>5667.109666666667</v>
+        <v>2481.7675</v>
       </c>
     </row>
     <row r="5">
@@ -1364,7 +1364,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>19980300022</v>
+        <v>19940300026</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1378,10 +1378,10 @@
         <v>0.61</v>
       </c>
       <c r="F5" t="n">
-        <v>5667.109666666667</v>
+        <v>7561.923333333333</v>
       </c>
       <c r="G5" t="n">
-        <v>5667.109666666667</v>
+        <v>7561.923333333333</v>
       </c>
     </row>
     <row r="6">
@@ -1389,7 +1389,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>19971700031</v>
+        <v>19920300041</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1397,10 +1397,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E6" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F6" t="n">
         <v>2481.7675</v>
@@ -1414,24 +1414,24 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>19942800026</v>
+        <v>19900300030</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E7" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F7" t="n">
-        <v>7561.923333333333</v>
+        <v>2704.666666666667</v>
       </c>
       <c r="G7" t="n">
-        <v>7561.923333333333</v>
+        <v>2704.666666666667</v>
       </c>
     </row>
     <row r="8">
@@ -1439,7 +1439,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>19930300037</v>
+        <v>19890300027</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1453,10 +1453,10 @@
         <v>0.61</v>
       </c>
       <c r="F8" t="n">
-        <v>5667.109666666667</v>
+        <v>1217.633333333333</v>
       </c>
       <c r="G8" t="n">
-        <v>5667.109666666667</v>
+        <v>1217.633333333333</v>
       </c>
     </row>
     <row r="9">
@@ -1464,7 +1464,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>19921700051</v>
+        <v>19890300033</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1472,16 +1472,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E9" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F9" t="n">
-        <v>2481.7675</v>
+        <v>7561.923333333333</v>
       </c>
       <c r="G9" t="n">
-        <v>2481.7675</v>
+        <v>7561.923333333333</v>
       </c>
     </row>
     <row r="10">
@@ -1489,24 +1489,24 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>19901400030</v>
+        <v>19870300029</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E10" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F10" t="n">
-        <v>2704.666666666667</v>
+        <v>6926.339999999999</v>
       </c>
       <c r="G10" t="n">
-        <v>2704.666666666667</v>
+        <v>6926.339999999999</v>
       </c>
     </row>
     <row r="11">
@@ -1514,24 +1514,24 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>19893000027</v>
+        <v>19850300040</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>4.2</v>
       </c>
       <c r="E11" t="n">
-        <v>0.35</v>
+        <v>0.61</v>
       </c>
       <c r="F11" t="n">
-        <v>1217.633333333333</v>
+        <v>2704.666666666667</v>
       </c>
       <c r="G11" t="n">
-        <v>1217.633333333333</v>
+        <v>2704.666666666667</v>
       </c>
     </row>
     <row r="12">
@@ -1539,24 +1539,24 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>19892800033</v>
+        <v>19840300037</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>HARD_COAL</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E12" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F12" t="n">
-        <v>7561.923333333333</v>
+        <v>1217.633333333333</v>
       </c>
       <c r="G12" t="n">
-        <v>7561.923333333333</v>
+        <v>1217.633333333333</v>
       </c>
     </row>
     <row r="13">
@@ -1564,18 +1564,18 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19872900029</v>
+        <v>19820300039</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>LIGNITE</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E13" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F13" t="n">
         <v>6926.339999999999</v>
@@ -1589,7 +1589,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19871700043</v>
+        <v>19690300028</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1597,16 +1597,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>4.5</v>
+        <v>4.2</v>
       </c>
       <c r="E14" t="n">
-        <v>0.43</v>
+        <v>0.61</v>
       </c>
       <c r="F14" t="n">
-        <v>2481.7675</v>
+        <v>2940.25</v>
       </c>
       <c r="G14" t="n">
-        <v>2481.7675</v>
+        <v>2940.25</v>
       </c>
     </row>
     <row r="15">
@@ -1614,174 +1614,24 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>19851400050</v>
+        <v>19640300038</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="E15" t="n">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="F15" t="n">
-        <v>2704.666666666667</v>
+        <v>2940.25</v>
       </c>
       <c r="G15" t="n">
-        <v>2704.666666666667</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>19842800038</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>HARD_COAL</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F16" t="n">
-        <v>7561.923333333333</v>
-      </c>
-      <c r="G16" t="n">
-        <v>7561.923333333333</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>19843000044</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>OIL</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>6</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="F17" t="n">
-        <v>1217.633333333333</v>
-      </c>
-      <c r="G17" t="n">
-        <v>1217.633333333333</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>19822900049</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>LIGNITE</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F18" t="n">
-        <v>6926.339999999999</v>
-      </c>
-      <c r="G18" t="n">
-        <v>6926.339999999999</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>19801400042</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>NUCLEAR</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2704.666666666667</v>
-      </c>
-      <c r="G19" t="n">
-        <v>2704.666666666667</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>19793000039</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>OIL</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>6</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="F20" t="n">
-        <v>1217.633333333333</v>
-      </c>
-      <c r="G20" t="n">
-        <v>1217.633333333333</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>19772900041</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>LIGNITE</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F21" t="n">
-        <v>6926.339999999999</v>
-      </c>
-      <c r="G21" t="n">
-        <v>6926.339999999999</v>
+        <v>2940.25</v>
       </c>
     </row>
   </sheetData>
@@ -1832,7 +1682,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1887,10 +1737,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99992100002</v>
+        <v>20202100034</v>
       </c>
       <c r="C2" t="n">
-        <v>500</v>
+        <v>2591.333333333333</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1926,17 +1776,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>99992400003</v>
+        <v>20152100032</v>
       </c>
       <c r="C3" t="n">
-        <v>500</v>
+        <v>18148.27119466832</v>
       </c>
       <c r="D3" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1965,17 +1815,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>99992300007</v>
+        <v>20152100043</v>
       </c>
       <c r="C4" t="n">
-        <v>500</v>
+        <v>2591.333333333333</v>
       </c>
       <c r="D4" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -2004,17 +1854,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20202300034</v>
+        <v>20112100035</v>
       </c>
       <c r="C5" t="n">
-        <v>2591.333333333333</v>
+        <v>17185.46324999998</v>
       </c>
       <c r="D5" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2043,10 +1893,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20152100032</v>
+        <v>20102100024</v>
       </c>
       <c r="C6" t="n">
-        <v>18148.27119466832</v>
+        <v>3232.501133333333</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -2082,17 +1932,17 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20152300053</v>
+        <v>20102100042</v>
       </c>
       <c r="C7" t="n">
-        <v>2591.333333333333</v>
+        <v>18148.27119466832</v>
       </c>
       <c r="D7" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -2121,17 +1971,17 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20112400035</v>
+        <v>20062100023</v>
       </c>
       <c r="C8" t="n">
         <v>17185.46324999998</v>
       </c>
       <c r="D8" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2160,17 +2010,17 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20102300046</v>
+        <v>20052100021</v>
       </c>
       <c r="C9" t="n">
-        <v>2591.333333333333</v>
+        <v>3232.501133333333</v>
       </c>
       <c r="D9" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2199,10 +2049,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20102100052</v>
+        <v>20002100036</v>
       </c>
       <c r="C10" t="n">
-        <v>18148.27119466832</v>
+        <v>3232.501133333333</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -2228,240 +2078,6 @@
         </is>
       </c>
       <c r="I10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>20062400023</v>
-      </c>
-      <c r="C11" t="n">
-        <v>17185.46324999998</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>WindOn</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="n">
-        <v>20052100045</v>
-      </c>
-      <c r="C12" t="n">
-        <v>18148.27119466832</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="n">
-        <v>20012400047</v>
-      </c>
-      <c r="C13" t="n">
-        <v>17185.46324999998</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>WindOn</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
-        <v>19691200028</v>
-      </c>
-      <c r="C14" t="n">
-        <v>2940.25</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>RunOfRiver</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="n">
-        <v>19641200048</v>
-      </c>
-      <c r="C15" t="n">
-        <v>2940.25</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>RunOfRiver</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>19591200040</v>
-      </c>
-      <c r="C16" t="n">
-        <v>2940.25</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>RunOfRiver</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -2478,7 +2094,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2521,34 +2137,6 @@
         <is>
           <t>InstalledPowerInMW</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>99992600009</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -2580,7 +2168,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2635,10 +2223,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99990100004</v>
+        <v>20280100043</v>
       </c>
       <c r="C2" t="n">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="D2" t="n">
         <v>1.9</v>
@@ -2674,10 +2262,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20100100024</v>
+        <v>99990100004</v>
       </c>
       <c r="C3" t="n">
-        <v>3232.501133333333</v>
+        <v>100</v>
       </c>
       <c r="D3" t="n">
         <v>1.9</v>
@@ -2713,10 +2301,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20050100021</v>
+        <v>20240100043</v>
       </c>
       <c r="C4" t="n">
-        <v>3232.501133333333</v>
+        <v>100</v>
       </c>
       <c r="D4" t="n">
         <v>1.9</v>
@@ -2742,45 +2330,6 @@
         </is>
       </c>
       <c r="I4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>20000100036</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3232.501133333333</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Biogas</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
resaving future market clearing
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="12315" yWindow="-16350" windowWidth="29040" windowHeight="15840" tabRatio="935" firstSheet="3" activeTab="8" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-16485" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="935" firstSheet="3" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_skeleton" sheetId="1" state="visible" r:id="rId1"/>
@@ -219,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -252,6 +252,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1157,42 +1158,42 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="16" t="inlineStr">
+      <c r="B1" s="17" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="16" t="inlineStr">
+      <c r="C1" s="17" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
-      <c r="D1" s="16" t="inlineStr">
+      <c r="D1" s="17" t="inlineStr">
         <is>
           <t>OpexVarInEURperMWH</t>
         </is>
       </c>
-      <c r="E1" s="16" t="inlineStr">
+      <c r="E1" s="17" t="inlineStr">
         <is>
           <t>Set</t>
         </is>
       </c>
-      <c r="F1" s="16" t="inlineStr">
+      <c r="F1" s="17" t="inlineStr">
         <is>
           <t>SupportInstrument</t>
         </is>
       </c>
-      <c r="G1" s="16" t="inlineStr">
+      <c r="G1" s="17" t="inlineStr">
         <is>
           <t>FIT</t>
         </is>
       </c>
-      <c r="H1" s="16" t="inlineStr">
+      <c r="H1" s="17" t="inlineStr">
         <is>
           <t>Premium</t>
         </is>
       </c>
-      <c r="I1" s="16" t="inlineStr">
+      <c r="I1" s="17" t="inlineStr">
         <is>
           <t>Lcoe</t>
         </is>
@@ -1534,28 +1535,28 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="16" t="n">
+      <c r="B1" s="17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="16" t="inlineStr">
+      <c r="A2" s="17" t="inlineStr">
         <is>
           <t>StartTime</t>
         </is>
       </c>
-      <c r="B2" s="18" t="n">
-        <v>56249.99861111111</v>
+      <c r="B2" s="19" t="n">
+        <v>57345.99861111111</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="16" t="inlineStr">
+      <c r="A3" s="17" t="inlineStr">
         <is>
           <t>StopTime</t>
         </is>
       </c>
-      <c r="B3" s="18" t="n">
-        <v>56613.99861111111</v>
+      <c r="B3" s="19" t="n">
+        <v>57709.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1687,64 +1688,64 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="16" t="inlineStr">
+      <c r="B1" s="17" t="inlineStr">
         <is>
           <t>AgentType</t>
         </is>
       </c>
-      <c r="C1" s="16" t="inlineStr">
+      <c r="C1" s="17" t="inlineStr">
         <is>
           <t>CO2</t>
         </is>
       </c>
-      <c r="D1" s="16" t="inlineStr">
+      <c r="D1" s="17" t="inlineStr">
         <is>
           <t>HARD_COAL</t>
         </is>
       </c>
-      <c r="E1" s="16" t="inlineStr">
+      <c r="E1" s="17" t="inlineStr">
         <is>
           <t>OIL</t>
         </is>
       </c>
-      <c r="F1" s="16" t="inlineStr">
+      <c r="F1" s="17" t="inlineStr">
         <is>
           <t>HYDROGEN</t>
         </is>
       </c>
-      <c r="G1" s="16" t="inlineStr">
+      <c r="G1" s="17" t="inlineStr">
         <is>
           <t>LIGNITE</t>
         </is>
       </c>
-      <c r="H1" s="16" t="inlineStr">
+      <c r="H1" s="17" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="I1" s="16" t="inlineStr">
+      <c r="I1" s="17" t="inlineStr">
         <is>
           <t>NUCLEAR</t>
         </is>
       </c>
-      <c r="J1" s="16" t="inlineStr">
+      <c r="J1" s="17" t="inlineStr">
         <is>
           <t>WASTE</t>
         </is>
       </c>
-      <c r="K1" s="16" t="inlineStr">
+      <c r="K1" s="17" t="inlineStr">
         <is>
           <t>BIOMASS</t>
         </is>
       </c>
-      <c r="L1" s="16" t="inlineStr">
+      <c r="L1" s="17" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="16" t="n">
+      <c r="A2" s="17" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -1766,7 +1767,7 @@
       <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="16" t="n">
+      <c r="A3" s="17" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -1814,7 +1815,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1823,68 +1824,68 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="16" t="inlineStr">
+      <c r="B1" s="17" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="16" t="inlineStr">
+      <c r="C1" s="17" t="inlineStr">
         <is>
           <t>FuelType</t>
         </is>
       </c>
-      <c r="D1" s="16" t="inlineStr">
+      <c r="D1" s="17" t="inlineStr">
         <is>
           <t>OpexVarInEURperMWH</t>
         </is>
       </c>
-      <c r="E1" s="16" t="inlineStr">
+      <c r="E1" s="17" t="inlineStr">
         <is>
           <t>Efficiency</t>
         </is>
       </c>
-      <c r="F1" s="16" t="inlineStr">
+      <c r="F1" s="17" t="inlineStr">
         <is>
           <t>BlockSizeInMW</t>
         </is>
       </c>
-      <c r="G1" s="16" t="inlineStr">
+      <c r="G1" s="17" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="16" t="n">
-        <v>1</v>
+      <c r="A2" s="17" t="n">
+        <v>16</v>
       </c>
       <c r="B2" t="n">
-        <v>99993300004</v>
+        <v>20501900040</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>HYDROGEN</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1.5</v>
+        <v>9.431790764000008</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4</v>
+        <v>0.110414839365</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>484</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>484</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="16" t="n">
-        <v>2</v>
+      <c r="A3" s="17" t="n">
+        <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>99990800005</v>
+        <v>20590800067</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1898,18 +1899,18 @@
         <v>0.61</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="16" t="n">
-        <v>3</v>
+      <c r="A4" s="17" t="n">
+        <v>23</v>
       </c>
       <c r="B4" t="n">
-        <v>99992200009</v>
+        <v>20340800044</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1917,49 +1918,49 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4.5</v>
+        <v>45.50576496223126</v>
       </c>
       <c r="E4" t="n">
-        <v>0.43</v>
+        <v>0.04379177724920303</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="16" t="n">
-        <v>4</v>
+      <c r="A5" s="17" t="n">
+        <v>21</v>
       </c>
       <c r="B5" t="n">
-        <v>20501900040</v>
+        <v>20380800043</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>31.08104976588433</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1869885</v>
+        <v>0.06674558337022257</v>
       </c>
       <c r="F5" t="n">
-        <v>484</v>
+        <v>1000</v>
       </c>
       <c r="G5" t="n">
-        <v>484</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="16" t="n">
-        <v>0</v>
+      <c r="A6" s="17" t="n">
+        <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>20542200054</v>
+        <v>20420800042</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1967,10 +1968,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4.5</v>
+        <v>21.22877519697037</v>
       </c>
       <c r="E6" t="n">
-        <v>0.43</v>
+        <v>0.1017308083679661</v>
       </c>
       <c r="F6" t="n">
         <v>1000</v>
@@ -1980,8 +1981,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="16" t="n">
-        <v>6</v>
+      <c r="A7" s="17" t="n">
+        <v>18</v>
       </c>
       <c r="B7" t="n">
         <v>20460800041</v>
@@ -1992,10 +1993,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4.2</v>
+        <v>14.49953910045104</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2625849981000001</v>
+        <v>0.155053815528069</v>
       </c>
       <c r="F7" t="n">
         <v>1000</v>
@@ -2005,252 +2006,527 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="16" t="n">
+      <c r="A8" s="17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20542200054</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>7.247295000000003</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.2539107</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="17" t="n">
+        <v>14</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20552200056</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>6.588450000000002</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.282123</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="17" t="n">
+        <v>12</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20562200059</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>5.989500000000001</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.31347</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="17" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20562200058</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>5.989500000000001</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.31347</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="17" t="n">
+        <v>13</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20550800055</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>6.149220000000002</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.400221</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="17" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20572200063</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>5.445000000000001</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.3483</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20572200062</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>5.445000000000001</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.3483</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
-        <v>20420800042</v>
-      </c>
-      <c r="C8" t="inlineStr">
+      <c r="B15" t="n">
+        <v>20572200061</v>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.1722820172534101</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="16" t="n">
-        <v>9</v>
-      </c>
-      <c r="B9" t="n">
-        <v>20380800043</v>
-      </c>
-      <c r="C9" t="inlineStr">
+      <c r="D15" t="n">
+        <v>5.445000000000001</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.3483</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20572200060</v>
+      </c>
+      <c r="C16" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.1130342315199623</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="16" t="n">
-        <v>11</v>
-      </c>
-      <c r="B10" t="n">
-        <v>20340800044</v>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="D16" t="n">
+        <v>5.445000000000001</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.3483</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20582200066</v>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.07416175930024731</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="16" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" t="n">
+      <c r="D17" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.387</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20582200065</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.387</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20580800064</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>4.620000000000001</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.549</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20592200069</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20592200068</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="17" t="n">
+        <v>10</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20560800057</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>5.590200000000002</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.44469</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="17" t="n">
+        <v>20</v>
+      </c>
+      <c r="B23" t="n">
         <v>20402200047</v>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.09837020755633234</v>
-      </c>
-      <c r="F11" t="n">
+      <c r="D23" t="n">
+        <v>27.52159070178659</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.05808662385993869</v>
+      </c>
+      <c r="F23" t="n">
         <v>1300</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G23" t="n">
         <v>1300</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="16" t="n">
-        <v>14</v>
-      </c>
-      <c r="B12" t="n">
+    <row r="24">
+      <c r="A24" s="17" t="n">
+        <v>26</v>
+      </c>
+      <c r="B24" t="n">
         <v>20302200046</v>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.0342995705230552</v>
-      </c>
-      <c r="F12" t="n">
+      <c r="D24" t="n">
+        <v>71.38391837271729</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.02025355339815887</v>
+      </c>
+      <c r="F24" t="n">
         <v>1300</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G24" t="n">
         <v>1300</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="16" t="n">
-        <v>10</v>
-      </c>
-      <c r="B13" t="n">
+    <row r="25">
+      <c r="A25" s="17" t="n">
+        <v>22</v>
+      </c>
+      <c r="B25" t="n">
         <v>20370900050</v>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.08838906300823286</v>
-      </c>
-      <c r="F13" t="n">
+      <c r="D25" t="n">
+        <v>34.18915474247277</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.05219285781573143</v>
+      </c>
+      <c r="F25" t="n">
         <v>1309</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G25" t="n">
         <v>1309</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="16" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="n">
+    <row r="26">
+      <c r="A26" s="17" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
         <v>20320900049</v>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.05219285781573143</v>
-      </c>
-      <c r="F14" t="n">
+      <c r="D26" t="n">
+        <v>55.06197560429983</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.03081936061161125</v>
+      </c>
+      <c r="F26" t="n">
         <v>1320</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G26" t="n">
         <v>1320</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B15" t="n">
-        <v>20280900048</v>
-      </c>
-      <c r="C15" t="inlineStr">
+    <row r="27">
+      <c r="A27" s="17" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>20300800045</v>
+      </c>
+      <c r="C27" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.03424373401290139</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1320</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="16" t="n">
-        <v>13</v>
-      </c>
-      <c r="B16" t="n">
-        <v>20300800045</v>
-      </c>
-      <c r="C16" t="inlineStr">
+      <c r="D27" t="n">
+        <v>66.6249904812028</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.02873178505320212</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1343</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="B28" t="n">
+        <v>20500800053</v>
+      </c>
+      <c r="C28" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.04865753027689226</v>
-      </c>
-      <c r="F16" t="n">
-        <v>1343</v>
-      </c>
-      <c r="G16" t="n">
-        <v>1343</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="16" t="n">
-        <v>5</v>
-      </c>
-      <c r="B17" t="n">
-        <v>20500800053</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.400221</v>
-      </c>
-      <c r="F17" t="n">
+      <c r="D28" t="n">
+        <v>9.903380302200008</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.23632649829</v>
+      </c>
+      <c r="F28" t="n">
         <v>15000</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G28" t="n">
         <v>15000</v>
       </c>
     </row>
@@ -2742,7 +3018,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2751,49 +3027,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="16" t="inlineStr">
+      <c r="B1" s="17" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="16" t="inlineStr">
+      <c r="C1" s="17" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
-      <c r="D1" s="16" t="inlineStr">
+      <c r="D1" s="17" t="inlineStr">
         <is>
           <t>OpexVarInEURperMWH</t>
         </is>
       </c>
-      <c r="E1" s="16" t="inlineStr">
+      <c r="E1" s="17" t="inlineStr">
         <is>
           <t>Set</t>
         </is>
       </c>
-      <c r="F1" s="16" t="inlineStr">
+      <c r="F1" s="17" t="inlineStr">
         <is>
           <t>SupportInstrument</t>
         </is>
       </c>
-      <c r="G1" s="16" t="inlineStr">
+      <c r="G1" s="17" t="inlineStr">
         <is>
           <t>FIT</t>
         </is>
       </c>
-      <c r="H1" s="16" t="inlineStr">
+      <c r="H1" s="17" t="inlineStr">
         <is>
           <t>Premium</t>
         </is>
       </c>
-      <c r="I1" s="16" t="inlineStr">
+      <c r="I1" s="17" t="inlineStr">
         <is>
           <t>Lcoe</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="16" t="n">
+      <c r="A2" s="17" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
@@ -2803,7 +3079,7 @@
         <v>4000</v>
       </c>
       <c r="D2" t="n">
-        <v>1.35</v>
+        <v>3.183229382850003</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -2832,7 +3108,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="16" t="n">
+      <c r="A3" s="17" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
@@ -2871,7 +3147,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="16" t="n">
+      <c r="A4" s="17" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
@@ -2881,7 +3157,7 @@
         <v>7000</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>7.073843073000006</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -2910,7 +3186,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="16" t="n">
+      <c r="A5" s="17" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="n">
@@ -2949,7 +3225,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="16" t="n">
+      <c r="A6" s="17" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="n">
@@ -2959,7 +3235,7 @@
         <v>7000</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>9.41528513016301</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -2988,7 +3264,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="16" t="n">
+      <c r="A7" s="17" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="n">
@@ -3027,7 +3303,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="16" t="n">
+      <c r="A8" s="17" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="n">
@@ -3037,7 +3313,7 @@
         <v>7000</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>12.53174450824697</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -3066,7 +3342,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="16" t="n">
+      <c r="A9" s="17" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="n">
@@ -3105,7 +3381,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="16" t="n">
+      <c r="A10" s="17" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="n">
@@ -3115,7 +3391,7 @@
         <v>7000</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>16.67975194047672</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -3144,7 +3420,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="16" t="n">
+      <c r="A11" s="17" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="n">
@@ -3154,7 +3430,7 @@
         <v>4000</v>
       </c>
       <c r="D11" t="n">
-        <v>1.35</v>
+        <v>8.256477210535976</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -3183,7 +3459,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="16" t="n">
+      <c r="A12" s="17" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="n">
@@ -3193,7 +3469,7 @@
         <v>7000</v>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>18.34772713452439</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -3222,7 +3498,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="16" t="n">
+      <c r="A13" s="17" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="n">
@@ -3261,7 +3537,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="16" t="n">
+      <c r="A14" s="17" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="n">
@@ -3271,7 +3547,7 @@
         <v>7000</v>
       </c>
       <c r="D14" t="n">
-        <v>3</v>
+        <v>22.20074983277452</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -3300,7 +3576,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="16" t="n">
+      <c r="A15" s="17" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="n">
@@ -3310,7 +3586,7 @@
         <v>7000</v>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>26.86290729765717</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -3339,21 +3615,21 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="16" t="n">
+      <c r="A16" s="17" t="n">
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20340300028</v>
+        <v>20340100037</v>
       </c>
       <c r="C16" t="n">
-        <v>16500</v>
+        <v>7000</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>32.50411783016519</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -3378,17 +3654,17 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="16" t="n">
+      <c r="A17" s="17" t="n">
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20340100037</v>
+        <v>20320100038</v>
       </c>
       <c r="C17" t="n">
         <v>7000</v>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>39.32998257449988</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -3417,17 +3693,17 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="16" t="n">
+      <c r="A18" s="17" t="n">
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20320100038</v>
+        <v>20300100039</v>
       </c>
       <c r="C18" t="n">
         <v>7000</v>
       </c>
       <c r="D18" t="n">
-        <v>3</v>
+        <v>47.58927891514486</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -3450,123 +3726,6 @@
         </is>
       </c>
       <c r="I18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="16" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>20300200022</v>
-      </c>
-      <c r="C19" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>WindOn</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="16" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>20300300029</v>
-      </c>
-      <c r="C20" t="n">
-        <v>17349</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="16" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>20300100039</v>
-      </c>
-      <c r="C21" t="n">
-        <v>7000</v>
-      </c>
-      <c r="D21" t="n">
-        <v>3</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>WindOff</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -3592,44 +3751,44 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="16" t="inlineStr">
+      <c r="B1" s="17" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="16" t="inlineStr">
+      <c r="C1" s="17" t="inlineStr">
         <is>
           <t>StorageType</t>
         </is>
       </c>
-      <c r="D1" s="16" t="inlineStr">
+      <c r="D1" s="17" t="inlineStr">
         <is>
           <t>EnergyToPowerRatio</t>
         </is>
       </c>
-      <c r="E1" s="16" t="inlineStr">
+      <c r="E1" s="17" t="inlineStr">
         <is>
           <t>ChargingEfficiency</t>
         </is>
       </c>
-      <c r="F1" s="16" t="inlineStr">
+      <c r="F1" s="17" t="inlineStr">
         <is>
           <t>DischargingEfficiency</t>
         </is>
       </c>
-      <c r="G1" s="16" t="inlineStr">
+      <c r="G1" s="17" t="inlineStr">
         <is>
           <t>InitialEnergyLevelInMWH</t>
         </is>
       </c>
-      <c r="H1" s="16" t="inlineStr">
+      <c r="H1" s="17" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="16" t="n">
+      <c r="A2" s="17" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
@@ -3644,7 +3803,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.92</v>
+        <v>0.3486784401000001</v>
       </c>
       <c r="F2" t="n">
         <v>0.92</v>

</xml_diff>

<commit_message>
testing industrial demand as hydrogen
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\amiris_workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4938E5-79A8-47D4-B940-5C3B0AEB59B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10A7A32-B5C8-4578-927A-1CFA321D7404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="993" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16485" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="993" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_skeleton" sheetId="1" r:id="rId1"/>
@@ -423,6 +423,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1267,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1327,10 +1328,10 @@
         <v>90</v>
       </c>
       <c r="B5" s="6">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1338,23 +1339,13 @@
         <v>90</v>
       </c>
       <c r="B6" s="6">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="6">
-        <v>60</v>
-      </c>
-      <c r="C7" s="6" t="s">
         <v>96</v>
       </c>
     </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1710,7 +1701,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1828,6 +1819,17 @@
       </c>
       <c r="C12" s="6" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="6">
+        <v>80</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -2598,9 +2600,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="14.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" s="10" t="s">
@@ -2633,7 +2640,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.74</v>
+        <v>0.99</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>

<commit_message>
reorganizing amiris config files
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28830" yWindow="-16350" windowWidth="29040" windowHeight="15840" tabRatio="993" firstSheet="0" activeTab="10" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="993" firstSheet="0" activeTab="10" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_skeleton" sheetId="1" state="visible" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
     <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -80,7 +80,11 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -189,7 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
@@ -210,10 +214,13 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1201,17 +1208,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="inlineStr">
+      <c r="A1" s="12" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>VOLL</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="12" t="inlineStr">
         <is>
           <t>TimeSeries</t>
         </is>
@@ -1224,12 +1231,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>60</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>amiris-config/data/LS_hydrogen_high.csv</t>
-        </is>
+        <v>47</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1239,12 +1244,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>40</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>amiris-config/data/LS_hydrogen_low.csv</t>
-        </is>
+        <v>4000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1254,12 +1257,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4000</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>amiris-config/data/load.csv</t>
-        </is>
+        <v>1500</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1269,12 +1270,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>amiris-config/data/LS_high.csv</t>
-        </is>
+        <v>250</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1286,10 +1285,8 @@
       <c r="B6" t="n">
         <v>500</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>amiris-config/data/LS_low.csv</t>
-        </is>
+      <c r="C6" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1876,27 +1873,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="n">
+      <c r="B1" s="12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="inlineStr">
+      <c r="A2" s="12" t="inlineStr">
         <is>
           <t>StartTime</t>
         </is>
       </c>
-      <c r="B2" s="13" t="n">
+      <c r="B2" s="14" t="n">
         <v>54788.99861111111</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="inlineStr">
+      <c r="A3" s="12" t="inlineStr">
         <is>
           <t>StopTime</t>
         </is>
       </c>
-      <c r="B3" s="13" t="n">
+      <c r="B3" s="14" t="n">
         <v>55152.99861111111</v>
       </c>
     </row>
@@ -2066,64 +2063,64 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>AgentType</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="12" t="inlineStr">
         <is>
           <t>CO2</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>HARD_COAL</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="F1" s="12" t="inlineStr">
         <is>
           <t>OIL</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="G1" s="12" t="inlineStr">
         <is>
           <t>HYDROGEN</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="H1" s="12" t="inlineStr">
         <is>
           <t>LIGNITE</t>
         </is>
       </c>
-      <c r="H1" s="11" t="inlineStr">
+      <c r="I1" s="12" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="I1" s="11" t="inlineStr">
+      <c r="J1" s="12" t="inlineStr">
         <is>
           <t>NUCLEAR</t>
         </is>
       </c>
-      <c r="J1" s="11" t="inlineStr">
+      <c r="K1" s="12" t="inlineStr">
         <is>
           <t>WASTE</t>
         </is>
       </c>
-      <c r="K1" s="11" t="inlineStr">
+      <c r="L1" s="12" t="inlineStr">
         <is>
           <t>BIOMASS</t>
         </is>
       </c>
-      <c r="L1" s="11" t="inlineStr">
-        <is>
-          <t>OTHER</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="12" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -2132,7 +2129,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>199.9999999999991</v>
+        <v>167.9999999999998</v>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
@@ -2145,7 +2142,7 @@
       <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="n">
+      <c r="A3" s="12" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -2155,31 +2152,31 @@
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>6.732000000039989</v>
+        <v>64.47999999998137</v>
       </c>
       <c r="E3" t="n">
+        <v>6.730000000001382</v>
+      </c>
+      <c r="F3" t="n">
         <v>79.69000000000142</v>
       </c>
-      <c r="F3" t="n">
-        <v>80.0000000000291</v>
-      </c>
       <c r="G3" t="n">
+        <v>48.57925285126839</v>
+      </c>
+      <c r="H3" t="n">
         <v>6.479999999999997</v>
       </c>
-      <c r="H3" t="n">
-        <v>41.9999999999709</v>
-      </c>
       <c r="I3" t="n">
+        <v>14.65000000003783</v>
+      </c>
+      <c r="J3" t="n">
         <v>1.689999999999999</v>
       </c>
-      <c r="J3" t="n">
-        <v>7.499999999999995</v>
-      </c>
       <c r="K3" t="n">
-        <v>34.99999999991269</v>
+        <v>7.499999999999996</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>34.99999999995634</v>
       </c>
     </row>
   </sheetData>
@@ -2193,7 +2190,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2202,60 +2199,260 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="12" t="inlineStr">
         <is>
           <t>FuelType</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>OpexVarInEURperMWH</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>Efficiency</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="12" t="inlineStr">
         <is>
           <t>BlockSizeInMW</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="G1" s="12" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="12" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20491900040</v>
+        <v>20383300053</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>OTHER</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.02</v>
+        <v>1.5</v>
       </c>
       <c r="E2" t="n">
-        <v>0.283575</v>
+        <v>0.4</v>
       </c>
       <c r="F2" t="n">
-        <v>5663</v>
+        <v>1500</v>
       </c>
       <c r="G2" t="n">
-        <v>5663</v>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>20323300052</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>20313300051</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>20303300050</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>20293300049</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20283300048</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20273300047</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20263300046</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="12" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20253300045</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>
@@ -2278,34 +2475,34 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="12" t="inlineStr">
         <is>
           <t>ElectrolyserType</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>PeakConsumptionInMW</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>ConversionFactor</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="12" t="inlineStr">
         <is>
           <t>HydrogenProductionTargetInMWH</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="12" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
@@ -2337,7 +2534,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2346,63 +2543,63 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="12" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>OpexVarInEURperMWH</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>Set</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="12" t="inlineStr">
         <is>
           <t>SupportInstrument</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="G1" s="12" t="inlineStr">
         <is>
           <t>FIT</t>
         </is>
       </c>
-      <c r="H1" s="11" t="inlineStr">
+      <c r="H1" s="12" t="inlineStr">
         <is>
           <t>Premium</t>
         </is>
       </c>
-      <c r="I1" s="11" t="inlineStr">
+      <c r="I1" s="12" t="inlineStr">
         <is>
           <t>Lcoe</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="12" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20500100030</v>
+        <v>20390200023</v>
       </c>
       <c r="C2" t="n">
-        <v>7000</v>
+        <v>4000</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>1.35</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2427,21 +2624,21 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="n">
+      <c r="A3" s="12" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20490200021</v>
+        <v>20390300033</v>
       </c>
       <c r="C3" t="n">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="D3" t="n">
-        <v>1.35675</v>
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2466,14 +2663,14 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="n">
+      <c r="A4" s="12" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20490300024</v>
+        <v>20380300032</v>
       </c>
       <c r="C4" t="n">
-        <v>5500</v>
+        <v>5000</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -2505,21 +2702,21 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="n">
+      <c r="A5" s="12" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20491500041</v>
+        <v>20370300031</v>
       </c>
       <c r="C5" t="n">
-        <v>41</v>
+        <v>5000</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>RunOfRiver</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2544,21 +2741,21 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="n">
+      <c r="A6" s="12" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20470100031</v>
+        <v>20360300030</v>
       </c>
       <c r="C6" t="n">
-        <v>7000</v>
+        <v>5500</v>
       </c>
       <c r="D6" t="n">
-        <v>3.045225374999999</v>
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -2583,14 +2780,14 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="n">
+      <c r="A7" s="12" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20460300025</v>
+        <v>20350300029</v>
       </c>
       <c r="C7" t="n">
-        <v>5500</v>
+        <v>4500</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -2622,21 +2819,21 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="11" t="n">
+      <c r="A8" s="12" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20440100032</v>
+        <v>20340200022</v>
       </c>
       <c r="C8" t="n">
-        <v>7000</v>
+        <v>4000</v>
       </c>
       <c r="D8" t="n">
-        <v>3.091132528181295</v>
+        <v>1.35</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2661,14 +2858,14 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="n">
+      <c r="A9" s="12" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20420300026</v>
+        <v>20340300028</v>
       </c>
       <c r="C9" t="n">
-        <v>5500</v>
+        <v>3257</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -2700,17 +2897,17 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11" t="n">
+      <c r="A10" s="12" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20410100033</v>
+        <v>20340100043</v>
       </c>
       <c r="C10" t="n">
         <v>7000</v>
       </c>
       <c r="D10" t="n">
-        <v>3.137731737435193</v>
+        <v>2.7</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -2739,21 +2936,21 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="n">
+      <c r="A11" s="12" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20400200023</v>
+        <v>20330300027</v>
       </c>
       <c r="C11" t="n">
-        <v>4000</v>
+        <v>4500</v>
       </c>
       <c r="D11" t="n">
-        <v>1.419039178255066</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -2778,17 +2975,17 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11" t="n">
+      <c r="A12" s="12" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20400100034</v>
+        <v>20330100042</v>
       </c>
       <c r="C12" t="n">
         <v>7000</v>
       </c>
       <c r="D12" t="n">
-        <v>3.153420396122369</v>
+        <v>2.7</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2817,14 +3014,14 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="n">
+      <c r="A13" s="12" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20380300027</v>
+        <v>20320300026</v>
       </c>
       <c r="C13" t="n">
-        <v>5500</v>
+        <v>4500</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -2856,17 +3053,17 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="n">
+      <c r="A14" s="12" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20380100035</v>
+        <v>20320100041</v>
       </c>
       <c r="C14" t="n">
         <v>7000</v>
       </c>
       <c r="D14" t="n">
-        <v>3.185033435593495</v>
+        <v>2.7</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2895,223 +3092,223 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="n">
+      <c r="A15" s="12" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20360100036</v>
+        <v>20310300025</v>
       </c>
       <c r="C15" t="n">
+        <v>4500</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="12" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20310100040</v>
+      </c>
+      <c r="C16" t="n">
         <v>7000</v>
       </c>
-      <c r="D15" t="n">
-        <v>3.216963395785319</v>
-      </c>
-      <c r="E15" t="inlineStr">
+      <c r="D16" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="11" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="n">
-        <v>20340300028</v>
-      </c>
-      <c r="C16" t="n">
-        <v>5500</v>
-      </c>
-      <c r="D16" t="n">
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20300200021</v>
+      </c>
+      <c r="C17" t="n">
+        <v>4000</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="12" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20300300024</v>
+      </c>
+      <c r="C18" t="n">
+        <v>4500</v>
+      </c>
+      <c r="D18" t="n">
         <v>0</v>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>OtherPV</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="11" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>20340100037</v>
-      </c>
-      <c r="C17" t="n">
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="12" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20300100039</v>
+      </c>
+      <c r="C19" t="n">
         <v>7000</v>
       </c>
-      <c r="D17" t="n">
-        <v>3.249213453828066</v>
-      </c>
-      <c r="E17" t="inlineStr">
+      <c r="D19" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="11" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>20320100038</v>
-      </c>
-      <c r="C18" t="n">
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="12" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20290100038</v>
+      </c>
+      <c r="C20" t="n">
         <v>7000</v>
       </c>
-      <c r="D18" t="n">
-        <v>3.281786818702691</v>
-      </c>
-      <c r="E18" t="inlineStr">
+      <c r="D20" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="11" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="n">
-        <v>20300200022</v>
-      </c>
-      <c r="C19" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1.491609029202083</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>WindOn</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="11" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>20300300029</v>
-      </c>
-      <c r="C20" t="n">
-        <v>5783</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>OtherPV</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>NONE</t>
-        </is>
-      </c>
       <c r="G20" t="inlineStr">
         <is>
           <t>-</t>
@@ -3129,17 +3326,17 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="11" t="n">
+      <c r="A21" s="12" t="n">
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20300100039</v>
+        <v>20280100037</v>
       </c>
       <c r="C21" t="n">
         <v>7000</v>
       </c>
       <c r="D21" t="n">
-        <v>3.314686731560185</v>
+        <v>2.7</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -3162,6 +3359,123 @@
         </is>
       </c>
       <c r="I21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="12" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20270100036</v>
+      </c>
+      <c r="C22" t="n">
+        <v>7000</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="12" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>20260100035</v>
+      </c>
+      <c r="C23" t="n">
+        <v>7000</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="12" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>20250100034</v>
+      </c>
+      <c r="C24" t="n">
+        <v>7000</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -3178,7 +3492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3187,48 +3501,48 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="12" t="inlineStr">
         <is>
           <t>StorageType</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>EnergyToPowerRatio</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>ChargingEfficiency</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="12" t="inlineStr">
         <is>
           <t>DischargingEfficiency</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="G1" s="12" t="inlineStr">
         <is>
           <t>InitialEnergyLevelInMWH</t>
         </is>
       </c>
-      <c r="H1" s="11" t="inlineStr">
+      <c r="H1" s="12" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="12" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>99992600008</v>
+        <v>20352600044</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -3236,10 +3550,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="F2" t="n">
         <v>0.92</v>
@@ -3248,35 +3562,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>20492600042</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.8955</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1736</v>
+        <v>1700</v>
       </c>
     </row>
   </sheetData>
@@ -3317,42 +3603,42 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="12" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="12" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="12" t="inlineStr">
         <is>
           <t>OpexVarInEURperMWH</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>Set</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="12" t="inlineStr">
         <is>
           <t>SupportInstrument</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="G1" s="12" t="inlineStr">
         <is>
           <t>FIT</t>
         </is>
       </c>
-      <c r="H1" s="11" t="inlineStr">
+      <c r="H1" s="12" t="inlineStr">
         <is>
           <t>Premium</t>
         </is>
       </c>
-      <c r="I1" s="11" t="inlineStr">
+      <c r="I1" s="12" t="inlineStr">
         <is>
           <t>Lcoe</t>
         </is>

</xml_diff>

<commit_message>
verification run with load shedders
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -33,8 +33,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -209,7 +209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -242,7 +242,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1581,7 +1582,7 @@
           <t>StartTime</t>
         </is>
       </c>
-      <c r="B2" s="16" t="n">
+      <c r="B2" s="17" t="n">
         <v>56249.99861111111</v>
       </c>
     </row>
@@ -1591,7 +1592,7 @@
           <t>StopTime</t>
         </is>
       </c>
-      <c r="B3" s="16" t="n">
+      <c r="B3" s="17" t="n">
         <v>56613.99861111111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
enabling stochastic increase demand
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1476,7 +1476,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>amiris-config/data/future_load.csv</t>
+          <t>amiris-config/data/load.csv</t>
         </is>
       </c>
     </row>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>amiris-config/data/future_LS_high.csv</t>
+          <t>amiris-config/data/LS_high.csv</t>
         </is>
       </c>
     </row>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>amiris-config/data/future_LS_low.csv</t>
+          <t>amiris-config/data/LS_low.csv</t>
         </is>
       </c>
     </row>
@@ -1548,7 +1548,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>amiris-config/data/future_LS_mid.csv</t>
+          <t>amiris-config/data/LS_mid.csv</t>
         </is>
       </c>
     </row>
@@ -1583,7 +1583,7 @@
         </is>
       </c>
       <c r="B2" s="17" t="n">
-        <v>56249.99861111111</v>
+        <v>54788.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1593,7 +1593,7 @@
         </is>
       </c>
       <c r="B3" s="17" t="n">
-        <v>56613.99861111111</v>
+        <v>55152.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1852,7 +1852,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2019,10 +2019,10 @@
     </row>
     <row r="7">
       <c r="A7" s="15" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>20493300068</v>
+        <v>20243300061</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -2036,18 +2036,18 @@
         <v>0.4</v>
       </c>
       <c r="F7" t="n">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="G7" t="n">
-        <v>2000</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>20463300067</v>
+        <v>20493300068</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -2069,26 +2069,51 @@
     </row>
     <row r="9">
       <c r="A9" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20463300067</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B10" t="n">
         <v>20491900021</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>NUCLEAR</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>4</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>0.285</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F10" t="n">
         <v>5663.943</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G10" t="n">
         <v>5663.943</v>
       </c>
     </row>
@@ -2504,7 +2529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3885,17 +3910,17 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>20280100050</v>
+        <v>20290300029</v>
       </c>
       <c r="C36" t="n">
         <v>3000</v>
       </c>
       <c r="D36" t="n">
-        <v>2.7</v>
+        <v>0</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3924,7 +3949,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>20260100049</v>
+        <v>20280100050</v>
       </c>
       <c r="C37" t="n">
         <v>3000</v>
@@ -3953,6 +3978,123 @@
         </is>
       </c>
       <c r="I37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="15" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>20270300028</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="15" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>20260300027</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="15" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>20260100049</v>
+      </c>
+      <c r="C40" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D40" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>

<commit_message>
Update to latest AMIRIS data structure
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\TradeRES\toolbox-amiris-emlab-new\toolbox-amiris-emlab\amiris_workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB415195-D413-4B18-A5B6-BAA0A800728E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8128B2-F74E-4DDF-B9AE-F932B64DF1AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="935" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="8325" tabRatio="880" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_skeleton" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="108">
   <si>
     <t>group</t>
   </si>
@@ -189,6 +189,9 @@
     <t>CO2</t>
   </si>
   <si>
+    <t>OTHER</t>
+  </si>
+  <si>
     <t>HARD_COAL</t>
   </si>
   <si>
@@ -213,9 +216,6 @@
     <t>BIOMASS</t>
   </si>
   <si>
-    <t>OTHER</t>
-  </si>
-  <si>
     <t>FuelsMarket</t>
   </si>
   <si>
@@ -255,15 +255,18 @@
     <t>Lcoe</t>
   </si>
   <si>
+    <t>PVRooftop</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>OtherPV</t>
   </si>
   <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>WindOn</t>
   </si>
   <si>
@@ -333,7 +336,19 @@
     <t>amiris-config/data/demand_processed/ind_cluster-2_shedding_timeseries.csv</t>
   </si>
   <si>
-    <t>amiris-config/data/load.csv</t>
+    <t>amiris-config/data/future_load.csv</t>
+  </si>
+  <si>
+    <t>amiris-config/data/future_LS_high.csv</t>
+  </si>
+  <si>
+    <t>amiris-config/data/LS_hydrogen.csv</t>
+  </si>
+  <si>
+    <t>amiris-config/data/future_LS_low.csv</t>
+  </si>
+  <si>
+    <t>amiris-config/data/future_LS_mid.csv</t>
   </si>
   <si>
     <t>StartTime</t>
@@ -345,7 +360,7 @@
     <t>Strategist</t>
   </si>
   <si>
-    <t>MULTI_AGENT_SIMPLE</t>
+    <t>SINGLE_AGENT_MIN_SYSTEM_COST</t>
   </si>
 </sst>
 </file>
@@ -401,7 +416,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -417,7 +431,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -488,38 +502,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -536,19 +524,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1205,31 +1185,31 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="9" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1324,7 +1304,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,83 +1316,83 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B2" s="7">
         <v>4000</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B3" s="7">
         <v>300</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B4" s="7">
         <v>300.7</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B5" s="7">
         <v>447.1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B6" s="7">
         <v>607.5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B7" s="7">
         <v>1151.9000000000001</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" s="11"/>
+      <c r="C15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1422,66 +1402,98 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="3" width="46.5703125" style="2" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="9" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="7">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>400000000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2">
         <v>4000</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>150000000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3">
+        <v>1500</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3300000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>25000000</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5">
+        <v>250</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50000000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6">
+        <v>500</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1491,27 +1503,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="12">
+      <c r="B1" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="13">
-        <v>54788.998611111107</v>
+      <c r="A2" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="10">
+        <v>58806.998611111107</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B3" s="13">
-        <v>55152.998611111107</v>
+      <c r="A3" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="10">
+        <v>59170.998611111107</v>
       </c>
     </row>
   </sheetData>
@@ -1600,87 +1612,87 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2">
-        <v>199.99999999999909</v>
+        <v>167.9999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>59</v>
       </c>
       <c r="D3">
-        <v>6.7320000000399887</v>
+        <v>45.100000000064028</v>
       </c>
       <c r="E3">
+        <v>6.7300000000013824</v>
+      </c>
+      <c r="F3">
         <v>79.690000000001419</v>
       </c>
-      <c r="F3">
-        <v>80.000000000029104</v>
-      </c>
       <c r="G3">
+        <v>48.579252851268393</v>
+      </c>
+      <c r="H3">
         <v>6.4799999999999969</v>
       </c>
-      <c r="H3">
-        <v>41.999999999970903</v>
-      </c>
       <c r="I3">
+        <v>14.65000000003783</v>
+      </c>
+      <c r="J3">
         <v>1.6899999999999991</v>
       </c>
-      <c r="J3">
-        <v>7.4999999999999947</v>
-      </c>
       <c r="K3">
-        <v>34.999999999912689</v>
+        <v>7.4999999999999956</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>34.999999999956337</v>
       </c>
     </row>
   </sheetData>
@@ -1690,41 +1702,41 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
       <c r="B2">
         <v>99993300004</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>1.5</v>
@@ -1740,20 +1752,20 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>99990300005</v>
+        <v>99990600006</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D3">
-        <v>4.2</v>
+        <v>1.9</v>
       </c>
       <c r="E3">
-        <v>0.61</v>
+        <v>0.309</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1763,325 +1775,233 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>99990100006</v>
+        <v>20523300069</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D4">
-        <v>1.9</v>
+        <v>1.5</v>
       </c>
       <c r="E4">
-        <v>0.309</v>
+        <v>0.4</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="9">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>20423300066</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5">
+        <v>1.5</v>
+      </c>
+      <c r="E5">
+        <v>0.4</v>
+      </c>
+      <c r="F5">
+        <v>1500</v>
+      </c>
+      <c r="G5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>20403300065</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>1.5</v>
+      </c>
+      <c r="E6">
+        <v>0.4</v>
+      </c>
+      <c r="F6">
+        <v>1500</v>
+      </c>
+      <c r="G6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>20363300064</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>1.5</v>
+      </c>
+      <c r="E7">
+        <v>0.4</v>
+      </c>
+      <c r="F7">
+        <v>1500</v>
+      </c>
+      <c r="G7">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>20323300063</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>1.5</v>
+      </c>
+      <c r="E8">
+        <v>0.4</v>
+      </c>
+      <c r="F8">
+        <v>1500</v>
+      </c>
+      <c r="G8">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>20283300062</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>1.5</v>
+      </c>
+      <c r="E9">
+        <v>0.4</v>
+      </c>
+      <c r="F9">
+        <v>1500</v>
+      </c>
+      <c r="G9">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>20243300061</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>1.5</v>
+      </c>
+      <c r="E10">
+        <v>0.4</v>
+      </c>
+      <c r="F10">
+        <v>1500</v>
+      </c>
+      <c r="G10">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>20493300068</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11">
+        <v>1.5</v>
+      </c>
+      <c r="E11">
+        <v>0.4</v>
+      </c>
+      <c r="F11">
+        <v>2000</v>
+      </c>
+      <c r="G11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>20463300067</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>1.5</v>
+      </c>
+      <c r="E12">
+        <v>0.4</v>
+      </c>
+      <c r="F12">
+        <v>2000</v>
+      </c>
+      <c r="G12">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>99991700009</v>
-      </c>
-      <c r="C5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5">
-        <v>4.5</v>
-      </c>
-      <c r="E5">
-        <v>0.43</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>20300300049</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6">
-        <v>4.2</v>
-      </c>
-      <c r="E6">
-        <v>0.58498853211009172</v>
-      </c>
-      <c r="F6">
-        <v>343</v>
-      </c>
-      <c r="G6">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="B13">
+        <v>20491900021</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>20501400044</v>
-      </c>
-      <c r="C7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>0.34</v>
-      </c>
-      <c r="F7">
-        <v>484</v>
-      </c>
-      <c r="G7">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>20460300045</v>
-      </c>
-      <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8">
-        <v>4.2</v>
-      </c>
-      <c r="E8">
-        <v>0.52</v>
-      </c>
-      <c r="F8">
-        <v>1000</v>
-      </c>
-      <c r="G8">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>20420300046</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9">
-        <v>4.2</v>
-      </c>
-      <c r="E9">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F9">
-        <v>1000</v>
-      </c>
-      <c r="G9">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>20380300047</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10">
-        <v>4.2</v>
-      </c>
-      <c r="E10">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="F10">
-        <v>1000</v>
-      </c>
-      <c r="G10">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>20340300048</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11">
-        <v>4.2</v>
-      </c>
-      <c r="E11">
-        <v>0.59</v>
-      </c>
-      <c r="F11">
-        <v>1000</v>
-      </c>
-      <c r="G11">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>20401700051</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12">
-        <v>4.5</v>
-      </c>
-      <c r="E12">
-        <v>0.36299999999999999</v>
-      </c>
-      <c r="F12">
-        <v>1300</v>
-      </c>
-      <c r="G12">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>14</v>
-      </c>
-      <c r="B13">
-        <v>20301700050</v>
-      </c>
-      <c r="C13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13">
-        <v>4.5</v>
-      </c>
       <c r="E13">
-        <v>0.38765163297045102</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F13">
-        <v>1300</v>
+        <v>5663.9430000000002</v>
       </c>
       <c r="G13">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>20370400054</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14">
-        <v>4.2</v>
-      </c>
-      <c r="E14">
-        <v>0.35211968384126402</v>
-      </c>
-      <c r="F14">
-        <v>1320</v>
-      </c>
-      <c r="G14">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>20320400053</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15">
-        <v>4.2</v>
-      </c>
-      <c r="E15">
-        <v>0.4374676880872479</v>
-      </c>
-      <c r="F15">
-        <v>1320</v>
-      </c>
-      <c r="G15">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>20280400052</v>
-      </c>
-      <c r="C16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16">
-        <v>4.2</v>
-      </c>
-      <c r="E16">
-        <v>0.35755348765669459</v>
-      </c>
-      <c r="F16">
-        <v>1320</v>
-      </c>
-      <c r="G16">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
-        <v>12</v>
-      </c>
-      <c r="B17">
-        <v>20300100021</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17">
-        <v>1.9</v>
-      </c>
-      <c r="E17">
-        <v>0.42</v>
-      </c>
-      <c r="F17">
-        <v>9000</v>
-      </c>
-      <c r="G17">
-        <v>9000</v>
+        <v>5663.9430000000002</v>
       </c>
     </row>
   </sheetData>
@@ -2105,11 +2025,11 @@
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <f>SUM(conventionals!G:G,renewables_full!C:C,biogas_full!C:C)</f>
-        <v>20391</v>
+        <v>19665.942999999999</v>
       </c>
       <c r="B1">
         <f>A1/1000</f>
-        <v>20.390999999999998</v>
+        <v>19.665942999999999</v>
       </c>
       <c r="C1" t="s">
         <v>66</v>
@@ -2466,44 +2386,44 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="9" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>99992100002</v>
+        <v>99990500001</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2528,17 +2448,17 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>99992400003</v>
+        <v>99990300002</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>75</v>
@@ -2557,17 +2477,17 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>99992300007</v>
+        <v>99990200003</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>1.35</v>
       </c>
       <c r="E4" t="s">
         <v>76</v>
@@ -2586,20 +2506,20 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>20502400025</v>
+        <v>99990100007</v>
       </c>
       <c r="C5">
-        <v>4000</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F5" t="s">
         <v>73</v>
@@ -2615,20 +2535,20 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>20502100028</v>
+        <v>20490300048</v>
       </c>
       <c r="C6">
-        <v>5500</v>
+        <v>3000</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F6" t="s">
         <v>73</v>
@@ -2644,17 +2564,17 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>20502300034</v>
+        <v>20480200026</v>
       </c>
       <c r="C7">
-        <v>7000</v>
+        <v>2400</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>1.35</v>
       </c>
       <c r="E7" t="s">
         <v>76</v>
@@ -2673,20 +2593,20 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>20472300035</v>
+        <v>20480300047</v>
       </c>
       <c r="C8">
-        <v>7000</v>
+        <v>3850</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" t="s">
         <v>73</v>
@@ -2702,49 +2622,49 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>20462100029</v>
+        <v>20480100060</v>
       </c>
       <c r="C9">
-        <v>5500</v>
+        <v>3000</v>
       </c>
       <c r="D9">
+        <v>2.7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>20470300046</v>
+      </c>
+      <c r="C10">
+        <v>3500</v>
+      </c>
+      <c r="D10">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H9" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>20442300036</v>
-      </c>
-      <c r="C10">
-        <v>7000</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" t="s">
         <v>73</v>
@@ -2760,49 +2680,49 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="9">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>20422100030</v>
+        <v>20470100059</v>
       </c>
       <c r="C11">
-        <v>5500</v>
+        <v>3000</v>
       </c>
       <c r="D11">
+        <v>2.7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>20460300045</v>
+      </c>
+      <c r="C12">
+        <v>3500</v>
+      </c>
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>20412300037</v>
-      </c>
-      <c r="C12">
-        <v>7000</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" t="s">
         <v>73</v>
@@ -2818,50 +2738,50 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="9">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>20402400027</v>
+        <v>20460100058</v>
       </c>
       <c r="C13">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D13">
-        <v>1.35</v>
+        <v>2.7</v>
       </c>
       <c r="E13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>20450300044</v>
+      </c>
+      <c r="C14">
+        <v>3500</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
         <v>75</v>
       </c>
-      <c r="F13" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" t="s">
-        <v>74</v>
-      </c>
-      <c r="I13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>20402300038</v>
-      </c>
-      <c r="C14">
-        <v>7000</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
-      </c>
       <c r="F14" t="s">
         <v>73</v>
       </c>
@@ -2876,20 +2796,20 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="9">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>20382100031</v>
+        <v>20440300043</v>
       </c>
       <c r="C15">
-        <v>5500</v>
+        <v>3500</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F15" t="s">
         <v>73</v>
@@ -2905,20 +2825,20 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="9">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>20382300039</v>
+        <v>20440100057</v>
       </c>
       <c r="C16">
-        <v>7000</v>
+        <v>4000</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
         <v>73</v>
@@ -2934,17 +2854,17 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
+      <c r="A17" s="9">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>20362300040</v>
+        <v>20430200025</v>
       </c>
       <c r="C17">
-        <v>7000</v>
+        <v>2400</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>1.35</v>
       </c>
       <c r="E17" t="s">
         <v>76</v>
@@ -2963,20 +2883,20 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="9">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>20342100032</v>
+        <v>20430300042</v>
       </c>
       <c r="C18">
-        <v>5500</v>
+        <v>3500</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F18" t="s">
         <v>73</v>
@@ -2992,20 +2912,20 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="A19" s="9">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>20342300041</v>
+        <v>20420300041</v>
       </c>
       <c r="C19">
-        <v>7000</v>
+        <v>3500</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F19" t="s">
         <v>73</v>
@@ -3021,20 +2941,20 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="9">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>20322300042</v>
+        <v>20420100056</v>
       </c>
       <c r="C20">
-        <v>7000</v>
+        <v>3000</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F20" t="s">
         <v>73</v>
@@ -3050,17 +2970,17 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+      <c r="A21" s="9">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>20302400026</v>
+        <v>20410300040</v>
       </c>
       <c r="C21">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="D21">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E21" t="s">
         <v>75</v>
@@ -3079,20 +2999,20 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="A22" s="9">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>20302100033</v>
+        <v>20400300039</v>
       </c>
       <c r="C22">
-        <v>5500</v>
+        <v>3500</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F22" t="s">
         <v>73</v>
@@ -3108,31 +3028,640 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
+      <c r="A23" s="9">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>20302300043</v>
+        <v>20400100055</v>
       </c>
       <c r="C23">
-        <v>7000</v>
+        <v>3000</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="E23" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>20390300038</v>
+      </c>
+      <c r="C24">
+        <v>3500</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" t="s">
+        <v>74</v>
+      </c>
+      <c r="I24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>20380200024</v>
+      </c>
+      <c r="C25">
+        <v>2400</v>
+      </c>
+      <c r="D25">
+        <v>1.35</v>
+      </c>
+      <c r="E25" t="s">
         <v>76</v>
       </c>
-      <c r="F23" t="s">
-        <v>73</v>
-      </c>
-      <c r="G23" t="s">
-        <v>74</v>
-      </c>
-      <c r="H23" t="s">
-        <v>74</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="F25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>20380300037</v>
+      </c>
+      <c r="C26">
+        <v>3000</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H26" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>20370300036</v>
+      </c>
+      <c r="C27">
+        <v>3000</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" t="s">
+        <v>74</v>
+      </c>
+      <c r="I27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>20360300035</v>
+      </c>
+      <c r="C28">
+        <v>3000</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>20360100054</v>
+      </c>
+      <c r="C29">
+        <v>3000</v>
+      </c>
+      <c r="D29">
+        <v>2.7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s">
+        <v>74</v>
+      </c>
+      <c r="I29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>20350300034</v>
+      </c>
+      <c r="C30">
+        <v>3000</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>20340200023</v>
+      </c>
+      <c r="C31">
+        <v>2400</v>
+      </c>
+      <c r="D31">
+        <v>1.35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" t="s">
+        <v>74</v>
+      </c>
+      <c r="H31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>20340300033</v>
+      </c>
+      <c r="C32">
+        <v>3000</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" t="s">
+        <v>74</v>
+      </c>
+      <c r="H32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>20340100053</v>
+      </c>
+      <c r="C33">
+        <v>3000</v>
+      </c>
+      <c r="D33">
+        <v>2.7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>20330300032</v>
+      </c>
+      <c r="C34">
+        <v>3000</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" t="s">
+        <v>74</v>
+      </c>
+      <c r="H34" t="s">
+        <v>74</v>
+      </c>
+      <c r="I34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>20320300031</v>
+      </c>
+      <c r="C35">
+        <v>3000</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" t="s">
+        <v>73</v>
+      </c>
+      <c r="G35" t="s">
+        <v>74</v>
+      </c>
+      <c r="H35" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>20320100052</v>
+      </c>
+      <c r="C36">
+        <v>3000</v>
+      </c>
+      <c r="D36">
+        <v>2.7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" t="s">
+        <v>73</v>
+      </c>
+      <c r="G36" t="s">
+        <v>74</v>
+      </c>
+      <c r="H36" t="s">
+        <v>74</v>
+      </c>
+      <c r="I36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>20310300030</v>
+      </c>
+      <c r="C37">
+        <v>3000</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37" t="s">
+        <v>74</v>
+      </c>
+      <c r="H37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>20300200022</v>
+      </c>
+      <c r="C38">
+        <v>2400</v>
+      </c>
+      <c r="D38">
+        <v>1.35</v>
+      </c>
+      <c r="E38" t="s">
+        <v>76</v>
+      </c>
+      <c r="F38" t="s">
+        <v>73</v>
+      </c>
+      <c r="G38" t="s">
+        <v>74</v>
+      </c>
+      <c r="H38" t="s">
+        <v>74</v>
+      </c>
+      <c r="I38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>20300100051</v>
+      </c>
+      <c r="C39">
+        <v>3000</v>
+      </c>
+      <c r="D39">
+        <v>2.7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G39" t="s">
+        <v>74</v>
+      </c>
+      <c r="H39" t="s">
+        <v>74</v>
+      </c>
+      <c r="I39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>20290300029</v>
+      </c>
+      <c r="C40">
+        <v>3000</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
+        <v>75</v>
+      </c>
+      <c r="F40" t="s">
+        <v>73</v>
+      </c>
+      <c r="G40" t="s">
+        <v>74</v>
+      </c>
+      <c r="H40" t="s">
+        <v>74</v>
+      </c>
+      <c r="I40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>20280100050</v>
+      </c>
+      <c r="C41">
+        <v>3000</v>
+      </c>
+      <c r="D41">
+        <v>2.7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" t="s">
+        <v>73</v>
+      </c>
+      <c r="G41" t="s">
+        <v>74</v>
+      </c>
+      <c r="H41" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>20270300028</v>
+      </c>
+      <c r="C42">
+        <v>2500</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" t="s">
+        <v>73</v>
+      </c>
+      <c r="G42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H42" t="s">
+        <v>74</v>
+      </c>
+      <c r="I42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>20260300027</v>
+      </c>
+      <c r="C43">
+        <v>1000</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" t="s">
+        <v>74</v>
+      </c>
+      <c r="H43" t="s">
+        <v>74</v>
+      </c>
+      <c r="I43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>20260100049</v>
+      </c>
+      <c r="C44">
+        <v>3000</v>
+      </c>
+      <c r="D44">
+        <v>2.7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" t="s">
+        <v>73</v>
+      </c>
+      <c r="G44" t="s">
+        <v>74</v>
+      </c>
+      <c r="H44" t="s">
+        <v>74</v>
+      </c>
+      <c r="I44" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3145,110 +3674,109 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5703125" style="2" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="9" t="s">
         <v>80</v>
       </c>
+      <c r="F1" s="9" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
       <c r="B2">
         <v>99999999999</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="10">
-        <v>41071</v>
-      </c>
-      <c r="E2" s="9">
-        <v>0.74</v>
-      </c>
-      <c r="F2" s="2">
-        <v>12901502.502842134</v>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2">
+        <v>11775</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>4297995</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I5"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="14" t="s">
-        <v>101</v>
+      <c r="I1" s="9" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
       <c r="B2">
         <v>99992600008</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <v>0.92</v>
@@ -3263,94 +3791,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>20402600022</v>
-      </c>
-      <c r="C3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>0.92</v>
-      </c>
-      <c r="F3">
-        <v>0.92</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>4500</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>20362600023</v>
-      </c>
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>0.92</v>
-      </c>
-      <c r="F4">
-        <v>0.92</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>3100</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>20322600024</v>
-      </c>
-      <c r="C5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>0.92</v>
-      </c>
-      <c r="F5">
-        <v>0.92</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>3000</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change storage strategist default option
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koch_j0\TradeRES\toolbox-amiris-emlab-new\toolbox-amiris-emlab\amiris_workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8128B2-F74E-4DDF-B9AE-F932B64DF1AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4122B0-F147-47E8-A612-D92DEED83618}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="8325" tabRatio="880" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,7 +360,7 @@
     <t>Strategist</t>
   </si>
   <si>
-    <t>SINGLE_AGENT_MIN_SYSTEM_COST</t>
+    <t>MULTI_AGENT_SIMPLE</t>
   </si>
 </sst>
 </file>
@@ -3725,7 +3725,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix load of capacity market
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1441,7 +1441,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>amiris-config/data/future_load.csv</t>
+          <t>amiris-config/data/load.csv</t>
         </is>
       </c>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>amiris-config/data/future_LS_high.csv</t>
+          <t>amiris-config/data/LS_high.csv</t>
         </is>
       </c>
     </row>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>amiris-config/data/future_LS_low.csv</t>
+          <t>amiris-config/data/LS_low.csv</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>amiris-config/data/future_LS_mid.csv</t>
+          <t>amiris-config/data/LS_mid.csv</t>
         </is>
       </c>
     </row>
@@ -1548,7 +1548,7 @@
         </is>
       </c>
       <c r="B2" s="13" t="n">
-        <v>59171.99861111111</v>
+        <v>55153.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1558,7 +1558,7 @@
         </is>
       </c>
       <c r="B3" s="13" t="n">
-        <v>59535.99861111111</v>
+        <v>55517.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1817,7 +1817,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1859,60 +1859,60 @@
     </row>
     <row r="2">
       <c r="A2" s="11" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>99993300004</v>
+        <v>20472200080</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1.5</v>
+        <v>4.590677252812498</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>700</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>700</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>99990600006</v>
+        <v>20491900021</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BIOMASS</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1.9</v>
+        <v>4.040099999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>0.309</v>
+        <v>0.285</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>900</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>99991900009</v>
+        <v>20491900022</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1920,124 +1920,124 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>4.040099999999999</v>
       </c>
       <c r="E4" t="n">
         <v>0.285</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>900</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>900</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>20553300084</v>
+        <v>20491900023</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.553294095411101</v>
+        <v>4.040099999999999</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4</v>
+        <v>0.285</v>
       </c>
       <c r="F5" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="G5" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="11" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="n">
-        <v>20543300077</v>
+        <v>20491900024</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1.561060565888156</v>
+        <v>4.040099999999999</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4</v>
+        <v>0.285</v>
       </c>
       <c r="F6" t="n">
-        <v>1000</v>
+        <v>984</v>
       </c>
       <c r="G6" t="n">
-        <v>1000</v>
+        <v>984</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="11" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20423300069</v>
+        <v>20492200078</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1.657343365780092</v>
+        <v>4.545112499999998</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="F7" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="G7" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="11" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20403300068</v>
+        <v>20482200079</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>OTHER</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1.673958233022038</v>
+        <v>4.567838062499998</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="F8" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="G8" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="11" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>20363300067</v>
+        <v>20283300071</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1.707689329442772</v>
+        <v>1.682328024187148</v>
       </c>
       <c r="E9" t="n">
         <v>0.4</v>
@@ -2059,21 +2059,21 @@
     </row>
     <row r="10">
       <c r="A10" s="11" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" t="n">
-        <v>20351900022</v>
+        <v>20243300070</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>OTHER</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4.576607402906627</v>
+        <v>1.716227776089985</v>
       </c>
       <c r="E10" t="n">
-        <v>0.285</v>
+        <v>0.4</v>
       </c>
       <c r="F10" t="n">
         <v>1500</v>
@@ -2084,60 +2084,60 @@
     </row>
     <row r="11">
       <c r="A11" s="11" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B11" t="n">
-        <v>20301900021</v>
+        <v>20493300077</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>OTHER</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>4.692172474905471</v>
+        <v>1.5150375</v>
       </c>
       <c r="E11" t="n">
-        <v>0.285</v>
+        <v>0.4</v>
       </c>
       <c r="F11" t="n">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="G11" t="n">
-        <v>1500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="11" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B12" t="n">
-        <v>20201900023</v>
+        <v>20463300076</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>NUCLEAR</t>
+          <t>OTHER</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4.932130794830295</v>
+        <v>1.537876879692186</v>
       </c>
       <c r="E12" t="n">
-        <v>0.285</v>
+        <v>0.4</v>
       </c>
       <c r="F12" t="n">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="G12" t="n">
-        <v>1500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="11" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>20583300110</v>
+        <v>20423300075</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -2145,7 +2145,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1.530225750937499</v>
+        <v>1.568865868717596</v>
       </c>
       <c r="E13" t="n">
         <v>0.4</v>
@@ -2159,10 +2159,10 @@
     </row>
     <row r="14">
       <c r="A14" s="11" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B14" t="n">
-        <v>20493300071</v>
+        <v>20403300074</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -2170,7 +2170,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1.600479301385731</v>
+        <v>1.58459374905149</v>
       </c>
       <c r="E14" t="n">
         <v>0.4</v>
@@ -2184,10 +2184,10 @@
     </row>
     <row r="15">
       <c r="A15" s="11" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B15" t="n">
-        <v>20463300070</v>
+        <v>20363300073</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -2195,7 +2195,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1.624606726914033</v>
+        <v>1.616524106382123</v>
       </c>
       <c r="E15" t="n">
         <v>0.4</v>
@@ -2204,6 +2204,31 @@
         <v>2000</v>
       </c>
       <c r="G15" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20323300072</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>OTHER</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1.649097876398102</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G16" t="n">
         <v>2000</v>
       </c>
     </row>
@@ -2619,7 +2644,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2674,17 +2699,17 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20610300131</v>
+        <v>20500200084</v>
       </c>
       <c r="C2" t="n">
         <v>3000</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1.35675</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2713,13 +2738,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20600100127</v>
+        <v>20500100064</v>
       </c>
       <c r="C3" t="n">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="D3" t="n">
-        <v>2.7270675</v>
+        <v>2.7135</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -2752,10 +2777,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20600300126</v>
+        <v>20490300051</v>
       </c>
       <c r="C4" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -2791,10 +2816,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20590200119</v>
+        <v>20480200029</v>
       </c>
       <c r="C5" t="n">
-        <v>2000</v>
+        <v>1580</v>
       </c>
       <c r="D5" t="n">
         <v>1.37035141875</v>
@@ -2830,10 +2855,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20590300118</v>
+        <v>20480300050</v>
       </c>
       <c r="C6" t="n">
-        <v>4000</v>
+        <v>1500</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -2869,17 +2894,17 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>99990500001</v>
+        <v>20480100063</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>3500</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>2.740702837499999</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>PVRooftop</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -2908,10 +2933,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>99990300002</v>
+        <v>20470300049</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -2947,17 +2972,17 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>99990200003</v>
+        <v>20460300048</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>2000</v>
       </c>
       <c r="D9" t="n">
-        <v>1.35</v>
+        <v>0</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2986,13 +3011,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>99990100007</v>
+        <v>20460100062</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>3500</v>
       </c>
       <c r="D10" t="n">
-        <v>2.7</v>
+        <v>2.768178383445936</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -3025,17 +3050,17 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>20580100111</v>
+        <v>20450300047</v>
       </c>
       <c r="C11" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D11" t="n">
-        <v>2.754406351687499</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -3064,7 +3089,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>20580300109</v>
+        <v>20440300046</v>
       </c>
       <c r="C12" t="n">
         <v>2000</v>
@@ -3103,17 +3128,17 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>20570300101</v>
+        <v>20440100061</v>
       </c>
       <c r="C13" t="n">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>2.795929371739981</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -3142,17 +3167,17 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>20560100097</v>
+        <v>20430200028</v>
       </c>
       <c r="C14" t="n">
-        <v>3000</v>
+        <v>1400</v>
       </c>
       <c r="D14" t="n">
-        <v>2.782019275363166</v>
+        <v>1.404954509299341</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -3181,10 +3206,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20560300096</v>
+        <v>20430300045</v>
       </c>
       <c r="C15" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -3220,17 +3245,17 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20550200089</v>
+        <v>20420300044</v>
       </c>
       <c r="C16" t="n">
         <v>2000</v>
       </c>
       <c r="D16" t="n">
-        <v>1.397964685869991</v>
+        <v>0</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -3259,17 +3284,17 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20550300088</v>
+        <v>20420100060</v>
       </c>
       <c r="C17" t="n">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>2.823958563691674</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -3298,10 +3323,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20540300081</v>
+        <v>20410300043</v>
       </c>
       <c r="C18" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -3337,17 +3362,17 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20520300076</v>
+        <v>20410100069</v>
       </c>
       <c r="C19" t="n">
-        <v>1000</v>
+        <v>3500</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>2.838078356510132</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -3376,17 +3401,17 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20500100075</v>
+        <v>20400300042</v>
       </c>
       <c r="C20" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D20" t="n">
-        <v>2.866530092034146</v>
+        <v>0</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -3415,17 +3440,17 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20490300051</v>
+        <v>20400100059</v>
       </c>
       <c r="C21" t="n">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>2.852268748292683</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -3454,17 +3479,17 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20480200029</v>
+        <v>20390300041</v>
       </c>
       <c r="C22" t="n">
-        <v>2400</v>
+        <v>2000</v>
       </c>
       <c r="D22" t="n">
-        <v>1.447633528103394</v>
+        <v>0</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -3493,17 +3518,17 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20480300050</v>
+        <v>20380200027</v>
       </c>
       <c r="C23" t="n">
-        <v>3850</v>
+        <v>1400</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>1.440431371247158</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -3532,17 +3557,17 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20480100063</v>
+        <v>20380300040</v>
       </c>
       <c r="C24" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D24" t="n">
-        <v>2.895267056206787</v>
+        <v>0</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -3571,17 +3596,17 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20470300049</v>
+        <v>20380100058</v>
       </c>
       <c r="C25" t="n">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>2.880862742494316</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3610,17 +3635,17 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20470100062</v>
+        <v>20370300039</v>
       </c>
       <c r="C26" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D26" t="n">
-        <v>2.909743391487821</v>
+        <v>0</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3649,17 +3674,17 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20460300048</v>
+        <v>20370100068</v>
       </c>
       <c r="C27" t="n">
         <v>3500</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>2.895267056206787</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -3688,17 +3713,17 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20460100061</v>
+        <v>20360300038</v>
       </c>
       <c r="C28" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D28" t="n">
-        <v>2.92429210844526</v>
+        <v>0</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -3727,17 +3752,17 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>20450300047</v>
+        <v>20360100057</v>
       </c>
       <c r="C29" t="n">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>2.909743391487821</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -3766,10 +3791,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>20440300046</v>
+        <v>20350300037</v>
       </c>
       <c r="C30" t="n">
-        <v>3500</v>
+        <v>2000</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
@@ -3805,17 +3830,17 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>20440100060</v>
+        <v>20340200026</v>
       </c>
       <c r="C31" t="n">
-        <v>4000</v>
+        <v>1400</v>
       </c>
       <c r="D31" t="n">
-        <v>2.953608136832422</v>
+        <v>1.469456784493743</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3844,17 +3869,17 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>20430200028</v>
+        <v>20340300036</v>
       </c>
       <c r="C32" t="n">
-        <v>2400</v>
+        <v>2000</v>
       </c>
       <c r="D32" t="n">
-        <v>1.484188088758292</v>
+        <v>0</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3883,17 +3908,17 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>20430300045</v>
+        <v>20340100056</v>
       </c>
       <c r="C33" t="n">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>2.938913568987485</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3922,10 +3947,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>20420300044</v>
+        <v>20330300035</v>
       </c>
       <c r="C34" t="n">
-        <v>3500</v>
+        <v>2000</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
@@ -3961,13 +3986,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>20420100059</v>
+        <v>20330100067</v>
       </c>
       <c r="C35" t="n">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="D35" t="n">
-        <v>2.983218058404167</v>
+        <v>2.953608136832422</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -4000,10 +4025,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>20410300043</v>
+        <v>20320300034</v>
       </c>
       <c r="C36" t="n">
-        <v>3500</v>
+        <v>2000</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
@@ -4039,17 +4064,17 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>20400300042</v>
+        <v>20320100055</v>
       </c>
       <c r="C37" t="n">
-        <v>3500</v>
+        <v>4000</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>2.968376177516584</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -4078,17 +4103,17 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>20400100058</v>
+        <v>20310300033</v>
       </c>
       <c r="C38" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D38" t="n">
-        <v>3.013124819439668</v>
+        <v>0</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -4117,17 +4142,17 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>20390300041</v>
+        <v>20310100066</v>
       </c>
       <c r="C39" t="n">
         <v>3500</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>2.983218058404167</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -4156,13 +4181,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>20380200027</v>
+        <v>20300200025</v>
       </c>
       <c r="C40" t="n">
-        <v>2400</v>
+        <v>1400</v>
       </c>
       <c r="D40" t="n">
-        <v>1.521665697877275</v>
+        <v>1.499067074348094</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -4195,17 +4220,17 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>20380300040</v>
+        <v>20300100054</v>
       </c>
       <c r="C41" t="n">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>2.998134148696188</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -4234,17 +4259,17 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20360100057</v>
+        <v>20290300032</v>
       </c>
       <c r="C42" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D42" t="n">
-        <v>3.073840792996989</v>
+        <v>0</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4273,13 +4298,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20340100056</v>
+        <v>20280100053</v>
       </c>
       <c r="C43" t="n">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="D43" t="n">
-        <v>3.104656046946783</v>
+        <v>3.028190443536866</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -4302,6 +4327,123 @@
         </is>
       </c>
       <c r="I43" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="11" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>20270300031</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2000</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="11" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>20270100065</v>
+      </c>
+      <c r="C45" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D45" t="n">
+        <v>3.04333139575455</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="11" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>20260100052</v>
+      </c>
+      <c r="C46" t="n">
+        <v>4000</v>
+      </c>
+      <c r="D46" t="n">
+        <v>3.058548052733322</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -4386,7 +4528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="B1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4436,39 +4578,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>99992600008</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>MULTI_AGENT_SIMPLE</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Allow for default usage of electrolysis
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TradeRES\toolbox-amiris-emlab-new\toolbox-amiris-emlab\amiris_workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374DABEF-08F2-4F32-895E-4DB43CE6C7CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0F2FD2-1817-4F56-99D1-061E18198E01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="8325" tabRatio="880" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3845,7 +3845,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3897,9 +3897,6 @@
       <c r="F2">
         <v>4297995</v>
       </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
upating to amiris 2.14
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1548,7 +1548,7 @@
         </is>
       </c>
       <c r="B2" s="13" t="n">
-        <v>58806.99861111111</v>
+        <v>56249.99861111111</v>
       </c>
     </row>
     <row r="3">
@@ -1558,7 +1558,7 @@
         </is>
       </c>
       <c r="B3" s="13" t="n">
-        <v>59170.99861111111</v>
+        <v>56613.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1817,7 +1817,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1862,7 +1862,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20473300034</v>
+        <v>99993300003</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1870,16 +1870,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1.608481697892659</v>
+        <v>1.5</v>
       </c>
       <c r="E2" t="n">
         <v>0.4</v>
       </c>
       <c r="F2" t="n">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>2000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -1887,24 +1887,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20453300033</v>
+        <v>99990600006</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>HYDROGEN</t>
+          <t>BIOMASS</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1.624606726914033</v>
+        <v>2.6</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4</v>
+        <v>0.309</v>
       </c>
       <c r="F3" t="n">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>2000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -1912,24 +1912,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20433300032</v>
+        <v>99991900008</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>HYDROGEN</t>
+          <t>NUCLEAR</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1.640893409351346</v>
+        <v>3.5</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="F4" t="n">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>2000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -1937,32 +1937,32 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20413300031</v>
+        <v>99992200009</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>HYDROGEN</t>
+          <t>NATURAL_GAS</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1.657343365780092</v>
+        <v>4.5</v>
       </c>
       <c r="E5" t="n">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="F5" t="n">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>2000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="11" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B6" t="n">
-        <v>20393300030</v>
+        <v>20253300023</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1970,7 +1970,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1.673958233022038</v>
+        <v>1.733432959545287</v>
       </c>
       <c r="E6" t="n">
         <v>0.4</v>
@@ -1984,10 +1984,10 @@
     </row>
     <row r="7">
       <c r="A7" s="11" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>20373300029</v>
+        <v>20273300024</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1995,7 +1995,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1.690739664308083</v>
+        <v>1.716227776089985</v>
       </c>
       <c r="E7" t="n">
         <v>0.4</v>
@@ -2009,10 +2009,10 @@
     </row>
     <row r="8">
       <c r="A8" s="11" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>20353300028</v>
+        <v>20293300025</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -2020,7 +2020,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1.707689329442772</v>
+        <v>1.699193362629623</v>
       </c>
       <c r="E8" t="n">
         <v>0.4</v>
@@ -2034,10 +2034,10 @@
     </row>
     <row r="9">
       <c r="A9" s="11" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>20333300027</v>
+        <v>20313300026</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1.724808914970435</v>
+        <v>1.682328024187148</v>
       </c>
       <c r="E9" t="n">
         <v>0.4</v>
@@ -2059,26 +2059,276 @@
     </row>
     <row r="10">
       <c r="A10" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20333300027</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>HYDROGEN</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1.665630082608993</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20353300028</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>HYDROGEN</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1.649097876398102</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20393300030</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>HYDROGEN</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1.616524106382123</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20233300022</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>HYDROGEN</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1.750810624964728</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20413300031</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>HYDROGEN</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1.600479301385731</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="B15" t="n">
+        <v>20433300032</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>HYDROGEN</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1.58459374905149</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20453300033</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>HYDROGEN</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1.568865868717596</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B17" t="n">
+        <v>20473300034</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>HYDROGEN</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1.553294095411101</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20373300029</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>HYDROGEN</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1.632729760548603</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="B19" t="n">
         <v>20401900035</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>NUCLEAR</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>3.886470192754317</v>
-      </c>
-      <c r="E10" t="n">
+      <c r="D19" t="n">
+        <v>3.753123961749539</v>
+      </c>
+      <c r="E19" t="n">
         <v>0.35</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F19" t="n">
         <v>5000</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G19" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20151900036</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>NUCLEAR</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>4.251522216620676</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5000</v>
+      </c>
+      <c r="G20" t="n">
         <v>5000</v>
       </c>
     </row>
@@ -2549,10 +2799,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20610100094</v>
+        <v>99990100002</v>
       </c>
       <c r="C2" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
         <v>0.5</v>
@@ -2588,17 +2838,17 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20610100095</v>
+        <v>99990300004</v>
       </c>
       <c r="C3" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>0.5</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2627,17 +2877,17 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>20610100096</v>
+        <v>99990200005</v>
       </c>
       <c r="C4" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>0.5</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -2666,17 +2916,17 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20600100093</v>
+        <v>99990500007</v>
       </c>
       <c r="C5" t="n">
-        <v>12000</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5024999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>PVRooftop</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -2705,17 +2955,17 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20550100060</v>
+        <v>20490200021</v>
       </c>
       <c r="C6" t="n">
-        <v>10000</v>
+        <v>12000</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5151887546968825</v>
+        <v>0.5126256265640622</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>WindOff</t>
+          <t>WindOn</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -2744,17 +2994,17 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20490200021</v>
+        <v>20490300037</v>
       </c>
       <c r="C7" t="n">
-        <v>12000</v>
+        <v>35000</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5308389059322491</v>
+        <v>0.5126256265640622</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -2783,13 +3033,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>20490300037</v>
+        <v>20400300038</v>
       </c>
       <c r="C8" t="n">
         <v>35000</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5308389059322491</v>
+        <v>0.5361605659642198</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -2822,17 +3072,17 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20400300038</v>
+        <v>20370100040</v>
       </c>
       <c r="C9" t="n">
-        <v>35000</v>
+        <v>25000</v>
       </c>
       <c r="D9" t="n">
-        <v>0.555210027536331</v>
+        <v>0.544243253516201</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>OtherPV</t>
+          <t>WindOff</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2861,13 +3111,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>20370100040</v>
+        <v>20250100039</v>
       </c>
       <c r="C10" t="n">
         <v>25000</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5635798881026944</v>
+        <v>0.5778109865150957</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -2982,7 +3232,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3037,7 +3287,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20612600097</v>
+        <v>99992600001</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -3057,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -3070,7 +3320,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20612600098</v>
+        <v>20502600043</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -3090,240 +3340,9 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I3" t="inlineStr">
-        <is>
-          <t>MULTI_AGENT_MEDIAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>20612600099</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>4</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>MULTI_AGENT_MEDIAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>20602600092</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>13000</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>MULTI_AGENT_MEDIAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>20592600066</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2000</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>MULTI_AGENT_MEDIAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>99992600001</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>MULTI_AGENT_MEDIAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>20572600063</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>2000</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>MULTI_AGENT_MEDIAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>20552600059</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>5000</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>MULTI_AGENT_MEDIAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="11" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>20502600043</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>2000</v>
-      </c>
-      <c r="I10" t="inlineStr">
         <is>
           <t>MULTI_AGENT_MEDIAN</t>
         </is>

</xml_diff>

<commit_message>
updating amiris data strucure
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="8325" tabRatio="880" firstSheet="4" activeTab="7" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-16515" windowWidth="29040" windowHeight="15840" tabRatio="880" firstSheet="3" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_skeleton" sheetId="1" state="visible" r:id="rId1"/>
@@ -25,7 +25,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'renewables_full'!$A$1:$I$60</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1" concurrentCalc="0"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1" calcOnSave="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -182,10 +182,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -200,10 +199,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -211,7 +210,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -593,10 +592,10 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
-    <col width="22.28515625" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="31.140625" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="22.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="31.140625" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -843,7 +842,7 @@
           <t>PredefinedPlantBuilder</t>
         </is>
       </c>
-      <c r="C15" s="3" t="inlineStr">
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>CyclingCostInEURperMW</t>
         </is>
@@ -1088,7 +1087,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1109,42 +1108,42 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>OpexVarInEURperMWH</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>Set</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>SupportInstrument</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>FIT</t>
         </is>
       </c>
-      <c r="H1" s="11" t="inlineStr">
+      <c r="H1" s="10" t="inlineStr">
         <is>
           <t>Premium</t>
         </is>
       </c>
-      <c r="I1" s="11" t="inlineStr">
+      <c r="I1" s="10" t="inlineStr">
         <is>
           <t>Lcoe</t>
         </is>
@@ -1167,87 +1166,87 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>OpexVarInEURperMWH</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Set</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>SupportInstrument</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>FIT</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Premium</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>Lcoe</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="n">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="n">
+      <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="n">
+      <c r="A6" s="3" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="3" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="n">
+      <c r="A8" s="3" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="n">
+      <c r="A9" s="3" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1268,122 +1267,122 @@
       <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
-    <col width="22.7109375" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="20.140625" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="82.42578125" customWidth="1" style="2" min="3" max="3"/>
+    <col width="22.7109375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="20.140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="82.42578125" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="2" thickBot="1">
-      <c r="A1" s="6" t="inlineStr">
+    <row r="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>VOLL</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>TimeSeries</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" s="2" thickBot="1">
-      <c r="A2" s="7" t="inlineStr">
+    <row r="2" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>SHEDDING</t>
         </is>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="6" t="n">
         <v>4000</v>
       </c>
-      <c r="C2" s="7" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>amiris-config/data/demand_processed/load.csv</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" s="2" thickBot="1">
-      <c r="A3" s="7" t="inlineStr">
+    <row r="3" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>SHEDDING</t>
         </is>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="6" t="n">
         <v>300</v>
       </c>
-      <c r="C3" s="7" t="inlineStr">
+      <c r="C3" s="6" t="inlineStr">
         <is>
           <t>amiris-config/data/demand_processed/hoho_cluster_shedding_timeseries.csv</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" s="2" thickBot="1">
-      <c r="A4" s="7" t="inlineStr">
+    <row r="4" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>SHEDDING</t>
         </is>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="6" t="n">
         <v>300.7</v>
       </c>
-      <c r="C4" s="7" t="inlineStr">
+      <c r="C4" s="6" t="inlineStr">
         <is>
           <t>amiris-config/data/demand_processed/tcs_hoho_cluster_shedding_timeseries.csv</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1" s="2" thickBot="1">
-      <c r="A5" s="7" t="inlineStr">
+    <row r="5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>SHEDDING</t>
         </is>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="6" t="n">
         <v>447.1</v>
       </c>
-      <c r="C5" s="7" t="inlineStr">
+      <c r="C5" s="6" t="inlineStr">
         <is>
           <t>amiris-config/data/demand_processed/tcs_cluster_shedding_timeseries.csv</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1" s="2" thickBot="1">
-      <c r="A6" s="7" t="inlineStr">
+    <row r="6" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>SHEDDING</t>
         </is>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="6" t="n">
         <v>607.5</v>
       </c>
-      <c r="C6" s="7" t="inlineStr">
+      <c r="C6" s="6" t="inlineStr">
         <is>
           <t>amiris-config/data/demand_processed/ind_cluster-1_shedding_timeseries.csv</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" s="2" thickBot="1">
-      <c r="A7" s="7" t="inlineStr">
+    <row r="7" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>SHEDDING</t>
         </is>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="6" t="n">
         <v>1151.9</v>
       </c>
-      <c r="C7" s="7" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>amiris-config/data/demand_processed/ind_cluster-2_shedding_timeseries.csv</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="C15" s="8" t="n"/>
+      <c r="C15" s="7" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
@@ -1406,22 +1405,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="inlineStr">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>VOLL</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>TimeSeries</t>
         </is>
@@ -1537,28 +1536,28 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="n">
+      <c r="B1" s="10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="inlineStr">
+      <c r="A2" s="10" t="inlineStr">
         <is>
           <t>StartTime</t>
         </is>
       </c>
-      <c r="B2" s="13" t="n">
-        <v>56249.99861111111</v>
+      <c r="B2" s="12" t="n">
+        <v>55884.99861111111</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="inlineStr">
+      <c r="A3" s="10" t="inlineStr">
         <is>
           <t>StopTime</t>
         </is>
       </c>
-      <c r="B3" s="13" t="n">
-        <v>56613.99861111111</v>
+      <c r="B3" s="12" t="n">
+        <v>56248.99861111111</v>
       </c>
     </row>
   </sheetData>
@@ -1578,11 +1577,11 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
-    <col width="13.42578125" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="22.28515625" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="31.140625" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="13.42578125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="22.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="31.140625" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1690,64 +1689,64 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>AgentType</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>CO2</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>HARD_COAL</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>OIL</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>HYDROGEN</t>
         </is>
       </c>
-      <c r="H1" s="11" t="inlineStr">
+      <c r="H1" s="10" t="inlineStr">
         <is>
           <t>LIGNITE</t>
         </is>
       </c>
-      <c r="I1" s="11" t="inlineStr">
+      <c r="I1" s="10" t="inlineStr">
         <is>
           <t>NATURAL_GAS</t>
         </is>
       </c>
-      <c r="J1" s="11" t="inlineStr">
+      <c r="J1" s="10" t="inlineStr">
         <is>
           <t>NUCLEAR</t>
         </is>
       </c>
-      <c r="K1" s="11" t="inlineStr">
+      <c r="K1" s="10" t="inlineStr">
         <is>
           <t>WASTE</t>
         </is>
       </c>
-      <c r="L1" s="11" t="inlineStr">
+      <c r="L1" s="10" t="inlineStr">
         <is>
           <t>BIOMASS</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="10" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -1769,7 +1768,7 @@
       <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="n">
+      <c r="A3" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -1817,7 +1816,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1826,40 +1825,40 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>FuelType</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>OpexVarInEURperMWH</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>Efficiency</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>BlockSizeInMW</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
-        <v>0</v>
+      <c r="A2" s="10" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>99993300003</v>
@@ -1883,8 +1882,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="n">
-        <v>1</v>
+      <c r="A3" s="10" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="n">
         <v>99990600006</v>
@@ -1908,8 +1907,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="n">
-        <v>2</v>
+      <c r="A4" s="10" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="n">
         <v>99991900008</v>
@@ -1933,8 +1932,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="n">
-        <v>3</v>
+      <c r="A5" s="10" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="n">
         <v>99992200009</v>
@@ -1958,61 +1957,61 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="n">
-        <v>16</v>
+      <c r="A6" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>20253300023</v>
+        <v>20522200077</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>NATURAL_GAS</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4.522499999999999</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="n">
+        <v>18</v>
+      </c>
+      <c r="B7" t="n">
+        <v>20243300065</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>HYDROGEN</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="D7" t="n">
         <v>1.733432959545287</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G6" t="n">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="11" t="n">
-        <v>15</v>
-      </c>
-      <c r="B7" t="n">
-        <v>20273300024</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>HYDROGEN</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1.716227776089985</v>
       </c>
       <c r="E7" t="n">
         <v>0.4</v>
       </c>
       <c r="F7" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G7" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="11" t="n">
-        <v>14</v>
+      <c r="A8" s="10" t="n">
+        <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>20293300025</v>
+        <v>20263300066</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -2020,24 +2019,24 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1.699193362629623</v>
+        <v>1.716227776089985</v>
       </c>
       <c r="E8" t="n">
         <v>0.4</v>
       </c>
       <c r="F8" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G8" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11" t="n">
-        <v>13</v>
+      <c r="A9" s="10" t="n">
+        <v>16</v>
       </c>
       <c r="B9" t="n">
-        <v>20313300026</v>
+        <v>20283300067</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -2045,24 +2044,24 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1.682328024187148</v>
+        <v>1.699193362629623</v>
       </c>
       <c r="E9" t="n">
         <v>0.4</v>
       </c>
       <c r="F9" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G9" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11" t="n">
-        <v>12</v>
+      <c r="A10" s="10" t="n">
+        <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>20333300027</v>
+        <v>20303300068</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -2070,24 +2069,24 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1.665630082608993</v>
+        <v>1.682328024187148</v>
       </c>
       <c r="E10" t="n">
         <v>0.4</v>
       </c>
       <c r="F10" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G10" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11" t="n">
-        <v>11</v>
+      <c r="A11" s="10" t="n">
+        <v>13</v>
       </c>
       <c r="B11" t="n">
-        <v>20353300028</v>
+        <v>20323300069</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -2095,24 +2094,24 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1.649097876398102</v>
+        <v>1.665630082608993</v>
       </c>
       <c r="E11" t="n">
         <v>0.4</v>
       </c>
       <c r="F11" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G11" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11" t="n">
-        <v>9</v>
+      <c r="A12" s="10" t="n">
+        <v>12</v>
       </c>
       <c r="B12" t="n">
-        <v>20393300030</v>
+        <v>20343300070</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -2120,24 +2119,24 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1.616524106382123</v>
+        <v>1.649097876398102</v>
       </c>
       <c r="E12" t="n">
         <v>0.4</v>
       </c>
       <c r="F12" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G12" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="n">
-        <v>17</v>
+      <c r="A13" s="10" t="n">
+        <v>10</v>
       </c>
       <c r="B13" t="n">
-        <v>20233300022</v>
+        <v>20363300071</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -2145,24 +2144,24 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1.750810624964728</v>
+        <v>1.632729760548603</v>
       </c>
       <c r="E13" t="n">
         <v>0.4</v>
       </c>
       <c r="F13" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G13" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="n">
-        <v>7</v>
+      <c r="A14" s="10" t="n">
+        <v>9</v>
       </c>
       <c r="B14" t="n">
-        <v>20413300031</v>
+        <v>20383300072</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -2170,24 +2169,24 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1.600479301385731</v>
+        <v>1.616524106382123</v>
       </c>
       <c r="E14" t="n">
         <v>0.4</v>
       </c>
       <c r="F14" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G14" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="n">
-        <v>6</v>
+      <c r="A15" s="10" t="n">
+        <v>8</v>
       </c>
       <c r="B15" t="n">
-        <v>20433300032</v>
+        <v>20403300073</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -2195,24 +2194,24 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>1.58459374905149</v>
+        <v>1.600479301385731</v>
       </c>
       <c r="E15" t="n">
         <v>0.4</v>
       </c>
       <c r="F15" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G15" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="11" t="n">
-        <v>5</v>
+      <c r="A16" s="10" t="n">
+        <v>7</v>
       </c>
       <c r="B16" t="n">
-        <v>20453300033</v>
+        <v>20423300074</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -2220,24 +2219,24 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1.568865868717596</v>
+        <v>1.58459374905149</v>
       </c>
       <c r="E16" t="n">
         <v>0.4</v>
       </c>
       <c r="F16" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G16" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11" t="n">
-        <v>4</v>
+      <c r="A17" s="10" t="n">
+        <v>6</v>
       </c>
       <c r="B17" t="n">
-        <v>20473300034</v>
+        <v>20443300075</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -2245,24 +2244,24 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1.553294095411101</v>
+        <v>1.568865868717596</v>
       </c>
       <c r="E17" t="n">
         <v>0.4</v>
       </c>
       <c r="F17" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G17" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="11" t="n">
-        <v>10</v>
+      <c r="A18" s="10" t="n">
+        <v>5</v>
       </c>
       <c r="B18" t="n">
-        <v>20373300029</v>
+        <v>20463300076</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -2270,24 +2269,24 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>1.632729760548603</v>
+        <v>1.553294095411101</v>
       </c>
       <c r="E18" t="n">
         <v>0.4</v>
       </c>
       <c r="F18" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G18" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="n">
-        <v>8</v>
+      <c r="A19" s="10" t="n">
+        <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>20401900035</v>
+        <v>20101900024</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -2295,24 +2294,24 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>3.753123961749539</v>
+        <v>4.337192517703889</v>
       </c>
       <c r="E19" t="n">
         <v>0.35</v>
       </c>
       <c r="F19" t="n">
-        <v>5000</v>
+        <v>1164</v>
       </c>
       <c r="G19" t="n">
-        <v>5000</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="11" t="n">
-        <v>18</v>
+      <c r="A20" s="10" t="n">
+        <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>20151900036</v>
+        <v>20201900023</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -2320,16 +2319,66 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4.251522216620676</v>
+        <v>4.126179170119998</v>
       </c>
       <c r="E20" t="n">
         <v>0.35</v>
       </c>
       <c r="F20" t="n">
-        <v>5000</v>
+        <v>1500</v>
       </c>
       <c r="G20" t="n">
-        <v>5000</v>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="n">
+        <v>14</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20301900021</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>NUCLEAR</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>3.925432056436678</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F21" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="n">
+        <v>11</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20351900022</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>NUCLEAR</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>3.828751288486473</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>
@@ -2349,9 +2398,9 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="20.42578125" customWidth="1" style="2" min="1" max="1"/>
+    <col width="20.42578125" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2386,349 +2435,349 @@
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col width="14" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="14" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>OpexVarInEURperMWH</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Set</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>SupportInstrument</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>FIT</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Premium</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>Lcoe</t>
         </is>
       </c>
-      <c r="K1" s="5" t="n"/>
+      <c r="K1" s="4" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="K2" s="1" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="n">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="K3" s="1" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="n">
+      <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
       <c r="K4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="n">
+      <c r="A6" s="3" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="3" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="n">
+      <c r="A8" s="3" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="n">
+      <c r="A9" s="3" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="n">
+      <c r="A10" s="3" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="n">
+      <c r="A11" s="3" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="n">
+      <c r="A12" s="3" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="n">
+      <c r="A13" s="3" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="n">
+      <c r="A14" s="3" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="n">
+      <c r="A15" s="3" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="n">
+      <c r="A16" s="3" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="n">
+      <c r="A17" s="3" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="n">
+      <c r="A18" s="3" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="n">
+      <c r="A19" s="3" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="n">
+      <c r="A20" s="3" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="n">
+      <c r="A21" s="3" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="n">
+      <c r="A22" s="3" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="n">
+      <c r="A23" s="3" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="n">
+      <c r="A24" s="3" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n">
+      <c r="A25" s="3" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="n">
+      <c r="A26" s="3" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="n">
+      <c r="A27" s="3" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="n">
+      <c r="A28" s="3" t="n">
         <v>26</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="n">
+      <c r="A29" s="3" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="n">
+      <c r="A30" s="3" t="n">
         <v>28</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="n">
+      <c r="A31" s="3" t="n">
         <v>29</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="n">
+      <c r="A32" s="3" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="n">
+      <c r="A33" s="3" t="n">
         <v>31</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="n">
+      <c r="A34" s="3" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="n">
+      <c r="A35" s="3" t="n">
         <v>33</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="n">
+      <c r="A36" s="3" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="n">
+      <c r="A37" s="3" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="n">
+      <c r="A38" s="3" t="n">
         <v>36</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="n">
+      <c r="A39" s="3" t="n">
         <v>37</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="n">
+      <c r="A40" s="3" t="n">
         <v>38</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="n">
+      <c r="A41" s="3" t="n">
         <v>39</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="n">
+      <c r="A42" s="3" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="n">
+      <c r="A43" s="3" t="n">
         <v>41</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="n">
+      <c r="A44" s="3" t="n">
         <v>42</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="n">
+      <c r="A45" s="3" t="n">
         <v>43</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="n">
+      <c r="A46" s="3" t="n">
         <v>44</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="4" t="n">
+      <c r="A47" s="3" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="4" t="n">
+      <c r="A48" s="3" t="n">
         <v>46</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="4" t="n">
+      <c r="A49" s="3" t="n">
         <v>47</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="n">
+      <c r="A50" s="3" t="n">
         <v>48</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="4" t="n">
+      <c r="A51" s="3" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="n">
+      <c r="A52" s="3" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="4" t="n">
+      <c r="A53" s="3" t="n">
         <v>51</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="n">
+      <c r="A54" s="3" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="4" t="n">
+      <c r="A55" s="3" t="n">
         <v>53</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="4" t="n">
+      <c r="A56" s="3" t="n">
         <v>54</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="4" t="n">
+      <c r="A57" s="3" t="n">
         <v>55</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="4" t="n">
+      <c r="A58" s="3" t="n">
         <v>56</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="4" t="n">
+      <c r="A59" s="3" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="4" t="n">
+      <c r="A60" s="3" t="n">
         <v>58</v>
       </c>
     </row>
@@ -2744,7 +2793,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2753,49 +2802,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>OpexVarInEURperMWH</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>Set</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>SupportInstrument</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>FIT</t>
         </is>
       </c>
-      <c r="H1" s="11" t="inlineStr">
+      <c r="H1" s="10" t="inlineStr">
         <is>
           <t>Premium</t>
         </is>
       </c>
-      <c r="I1" s="11" t="inlineStr">
+      <c r="I1" s="10" t="inlineStr">
         <is>
           <t>Lcoe</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="10" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
@@ -2834,7 +2883,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11" t="n">
+      <c r="A3" s="10" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
@@ -2873,7 +2922,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11" t="n">
+      <c r="A4" s="10" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
@@ -2912,7 +2961,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="n">
+      <c r="A5" s="10" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="n">
@@ -2951,21 +3000,21 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11" t="n">
+      <c r="A6" s="10" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20490200021</v>
+        <v>20490300051</v>
       </c>
       <c r="C6" t="n">
-        <v>12000</v>
+        <v>3000</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5126256265640622</v>
+        <v>0.5100752503124998</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>WindOn</t>
+          <t>OtherPV</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -2990,156 +3039,1404 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="n">
+      <c r="A7" s="10" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>20490300037</v>
+        <v>20480200029</v>
       </c>
       <c r="C7" t="n">
-        <v>35000</v>
+        <v>2400</v>
       </c>
       <c r="D7" t="n">
         <v>0.5126256265640622</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>20480300050</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3850</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.5126256265640622</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>OtherPV</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>20400300038</v>
-      </c>
-      <c r="C8" t="n">
-        <v>35000</v>
-      </c>
-      <c r="D8" t="n">
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20480100063</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5126256265640622</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20470300049</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5151887546968825</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>20470100062</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.5151887546968825</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>20460300048</v>
+      </c>
+      <c r="C12" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.5177646984703669</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>20460100061</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.5177646984703669</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>20450300047</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.5203535219627187</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>20440300046</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.5229552895725321</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>20440100060</v>
+      </c>
+      <c r="C16" t="n">
+        <v>4000</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.5229552895725321</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>20430200028</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2400</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.5255700660203948</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>20430300045</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.5255700660203948</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>20420300044</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.5281979163504967</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>20420100059</v>
+      </c>
+      <c r="C20" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.5281979163504967</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20410300043</v>
+      </c>
+      <c r="C21" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.5308389059322491</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>20400300042</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.5334931004619103</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>20400100058</v>
+      </c>
+      <c r="C23" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.5334931004619103</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>20390300041</v>
+      </c>
+      <c r="C24" t="n">
+        <v>3500</v>
+      </c>
+      <c r="D24" t="n">
         <v>0.5361605659642198</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>OtherPV</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>20370100040</v>
-      </c>
-      <c r="C9" t="n">
-        <v>25000</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="10" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>20380200027</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2400</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.5388413687940409</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="10" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>20380300040</v>
+      </c>
+      <c r="C26" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.5388413687940409</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="10" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>20370300039</v>
+      </c>
+      <c r="C27" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.541535575638011</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="10" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>20360300038</v>
+      </c>
+      <c r="C28" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D28" t="n">
         <v>0.544243253516201</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="10" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>20360100057</v>
+      </c>
+      <c r="C29" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.544243253516201</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="11" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>20250100039</v>
-      </c>
-      <c r="C10" t="n">
-        <v>25000</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.5778109865150957</v>
-      </c>
-      <c r="E10" t="inlineStr">
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="10" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>20350300037</v>
+      </c>
+      <c r="C30" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.5469644697837819</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="10" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>20340200026</v>
+      </c>
+      <c r="C31" t="n">
+        <v>2400</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.5496992921327007</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="10" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>20340300036</v>
+      </c>
+      <c r="C32" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.5496992921327007</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="10" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>20340100056</v>
+      </c>
+      <c r="C33" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.5496992921327007</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>WindOff</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="10" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>20330300035</v>
+      </c>
+      <c r="C34" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.5524477885933642</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="10" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>20320300034</v>
+      </c>
+      <c r="C35" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.555210027536331</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="10" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>20320100055</v>
+      </c>
+      <c r="C36" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.555210027536331</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="10" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>20310300033</v>
+      </c>
+      <c r="C37" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.5579860776740125</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="10" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>20300200025</v>
+      </c>
+      <c r="C38" t="n">
+        <v>2400</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.5607760080623826</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>WindOn</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="10" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>20300100054</v>
+      </c>
+      <c r="C39" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.5607760080623826</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="10" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>20290300032</v>
+      </c>
+      <c r="C40" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.5635798881026944</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>OtherPV</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="10" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>20280100053</v>
+      </c>
+      <c r="C41" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.5663977875432078</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="10" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>20260100052</v>
+      </c>
+      <c r="C42" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.5720759253633284</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>WindOff</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
         <is>
           <t>-</t>
         </is>
@@ -3165,39 +4462,39 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>ElectrolyserType</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>PeakConsumptionInMW</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>ConversionFactor</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>HydrogenProductionTargetInMWH</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>PriceLimitOverrideInEURperMWH</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="10" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
@@ -3215,7 +4512,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>3166666</v>
+        <v>4297995</v>
       </c>
       <c r="G2" t="n">
         <v>60.40312774153847</v>
@@ -3232,7 +4529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3241,49 +4538,49 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>identifier</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>StorageType</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>EnergyToPowerRatio</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>ChargingEfficiency</t>
         </is>
       </c>
-      <c r="F1" s="11" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>DischargingEfficiency</t>
         </is>
       </c>
-      <c r="G1" s="11" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>InitialEnergyLevelInMWH</t>
         </is>
       </c>
-      <c r="H1" s="11" t="inlineStr">
+      <c r="H1" s="10" t="inlineStr">
         <is>
           <t>InstalledPowerInMW</t>
         </is>
       </c>
-      <c r="I1" s="11" t="inlineStr">
+      <c r="I1" s="10" t="inlineStr">
         <is>
           <t>Strategist</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="n">
+      <c r="A2" s="10" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
@@ -3310,39 +4607,6 @@
         <v>1</v>
       </c>
       <c r="I2" t="inlineStr">
-        <is>
-          <t>MULTI_AGENT_MEDIAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>20502600043</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>STORAGE</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>2000</v>
-      </c>
-      <c r="I3" t="inlineStr">
         <is>
           <t>MULTI_AGENT_MEDIAN</t>
         </is>

</xml_diff>

<commit_message>
Define strike price for revenue obligations per plant (conventionals or res)
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TradeRES\toolbox-amiris-emlab-new\toolbox-amiris-emlab\amiris_workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370B62AB-AEFB-4C59-9ACE-6849A5A2CB18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9138A9B-3A0B-4DBB-9C50-147E5504FB12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-16515" windowWidth="29040" windowHeight="15840" tabRatio="880" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-16515" windowWidth="29040" windowHeight="15840" tabRatio="880" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_skeleton" sheetId="1" r:id="rId1"/>
@@ -28,17 +28,16 @@
     <sheet name="load_shedding(notactive)" sheetId="13" r:id="rId13"/>
     <sheet name="load_shedding" sheetId="14" r:id="rId14"/>
     <sheet name="times" sheetId="15" r:id="rId15"/>
-    <sheet name="capacity_remuneration" sheetId="16" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">renewables_full!$A$1:$I$60</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="110">
   <si>
     <t>group</t>
   </si>
@@ -438,7 +437,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -509,12 +508,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
@@ -535,6 +545,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1187,13 +1200,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="B1:I1"/>
+  <dimension ref="B1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>60</v>
       </c>
@@ -1217,6 +1232,9 @@
       </c>
       <c r="I1" s="8" t="s">
         <v>71</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1507,7 +1525,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1534,29 +1554,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFD3275-39F2-44A7-AE7F-B90340B7D360}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B1">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1731,13 +1728,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>60</v>
       </c>
@@ -1756,8 +1758,11 @@
       <c r="G1" s="8" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1779,8 +1784,11 @@
       <c r="G2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -1802,8 +1810,11 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -1825,8 +1836,11 @@
       <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -1848,8 +1862,11 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>0</v>
       </c>
@@ -1871,8 +1888,11 @@
       <c r="G6">
         <v>1000</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>18</v>
       </c>
@@ -1894,8 +1914,11 @@
       <c r="G7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>17</v>
       </c>
@@ -1917,8 +1940,11 @@
       <c r="G8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>16</v>
       </c>
@@ -1940,8 +1966,11 @@
       <c r="G9">
         <v>1000</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>15</v>
       </c>
@@ -1963,8 +1992,11 @@
       <c r="G10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>13</v>
       </c>
@@ -1986,8 +2018,11 @@
       <c r="G11">
         <v>1000</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>12</v>
       </c>
@@ -2009,8 +2044,11 @@
       <c r="G12">
         <v>1000</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>10</v>
       </c>
@@ -2032,8 +2070,11 @@
       <c r="G13">
         <v>1000</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>9</v>
       </c>
@@ -2055,8 +2096,11 @@
       <c r="G14">
         <v>1000</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>8</v>
       </c>
@@ -2078,8 +2122,11 @@
       <c r="G15">
         <v>1000</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>7</v>
       </c>
@@ -2101,8 +2148,11 @@
       <c r="G16">
         <v>1000</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>6</v>
       </c>
@@ -2124,8 +2174,11 @@
       <c r="G17">
         <v>1000</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>5</v>
       </c>
@@ -2148,7 +2201,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>20</v>
       </c>
@@ -2171,7 +2224,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -2194,7 +2247,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>14</v>
       </c>
@@ -2217,7 +2270,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>11</v>
       </c>
@@ -2622,13 +2675,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>60</v>
       </c>
@@ -2653,8 +2708,11 @@
       <c r="I1" s="8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>0</v>
       </c>
@@ -2682,8 +2740,11 @@
       <c r="I2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -2711,8 +2772,11 @@
       <c r="I3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -2740,8 +2804,11 @@
       <c r="I4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -2769,8 +2836,11 @@
       <c r="I5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -2798,8 +2868,11 @@
       <c r="I6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -2828,7 +2901,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -2857,7 +2930,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -2886,7 +2959,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -2915,7 +2988,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -2944,7 +3017,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -2973,7 +3046,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -3002,7 +3075,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -3031,7 +3104,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -3060,7 +3133,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
last files to add in this branch
</commit_message>
<xml_diff>
--- a/amiris_workflow/amiris_data_structure.xlsx
+++ b/amiris_workflow/amiris_data_structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TradeRES\toolbox-amiris-emlab-new\toolbox-amiris-emlab\amiris_workflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\amiris_workflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9378B1-DBA9-44EA-8ADC-C9F8222D2EBF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8B9A95-B6B9-483C-B19C-4EB10296BCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_skeleton" sheetId="1" r:id="rId1"/>
@@ -33,11 +33,24 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">renewables_full!$A$1:$I$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="108">
   <si>
     <t>group</t>
   </si>
@@ -258,18 +271,18 @@
     <t>Lcoe</t>
   </si>
   <si>
+    <t>WindOff</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>OtherPV</t>
   </si>
   <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>WindOff</t>
-  </si>
-  <si>
     <t>WindOn</t>
   </si>
   <si>
@@ -345,22 +358,22 @@
     <t>amiris-config/data/demand_processed/ind_cluster-2_shedding_timeseries.csv</t>
   </si>
   <si>
-    <t>amiris-config/data/LS_3.csv</t>
-  </si>
-  <si>
-    <t>amiris-config/data/LS_2.csv</t>
-  </si>
-  <si>
-    <t>amiris-config/data/LS_1.csv</t>
-  </si>
-  <si>
-    <t>amiris-config/data/LS_hydrogen.csv</t>
+    <t>amiris-config/data/future_LS_2.csv</t>
+  </si>
+  <si>
+    <t>amiris-config/data/future_LS_1.csv</t>
+  </si>
+  <si>
+    <t>amiris-config/data/future_LS_hydrogen.csv</t>
   </si>
   <si>
     <t>StartTime</t>
   </si>
   <si>
     <t>StopTime</t>
+  </si>
+  <si>
+    <t>storage</t>
   </si>
 </sst>
 </file>
@@ -370,7 +383,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,11 +430,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -436,7 +444,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -499,17 +507,6 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -523,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
@@ -540,17 +537,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -868,7 +862,7 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
@@ -1191,7 +1185,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1203,31 +1197,31 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1244,7 +1238,7 @@
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
@@ -1322,10 +1316,10 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
@@ -1420,29 +1414,29 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>300000</v>
+        <v>200000</v>
       </c>
       <c r="B2" t="s">
         <v>95</v>
@@ -1456,13 +1450,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="B3" t="s">
         <v>95</v>
       </c>
       <c r="C3">
-        <v>4000</v>
+        <v>4001</v>
       </c>
       <c r="D3" t="s">
         <v>103</v>
@@ -1470,30 +1464,16 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>100000</v>
+        <v>8888888</v>
       </c>
       <c r="B4" t="s">
         <v>95</v>
       </c>
       <c r="C4">
-        <v>4001</v>
+        <v>33.351799999999614</v>
       </c>
       <c r="D4" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>8888888</v>
-      </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5">
-        <v>33.351799999999614</v>
-      </c>
-      <c r="D5" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1507,27 +1487,27 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="8">
+      <c r="B1" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="8">
+        <v>54788.998611111107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="9">
-        <v>56614.998611111107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3" s="9">
-        <v>56978.998611111107</v>
+      <c r="B3" s="8">
+        <v>55152.998611111107</v>
       </c>
     </row>
   </sheetData>
@@ -1543,7 +1523,7 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -1616,56 +1596,56 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2">
-        <v>168</v>
+        <v>204.2781719838913</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1706,52 +1686,52 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>1</v>
+      <c r="A2" s="9">
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>20490100069</v>
+        <v>99990800003</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D2">
-        <v>2.6789815244237891</v>
+        <v>4.24</v>
       </c>
       <c r="E2">
-        <v>0.309</v>
+        <v>0.6</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1759,42 +1739,36 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2">
-        <v>50</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>8</v>
+      <c r="A3" s="9">
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>20351200031</v>
+        <v>99990100006</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D3">
-        <v>3.8671345201535492</v>
+        <v>1.83</v>
       </c>
       <c r="E3">
-        <v>0.35</v>
+        <v>0.309</v>
       </c>
       <c r="F3">
-        <v>400</v>
+        <v>1</v>
       </c>
       <c r="G3">
-        <v>400</v>
-      </c>
-      <c r="H3">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>0</v>
+      <c r="A4" s="9">
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>20550700100</v>
+        <v>99990700007</v>
       </c>
       <c r="C4" t="s">
         <v>53</v>
@@ -1806,212 +1780,516 @@
         <v>0.43</v>
       </c>
       <c r="F4">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>2000</v>
-      </c>
-      <c r="H4">
-        <v>150</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>2</v>
+      <c r="A5" s="9">
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>20480800030</v>
+        <v>20490100021</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5">
-        <v>4.3906446430287112</v>
+        <v>1.8318300000000001</v>
       </c>
       <c r="E5">
-        <v>0.6</v>
+        <v>0.309</v>
       </c>
       <c r="F5">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>2000</v>
-      </c>
-      <c r="H5">
-        <v>200</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>3</v>
+      <c r="A6" s="9">
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>20470700029</v>
+        <v>20351200052</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D6">
-        <v>4.984986740402845</v>
+        <v>3.5528690972880219</v>
       </c>
       <c r="E6">
-        <v>0.43</v>
+        <v>0.35</v>
       </c>
       <c r="F6">
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="G6">
-        <v>2000</v>
-      </c>
-      <c r="H6">
-        <v>250</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>4</v>
+      <c r="A7" s="9">
+        <v>22</v>
       </c>
       <c r="B7">
-        <v>20450700028</v>
+        <v>20300700025</v>
       </c>
       <c r="C7" t="s">
         <v>53</v>
       </c>
       <c r="D7">
-        <v>5.0349612324753821</v>
+        <v>4.8867155838819896</v>
       </c>
       <c r="E7">
         <v>0.43</v>
       </c>
       <c r="F7">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G7">
-        <v>2000</v>
-      </c>
-      <c r="H7">
-        <v>300</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>5</v>
+      <c r="A8" s="9">
+        <v>21</v>
       </c>
       <c r="B8">
-        <v>20430700027</v>
+        <v>20300800023</v>
       </c>
       <c r="C8" t="s">
         <v>53</v>
       </c>
       <c r="D8">
-        <v>5.0854367188309464</v>
+        <v>4.3256104542086922</v>
       </c>
       <c r="E8">
-        <v>0.43</v>
+        <v>0.6</v>
       </c>
       <c r="F8">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G8">
-        <v>2000</v>
-      </c>
-      <c r="H8">
-        <v>350</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>6</v>
+      <c r="A9" s="9">
+        <v>20</v>
       </c>
       <c r="B9">
-        <v>20400700026</v>
+        <v>20310700035</v>
       </c>
       <c r="C9" t="s">
         <v>53</v>
       </c>
       <c r="D9">
-        <v>5.1621003130469116</v>
+        <v>4.8818337501318583</v>
       </c>
       <c r="E9">
         <v>0.43</v>
       </c>
       <c r="F9">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G9">
-        <v>2000</v>
-      </c>
-      <c r="H9">
-        <v>400</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>7</v>
+      <c r="A10" s="9">
+        <v>19</v>
       </c>
       <c r="B10">
-        <v>20370700025</v>
+        <v>20310700033</v>
       </c>
       <c r="C10" t="s">
         <v>53</v>
       </c>
       <c r="D10">
-        <v>5.2399196205286307</v>
+        <v>4.8818337501318583</v>
       </c>
       <c r="E10">
         <v>0.43</v>
       </c>
       <c r="F10">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G10">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
-        <v>9</v>
+      <c r="A11" s="9">
+        <v>18</v>
       </c>
       <c r="B11">
-        <v>20340700024</v>
+        <v>20340700027</v>
       </c>
       <c r="C11" t="s">
         <v>53</v>
       </c>
       <c r="D11">
-        <v>5.3189120637980496</v>
+        <v>4.8672174911387529</v>
       </c>
       <c r="E11">
         <v>0.43</v>
       </c>
       <c r="F11">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G11">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
-        <v>10</v>
+      <c r="A12" s="9">
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>20320700023</v>
+        <v>20350700037</v>
       </c>
       <c r="C12" t="s">
         <v>53</v>
       </c>
       <c r="D12">
-        <v>5.3722341572376253</v>
+        <v>4.8623551360027504</v>
       </c>
       <c r="E12">
         <v>0.43</v>
       </c>
       <c r="F12">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="G12">
-        <v>2000</v>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>20350800022</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13">
+        <v>4.3040471350003484</v>
+      </c>
+      <c r="E13">
+        <v>0.6</v>
+      </c>
+      <c r="F13">
+        <v>1000</v>
+      </c>
+      <c r="G13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>20370700028</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14">
+        <v>4.8526449933710163</v>
+      </c>
+      <c r="E14">
+        <v>0.43</v>
+      </c>
+      <c r="F14">
+        <v>1000</v>
+      </c>
+      <c r="G14">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>20400700029</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15">
+        <v>4.8381161258071028</v>
+      </c>
+      <c r="E15">
+        <v>0.43</v>
+      </c>
+      <c r="F15">
+        <v>1000</v>
+      </c>
+      <c r="G15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>20280700034</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16">
+        <v>4.8964939017653357</v>
+      </c>
+      <c r="E16">
+        <v>0.43</v>
+      </c>
+      <c r="F16">
+        <v>1000</v>
+      </c>
+      <c r="G16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>20410700039</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17">
+        <v>4.833282842964139</v>
+      </c>
+      <c r="E17">
+        <v>0.43</v>
+      </c>
+      <c r="F17">
+        <v>1000</v>
+      </c>
+      <c r="G17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>20430700030</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18">
+        <v>4.8236307578177469</v>
+      </c>
+      <c r="E18">
+        <v>0.43</v>
+      </c>
+      <c r="F18">
+        <v>1000</v>
+      </c>
+      <c r="G18">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>20440700040</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19">
+        <v>4.8188119458718752</v>
+      </c>
+      <c r="E19">
+        <v>0.43</v>
+      </c>
+      <c r="F19">
+        <v>1000</v>
+      </c>
+      <c r="G19">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>20450700031</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20">
+        <v>4.8139979479239514</v>
+      </c>
+      <c r="E20">
+        <v>0.43</v>
+      </c>
+      <c r="F20">
+        <v>1000</v>
+      </c>
+      <c r="G20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>20460700041</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21">
+        <v>4.8091887591647877</v>
+      </c>
+      <c r="E21">
+        <v>0.43</v>
+      </c>
+      <c r="F21">
+        <v>1000</v>
+      </c>
+      <c r="G21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>20470700032</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22">
+        <v>4.8043843747899988</v>
+      </c>
+      <c r="E22">
+        <v>0.43</v>
+      </c>
+      <c r="F22">
+        <v>1000</v>
+      </c>
+      <c r="G22">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>20490700026</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23">
+        <v>4.7947899999999999</v>
+      </c>
+      <c r="E23">
+        <v>0.43</v>
+      </c>
+      <c r="F23">
+        <v>1000</v>
+      </c>
+      <c r="G23">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>20500700036</v>
+      </c>
+      <c r="C24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24">
+        <v>4.79</v>
+      </c>
+      <c r="E24">
+        <v>0.43</v>
+      </c>
+      <c r="F24">
+        <v>1000</v>
+      </c>
+      <c r="G24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>20380700038</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25">
+        <v>4.8477971961748416</v>
+      </c>
+      <c r="E25">
+        <v>0.43</v>
+      </c>
+      <c r="F25">
+        <v>1000</v>
+      </c>
+      <c r="G25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>20270700024</v>
+      </c>
+      <c r="C26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26">
+        <v>4.9013903956671019</v>
+      </c>
+      <c r="E26">
+        <v>0.43</v>
+      </c>
+      <c r="F26">
+        <v>1000</v>
+      </c>
+      <c r="G26">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -2021,27 +2299,62 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="B1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <f>SUM(conventionals!G:G,renewables_full!C:C,biogas_full!C:C)</f>
-        <v>18401</v>
-      </c>
-      <c r="B1">
-        <f>A1/1000</f>
-        <v>18.401</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1">
+        <f>SUM(conventionals!G:G,)</f>
+        <v>20404</v>
+      </c>
+      <c r="D1">
+        <f>C1/1000</f>
+        <v>20.404</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2">
+        <f>SUM(renewables!C:C)</f>
+        <v>120003</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D3" si="0">C2/1000</f>
+        <v>120.003</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3">
+        <f>SUM(storages!H:H)</f>
+        <v>10002</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>10.002000000000001</v>
+      </c>
+      <c r="E3" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2058,7 +2371,7 @@
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
@@ -2396,53 +2709,53 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>20531600096</v>
+        <v>99991800002</v>
       </c>
       <c r="C2">
-        <v>2400</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0.50501249999999986</v>
+        <v>3.25</v>
       </c>
       <c r="E2" t="s">
         <v>73</v>
@@ -2461,17 +2774,17 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>20531800090</v>
+        <v>99991600004</v>
       </c>
       <c r="C3">
-        <v>500</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0.50501249999999986</v>
+        <v>0.5</v>
       </c>
       <c r="E3" t="s">
         <v>76</v>
@@ -2490,17 +2803,17 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>20531900097</v>
+        <v>99991900005</v>
       </c>
       <c r="C4">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>2.020049999999999</v>
+        <v>1.3</v>
       </c>
       <c r="E4" t="s">
         <v>77</v>
@@ -2519,20 +2832,20 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>20521600084</v>
+        <v>20491600053</v>
       </c>
       <c r="C5">
-        <v>3400</v>
+        <v>3000</v>
       </c>
       <c r="D5">
-        <v>0.50753756249999982</v>
+        <v>0.50049999999999994</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F5" t="s">
         <v>74</v>
@@ -2548,20 +2861,20 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>20511600079</v>
+        <v>20481600054</v>
       </c>
       <c r="C6">
-        <v>2400</v>
+        <v>3000</v>
       </c>
       <c r="D6">
-        <v>0.51007525031249978</v>
+        <v>0.50100049999999985</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
         <v>74</v>
@@ -2577,17 +2890,17 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>20501600075</v>
+        <v>20481800089</v>
       </c>
       <c r="C7">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="D7">
-        <v>0.51262562656406219</v>
+        <v>3.2565032499999989</v>
       </c>
       <c r="E7" t="s">
         <v>73</v>
@@ -2606,20 +2919,20 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>20481800063</v>
+        <v>20481900094</v>
       </c>
       <c r="C8">
-        <v>4000</v>
+        <v>2400</v>
       </c>
       <c r="D8">
-        <v>0.51776469847036688</v>
+        <v>1.3026013000000001</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F8" t="s">
         <v>74</v>
@@ -2635,20 +2948,20 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>20481900068</v>
+        <v>20471600055</v>
       </c>
       <c r="C9">
-        <v>2400</v>
+        <v>3000</v>
       </c>
       <c r="D9">
-        <v>2.071058793881468</v>
+        <v>0.50150150049999986</v>
       </c>
       <c r="E9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F9" t="s">
         <v>74</v>
@@ -2664,20 +2977,20 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>20471600051</v>
+        <v>20461600056</v>
       </c>
       <c r="C10">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D10">
-        <v>0.52035352196271867</v>
+        <v>0.50200300200049974</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
         <v>74</v>
@@ -2693,20 +3006,20 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="9">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>20471800062</v>
+        <v>20461800088</v>
       </c>
       <c r="C11">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D11">
-        <v>0.52035352196271867</v>
+        <v>3.2630195130032482</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F11" t="s">
         <v>74</v>
@@ -2722,20 +3035,20 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="9">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>20461600050</v>
+        <v>20451600057</v>
       </c>
       <c r="C12">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D12">
-        <v>0.52295528957253212</v>
+        <v>0.50250500500250017</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
         <v>74</v>
@@ -2751,17 +3064,17 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="9">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>20461800061</v>
+        <v>20441600059</v>
       </c>
       <c r="C13">
         <v>3000</v>
       </c>
       <c r="D13">
-        <v>0.52295528957253212</v>
+        <v>0.50300751000750266</v>
       </c>
       <c r="E13" t="s">
         <v>76</v>
@@ -2780,17 +3093,17 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="9">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>20451600049</v>
+        <v>20441800087</v>
       </c>
       <c r="C14">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D14">
-        <v>0.5255700660203948</v>
+        <v>3.269548815048767</v>
       </c>
       <c r="E14" t="s">
         <v>73</v>
@@ -2809,20 +3122,20 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="9">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>20441600048</v>
+        <v>20431600060</v>
       </c>
       <c r="C15">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D15">
-        <v>0.52819791635049673</v>
+        <v>0.50351051751751008</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F15" t="s">
         <v>74</v>
@@ -2838,20 +3151,20 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="9">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>20441800060</v>
+        <v>20431900093</v>
       </c>
       <c r="C16">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="D16">
-        <v>0.52819791635049673</v>
+        <v>1.3091273455455259</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
         <v>74</v>
@@ -2867,20 +3180,20 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="9">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>20431600047</v>
+        <v>20421600061</v>
       </c>
       <c r="C17">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D17">
-        <v>0.53083890593224914</v>
+        <v>0.50401402803502759</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F17" t="s">
         <v>74</v>
@@ -2896,20 +3209,20 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="9">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>20431900067</v>
+        <v>20411600063</v>
       </c>
       <c r="C18">
-        <v>2400</v>
+        <v>3000</v>
       </c>
       <c r="D18">
-        <v>2.123355623728997</v>
+        <v>0.5045180420630625</v>
       </c>
       <c r="E18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F18" t="s">
         <v>74</v>
@@ -2925,20 +3238,20 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="9">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>20421600046</v>
+        <v>20401600064</v>
       </c>
       <c r="C19">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D19">
-        <v>0.53349310046191034</v>
+        <v>0.50502256010512558</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F19" t="s">
         <v>74</v>
@@ -2954,20 +3267,20 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="9">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>20421800059</v>
+        <v>20401800086</v>
       </c>
       <c r="C20">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D20">
-        <v>0.53349310046191034</v>
+        <v>3.2826466406833159</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F20" t="s">
         <v>74</v>
@@ -2983,20 +3296,20 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="9">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>20411600045</v>
+        <v>20391600065</v>
       </c>
       <c r="C21">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D21">
-        <v>0.53616056596421979</v>
+        <v>0.50552758266523057</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F21" t="s">
         <v>74</v>
@@ -3012,20 +3325,20 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="9">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>20401600044</v>
+        <v>20381600066</v>
       </c>
       <c r="C22">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D22">
-        <v>0.53884136879404088</v>
+        <v>0.50603311024789577</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F22" t="s">
         <v>74</v>
@@ -3041,20 +3354,20 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="9">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>20401800058</v>
+        <v>20381800085</v>
       </c>
       <c r="C23">
         <v>3000</v>
       </c>
       <c r="D23">
-        <v>0.53884136879404088</v>
+        <v>3.2892152166113231</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
         <v>74</v>
@@ -3070,20 +3383,20 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="A24" s="9">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>20391600043</v>
+        <v>20371600067</v>
       </c>
       <c r="C24">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D24">
-        <v>0.54153557563801102</v>
+        <v>0.50653914335814365</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F24" t="s">
         <v>74</v>
@@ -3099,20 +3412,20 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+      <c r="A25" s="9">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>20381600042</v>
+        <v>20361600068</v>
       </c>
       <c r="C25">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D25">
-        <v>0.54424325351620095</v>
+        <v>0.50704568250150173</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F25" t="s">
         <v>74</v>
@@ -3128,17 +3441,17 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="A26" s="9">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>20371600041</v>
+        <v>20361800084</v>
       </c>
       <c r="C26">
         <v>3000</v>
       </c>
       <c r="D26">
-        <v>0.54696446978378188</v>
+        <v>3.295796936259761</v>
       </c>
       <c r="E26" t="s">
         <v>73</v>
@@ -3157,20 +3470,20 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="9">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>20361600040</v>
+        <v>20351600069</v>
       </c>
       <c r="C27">
         <v>3000</v>
       </c>
       <c r="D27">
-        <v>0.54969929213270075</v>
+        <v>0.50755272818400321</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F27" t="s">
         <v>74</v>
@@ -3186,17 +3499,17 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+      <c r="A28" s="9">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>20361800057</v>
+        <v>20341600070</v>
       </c>
       <c r="C28">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D28">
-        <v>0.54969929213270075</v>
+        <v>0.50806028091218713</v>
       </c>
       <c r="E28" t="s">
         <v>76</v>
@@ -3215,20 +3528,20 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
+      <c r="A29" s="9">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>20351600039</v>
+        <v>20341900092</v>
       </c>
       <c r="C29">
-        <v>3000</v>
+        <v>2400</v>
       </c>
       <c r="D29">
-        <v>0.55244778859336419</v>
+        <v>1.3209567303716869</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F29" t="s">
         <v>74</v>
@@ -3244,20 +3557,20 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="9">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>20341600038</v>
+        <v>20331600071</v>
       </c>
       <c r="C30">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D30">
-        <v>0.55521002753633097</v>
+        <v>0.50856834119309924</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F30" t="s">
         <v>74</v>
@@ -3273,20 +3586,20 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="A31" s="9">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>20341800056</v>
+        <v>20331800083</v>
       </c>
       <c r="C31">
         <v>3000</v>
       </c>
       <c r="D31">
-        <v>0.55521002753633097</v>
+        <v>3.3056942177551449</v>
       </c>
       <c r="E31" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F31" t="s">
         <v>74</v>
@@ -3302,20 +3615,20 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="9">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>20341900066</v>
+        <v>20321600072</v>
       </c>
       <c r="C32">
-        <v>2400</v>
+        <v>3000</v>
       </c>
       <c r="D32">
-        <v>2.2208401101453239</v>
+        <v>0.5090769095342923</v>
       </c>
       <c r="E32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F32" t="s">
         <v>74</v>
@@ -3331,20 +3644,20 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="A33" s="9">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>20331600037</v>
+        <v>20311600073</v>
       </c>
       <c r="C33">
         <v>3000</v>
       </c>
       <c r="D33">
-        <v>0.55798607767401254</v>
+        <v>0.50958598644382658</v>
       </c>
       <c r="E33" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F33" t="s">
         <v>74</v>
@@ -3360,17 +3673,17 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
+      <c r="A34" s="9">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>20321600036</v>
+        <v>20311800082</v>
       </c>
       <c r="C34">
         <v>3000</v>
       </c>
       <c r="D34">
-        <v>0.56077600806238259</v>
+        <v>3.3123089118848732</v>
       </c>
       <c r="E34" t="s">
         <v>73</v>
@@ -3389,17 +3702,17 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+      <c r="A35" s="9">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>20321800055</v>
+        <v>20301600062</v>
       </c>
       <c r="C35">
         <v>3000</v>
       </c>
       <c r="D35">
-        <v>0.56077600806238259</v>
+        <v>0.51009557243027026</v>
       </c>
       <c r="E35" t="s">
         <v>76</v>
@@ -3418,20 +3731,20 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+      <c r="A36" s="9">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>20311600035</v>
+        <v>20291600074</v>
       </c>
       <c r="C36">
         <v>3000</v>
       </c>
       <c r="D36">
-        <v>0.56357988810269444</v>
+        <v>0.51060566800270046</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F36" t="s">
         <v>74</v>
@@ -3447,17 +3760,17 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="8">
+      <c r="A37" s="9">
         <v>35</v>
       </c>
       <c r="B37">
-        <v>20291600034</v>
+        <v>20291800081</v>
       </c>
       <c r="C37">
         <v>3000</v>
       </c>
       <c r="D37">
-        <v>0.56922977648092388</v>
+        <v>3.3189368420175529</v>
       </c>
       <c r="E37" t="s">
         <v>73</v>
@@ -3476,17 +3789,17 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+      <c r="A38" s="9">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>20291800054</v>
+        <v>20281600075</v>
       </c>
       <c r="C38">
         <v>3000</v>
       </c>
       <c r="D38">
-        <v>0.56922977648092388</v>
+        <v>0.51111627367070311</v>
       </c>
       <c r="E38" t="s">
         <v>76</v>
@@ -3505,17 +3818,17 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
+      <c r="A39" s="9">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>20281900065</v>
+        <v>20281900091</v>
       </c>
       <c r="C39">
         <v>2400</v>
       </c>
       <c r="D39">
-        <v>2.2883037014533141</v>
+        <v>1.3289023115438281</v>
       </c>
       <c r="E39" t="s">
         <v>77</v>
@@ -3534,17 +3847,17 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
+      <c r="A40" s="9">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>20241800053</v>
+        <v>20271600076</v>
       </c>
       <c r="C40">
         <v>3000</v>
       </c>
       <c r="D40">
-        <v>0.58360354165490935</v>
+        <v>0.51162738994437384</v>
       </c>
       <c r="E40" t="s">
         <v>76</v>
@@ -3559,6 +3872,180 @@
         <v>75</v>
       </c>
       <c r="I40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>20271800080</v>
+      </c>
+      <c r="C41">
+        <v>3000</v>
+      </c>
+      <c r="D41">
+        <v>3.32557803463843</v>
+      </c>
+      <c r="E41" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" t="s">
+        <v>74</v>
+      </c>
+      <c r="G41" t="s">
+        <v>75</v>
+      </c>
+      <c r="H41" t="s">
+        <v>75</v>
+      </c>
+      <c r="I41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>20261600058</v>
+      </c>
+      <c r="C42">
+        <v>3000</v>
+      </c>
+      <c r="D42">
+        <v>0.5121390173343181</v>
+      </c>
+      <c r="E42" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" t="s">
+        <v>74</v>
+      </c>
+      <c r="G42" t="s">
+        <v>75</v>
+      </c>
+      <c r="H42" t="s">
+        <v>75</v>
+      </c>
+      <c r="I42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>20251800079</v>
+      </c>
+      <c r="C43">
+        <v>3000</v>
+      </c>
+      <c r="D43">
+        <v>3.3322325162857398</v>
+      </c>
+      <c r="E43" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" t="s">
+        <v>74</v>
+      </c>
+      <c r="G43" t="s">
+        <v>75</v>
+      </c>
+      <c r="H43" t="s">
+        <v>75</v>
+      </c>
+      <c r="I43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>20231800078</v>
+      </c>
+      <c r="C44">
+        <v>3000</v>
+      </c>
+      <c r="D44">
+        <v>3.3389003135508282</v>
+      </c>
+      <c r="E44" t="s">
+        <v>73</v>
+      </c>
+      <c r="F44" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" t="s">
+        <v>75</v>
+      </c>
+      <c r="H44" t="s">
+        <v>75</v>
+      </c>
+      <c r="I44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>20231900090</v>
+      </c>
+      <c r="C45">
+        <v>2400</v>
+      </c>
+      <c r="D45">
+        <v>1.3355601254203311</v>
+      </c>
+      <c r="E45" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H45" t="s">
+        <v>75</v>
+      </c>
+      <c r="I45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>20211800077</v>
+      </c>
+      <c r="C46">
+        <v>3000</v>
+      </c>
+      <c r="D46">
+        <v>3.3455814530782422</v>
+      </c>
+      <c r="E46" t="s">
+        <v>73</v>
+      </c>
+      <c r="F46" t="s">
+        <v>74</v>
+      </c>
+      <c r="G46" t="s">
+        <v>75</v>
+      </c>
+      <c r="H46" t="s">
+        <v>75</v>
+      </c>
+      <c r="I46" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3573,30 +4060,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
       <c r="B2">
@@ -3615,7 +4102,7 @@
         <v>3063080</v>
       </c>
       <c r="G2">
-        <v>60.657940606042168</v>
+        <v>67.702876905382652</v>
       </c>
     </row>
   </sheetData>
@@ -3625,61 +4112,56 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="9">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>20481100074</v>
+        <v>99991100001</v>
       </c>
       <c r="C2" t="s">
         <v>90</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>117.76</v>
+        <v>0.92</v>
       </c>
       <c r="F2">
         <v>0.92</v>
@@ -3688,18 +4170,18 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>20451100073</v>
+        <v>99991100008</v>
       </c>
       <c r="C3" t="s">
         <v>90</v>
@@ -3708,7 +4190,7 @@
         <v>4</v>
       </c>
       <c r="E3">
-        <v>942.08</v>
+        <v>0.92</v>
       </c>
       <c r="F3">
         <v>0.92</v>
@@ -3717,18 +4199,18 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>2000</v>
+        <v>1</v>
       </c>
       <c r="I3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>20401100072</v>
+        <v>20491100051</v>
       </c>
       <c r="C4" t="s">
         <v>90</v>
@@ -3737,7 +4219,7 @@
         <v>4</v>
       </c>
       <c r="E4">
-        <v>30146.560000000001</v>
+        <v>0.92</v>
       </c>
       <c r="F4">
         <v>0.92</v>
@@ -3746,18 +4228,18 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>20351100071</v>
+        <v>20471100050</v>
       </c>
       <c r="C5" t="s">
         <v>90</v>
@@ -3766,7 +4248,7 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>964689.92000000004</v>
+        <v>0.92</v>
       </c>
       <c r="F5">
         <v>0.92</v>
@@ -3775,9 +4257,241 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>20441100049</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>0.92</v>
+      </c>
+      <c r="F6">
+        <v>0.92</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>1000</v>
+      </c>
+      <c r="I6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>20411100048</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>0.92</v>
+      </c>
+      <c r="F7">
+        <v>0.92</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>1000</v>
+      </c>
+      <c r="I7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>20381100047</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>0.92</v>
+      </c>
+      <c r="F8">
+        <v>0.92</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1000</v>
+      </c>
+      <c r="I8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>20351100046</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>0.92</v>
+      </c>
+      <c r="F9">
+        <v>0.92</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1000</v>
+      </c>
+      <c r="I9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>20321100045</v>
+      </c>
+      <c r="C10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>0.92</v>
+      </c>
+      <c r="F10">
+        <v>0.92</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1000</v>
+      </c>
+      <c r="I10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>20291100044</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0.92</v>
+      </c>
+      <c r="F11">
+        <v>0.92</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1000</v>
+      </c>
+      <c r="I11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>20271100043</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>0.92</v>
+      </c>
+      <c r="F12">
+        <v>0.92</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1000</v>
+      </c>
+      <c r="I12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>20261100042</v>
+      </c>
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>0.92</v>
+      </c>
+      <c r="F13">
+        <v>0.92</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1000</v>
+      </c>
+      <c r="I13" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>